<commit_message>
everything seems to run ok
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="0" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="3380" yWindow="3980" windowWidth="19420" windowHeight="10960" tabRatio="901" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="132">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -504,7 +504,10 @@
     <t>People who inject drugs</t>
   </si>
   <si>
-    <t>Births and aging</t>
+    <t>Births</t>
+  </si>
+  <si>
+    <t>Aging</t>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="256">
+  <cellStyleXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -871,6 +874,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1116,7 +1121,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="256">
+  <cellStyles count="258">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="4"/>
@@ -1225,6 +1230,7 @@
     <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="79"/>
     <cellStyle name="Followed Hyperlink 11" xfId="80"/>
     <cellStyle name="Followed Hyperlink 12" xfId="81"/>
@@ -1366,6 +1372,7 @@
     <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="7"/>
     <cellStyle name="Normal 3" xfId="8"/>
@@ -2523,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3227,8 +3234,8 @@
     </row>
     <row r="56" spans="1:10" s="53" customFormat="1">
       <c r="B56" s="3" t="str">
-        <f>Populations!$C$4</f>
-        <v>Clients</v>
+        <f>Populations!$C$8</f>
+        <v>F 0-14</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -3241,142 +3248,140 @@
     </row>
     <row r="57" spans="1:10" s="53" customFormat="1">
       <c r="B57" s="3" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
+        <f>Populations!$C$10</f>
+        <v>F 15+</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
+      <c r="G57" s="4">
+        <v>1</v>
+      </c>
+      <c r="H57" s="4">
+        <v>1</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" s="53" customFormat="1">
-      <c r="B58" s="3" t="str">
+    <row r="58" spans="1:10" s="53" customFormat="1"/>
+    <row r="59" spans="1:10" s="53" customFormat="1"/>
+    <row r="60" spans="1:10" s="53" customFormat="1"/>
+    <row r="61" spans="1:10" s="53" customFormat="1">
+      <c r="A61" s="54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="53" customFormat="1">
+      <c r="C62" s="3" t="str">
+        <f>Populations!$C$3</f>
+        <v>FSW</v>
+      </c>
+      <c r="D62" s="3" t="str">
+        <f>Populations!$C$4</f>
+        <v>Clients</v>
+      </c>
+      <c r="E62" s="3" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
+      </c>
+      <c r="F62" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-    </row>
-    <row r="59" spans="1:10" s="53" customFormat="1">
-      <c r="B59" s="3" t="str">
+      <c r="G62" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4">
-        <v>1</v>
-      </c>
-      <c r="J59" s="4"/>
-    </row>
-    <row r="60" spans="1:10" s="53" customFormat="1">
-      <c r="B60" s="3" t="str">
+      <c r="H62" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="53" customFormat="1">
-      <c r="B61" s="3" t="str">
+      <c r="I62" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-    </row>
-    <row r="62" spans="1:10" s="53" customFormat="1">
-      <c r="B62" s="3" t="str">
+      <c r="J62" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4">
-        <v>1</v>
-      </c>
-      <c r="H62" s="4">
-        <v>1</v>
-      </c>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" s="53" customFormat="1"/>
-    <row r="64" spans="1:10" s="53" customFormat="1"/>
-    <row r="65" spans="1:10" s="53" customFormat="1"/>
-    <row r="66" spans="1:10">
-      <c r="A66" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="C67" s="3" t="str">
+    </row>
+    <row r="63" spans="1:10" s="53" customFormat="1">
+      <c r="B63" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="D67" s="3" t="str">
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" s="53" customFormat="1">
+      <c r="B64" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
-      <c r="E67" s="3" t="str">
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" s="53" customFormat="1">
+      <c r="B65" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
-      <c r="F67" s="3" t="str">
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" s="53" customFormat="1">
+      <c r="B66" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
       </c>
-      <c r="G67" s="3" t="str">
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="1:10" s="53" customFormat="1">
+      <c r="B67" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
       </c>
-      <c r="H67" s="3" t="str">
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4">
+        <v>1</v>
+      </c>
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68" spans="1:10" s="53" customFormat="1">
+      <c r="B68" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
-      </c>
-      <c r="I67" s="3" t="str">
-        <f>Populations!$C$9</f>
-        <v>M 15+</v>
-      </c>
-      <c r="J67" s="3" t="str">
-        <f>Populations!$C$10</f>
-        <v>F 15+</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="B68" s="3" t="str">
-        <f>Populations!$C$3</f>
-        <v>FSW</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -3386,13 +3391,13 @@
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="J68" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="53" customFormat="1">
       <c r="B69" s="3" t="str">
-        <f>Populations!$C$4</f>
-        <v>Clients</v>
+        <f>Populations!$C$9</f>
+        <v>M 15+</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -3400,15 +3405,13 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-      <c r="I69" s="4">
-        <v>15</v>
-      </c>
+      <c r="I69" s="4"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" s="53" customFormat="1">
       <c r="B70" s="3" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
+        <f>Populations!$C$10</f>
+        <v>F 15+</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -3416,80 +3419,168 @@
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="4">
-        <v>15</v>
-      </c>
+      <c r="I70" s="4"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" s="53" customFormat="1">
-      <c r="B71" s="3" t="str">
+    <row r="71" spans="1:10" s="53" customFormat="1"/>
+    <row r="72" spans="1:10" s="53" customFormat="1"/>
+    <row r="73" spans="1:10" s="53" customFormat="1"/>
+    <row r="74" spans="1:10">
+      <c r="A74" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="C75" s="3" t="str">
+        <f>Populations!$C$3</f>
+        <v>FSW</v>
+      </c>
+      <c r="D75" s="3" t="str">
+        <f>Populations!$C$4</f>
+        <v>Clients</v>
+      </c>
+      <c r="E75" s="3" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
+      </c>
+      <c r="F75" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
       </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="B72" s="3" t="str">
+      <c r="G75" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="B73" s="3" t="str">
+      <c r="H75" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="B74" s="3" t="str">
+      <c r="I75" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
       </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="B75" s="3" t="str">
+      <c r="J75" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
       </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="B76" s="3" t="str">
+        <f>Populations!$C$3</f>
+        <v>FSW</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="B77" s="3" t="str">
+        <f>Populations!$C$4</f>
+        <v>Clients</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4">
+        <v>15</v>
+      </c>
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="B78" s="3" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
+      </c>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4">
+        <v>15</v>
+      </c>
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79" spans="1:10" s="53" customFormat="1">
+      <c r="B79" s="3" t="str">
+        <f>Populations!$C$6</f>
+        <v>PWID</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="B80" s="3" t="str">
+        <f>Populations!$C$7</f>
+        <v>M 0-14</v>
+      </c>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+    </row>
+    <row r="81" spans="2:10">
+      <c r="B81" s="3" t="str">
+        <f>Populations!$C$8</f>
+        <v>F 0-14</v>
+      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+    </row>
+    <row r="82" spans="2:10">
+      <c r="B82" s="3" t="str">
+        <f>Populations!$C$9</f>
+        <v>M 15+</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+    </row>
+    <row r="83" spans="2:10">
+      <c r="B83" s="3" t="str">
+        <f>Populations!$C$10</f>
+        <v>F 15+</v>
+      </c>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
introducing new numcirc param
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14160" tabRatio="901" activeTab="5"/>
+    <workbookView xWindow="555" yWindow="555" windowWidth="25035" windowHeight="14160" tabRatio="901" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -112,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="138">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -524,14 +519,17 @@
   <si>
     <t>Number of women on PMTCT (Option B/B+)</t>
   </si>
+  <si>
+    <t>Number of voluntary medical male circumcisions performed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="8">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
@@ -774,14 +772,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="638">
+  <cellStyleXfs count="652">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -844,7 +842,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1385,6 +1383,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1414,7 +1426,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1450,7 +1462,7 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1611,8 +1623,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="638">
+  <cellStyles count="652">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="4"/>
@@ -1970,6 +1983,13 @@
     <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="79"/>
     <cellStyle name="Followed Hyperlink 11" xfId="80"/>
     <cellStyle name="Followed Hyperlink 12" xfId="81"/>
@@ -2242,6 +2262,13 @@
     <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="7"/>
     <cellStyle name="Normal 3" xfId="8"/>
@@ -2555,34 +2582,34 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.33203125" customWidth="1"/>
+    <col min="1" max="1" width="89.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="84"/>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="84"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
     </row>
-    <row r="5" spans="1:1" ht="28">
+    <row r="5" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>102</v>
       </c>
@@ -2609,14 +2636,14 @@
       <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -2684,7 +2711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2717,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2750,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2783,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="52" customFormat="1">
+    <row r="6" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="54" t="s">
         <v>123</v>
       </c>
@@ -2815,7 +2842,7 @@
       </c>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -2848,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -2881,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -2914,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -2947,12 +2974,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
         <v>2000</v>
       </c>
@@ -3020,7 +3047,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3053,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3086,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3119,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="52" customFormat="1">
+    <row r="19" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="54" t="s">
         <v>123</v>
       </c>
@@ -3151,7 +3178,7 @@
       </c>
       <c r="Y19" s="9"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -3184,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -3217,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -3250,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -3283,12 +3310,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C28" s="3">
         <v>2000</v>
       </c>
@@ -3356,7 +3383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>38</v>
       </c>
@@ -3407,19 +3434,19 @@
       <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="52" customWidth="1"/>
-    <col min="7" max="10" width="12.6640625" customWidth="1"/>
+    <col min="3" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="52" customWidth="1"/>
+    <col min="7" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3453,7 +3480,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3467,7 +3494,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3485,7 +3512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3501,7 +3528,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" s="52" customFormat="1">
+    <row r="6" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3517,7 +3544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -3531,7 +3558,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -3545,7 +3572,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -3563,7 +3590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -3577,12 +3604,12 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3616,7 +3643,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3630,7 +3657,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3648,7 +3675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3664,7 +3691,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" s="52" customFormat="1">
+    <row r="19" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3680,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -3694,7 +3721,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -3708,7 +3735,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -3726,7 +3753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -3740,12 +3767,12 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3779,7 +3806,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3793,7 +3820,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3809,7 +3836,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3823,7 +3850,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" s="52" customFormat="1">
+    <row r="32" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3837,7 +3864,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -3851,7 +3878,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -3865,7 +3892,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -3879,7 +3906,7 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -3893,12 +3920,12 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C41" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3932,7 +3959,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3946,7 +3973,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3960,7 +3987,7 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3974,7 +4001,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" s="52" customFormat="1">
+    <row r="45" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3990,7 +4017,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -4004,7 +4031,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -4018,7 +4045,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -4032,7 +4059,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -4046,12 +4073,12 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="53" spans="1:10" s="52" customFormat="1">
+    <row r="53" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="53" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="52" customFormat="1">
+    <row r="54" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4085,7 +4112,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="52" customFormat="1">
+    <row r="55" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4103,7 +4130,7 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" s="52" customFormat="1">
+    <row r="56" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -4117,7 +4144,7 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" s="52" customFormat="1">
+    <row r="57" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -4135,15 +4162,15 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" s="52" customFormat="1"/>
-    <row r="59" spans="1:10" s="52" customFormat="1"/>
-    <row r="60" spans="1:10" s="52" customFormat="1"/>
-    <row r="61" spans="1:10" s="52" customFormat="1">
+    <row r="58" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="53" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="52" customFormat="1">
+    <row r="62" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4177,7 +4204,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="52" customFormat="1">
+    <row r="63" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4191,7 +4218,7 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="1:10" s="52" customFormat="1">
+    <row r="64" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4205,7 +4232,7 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
     </row>
-    <row r="65" spans="1:10" s="52" customFormat="1">
+    <row r="65" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -4219,7 +4246,7 @@
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
     </row>
-    <row r="66" spans="1:10" s="52" customFormat="1">
+    <row r="66" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -4233,7 +4260,7 @@
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
     </row>
-    <row r="67" spans="1:10" s="52" customFormat="1">
+    <row r="67" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -4249,7 +4276,7 @@
       </c>
       <c r="J67" s="4"/>
     </row>
-    <row r="68" spans="1:10" s="52" customFormat="1">
+    <row r="68" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -4265,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="52" customFormat="1">
+    <row r="69" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -4279,7 +4306,7 @@
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10" s="52" customFormat="1">
+    <row r="70" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -4293,15 +4320,15 @@
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" s="52" customFormat="1"/>
-    <row r="72" spans="1:10" s="52" customFormat="1"/>
-    <row r="73" spans="1:10" s="52" customFormat="1"/>
-    <row r="74" spans="1:10">
+    <row r="71" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C75" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4335,7 +4362,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4351,7 +4378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4367,7 +4394,7 @@
       </c>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -4383,7 +4410,7 @@
       </c>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" s="52" customFormat="1">
+    <row r="79" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -4397,7 +4424,7 @@
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -4411,7 +4438,7 @@
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="2:10">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -4425,7 +4452,7 @@
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="2:10">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -4439,7 +4466,7 @@
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
     </row>
-    <row r="83" spans="2:10">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -4472,12 +4499,12 @@
       <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>57</v>
       </c>
@@ -4486,7 +4513,7 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="48" t="s">
@@ -4499,7 +4526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="45"/>
       <c r="B3" s="47" t="s">
         <v>58</v>
@@ -4514,7 +4541,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="47" t="s">
         <v>59</v>
@@ -4529,7 +4556,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
       <c r="B5" s="47" t="s">
         <v>60</v>
@@ -4544,7 +4571,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="47" t="s">
         <v>61</v>
@@ -4559,7 +4586,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="47" t="s">
         <v>62</v>
@@ -4574,7 +4601,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="47" t="s">
         <v>63</v>
@@ -4589,7 +4616,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="47" t="s">
         <v>64</v>
@@ -4604,28 +4631,28 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="39"/>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="39"/>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="37"/>
       <c r="B12" s="39"/>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
         <v>65</v>
       </c>
@@ -4634,7 +4661,7 @@
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="45"/>
       <c r="B14" s="45"/>
       <c r="C14" s="48" t="s">
@@ -4647,7 +4674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="45"/>
       <c r="B15" s="47" t="s">
         <v>66</v>
@@ -4662,7 +4689,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="45"/>
       <c r="B16" s="47" t="s">
         <v>67</v>
@@ -4677,7 +4704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="45"/>
       <c r="B17" s="47" t="s">
         <v>68</v>
@@ -4692,7 +4719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
       <c r="B18" s="47" t="s">
         <v>69</v>
@@ -4707,7 +4734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="45"/>
       <c r="B19" s="47" t="s">
         <v>70</v>
@@ -4722,7 +4749,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="45"/>
       <c r="B20" s="47" t="s">
         <v>71</v>
@@ -4737,28 +4764,28 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="39"/>
       <c r="C21" s="37"/>
       <c r="D21" s="37"/>
       <c r="E21" s="37"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
       <c r="B22" s="39"/>
       <c r="C22" s="37"/>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="39"/>
       <c r="C23" s="37"/>
       <c r="D23" s="37"/>
       <c r="E23" s="37"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>72</v>
       </c>
@@ -4767,7 +4794,7 @@
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="45"/>
       <c r="B25" s="45"/>
       <c r="C25" s="48" t="s">
@@ -4780,7 +4807,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="45"/>
       <c r="B26" s="47" t="s">
         <v>73</v>
@@ -4795,7 +4822,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="45"/>
       <c r="B27" s="47" t="s">
         <v>68</v>
@@ -4810,7 +4837,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="B28" s="47" t="s">
         <v>110</v>
@@ -4825,7 +4852,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
       <c r="B29" s="47" t="s">
         <v>74</v>
@@ -4840,7 +4867,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
       <c r="B30" s="47" t="s">
         <v>75</v>
@@ -4855,28 +4882,28 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" s="39"/>
       <c r="C31" s="37"/>
       <c r="D31" s="37"/>
       <c r="E31" s="37"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" s="39"/>
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" s="39"/>
       <c r="C33" s="37"/>
       <c r="D33" s="37"/>
       <c r="E33" s="37"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
         <v>76</v>
       </c>
@@ -4885,7 +4912,7 @@
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="45"/>
       <c r="B35" s="45"/>
       <c r="C35" s="48" t="s">
@@ -4898,7 +4925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="45"/>
       <c r="B36" s="47" t="s">
         <v>77</v>
@@ -4913,7 +4940,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="45"/>
       <c r="B37" s="47" t="s">
         <v>78</v>
@@ -4928,7 +4955,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="45"/>
       <c r="B38" s="47" t="s">
         <v>79</v>
@@ -4943,7 +4970,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
       <c r="B39" s="47" t="s">
         <v>80</v>
@@ -4958,28 +4985,28 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="37"/>
       <c r="B40" s="39"/>
       <c r="C40" s="37"/>
       <c r="D40" s="37"/>
       <c r="E40" s="37"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="37"/>
       <c r="B41" s="39"/>
       <c r="C41" s="37"/>
       <c r="D41" s="37"/>
       <c r="E41" s="37"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="37"/>
       <c r="B42" s="39"/>
       <c r="C42" s="37"/>
       <c r="D42" s="37"/>
       <c r="E42" s="37"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
         <v>81</v>
       </c>
@@ -4988,7 +5015,7 @@
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="45"/>
       <c r="B44" s="45"/>
       <c r="C44" s="48" t="s">
@@ -5001,7 +5028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="45"/>
       <c r="B45" s="47" t="s">
         <v>66</v>
@@ -5016,7 +5043,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="45"/>
       <c r="B46" s="47" t="s">
         <v>67</v>
@@ -5031,7 +5058,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="45"/>
       <c r="B47" s="47" t="s">
         <v>82</v>
@@ -5046,7 +5073,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="45"/>
       <c r="B48" s="47" t="s">
         <v>69</v>
@@ -5061,7 +5088,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="45"/>
       <c r="B49" s="47" t="s">
         <v>70</v>
@@ -5080,7 +5107,7 @@
       <c r="H49" s="37"/>
       <c r="I49" s="37"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="45"/>
       <c r="B50" s="47" t="s">
         <v>71</v>
@@ -5099,7 +5126,7 @@
       <c r="H50" s="37"/>
       <c r="I50" s="37"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="45"/>
       <c r="B51" s="47" t="s">
         <v>83</v>
@@ -5118,7 +5145,7 @@
       <c r="H51" s="37"/>
       <c r="I51" s="37"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="45"/>
       <c r="B52" s="47" t="s">
         <v>84</v>
@@ -5137,7 +5164,7 @@
       <c r="H52" s="37"/>
       <c r="I52" s="37"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="37"/>
       <c r="B53" s="39"/>
       <c r="C53" s="37"/>
@@ -5148,7 +5175,7 @@
       <c r="H53" s="37"/>
       <c r="I53" s="37"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="37"/>
       <c r="B54" s="39"/>
       <c r="C54" s="37"/>
@@ -5159,7 +5186,7 @@
       <c r="H54" s="37"/>
       <c r="I54" s="37"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="37"/>
       <c r="B55" s="39"/>
       <c r="C55" s="37"/>
@@ -5170,7 +5197,7 @@
       <c r="H55" s="37"/>
       <c r="I55" s="37"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
         <v>111</v>
       </c>
@@ -5183,7 +5210,7 @@
       <c r="H56" s="37"/>
       <c r="I56" s="37"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="45"/>
       <c r="B57" s="45"/>
       <c r="C57" s="48" t="s">
@@ -5200,7 +5227,7 @@
       <c r="H57" s="37"/>
       <c r="I57" s="37"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="45"/>
       <c r="B58" s="47" t="s">
         <v>85</v>
@@ -5219,7 +5246,7 @@
       <c r="H58" s="41"/>
       <c r="I58" s="41"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="45"/>
       <c r="B59" s="47" t="s">
         <v>86</v>
@@ -5238,7 +5265,7 @@
       <c r="H59" s="41"/>
       <c r="I59" s="41"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="45"/>
       <c r="B60" s="47" t="s">
         <v>87</v>
@@ -5254,7 +5281,7 @@
       </c>
       <c r="F60" s="37"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="45"/>
       <c r="B61" s="47" t="s">
         <v>105</v>
@@ -5273,7 +5300,7 @@
       <c r="H61" s="41"/>
       <c r="I61" s="41"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="45"/>
       <c r="B62" s="47" t="s">
         <v>88</v>
@@ -5292,7 +5319,7 @@
       <c r="H62" s="41"/>
       <c r="I62" s="41"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="45"/>
       <c r="B63" s="47" t="s">
         <v>18</v>
@@ -5311,7 +5338,7 @@
       <c r="H63" s="41"/>
       <c r="I63" s="41"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="45"/>
       <c r="B64" s="47" t="s">
         <v>89</v>
@@ -5330,7 +5357,7 @@
       <c r="H64" s="41"/>
       <c r="I64" s="41"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="45"/>
       <c r="B65" s="47" t="s">
         <v>112</v>
@@ -5349,7 +5376,7 @@
       <c r="H65" s="41"/>
       <c r="I65" s="41"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="45"/>
       <c r="B66" s="47" t="s">
         <v>113</v>
@@ -5368,7 +5395,7 @@
       <c r="H66" s="37"/>
       <c r="I66" s="37"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="37"/>
       <c r="B67" s="39"/>
       <c r="C67" s="37"/>
@@ -5379,7 +5406,7 @@
       <c r="H67" s="37"/>
       <c r="I67" s="37"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="38"/>
       <c r="B68" s="39"/>
       <c r="C68" s="37"/>
@@ -5390,7 +5417,7 @@
       <c r="H68" s="37"/>
       <c r="I68" s="37"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="37"/>
       <c r="B69" s="39"/>
       <c r="C69" s="40"/>
@@ -5401,7 +5428,7 @@
       <c r="H69" s="37"/>
       <c r="I69" s="37"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="46" t="s">
         <v>90</v>
       </c>
@@ -5415,7 +5442,7 @@
       <c r="I70" s="37"/>
       <c r="J70" s="26"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="45"/>
       <c r="B71" s="45"/>
       <c r="C71" s="48" t="s">
@@ -5433,7 +5460,7 @@
       <c r="I71" s="37"/>
       <c r="J71" s="26"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="45"/>
       <c r="B72" s="47" t="s">
         <v>91</v>
@@ -5453,7 +5480,7 @@
       <c r="I72" s="37"/>
       <c r="J72" s="26"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="45"/>
       <c r="B73" s="47" t="s">
         <v>92</v>
@@ -5472,7 +5499,7 @@
       <c r="H73" s="37"/>
       <c r="I73" s="37"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="45"/>
       <c r="B74" s="47" t="s">
         <v>93</v>
@@ -5491,7 +5518,7 @@
       <c r="H74" s="37"/>
       <c r="I74" s="37"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="45"/>
       <c r="B75" s="47" t="s">
         <v>94</v>
@@ -5510,7 +5537,7 @@
       <c r="H75" s="37"/>
       <c r="I75" s="37"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="45"/>
       <c r="B76" s="47" t="s">
         <v>95</v>
@@ -5529,7 +5556,7 @@
       <c r="H76" s="37"/>
       <c r="I76" s="37"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="45"/>
       <c r="B77" s="47" t="s">
         <v>96</v>
@@ -5544,7 +5571,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="45"/>
       <c r="B78" s="47" t="s">
         <v>97</v>
@@ -5578,20 +5605,20 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -5617,7 +5644,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -5646,7 +5673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -5675,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -5704,7 +5731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="52" customFormat="1">
+    <row r="6" spans="1:10" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -5733,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -5762,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -5791,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>7</v>
       </c>
@@ -5820,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>8</v>
       </c>
@@ -5868,21 +5895,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="12" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="3">
         <v>2000</v>
       </c>
@@ -5950,7 +5977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5984,7 +6011,7 @@
       </c>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6040,7 +6067,7 @@
       </c>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6074,7 +6101,7 @@
       </c>
       <c r="Z5" s="7"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6108,7 +6135,7 @@
       </c>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6164,7 +6191,7 @@
       </c>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6198,7 +6225,7 @@
       </c>
       <c r="Z9" s="7"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6232,7 +6259,7 @@
       </c>
       <c r="Z11" s="7"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6288,7 +6315,7 @@
       </c>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6322,7 +6349,7 @@
       </c>
       <c r="Z13" s="7"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -6335,7 +6362,7 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:26" s="52" customFormat="1">
+    <row r="15" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="54" t="s">
         <v>123</v>
       </c>
@@ -6368,7 +6395,7 @@
       </c>
       <c r="Z15" s="7"/>
     </row>
-    <row r="16" spans="1:26" s="52" customFormat="1">
+    <row r="16" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="54" t="s">
         <v>123</v>
       </c>
@@ -6423,7 +6450,7 @@
       </c>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="2:26" s="52" customFormat="1">
+    <row r="17" spans="2:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="54" t="s">
         <v>123</v>
       </c>
@@ -6456,7 +6483,7 @@
       </c>
       <c r="Z17" s="7"/>
     </row>
-    <row r="18" spans="2:26" s="52" customFormat="1">
+    <row r="18" spans="2:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -6469,7 +6496,7 @@
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -6503,7 +6530,7 @@
       </c>
       <c r="Z19" s="7"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -6559,7 +6586,7 @@
       </c>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -6593,7 +6620,7 @@
       </c>
       <c r="Z21" s="7"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -6627,7 +6654,7 @@
       </c>
       <c r="Z23" s="7"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -6683,7 +6710,7 @@
       </c>
       <c r="Z24" s="7"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -6717,7 +6744,7 @@
       </c>
       <c r="Z25" s="7"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -6751,7 +6778,7 @@
       </c>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -6807,7 +6834,7 @@
       </c>
       <c r="Z28" s="7"/>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -6841,7 +6868,7 @@
       </c>
       <c r="Z29" s="7"/>
     </row>
-    <row r="31" spans="2:26">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -6875,7 +6902,7 @@
       </c>
       <c r="Z31" s="7"/>
     </row>
-    <row r="32" spans="2:26">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -6931,7 +6958,7 @@
       </c>
       <c r="Z32" s="7"/>
     </row>
-    <row r="33" spans="2:26">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -6965,7 +6992,7 @@
       </c>
       <c r="Z33" s="7"/>
     </row>
-    <row r="35" spans="2:26">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M35" t="s">
         <v>101</v>
       </c>
@@ -6974,7 +7001,7 @@
         <v>36960583.295806497</v>
       </c>
     </row>
-    <row r="36" spans="2:26">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M36" t="s">
         <v>100</v>
       </c>
@@ -6990,7 +7017,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="2:26">
+    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="N37">
         <f>3529/N36*100</f>
         <v>4.1513084731567043</v>
@@ -7018,19 +7045,19 @@
       <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="3">
         <v>2000</v>
       </c>
@@ -7098,7 +7125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7138,7 +7165,7 @@
       </c>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7178,7 +7205,7 @@
       </c>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7218,7 +7245,7 @@
       </c>
       <c r="Z5" s="5"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7252,7 +7279,7 @@
       </c>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7288,7 +7315,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7322,7 +7349,7 @@
       </c>
       <c r="Z9" s="5"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7358,7 +7385,7 @@
       </c>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7400,7 +7427,7 @@
       </c>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7436,7 +7463,7 @@
       </c>
       <c r="Z13" s="5"/>
     </row>
-    <row r="15" spans="1:26" s="52" customFormat="1">
+    <row r="15" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="54" t="s">
         <v>123</v>
       </c>
@@ -7471,7 +7498,7 @@
       </c>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26" s="52" customFormat="1">
+    <row r="16" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="54" t="s">
         <v>123</v>
       </c>
@@ -7512,7 +7539,7 @@
       </c>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="2:26" s="52" customFormat="1">
+    <row r="17" spans="2:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="54" t="s">
         <v>123</v>
       </c>
@@ -7547,8 +7574,8 @@
       </c>
       <c r="Z17" s="5"/>
     </row>
-    <row r="18" spans="2:26" s="52" customFormat="1"/>
-    <row r="19" spans="2:26">
+    <row r="18" spans="2:26" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -7582,7 +7609,7 @@
       </c>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -7618,7 +7645,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -7652,7 +7679,7 @@
       </c>
       <c r="Z21" s="5"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -7686,7 +7713,7 @@
       </c>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -7722,7 +7749,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -7756,7 +7783,7 @@
       </c>
       <c r="Z25" s="5"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -7790,7 +7817,7 @@
       </c>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -7838,7 +7865,7 @@
       </c>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -7872,7 +7899,7 @@
       </c>
       <c r="Z29" s="5"/>
     </row>
-    <row r="31" spans="2:26">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -7906,7 +7933,7 @@
       </c>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="2:26">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -7954,7 +7981,7 @@
       </c>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="2:26">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -8007,14 +8034,14 @@
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -8082,7 +8109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8115,7 +8142,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8148,7 +8175,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8181,7 +8208,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="52" customFormat="1">
+    <row r="6" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="54" t="s">
         <v>123</v>
       </c>
@@ -8213,7 +8240,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -8246,7 +8273,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -8279,7 +8306,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -8312,7 +8339,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -8345,12 +8372,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
         <v>2000</v>
       </c>
@@ -8418,7 +8445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8451,7 +8478,7 @@
       </c>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8484,7 +8511,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8517,7 +8544,7 @@
       </c>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25" s="52" customFormat="1">
+    <row r="19" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="54" t="s">
         <v>123</v>
       </c>
@@ -8549,7 +8576,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -8582,7 +8609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -8615,7 +8642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -8648,7 +8675,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -8681,12 +8708,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C28" s="3">
         <v>2000</v>
       </c>
@@ -8754,7 +8781,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8787,7 +8814,7 @@
       </c>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8820,7 +8847,7 @@
       </c>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8853,7 +8880,7 @@
       </c>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25" s="52" customFormat="1">
+    <row r="32" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="54" t="s">
         <v>123</v>
       </c>
@@ -8885,7 +8912,7 @@
       </c>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="2:25">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -8918,7 +8945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:25">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -8951,7 +8978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:25">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -8984,7 +9011,7 @@
       </c>
       <c r="Y35" s="5"/>
     </row>
-    <row r="36" spans="2:25">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -9032,18 +9059,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -9111,7 +9138,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9146,7 +9173,7 @@
       </c>
       <c r="Y3" s="9"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9183,7 +9210,7 @@
       </c>
       <c r="Y4" s="9"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9216,7 +9243,7 @@
       </c>
       <c r="Y5" s="9"/>
     </row>
-    <row r="6" spans="1:25" s="52" customFormat="1">
+    <row r="6" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="54" t="s">
         <v>123</v>
       </c>
@@ -9248,7 +9275,7 @@
       </c>
       <c r="Y6" s="9"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -9281,7 +9308,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -9314,7 +9341,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -9351,7 +9378,7 @@
       </c>
       <c r="Y9" s="9"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -9388,12 +9415,12 @@
       </c>
       <c r="Y10" s="9"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
         <v>2000</v>
       </c>
@@ -9461,7 +9488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>38</v>
       </c>
@@ -9493,12 +9520,12 @@
       </c>
       <c r="Y16" s="4"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C21" s="3">
         <v>2000</v>
       </c>
@@ -9566,7 +9593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
@@ -9614,12 +9641,12 @@
       </c>
       <c r="Y22" s="4"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C28" s="3">
         <v>2000</v>
       </c>
@@ -9687,7 +9714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -9720,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -9753,7 +9780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -9786,7 +9813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="52" customFormat="1">
+    <row r="32" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="54" t="s">
         <v>123</v>
       </c>
@@ -9818,7 +9845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -9851,7 +9878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -9884,7 +9911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -9917,7 +9944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -9950,12 +9977,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="53" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C41" s="3">
         <v>2000</v>
       </c>
@@ -10023,7 +10050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>27</v>
       </c>
@@ -10057,12 +10084,12 @@
       </c>
       <c r="Y42" s="4"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C47" s="3">
         <v>2000</v>
       </c>
@@ -10130,7 +10157,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10183,7 +10210,7 @@
       </c>
       <c r="Y48" s="8"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -10216,7 +10243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -10269,12 +10296,12 @@
       </c>
       <c r="Y50" s="8"/>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C55" s="3">
         <v>2000</v>
       </c>
@@ -10342,7 +10369,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>27</v>
       </c>
@@ -10393,20 +10420,20 @@
       <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -10474,7 +10501,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
@@ -10518,12 +10545,12 @@
       </c>
       <c r="Y3" s="8"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <v>2000</v>
       </c>
@@ -10591,7 +10618,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
@@ -10625,12 +10652,12 @@
       </c>
       <c r="Y9" s="8"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C14" s="3">
         <v>2000</v>
       </c>
@@ -10698,7 +10725,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
@@ -10756,12 +10783,12 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C20" s="3">
         <v>2000</v>
       </c>
@@ -10829,7 +10856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
@@ -10887,7 +10914,7 @@
       </c>
       <c r="Y21" s="42"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>103</v>
       </c>
@@ -10926,7 +10953,7 @@
       <c r="AH25" s="31"/>
       <c r="AI25" s="31"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26" s="31"/>
       <c r="C26" s="33">
@@ -11027,7 +11054,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="33" t="s">
         <v>27</v>
@@ -11068,12 +11095,12 @@
       </c>
       <c r="AI27" s="34"/>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C31" s="3">
         <v>2000</v>
       </c>
@@ -11141,7 +11168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -11199,12 +11226,12 @@
       </c>
       <c r="Y32" s="8"/>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C37" s="3">
         <v>2000</v>
       </c>
@@ -11272,7 +11299,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>27</v>
       </c>
@@ -11310,7 +11337,7 @@
       </c>
       <c r="Y38" s="8"/>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="71"/>
       <c r="B39" s="71"/>
       <c r="C39" s="71"/>
@@ -11337,7 +11364,7 @@
       <c r="X39" s="71"/>
       <c r="Y39" s="71"/>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="71"/>
       <c r="B40" s="71"/>
       <c r="C40" s="71"/>
@@ -11364,7 +11391,7 @@
       <c r="X40" s="71"/>
       <c r="Y40" s="71"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="71"/>
       <c r="B41" s="71"/>
       <c r="C41" s="71"/>
@@ -11391,7 +11418,7 @@
       <c r="X41" s="71"/>
       <c r="Y41" s="71"/>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="72" t="s">
         <v>131</v>
       </c>
@@ -11420,7 +11447,7 @@
       <c r="X42" s="71"/>
       <c r="Y42" s="71"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="71"/>
       <c r="B43" s="71"/>
       <c r="C43" s="73">
@@ -11491,7 +11518,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="71"/>
       <c r="B44" s="73" t="s">
         <v>38</v>
@@ -11522,7 +11549,7 @@
       </c>
       <c r="Y44" s="74"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="71"/>
       <c r="B45" s="71"/>
       <c r="C45" s="71"/>
@@ -11549,7 +11576,7 @@
       <c r="X45" s="71"/>
       <c r="Y45" s="71"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="71"/>
       <c r="B46" s="71"/>
       <c r="C46" s="71"/>
@@ -11576,7 +11603,7 @@
       <c r="X46" s="71"/>
       <c r="Y46" s="71"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="71"/>
       <c r="B47" s="71"/>
       <c r="C47" s="71"/>
@@ -11603,7 +11630,7 @@
       <c r="X47" s="71"/>
       <c r="Y47" s="71"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="82" t="s">
         <v>134</v>
       </c>
@@ -11632,7 +11659,7 @@
       <c r="X48" s="78"/>
       <c r="Y48" s="78"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="78"/>
       <c r="B49" s="78"/>
       <c r="C49" s="79">
@@ -11703,7 +11730,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="78"/>
       <c r="B50" s="79" t="s">
         <v>38</v>
@@ -11734,7 +11761,7 @@
       </c>
       <c r="Y50" s="81"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="77"/>
       <c r="B51" s="77"/>
       <c r="C51" s="77"/>
@@ -11761,7 +11788,7 @@
       <c r="X51" s="77"/>
       <c r="Y51" s="77"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="77"/>
       <c r="B52" s="77"/>
       <c r="C52" s="77"/>
@@ -11788,7 +11815,7 @@
       <c r="X52" s="77"/>
       <c r="Y52" s="77"/>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="77"/>
       <c r="B53" s="77"/>
       <c r="C53" s="77"/>
@@ -11815,7 +11842,7 @@
       <c r="X53" s="77"/>
       <c r="Y53" s="77"/>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="82" t="s">
         <v>135</v>
       </c>
@@ -11844,7 +11871,7 @@
       <c r="X54" s="78"/>
       <c r="Y54" s="78"/>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="78"/>
       <c r="B55" s="78"/>
       <c r="C55" s="79">
@@ -11915,7 +11942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="78"/>
       <c r="B56" s="79" t="s">
         <v>38</v>
@@ -11964,9 +11991,9 @@
       <selection activeCell="A77" sqref="A77:XFD82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
         <v>115</v>
       </c>
@@ -11995,7 +12022,7 @@
       <c r="X1" s="52"/>
       <c r="Y1" s="52"/>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="62"/>
       <c r="B2" s="52"/>
       <c r="C2" s="54">
@@ -12066,7 +12093,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="62"/>
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -12100,7 +12127,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="62"/>
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -12134,7 +12161,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="61"/>
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12168,7 +12195,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="52" customFormat="1">
+    <row r="6" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="61"/>
       <c r="B6" s="54" t="s">
         <v>123</v>
@@ -12201,7 +12228,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="61"/>
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12235,7 +12262,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="61"/>
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -12269,7 +12296,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="62"/>
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12303,7 +12330,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="62"/>
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
@@ -12337,10 +12364,10 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="62"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
         <v>127</v>
       </c>
@@ -12369,7 +12396,7 @@
       <c r="X14" s="52"/>
       <c r="Y14" s="52"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="52"/>
       <c r="C15" s="54">
         <v>2000</v>
@@ -12439,7 +12466,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="62"/>
       <c r="B16" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -12473,7 +12500,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="61"/>
       <c r="B17" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -12507,7 +12534,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="62"/>
       <c r="B18" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12541,7 +12568,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="52" customFormat="1">
+    <row r="19" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="61"/>
       <c r="B19" s="54" t="s">
         <v>123</v>
@@ -12574,7 +12601,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="61"/>
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12608,7 +12635,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="61"/>
       <c r="B21" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -12642,7 +12669,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="61"/>
       <c r="B22" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -12676,7 +12703,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="61"/>
       <c r="B23" s="3" t="str">
         <f>Populations!$C$10</f>
@@ -12710,13 +12737,13 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="61"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="61"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="63" t="s">
         <v>116</v>
       </c>
@@ -12745,7 +12772,7 @@
       <c r="X27" s="52"/>
       <c r="Y27" s="52"/>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="52"/>
       <c r="B28" s="52"/>
       <c r="C28" s="54">
@@ -12816,7 +12843,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12849,7 +12876,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="3" t="str">
         <f>Populations!$C$4</f>
@@ -12883,7 +12910,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="61"/>
       <c r="B31" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -12917,7 +12944,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="52" customFormat="1">
+    <row r="32" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="61"/>
       <c r="B32" s="54" t="s">
         <v>123</v>
@@ -12950,7 +12977,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
       <c r="B33" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -12984,7 +13011,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -13018,7 +13045,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -13052,7 +13079,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="61"/>
       <c r="B36" s="3" t="str">
         <f>Populations!$C$10</f>
@@ -13086,16 +13113,16 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="61"/>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="61"/>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="61"/>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="63" t="s">
         <v>117</v>
       </c>
@@ -13124,7 +13151,7 @@
       <c r="X40" s="52"/>
       <c r="Y40" s="52"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="52"/>
       <c r="B41" s="52"/>
       <c r="C41" s="54">
@@ -13195,7 +13222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="52"/>
       <c r="B42" s="3" t="str">
         <f>Populations!$C$3</f>
@@ -13229,7 +13256,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13262,7 +13289,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="52"/>
       <c r="B44" s="3" t="str">
         <f>Populations!$C$5</f>
@@ -13296,7 +13323,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="52" customFormat="1">
+    <row r="45" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="54" t="s">
         <v>123</v>
       </c>
@@ -13328,7 +13355,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="52"/>
       <c r="B46" s="3" t="str">
         <f>Populations!$C$7</f>
@@ -13362,7 +13389,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="52"/>
       <c r="B47" s="3" t="str">
         <f>Populations!$C$8</f>
@@ -13396,7 +13423,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="52"/>
       <c r="B48" s="3" t="str">
         <f>Populations!$C$9</f>
@@ -13430,7 +13457,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="52"/>
       <c r="B49" s="3" t="str">
         <f>Populations!$C$10</f>
@@ -13464,7 +13491,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="65" t="s">
         <v>128</v>
       </c>
@@ -13493,7 +13520,7 @@
       <c r="X53" s="64"/>
       <c r="Y53" s="64"/>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="64"/>
       <c r="B54" s="64"/>
       <c r="C54" s="66">
@@ -13564,7 +13591,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="64"/>
       <c r="B55" s="66" t="s">
         <v>38</v>
@@ -13597,7 +13624,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="65" t="s">
         <v>114</v>
       </c>
@@ -13626,7 +13653,7 @@
       <c r="X59" s="64"/>
       <c r="Y59" s="64"/>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="64"/>
       <c r="B60" s="64"/>
       <c r="C60" s="66">
@@ -13697,7 +13724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="64"/>
       <c r="B61" s="66" t="s">
         <v>38</v>
@@ -13730,7 +13757,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="65" t="s">
         <v>129</v>
       </c>
@@ -13759,7 +13786,7 @@
       <c r="X65" s="64"/>
       <c r="Y65" s="64"/>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="64"/>
       <c r="B66" s="64"/>
       <c r="C66" s="66">
@@ -13830,7 +13857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="64"/>
       <c r="B67" s="66" t="s">
         <v>38</v>
@@ -13863,7 +13890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="65" t="s">
         <v>130</v>
       </c>
@@ -13892,7 +13919,7 @@
       <c r="X71" s="64"/>
       <c r="Y71" s="64"/>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="64"/>
       <c r="B72" s="64"/>
       <c r="C72" s="66">
@@ -13963,7 +13990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="64"/>
       <c r="B73" s="66" t="s">
         <v>38</v>
@@ -13996,7 +14023,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="65" t="s">
         <v>132</v>
       </c>
@@ -14025,7 +14052,7 @@
       <c r="X77" s="64"/>
       <c r="Y77" s="64"/>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="64"/>
       <c r="B78" s="64"/>
       <c r="C78" s="66">
@@ -14096,7 +14123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="64"/>
       <c r="B79" s="66" t="s">
         <v>38</v>
@@ -14129,7 +14156,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="65" t="s">
         <v>133</v>
       </c>
@@ -14158,7 +14185,7 @@
       <c r="X83" s="64"/>
       <c r="Y83" s="64"/>
     </row>
-    <row r="84" spans="1:25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" s="64"/>
       <c r="B84" s="64"/>
       <c r="C84" s="66">
@@ -14229,7 +14256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="64"/>
       <c r="B85" s="66" t="s">
         <v>38</v>
@@ -14275,20 +14302,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y85"/>
+  <dimension ref="A1:Y95"/>
   <sheetViews>
-    <sheetView topLeftCell="J56" workbookViewId="0">
-      <selection activeCell="X83" sqref="X83:Y83"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
         <v>2000</v>
       </c>
@@ -14356,7 +14383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14389,7 +14416,7 @@
       </c>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14422,7 +14449,7 @@
       </c>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14455,7 +14482,7 @@
       </c>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:25" s="52" customFormat="1">
+    <row r="6" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="54" t="s">
         <v>123</v>
       </c>
@@ -14487,7 +14514,7 @@
       </c>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -14520,7 +14547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -14553,7 +14580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -14586,7 +14613,7 @@
       </c>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -14619,12 +14646,12 @@
       </c>
       <c r="Y10" s="4"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
         <v>2000</v>
       </c>
@@ -14692,7 +14719,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -14725,7 +14752,7 @@
       </c>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -14758,7 +14785,7 @@
       </c>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -14791,7 +14818,7 @@
       </c>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" spans="1:25" s="52" customFormat="1">
+    <row r="19" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="54" t="s">
         <v>123</v>
       </c>
@@ -14823,7 +14850,7 @@
       </c>
       <c r="Y19" s="4"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -14856,7 +14883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -14889,7 +14916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -14922,7 +14949,7 @@
       </c>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -14955,12 +14982,12 @@
       </c>
       <c r="Y23" s="4"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C28" s="3">
         <v>2000</v>
       </c>
@@ -15028,7 +15055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15061,7 +15088,7 @@
       </c>
       <c r="Y29" s="4"/>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15094,7 +15121,7 @@
       </c>
       <c r="Y30" s="4"/>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15127,7 +15154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="52" customFormat="1">
+    <row r="32" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="54" t="s">
         <v>123</v>
       </c>
@@ -15159,7 +15186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -15192,7 +15219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -15225,7 +15252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -15258,7 +15285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -15291,12 +15318,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C41" s="3">
         <v>2000</v>
       </c>
@@ -15364,7 +15391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15397,7 +15424,7 @@
       </c>
       <c r="Y42" s="9"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15430,7 +15457,7 @@
       </c>
       <c r="Y43" s="9"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15463,7 +15490,7 @@
       </c>
       <c r="Y44" s="9"/>
     </row>
-    <row r="45" spans="1:25" s="52" customFormat="1">
+    <row r="45" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="54" t="s">
         <v>123</v>
       </c>
@@ -15495,7 +15522,7 @@
       </c>
       <c r="Y45" s="9"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -15528,7 +15555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -15561,7 +15588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -15594,7 +15621,7 @@
       </c>
       <c r="Y48" s="9"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -15627,12 +15654,12 @@
       </c>
       <c r="Y49" s="9"/>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C54" s="3">
         <v>2000</v>
       </c>
@@ -15700,7 +15727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -15733,7 +15760,7 @@
       </c>
       <c r="Y55" s="9"/>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -15770,7 +15797,7 @@
       </c>
       <c r="Y56" s="9"/>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -15803,7 +15830,7 @@
       </c>
       <c r="Y57" s="9"/>
     </row>
-    <row r="58" spans="1:25" s="52" customFormat="1">
+    <row r="58" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="54" t="s">
         <v>123</v>
       </c>
@@ -15835,7 +15862,7 @@
       </c>
       <c r="Y58" s="9"/>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -15868,7 +15895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -15901,7 +15928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -15938,7 +15965,7 @@
       </c>
       <c r="Y61" s="9"/>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -15975,12 +16002,12 @@
       </c>
       <c r="Y62" s="9"/>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C67" s="3">
         <v>2000</v>
       </c>
@@ -16048,7 +16075,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -16083,7 +16110,7 @@
       </c>
       <c r="Y68" s="9"/>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -16116,7 +16143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -16149,7 +16176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" s="52" customFormat="1">
+    <row r="71" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="54" t="s">
         <v>123</v>
       </c>
@@ -16181,7 +16208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -16214,7 +16241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="str">
         <f>Populations!$C$8</f>
         <v>F 0-14</v>
@@ -16247,7 +16274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -16280,7 +16307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="str">
         <f>Populations!$C$10</f>
         <v>F 15+</v>
@@ -16313,12 +16340,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C80" s="3">
         <v>2000</v>
       </c>
@@ -16386,7 +16413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="2:25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -16419,7 +16446,7 @@
       </c>
       <c r="Y81" s="9"/>
     </row>
-    <row r="82" spans="2:25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -16452,7 +16479,7 @@
       </c>
       <c r="Y82" s="9"/>
     </row>
-    <row r="83" spans="2:25" s="52" customFormat="1">
+    <row r="83" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="54" t="s">
         <v>123</v>
       </c>
@@ -16484,7 +16511,7 @@
       </c>
       <c r="Y83" s="9"/>
     </row>
-    <row r="84" spans="2:25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="str">
         <f>Populations!$C$7</f>
         <v>M 0-14</v>
@@ -16517,7 +16544,7 @@
       </c>
       <c r="Y84" s="9"/>
     </row>
-    <row r="85" spans="2:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="str">
         <f>Populations!$C$9</f>
         <v>M 15+</v>
@@ -16550,14 +16577,236 @@
       </c>
       <c r="Y85" s="9"/>
     </row>
+    <row r="89" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="85" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C90" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D90" s="3">
+        <v>2001</v>
+      </c>
+      <c r="E90" s="3">
+        <v>2002</v>
+      </c>
+      <c r="F90" s="3">
+        <v>2003</v>
+      </c>
+      <c r="G90" s="3">
+        <v>2004</v>
+      </c>
+      <c r="H90" s="3">
+        <v>2005</v>
+      </c>
+      <c r="I90" s="3">
+        <v>2006</v>
+      </c>
+      <c r="J90" s="3">
+        <v>2007</v>
+      </c>
+      <c r="K90" s="3">
+        <v>2008</v>
+      </c>
+      <c r="L90" s="3">
+        <v>2009</v>
+      </c>
+      <c r="M90" s="3">
+        <v>2010</v>
+      </c>
+      <c r="N90" s="3">
+        <v>2011</v>
+      </c>
+      <c r="O90" s="3">
+        <v>2012</v>
+      </c>
+      <c r="P90" s="3">
+        <v>2013</v>
+      </c>
+      <c r="Q90" s="3">
+        <v>2014</v>
+      </c>
+      <c r="R90" s="3">
+        <v>2015</v>
+      </c>
+      <c r="S90" s="3">
+        <v>2016</v>
+      </c>
+      <c r="T90" s="3">
+        <v>2017</v>
+      </c>
+      <c r="U90" s="3">
+        <v>2018</v>
+      </c>
+      <c r="V90" s="3">
+        <v>2019</v>
+      </c>
+      <c r="W90" s="3">
+        <v>2020</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="3" t="str">
+        <f>Populations!$C$4</f>
+        <v>Clients</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="9"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="9"/>
+      <c r="R91" s="9"/>
+      <c r="S91" s="9"/>
+      <c r="T91" s="9"/>
+      <c r="U91" s="9"/>
+      <c r="V91" s="9"/>
+      <c r="W91" s="9"/>
+      <c r="X91" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y91" s="9"/>
+    </row>
+    <row r="92" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="3" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="9"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="9"/>
+      <c r="P92" s="9"/>
+      <c r="Q92" s="9"/>
+      <c r="R92" s="9"/>
+      <c r="S92" s="9"/>
+      <c r="T92" s="9"/>
+      <c r="U92" s="9"/>
+      <c r="V92" s="9"/>
+      <c r="W92" s="9"/>
+      <c r="X92" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y92" s="9"/>
+    </row>
+    <row r="93" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="9"/>
+      <c r="O93" s="9"/>
+      <c r="P93" s="9"/>
+      <c r="Q93" s="9"/>
+      <c r="R93" s="9"/>
+      <c r="S93" s="9"/>
+      <c r="T93" s="9"/>
+      <c r="U93" s="9"/>
+      <c r="V93" s="9"/>
+      <c r="W93" s="9"/>
+      <c r="X93" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y93" s="9"/>
+    </row>
+    <row r="94" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="str">
+        <f>Populations!$C$7</f>
+        <v>M 0-14</v>
+      </c>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="9"/>
+      <c r="K94" s="9"/>
+      <c r="L94" s="9"/>
+      <c r="M94" s="9"/>
+      <c r="N94" s="9"/>
+      <c r="O94" s="9"/>
+      <c r="P94" s="9"/>
+      <c r="Q94" s="9"/>
+      <c r="R94" s="9"/>
+      <c r="S94" s="9"/>
+      <c r="T94" s="9"/>
+      <c r="U94" s="9"/>
+      <c r="V94" s="9"/>
+      <c r="W94" s="9"/>
+      <c r="X94" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y94" s="9"/>
+    </row>
+    <row r="95" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="3" t="str">
+        <f>Populations!$C$9</f>
+        <v>M 15+</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="9"/>
+      <c r="M95" s="9"/>
+      <c r="N95" s="9"/>
+      <c r="O95" s="9"/>
+      <c r="P95" s="9"/>
+      <c r="Q95" s="9"/>
+      <c r="R95" s="9"/>
+      <c r="S95" s="9"/>
+      <c r="T95" s="9"/>
+      <c r="U95" s="9"/>
+      <c r="V95" s="9"/>
+      <c r="W95" s="9"/>
+      <c r="X95" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y95" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
broke epi dynamics but otherwise working
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1617,13 +1617,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="493" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="67" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="67" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="652">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2588,15 +2588,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84"/>
+      <c r="A2" s="85"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
+      <c r="A3" s="85"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
@@ -14305,7 +14305,7 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+      <selection activeCell="Q88" sqref="Q88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16578,7 +16578,7 @@
       <c r="Y85" s="9"/>
     </row>
     <row r="89" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="85" t="s">
+      <c r="A89" s="83" t="s">
         <v>137</v>
       </c>
     </row>
@@ -16679,7 +16679,9 @@
       <c r="X91" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y91" s="9"/>
+      <c r="Y91" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="str">
@@ -16710,7 +16712,9 @@
       <c r="X92" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y92" s="9"/>
+      <c r="Y92" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="54" t="s">
@@ -16740,7 +16744,9 @@
       <c r="X93" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y93" s="9"/>
+      <c r="Y93" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="str">
@@ -16771,7 +16777,9 @@
       <c r="X94" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y94" s="9"/>
+      <c r="Y94" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:25" s="61" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="str">
@@ -16802,7 +16810,9 @@
       <c r="X95" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y95" s="9"/>
+      <c r="Y95" s="9">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
getting there, still inconsistencies
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="737" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="737" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -4883,7 +4883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -6490,8 +6490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6620,17 +6620,17 @@
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21">
-        <v>0.2215</v>
+        <v>0.06</v>
       </c>
       <c r="K4" s="21"/>
       <c r="L4" s="21">
-        <v>0.35849999999999999</v>
+        <v>0.08</v>
       </c>
       <c r="M4" s="21"/>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
       <c r="P4" s="22">
-        <v>0.42599999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
@@ -6663,7 +6663,7 @@
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
       <c r="P5" s="22">
-        <v>2.5000000000000001E-2</v>
+        <v>0.23</v>
       </c>
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
@@ -6695,7 +6695,7 @@
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
       <c r="P6" s="22">
-        <v>0.05</v>
+        <v>0.17</v>
       </c>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
@@ -6721,19 +6721,13 @@
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
-      <c r="J7" s="21">
-        <v>0.23200000000000001</v>
-      </c>
+      <c r="J7" s="21"/>
       <c r="K7" s="21"/>
-      <c r="L7" s="21">
-        <v>0.38650000000000001</v>
-      </c>
+      <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="22"/>
       <c r="O7" s="21"/>
-      <c r="P7" s="22">
-        <v>0.46350000000000002</v>
-      </c>
+      <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
@@ -6744,7 +6738,9 @@
       <c r="X7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y7" s="22"/>
+      <c r="Y7" s="22">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
@@ -6758,19 +6754,13 @@
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="21">
-        <v>0.22900000000000001</v>
-      </c>
+      <c r="J8" s="21"/>
       <c r="K8" s="21"/>
-      <c r="L8" s="21">
-        <v>0.38250000000000001</v>
-      </c>
+      <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="22"/>
       <c r="O8" s="21"/>
-      <c r="P8" s="22">
-        <v>0.46250000000000002</v>
-      </c>
+      <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
@@ -6781,7 +6771,9 @@
       <c r="X8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y8" s="22"/>
+      <c r="Y8" s="22">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">

</xml_diff>

<commit_message>
aha, single missing parameter
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="737" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="737" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -6490,8 +6490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6969,25 +6969,25 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8">
-        <v>616</v>
+        <v>6160</v>
       </c>
       <c r="K20" s="8">
-        <v>1160</v>
+        <v>11600</v>
       </c>
       <c r="L20" s="8">
-        <v>1996</v>
+        <v>19960</v>
       </c>
       <c r="M20" s="8">
-        <v>2122</v>
+        <v>21220</v>
       </c>
       <c r="N20" s="8">
-        <v>2377</v>
+        <v>23770</v>
       </c>
       <c r="O20" s="8">
-        <v>2575</v>
+        <v>25750</v>
       </c>
       <c r="P20" s="8">
-        <v>3308</v>
+        <v>33080</v>
       </c>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
@@ -10856,8 +10856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N73" sqref="N73"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12030,7 +12030,7 @@
       <c r="J47" s="22"/>
       <c r="K47" s="22"/>
       <c r="L47" s="49">
-        <v>0.378</v>
+        <v>0.8</v>
       </c>
       <c r="M47" s="49"/>
       <c r="N47" s="22"/>
@@ -12065,13 +12065,13 @@
       </c>
       <c r="K48" s="22"/>
       <c r="L48" s="28">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="M48" s="28"/>
       <c r="N48" s="22"/>
       <c r="O48" s="22"/>
       <c r="P48" s="22">
-        <v>0.51249999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
@@ -12167,13 +12167,13 @@
       </c>
       <c r="K51" s="22"/>
       <c r="L51" s="22">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
       <c r="P51" s="22">
-        <v>0.53749999999999998</v>
+        <v>0.25</v>
       </c>
       <c r="Q51" s="22"/>
       <c r="R51" s="22"/>
@@ -12204,13 +12204,13 @@
       </c>
       <c r="K52" s="22"/>
       <c r="L52" s="28">
-        <v>0.39500000000000002</v>
+        <v>0.12</v>
       </c>
       <c r="M52" s="28"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
       <c r="P52" s="22">
-        <v>0.53500000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="Q52" s="22"/>
       <c r="R52" s="22"/>
@@ -12344,13 +12344,17 @@
       <c r="G59" s="22"/>
       <c r="H59" s="22"/>
       <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
+      <c r="J59" s="22">
+        <v>0.45750000000000002</v>
+      </c>
       <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="28"/>
       <c r="N59" s="22"/>
       <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
+      <c r="P59" s="22">
+        <v>0.70499999999999996</v>
+      </c>
       <c r="Q59" s="22"/>
       <c r="R59" s="22"/>
       <c r="S59" s="22"/>
@@ -12361,9 +12365,7 @@
       <c r="X59" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y59" s="22">
-        <v>0</v>
-      </c>
+      <c r="Y59" s="22"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="str">

</xml_diff>

<commit_message>
calibration still looks nice
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -10856,8 +10856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P59" sqref="P59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12310,7 +12310,7 @@
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
       <c r="J58" s="22">
-        <v>0.45750000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="K58" s="22"/>
       <c r="L58" s="28"/>
@@ -12318,7 +12318,7 @@
       <c r="N58" s="22"/>
       <c r="O58" s="22"/>
       <c r="P58" s="22">
-        <v>0.70499999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="Q58" s="22"/>
       <c r="R58" s="22"/>
@@ -12345,7 +12345,7 @@
       <c r="H59" s="22"/>
       <c r="I59" s="22"/>
       <c r="J59" s="22">
-        <v>0.45750000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="K59" s="22"/>
       <c r="L59" s="28"/>
@@ -12353,7 +12353,7 @@
       <c r="N59" s="22"/>
       <c r="O59" s="22"/>
       <c r="P59" s="22">
-        <v>0.70499999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="Q59" s="22"/>
       <c r="R59" s="22"/>

</xml_diff>

<commit_message>
fixed negs (for now) but plotting does not work
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -792,7 +792,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -922,6 +922,8 @@
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1121,7 +1123,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="135">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1136,6 +1138,7 @@
     <cellStyle name="Explanatory Text 3" xfId="118"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1235,6 +1238,7 @@
     <cellStyle name="Followed Hyperlink 98" xfId="113"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -10254,7 +10258,7 @@
         <v>29</v>
       </c>
       <c r="Y3" s="81">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -10288,7 +10292,7 @@
         <v>29</v>
       </c>
       <c r="Y4" s="81">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -10321,7 +10325,7 @@
         <v>29</v>
       </c>
       <c r="Y5" s="81">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -10353,7 +10357,7 @@
         <v>29</v>
       </c>
       <c r="Y6" s="81">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -10387,7 +10391,7 @@
         <v>29</v>
       </c>
       <c r="Y7" s="81">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -10421,7 +10425,7 @@
         <v>29</v>
       </c>
       <c r="Y8" s="81">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:25">

</xml_diff>

<commit_message>
starting to make transitions
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12580" tabRatio="805" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -441,9 +441,6 @@
     <t>CD4(&lt;50)</t>
   </si>
   <si>
-    <t>Disease progression rate (% per year)</t>
-  </si>
-  <si>
     <t>Acute to CD4(&gt;500)</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
   </si>
   <si>
     <t>CD4(50-200) to CD4(&lt;50)</t>
-  </si>
-  <si>
-    <t>Treatment recovery rate (% per year)</t>
   </si>
   <si>
     <t>CD4(350-500) to CD4(&gt;500)</t>
@@ -540,9 +534,6 @@
     <t>Cascade parameters</t>
   </si>
   <si>
-    <t>People on unsuppressive ART who progress (%)</t>
-  </si>
-  <si>
     <t>People on unsuppressive ART who recover (%)</t>
   </si>
   <si>
@@ -553,6 +544,15 @@
   </si>
   <si>
     <t>Average time taken to be linked to care (years)</t>
+  </si>
+  <si>
+    <t>Treatment recovery (average years spent to move)</t>
+  </si>
+  <si>
+    <t>Disease progression (average years to move)</t>
+  </si>
+  <si>
+    <t>Probability of increasing CD4 count when on unsuppressive ART (%)</t>
   </si>
 </sst>
 </file>
@@ -792,7 +792,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -928,8 +928,26 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1122,8 +1140,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="153">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1139,6 +1158,15 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1239,6 +1267,15 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -3204,10 +3241,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3404,7 +3441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:7">
       <c r="B17" s="3" t="s">
         <v>94</v>
       </c>
@@ -3418,7 +3455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:7">
       <c r="B18" s="3" t="s">
         <v>95</v>
       </c>
@@ -3432,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:7">
       <c r="B19" s="3" t="s">
         <v>96</v>
       </c>
@@ -3446,7 +3483,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:7">
       <c r="B20" s="3" t="s">
         <v>97</v>
       </c>
@@ -3460,33 +3497,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:7">
       <c r="A21" s="38"/>
       <c r="B21" s="52"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:7">
       <c r="A22" s="38"/>
       <c r="B22" s="52"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:7">
       <c r="A23" s="38"/>
       <c r="B23" s="52"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="C25" s="7" t="s">
         <v>30</v>
       </c>
@@ -3497,103 +3534,107 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="45">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="D26" s="45">
-        <v>2</v>
-      </c>
-      <c r="E26" s="45">
-        <v>9.76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>98</v>
+      </c>
+      <c r="C26" s="81">
+        <f>2.9/12</f>
+        <v>0.24166666666666667</v>
+      </c>
+      <c r="D26" s="81">
+        <f>1.23/12</f>
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="E26" s="81">
+        <f>6/12</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="45">
-        <v>1.05</v>
-      </c>
-      <c r="D27" s="45">
-        <v>0.86</v>
-      </c>
-      <c r="E27" s="45">
-        <v>1.61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="C27" s="81">
+        <v>0.95</v>
+      </c>
+      <c r="D27" s="81">
+        <v>0.62</v>
+      </c>
+      <c r="E27" s="81">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G27" s="83"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="81">
+        <v>3</v>
+      </c>
+      <c r="D28" s="81">
+        <v>2.83</v>
+      </c>
+      <c r="E28" s="81">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="45">
-        <v>0.33</v>
-      </c>
-      <c r="D28" s="45">
-        <v>0.32</v>
-      </c>
-      <c r="E28" s="45">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="81">
+        <v>3.74</v>
+      </c>
+      <c r="D29" s="81">
+        <v>3.48</v>
+      </c>
+      <c r="E29" s="81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="45">
-        <v>0.27</v>
-      </c>
-      <c r="D29" s="45">
-        <v>0.25</v>
-      </c>
-      <c r="E29" s="45">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="45">
-        <v>0.67</v>
-      </c>
-      <c r="D30" s="45">
-        <v>0.44</v>
-      </c>
-      <c r="E30" s="45">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="C30" s="81">
+        <v>1.5</v>
+      </c>
+      <c r="D30" s="81">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E30" s="81">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="38"/>
       <c r="B31" s="52"/>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:7">
       <c r="A32" s="38"/>
       <c r="B32" s="52"/>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
       <c r="E32" s="38"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:14">
       <c r="A33" s="38"/>
       <c r="B33" s="52"/>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:14">
       <c r="A34" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="C35" s="7" t="s">
         <v>30</v>
       </c>
@@ -3604,89 +3645,137 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:14">
       <c r="B36" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="81">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D36" s="81">
+        <v>1.07</v>
+      </c>
+      <c r="E36" s="81">
+        <v>7.28</v>
+      </c>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="B37" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="81">
+        <v>1.42</v>
+      </c>
+      <c r="D37" s="81">
+        <v>0.9</v>
+      </c>
+      <c r="E37" s="81">
+        <v>3.42</v>
+      </c>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="B38" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="45">
-        <v>0.45</v>
-      </c>
-      <c r="D36" s="45">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E36" s="45">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="B37" s="3" t="s">
+      <c r="C38" s="81">
+        <v>2.14</v>
+      </c>
+      <c r="D38" s="81">
+        <v>1.39</v>
+      </c>
+      <c r="E38" s="81">
+        <v>3.58</v>
+      </c>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="55"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="B39" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="45">
-        <v>0.7</v>
-      </c>
-      <c r="D37" s="45">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E37" s="45">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="B38" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="45">
-        <v>0.47</v>
-      </c>
-      <c r="D38" s="45">
-        <v>0.33</v>
-      </c>
-      <c r="E38" s="45">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="B39" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="45">
-        <v>1.52</v>
-      </c>
-      <c r="D39" s="45">
-        <v>1.06</v>
-      </c>
-      <c r="E39" s="45">
-        <v>1.96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="C39" s="81">
+        <v>0.66</v>
+      </c>
+      <c r="D39" s="81">
+        <v>0.51</v>
+      </c>
+      <c r="E39" s="81">
+        <v>0.94</v>
+      </c>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="55"/>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="38"/>
       <c r="B40" s="52"/>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="38"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="55"/>
+      <c r="N40" s="55"/>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="38"/>
       <c r="B41" s="52"/>
       <c r="C41" s="38"/>
       <c r="D41" s="38"/>
       <c r="E41" s="38"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="55"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="38"/>
       <c r="B42" s="52"/>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:14">
       <c r="A43" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="C44" s="7" t="s">
         <v>30</v>
       </c>
@@ -3697,7 +3786,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:14">
       <c r="B45" s="3" t="s">
         <v>92</v>
       </c>
@@ -3711,7 +3800,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:14">
       <c r="B46" s="3" t="s">
         <v>93</v>
       </c>
@@ -3725,9 +3814,9 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:14">
       <c r="B47" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C47" s="51">
         <v>5.7999999999999996E-3</v>
@@ -3739,7 +3828,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:14">
       <c r="B48" s="3" t="s">
         <v>95</v>
       </c>
@@ -3791,7 +3880,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="B51" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C51" s="51">
         <v>0.23</v>
@@ -3809,7 +3898,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="B52" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C52" s="51">
         <v>2.17</v>
@@ -3860,7 +3949,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F56" s="38"/>
       <c r="G56" s="38"/>
@@ -3884,7 +3973,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="B58" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C58" s="45">
         <v>0.95</v>
@@ -3902,7 +3991,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="B59" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C59" s="45">
         <v>0.57999999999999996</v>
@@ -3920,7 +4009,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="B60" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C60" s="45">
         <v>0</v>
@@ -3935,7 +4024,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="B61" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C61" s="45">
         <v>2.65</v>
@@ -3953,7 +4042,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="B62" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C62" s="45">
         <v>0.54</v>
@@ -3971,7 +4060,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="B63" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C63" s="45">
         <v>0.9</v>
@@ -3989,7 +4078,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="B64" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C64" s="45">
         <v>0.73</v>
@@ -4007,7 +4096,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="B65" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C65" s="45">
         <v>0.5</v>
@@ -4025,7 +4114,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="B66" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C66" s="45">
         <v>0.92</v>
@@ -4076,7 +4165,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="57" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B70" s="68"/>
       <c r="C70" s="68"/>
@@ -4109,7 +4198,7 @@
     <row r="72" spans="1:10">
       <c r="A72" s="68"/>
       <c r="B72" s="59" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C72" s="69">
         <v>0.4</v>
@@ -4129,7 +4218,7 @@
     <row r="73" spans="1:10">
       <c r="A73" s="68"/>
       <c r="B73" s="59" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C73" s="69">
         <v>0.4</v>
@@ -4148,7 +4237,7 @@
     <row r="74" spans="1:10">
       <c r="A74" s="68"/>
       <c r="B74" s="59" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C74" s="69">
         <v>0.4</v>
@@ -4198,7 +4287,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="63" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B78" s="56"/>
       <c r="C78" s="56"/>
@@ -4227,7 +4316,7 @@
     <row r="80" spans="1:10">
       <c r="A80" s="56"/>
       <c r="B80" s="65" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C80" s="66">
         <v>0.14599999999999999</v>
@@ -4245,7 +4334,7 @@
     <row r="81" spans="1:8">
       <c r="A81" s="56"/>
       <c r="B81" s="65" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C81" s="66">
         <v>8.0000000000000002E-3</v>
@@ -4263,7 +4352,7 @@
     <row r="82" spans="1:8">
       <c r="A82" s="56"/>
       <c r="B82" s="65" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C82" s="66">
         <v>0.02</v>
@@ -4281,7 +4370,7 @@
     <row r="83" spans="1:8">
       <c r="A83" s="56"/>
       <c r="B83" s="65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C83" s="66">
         <v>7.0000000000000007E-2</v>
@@ -4299,7 +4388,7 @@
     <row r="84" spans="1:8">
       <c r="A84" s="56"/>
       <c r="B84" s="65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C84" s="66">
         <v>0.26500000000000001</v>
@@ -4317,7 +4406,7 @@
     <row r="85" spans="1:8">
       <c r="A85" s="56"/>
       <c r="B85" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C85" s="66">
         <v>0.54700000000000004</v>
@@ -4335,7 +4424,7 @@
     <row r="86" spans="1:8">
       <c r="A86" s="56"/>
       <c r="B86" s="65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C86" s="66">
         <v>5.2999999999999999E-2</v>
@@ -4367,7 +4456,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9951,7 +10040,7 @@
     </row>
     <row r="60" spans="1:35">
       <c r="A60" s="71" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B60" s="70"/>
       <c r="C60" s="70"/>
@@ -10147,7 +10236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y3" sqref="Y3:Y8"/>
     </sheetView>
   </sheetViews>
@@ -10155,7 +10244,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:25">

</xml_diff>

<commit_message>
turn off age and risk transitions for now
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="134">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -531,13 +531,7 @@
     <t>Treated HIV</t>
   </si>
   <si>
-    <t>Cascade parameters</t>
-  </si>
-  <si>
     <t>People on unsuppressive ART who recover (%)</t>
-  </si>
-  <si>
-    <t>People lost to follow up who are still in care (%)</t>
   </si>
   <si>
     <t>People on ART with viral suppression (%)</t>
@@ -546,13 +540,13 @@
     <t>Average time taken to be linked to care (years)</t>
   </si>
   <si>
-    <t>Treatment recovery (average years spent to move)</t>
-  </si>
-  <si>
     <t>Disease progression (average years to move)</t>
   </si>
   <si>
-    <t>Probability of increasing CD4 count when on unsuppressive ART (%)</t>
+    <t>Treatment recovery on suppressive ART (average years to move)</t>
+  </si>
+  <si>
+    <t>Treatment recovery on unsuppressive ART</t>
   </si>
 </sst>
 </file>
@@ -792,7 +786,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -922,6 +916,14 @@
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1142,7 +1144,7 @@
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="161">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1167,6 +1169,10 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1276,6 +1282,10 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -3241,13 +3251,16 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N89"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="77" t="s">
@@ -3520,7 +3533,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3539,15 +3552,12 @@
         <v>98</v>
       </c>
       <c r="C26" s="81">
-        <f>2.9/12</f>
-        <v>0.24166666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="D26" s="81">
-        <f>1.23/12</f>
-        <v>0.10249999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="E26" s="81">
-        <f>6/12</f>
         <v>0.5</v>
       </c>
     </row>
@@ -3631,7 +3641,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -3771,185 +3781,191 @@
       <c r="E42" s="38"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="55"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="68"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="55"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="68"/>
+      <c r="B45" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="69">
+        <v>0.4</v>
+      </c>
+      <c r="D45" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="E45" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="55"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="56"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="56"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="38"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="56"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="56"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
-      <c r="C44" s="7" t="s">
+    <row r="50" spans="1:9">
+      <c r="C50" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D50" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E50" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
-      <c r="B45" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="51">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D45" s="51">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E45" s="51">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="B46" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="51">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D46" s="51">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E46" s="51">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="B47" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" s="51">
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="D47" s="51">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="E47" s="51">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="B48" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="51">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="D48" s="51">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E48" s="51">
-        <v>1.01E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="B49" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="51">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="D49" s="51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E49" s="51">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="B50" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="51">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="D50" s="51">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="E50" s="51">
-        <v>0.432</v>
-      </c>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
     </row>
     <row r="51" spans="1:9">
       <c r="B51" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C51" s="51">
-        <v>0.23</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="D51" s="51">
-        <v>0.15</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="E51" s="51">
-        <v>0.3</v>
-      </c>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
+        <v>4.4000000000000003E-3</v>
+      </c>
     </row>
     <row r="52" spans="1:9">
       <c r="B52" s="3" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C52" s="51">
-        <v>2.17</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="D52" s="51">
-        <v>1.27</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="E52" s="51">
-        <v>3.71</v>
-      </c>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
+        <v>4.4000000000000003E-3</v>
+      </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="38"/>
-      <c r="B53" s="52"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
+      <c r="B53" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="51">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D53" s="51">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E53" s="51">
+        <v>7.1000000000000004E-3</v>
+      </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="38"/>
-      <c r="B54" s="52"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
+      <c r="B54" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="51">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D54" s="51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E54" s="51">
+        <v>1.01E-2</v>
+      </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="38"/>
-      <c r="B55" s="52"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
+      <c r="B55" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="51">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D55" s="51">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E55" s="51">
+        <v>7.9000000000000001E-2</v>
+      </c>
       <c r="F55" s="38"/>
       <c r="G55" s="38"/>
       <c r="H55" s="38"/>
       <c r="I55" s="38"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="2" t="s">
-        <v>110</v>
+      <c r="B56" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="51">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D56" s="51">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E56" s="51">
+        <v>0.432</v>
       </c>
       <c r="F56" s="38"/>
       <c r="G56" s="38"/>
@@ -3957,14 +3973,17 @@
       <c r="I56" s="38"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="C57" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>28</v>
+      <c r="B57" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="51">
+        <v>0.23</v>
+      </c>
+      <c r="D57" s="51">
+        <v>0.15</v>
+      </c>
+      <c r="E57" s="51">
+        <v>0.3</v>
       </c>
       <c r="F57" s="38"/>
       <c r="G57" s="38"/>
@@ -3973,359 +3992,348 @@
     </row>
     <row r="58" spans="1:9">
       <c r="B58" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="D58" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="E58" s="45">
-        <v>0.98</v>
+        <v>109</v>
+      </c>
+      <c r="C58" s="51">
+        <v>2.17</v>
+      </c>
+      <c r="D58" s="51">
+        <v>1.27</v>
+      </c>
+      <c r="E58" s="51">
+        <v>3.71</v>
       </c>
       <c r="F58" s="38"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
-      <c r="I58" s="54"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="B59" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C59" s="45">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D59" s="45">
-        <v>0.47</v>
-      </c>
-      <c r="E59" s="45">
-        <v>0.67</v>
-      </c>
+      <c r="A59" s="38"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
       <c r="F59" s="38"/>
-      <c r="G59" s="54"/>
-      <c r="H59" s="54"/>
-      <c r="I59" s="54"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="B60" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" s="45">
-        <v>0</v>
-      </c>
-      <c r="D60" s="45">
-        <v>0</v>
-      </c>
-      <c r="E60" s="45">
-        <v>0.68</v>
-      </c>
+      <c r="A60" s="38"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
       <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="B61" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C61" s="45">
-        <v>2.65</v>
-      </c>
-      <c r="D61" s="45">
-        <v>1.35</v>
-      </c>
-      <c r="E61" s="45">
-        <v>5.19</v>
-      </c>
+      <c r="A61" s="38"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
       <c r="F61" s="38"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="54"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="B62" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C62" s="45">
-        <v>0.54</v>
-      </c>
-      <c r="D62" s="45">
-        <v>0.33</v>
-      </c>
-      <c r="E62" s="45">
-        <v>0.68</v>
+      <c r="A62" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="F62" s="38"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="54"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="B63" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C63" s="45">
-        <v>0.9</v>
-      </c>
-      <c r="D63" s="45">
-        <v>0.82</v>
-      </c>
-      <c r="E63" s="45">
-        <v>0.93</v>
+      <c r="C63" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F63" s="38"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="54"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
     </row>
     <row r="64" spans="1:9">
       <c r="B64" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C64" s="45">
-        <v>0.73</v>
+        <v>0.95</v>
       </c>
       <c r="D64" s="45">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="E64" s="45">
-        <v>0.8</v>
+        <v>0.98</v>
       </c>
       <c r="F64" s="38"/>
       <c r="G64" s="54"/>
       <c r="H64" s="54"/>
       <c r="I64" s="54"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C65" s="45">
-        <v>0.5</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D65" s="45">
-        <v>0.3</v>
+        <v>0.47</v>
       </c>
       <c r="E65" s="45">
-        <v>0.8</v>
+        <v>0.67</v>
       </c>
       <c r="F65" s="38"/>
       <c r="G65" s="54"/>
       <c r="H65" s="54"/>
       <c r="I65" s="54"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:9">
       <c r="B66" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" s="45">
+        <v>0</v>
+      </c>
+      <c r="D66" s="45">
+        <v>0</v>
+      </c>
+      <c r="E66" s="45">
+        <v>0.68</v>
+      </c>
+      <c r="F66" s="38"/>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="B67" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" s="45">
+        <v>2.65</v>
+      </c>
+      <c r="D67" s="45">
+        <v>1.35</v>
+      </c>
+      <c r="E67" s="45">
+        <v>5.19</v>
+      </c>
+      <c r="F67" s="38"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="54"/>
+      <c r="I67" s="54"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="B68" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="45">
+        <v>0.54</v>
+      </c>
+      <c r="D68" s="45">
+        <v>0.33</v>
+      </c>
+      <c r="E68" s="45">
+        <v>0.68</v>
+      </c>
+      <c r="F68" s="38"/>
+      <c r="G68" s="54"/>
+      <c r="H68" s="54"/>
+      <c r="I68" s="54"/>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="B69" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" s="45">
+        <v>0.9</v>
+      </c>
+      <c r="D69" s="45">
+        <v>0.82</v>
+      </c>
+      <c r="E69" s="45">
+        <v>0.93</v>
+      </c>
+      <c r="F69" s="38"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="54"/>
+      <c r="I69" s="54"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="B70" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="45">
+        <v>0.73</v>
+      </c>
+      <c r="D70" s="45">
+        <v>0.65</v>
+      </c>
+      <c r="E70" s="45">
+        <v>0.8</v>
+      </c>
+      <c r="F70" s="38"/>
+      <c r="G70" s="54"/>
+      <c r="H70" s="54"/>
+      <c r="I70" s="54"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="B71" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="D71" s="45">
+        <v>0.3</v>
+      </c>
+      <c r="E71" s="45">
+        <v>0.8</v>
+      </c>
+      <c r="F71" s="38"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="54"/>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="B72" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C66" s="45">
+      <c r="C72" s="45">
         <v>0.92</v>
       </c>
-      <c r="D66" s="45">
+      <c r="D72" s="45">
         <v>0.8</v>
       </c>
-      <c r="E66" s="45">
+      <c r="E72" s="45">
         <v>0.95</v>
       </c>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" s="38"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="38"/>
-      <c r="I67" s="38"/>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" s="60"/>
-      <c r="B68" s="61"/>
-      <c r="C68" s="67"/>
-      <c r="D68" s="67"/>
-      <c r="E68" s="67"/>
-      <c r="F68" s="67"/>
-      <c r="G68" s="67"/>
-      <c r="H68" s="67"/>
-      <c r="I68" s="38"/>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" s="67"/>
-      <c r="B69" s="61"/>
-      <c r="C69" s="62"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="67"/>
-      <c r="G69" s="67"/>
-      <c r="H69" s="67"/>
-      <c r="I69" s="38"/>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="B70" s="68"/>
-      <c r="C70" s="68"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="68"/>
-      <c r="F70" s="67"/>
-      <c r="G70" s="67"/>
-      <c r="H70" s="67"/>
-      <c r="I70" s="38"/>
-      <c r="J70" s="55"/>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="68"/>
-      <c r="B71" s="68"/>
-      <c r="C71" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E71" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="F71" s="67"/>
-      <c r="G71" s="67"/>
-      <c r="H71" s="67"/>
-      <c r="I71" s="38"/>
-      <c r="J71" s="55"/>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="68"/>
-      <c r="B72" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="C72" s="69">
-        <v>0.4</v>
-      </c>
-      <c r="D72" s="69">
-        <v>0.3</v>
-      </c>
-      <c r="E72" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="F72" s="67"/>
-      <c r="G72" s="67"/>
-      <c r="H72" s="67"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
       <c r="I72" s="38"/>
-      <c r="J72" s="55"/>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="68"/>
-      <c r="B73" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" s="69">
-        <v>0.4</v>
-      </c>
-      <c r="D73" s="69">
-        <v>0.3</v>
-      </c>
-      <c r="E73" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="F73" s="67"/>
-      <c r="G73" s="67"/>
-      <c r="H73" s="67"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="38"/>
+      <c r="B73" s="52"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
       <c r="I73" s="38"/>
     </row>
-    <row r="74" spans="1:10">
-      <c r="A74" s="68"/>
-      <c r="B74" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" s="69">
-        <v>0.4</v>
-      </c>
-      <c r="D74" s="69">
-        <v>0.3</v>
-      </c>
-      <c r="E74" s="69">
-        <v>0.5</v>
-      </c>
+    <row r="74" spans="1:9">
+      <c r="A74" s="60"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="67"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="67"/>
       <c r="F74" s="67"/>
       <c r="G74" s="67"/>
       <c r="H74" s="67"/>
       <c r="I74" s="38"/>
     </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="56"/>
-      <c r="B75" s="56"/>
-      <c r="C75" s="56"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="56"/>
+    <row r="75" spans="1:9">
+      <c r="A75" s="67"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="62"/>
+      <c r="D75" s="62"/>
+      <c r="E75" s="62"/>
       <c r="F75" s="67"/>
       <c r="G75" s="67"/>
       <c r="H75" s="67"/>
       <c r="I75" s="38"/>
     </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="56"/>
+    <row r="76" spans="1:9">
+      <c r="A76" s="63" t="s">
+        <v>120</v>
+      </c>
       <c r="B76" s="56"/>
       <c r="C76" s="56"/>
       <c r="D76" s="56"/>
       <c r="E76" s="56"/>
-      <c r="F76" s="67"/>
-      <c r="G76" s="67"/>
-      <c r="H76" s="67"/>
-      <c r="I76" s="38"/>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="F76" s="56"/>
+      <c r="G76" s="56"/>
+      <c r="H76" s="56"/>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" s="56"/>
       <c r="B77" s="56"/>
-      <c r="C77" s="56"/>
-      <c r="D77" s="56"/>
-      <c r="E77" s="56"/>
+      <c r="C77" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" s="64" t="s">
+        <v>28</v>
+      </c>
       <c r="F77" s="56"/>
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
     </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="63" t="s">
-        <v>120</v>
-      </c>
-      <c r="B78" s="56"/>
-      <c r="C78" s="56"/>
-      <c r="D78" s="56"/>
-      <c r="E78" s="56"/>
+    <row r="78" spans="1:9">
+      <c r="A78" s="56"/>
+      <c r="B78" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" s="66">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D78" s="66">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E78" s="66">
+        <v>0.20499999999999999</v>
+      </c>
       <c r="F78" s="56"/>
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:9">
       <c r="A79" s="56"/>
-      <c r="B79" s="56"/>
-      <c r="C79" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D79" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="E79" s="64" t="s">
-        <v>28</v>
+      <c r="B79" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="66">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D79" s="66">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E79" s="66">
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F79" s="56"/>
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:9">
       <c r="A80" s="56"/>
       <c r="B80" s="65" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C80" s="66">
-        <v>0.14599999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="D80" s="66">
-        <v>9.6000000000000002E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="E80" s="66">
-        <v>0.20499999999999999</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F80" s="56"/>
       <c r="G80" s="56"/>
@@ -4334,16 +4342,16 @@
     <row r="81" spans="1:8">
       <c r="A81" s="56"/>
       <c r="B81" s="65" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C81" s="66">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D81" s="66">
-        <v>5.0000000000000001E-3</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E81" s="66">
-        <v>1.0999999999999999E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="F81" s="56"/>
       <c r="G81" s="56"/>
@@ -4352,16 +4360,16 @@
     <row r="82" spans="1:8">
       <c r="A82" s="56"/>
       <c r="B82" s="65" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C82" s="66">
-        <v>0.02</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="D82" s="66">
-        <v>1.2999999999999999E-2</v>
+        <v>0.114</v>
       </c>
       <c r="E82" s="66">
-        <v>2.9000000000000001E-2</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="F82" s="56"/>
       <c r="G82" s="56"/>
@@ -4370,16 +4378,16 @@
     <row r="83" spans="1:8">
       <c r="A83" s="56"/>
       <c r="B83" s="65" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C83" s="66">
-        <v>7.0000000000000007E-2</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="D83" s="66">
-        <v>4.8000000000000001E-2</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="E83" s="66">
-        <v>9.4E-2</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="F83" s="56"/>
       <c r="G83" s="56"/>
@@ -4388,53 +4396,27 @@
     <row r="84" spans="1:8">
       <c r="A84" s="56"/>
       <c r="B84" s="65" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C84" s="66">
-        <v>0.26500000000000001</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D84" s="66">
-        <v>0.114</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E84" s="66">
-        <v>0.47399999999999998</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F84" s="56"/>
       <c r="G84" s="56"/>
       <c r="H84" s="56"/>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="56"/>
-      <c r="B85" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="C85" s="66">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="D85" s="66">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="E85" s="66">
-        <v>0.71499999999999997</v>
-      </c>
       <c r="F85" s="56"/>
       <c r="G85" s="56"/>
       <c r="H85" s="56"/>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="56"/>
-      <c r="B86" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="C86" s="66">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D86" s="66">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="E86" s="66">
-        <v>7.9000000000000001E-2</v>
-      </c>
       <c r="F86" s="56"/>
       <c r="G86" s="56"/>
       <c r="H86" s="56"/>
@@ -4443,16 +4425,6 @@
       <c r="F87" s="56"/>
       <c r="G87" s="56"/>
       <c r="H87" s="56"/>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="F88" s="56"/>
-      <c r="G88" s="56"/>
-      <c r="H88" s="56"/>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="F89" s="56"/>
-      <c r="G89" s="56"/>
-      <c r="H89" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -10040,7 +10012,7 @@
     </row>
     <row r="60" spans="1:35">
       <c r="A60" s="71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B60" s="70"/>
       <c r="C60" s="70"/>
@@ -10244,7 +10216,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:25">

</xml_diff>

<commit_message>
very reduced model runs now
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="133">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -531,9 +531,6 @@
     <t>Treated HIV</t>
   </si>
   <si>
-    <t>People on unsuppressive ART who recover (%)</t>
-  </si>
-  <si>
     <t>People on ART with viral suppression (%)</t>
   </si>
   <si>
@@ -546,7 +543,7 @@
     <t>Treatment recovery on suppressive ART (average years to move)</t>
   </si>
   <si>
-    <t>Treatment recovery on unsuppressive ART</t>
+    <t>CD4 change due to non-suppressive ART (% per year)</t>
   </si>
 </sst>
 </file>
@@ -949,7 +946,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1092,7 +1089,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1110,9 +1106,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="9" fontId="12" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
@@ -1139,10 +1132,15 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="12" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="161">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1815,15 +1813,15 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="82"/>
+      <c r="A2" s="81"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="82"/>
+      <c r="A3" s="81"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
@@ -3251,10 +3249,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3263,129 +3261,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="76" t="s">
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="76" t="s">
+      <c r="E2" s="74" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="75"/>
-      <c r="B3" s="78" t="s">
+      <c r="A3" s="73"/>
+      <c r="B3" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="79">
+      <c r="C3" s="77">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="77">
         <v>1E-4</v>
       </c>
-      <c r="E3" s="79">
+      <c r="E3" s="77">
         <v>1.4E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="75"/>
-      <c r="B4" s="78" t="s">
+      <c r="A4" s="73"/>
+      <c r="B4" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="77">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D4" s="79">
+      <c r="D4" s="77">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="77">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="75"/>
-      <c r="B5" s="78" t="s">
+      <c r="A5" s="73"/>
+      <c r="B5" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="77">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="D5" s="79">
+      <c r="D5" s="77">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="E5" s="79">
+      <c r="E5" s="77">
         <v>2.8E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="75"/>
-      <c r="B6" s="78" t="s">
+      <c r="A6" s="73"/>
+      <c r="B6" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="77">
         <v>1.38E-2</v>
       </c>
-      <c r="D6" s="79">
+      <c r="D6" s="77">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="E6" s="79">
+      <c r="E6" s="77">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="75"/>
-      <c r="B7" s="78" t="s">
+      <c r="A7" s="73"/>
+      <c r="B7" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="77">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D7" s="79">
+      <c r="D7" s="77">
         <v>6.3E-3</v>
       </c>
-      <c r="E7" s="79">
+      <c r="E7" s="77">
         <v>2.4E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="75"/>
-      <c r="B8" s="78" t="s">
+      <c r="A8" s="73"/>
+      <c r="B8" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="77">
         <v>0.36699999999999999</v>
       </c>
-      <c r="D8" s="79">
+      <c r="D8" s="77">
         <v>0.29399999999999998</v>
       </c>
-      <c r="E8" s="79">
+      <c r="E8" s="77">
         <v>0.44</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="75"/>
-      <c r="B9" s="78" t="s">
+      <c r="A9" s="73"/>
+      <c r="B9" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="77">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D9" s="79">
+      <c r="D9" s="77">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E9" s="79">
+      <c r="E9" s="77">
         <v>0.27</v>
       </c>
     </row>
@@ -3430,13 +3428,13 @@
       <c r="B15" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="80">
+      <c r="C15" s="78">
         <v>5.6</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="78">
         <v>3.3</v>
       </c>
-      <c r="E15" s="80">
+      <c r="E15" s="78">
         <v>9.1</v>
       </c>
     </row>
@@ -3533,7 +3531,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3551,13 +3549,13 @@
       <c r="B26" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="79">
         <v>0.24</v>
       </c>
-      <c r="D26" s="81">
+      <c r="D26" s="79">
         <v>0.1</v>
       </c>
-      <c r="E26" s="81">
+      <c r="E26" s="79">
         <v>0.5</v>
       </c>
     </row>
@@ -3565,28 +3563,28 @@
       <c r="B27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="81">
+      <c r="C27" s="79">
         <v>0.95</v>
       </c>
-      <c r="D27" s="81">
+      <c r="D27" s="79">
         <v>0.62</v>
       </c>
-      <c r="E27" s="81">
+      <c r="E27" s="79">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G27" s="83"/>
+      <c r="G27" s="80"/>
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="81">
+      <c r="C28" s="79">
         <v>3</v>
       </c>
-      <c r="D28" s="81">
+      <c r="D28" s="79">
         <v>2.83</v>
       </c>
-      <c r="E28" s="81">
+      <c r="E28" s="79">
         <v>3.16</v>
       </c>
     </row>
@@ -3594,13 +3592,13 @@
       <c r="B29" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="81">
+      <c r="C29" s="79">
         <v>3.74</v>
       </c>
-      <c r="D29" s="81">
+      <c r="D29" s="79">
         <v>3.48</v>
       </c>
-      <c r="E29" s="81">
+      <c r="E29" s="79">
         <v>4</v>
       </c>
     </row>
@@ -3608,13 +3606,13 @@
       <c r="B30" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="81">
+      <c r="C30" s="79">
         <v>1.5</v>
       </c>
-      <c r="D30" s="81">
+      <c r="D30" s="79">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E30" s="81">
+      <c r="E30" s="79">
         <v>2.25</v>
       </c>
     </row>
@@ -3641,7 +3639,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -3659,13 +3657,13 @@
       <c r="B36" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="81">
+      <c r="C36" s="79">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D36" s="81">
+      <c r="D36" s="79">
         <v>1.07</v>
       </c>
-      <c r="E36" s="81">
+      <c r="E36" s="79">
         <v>7.28</v>
       </c>
       <c r="G36" s="55"/>
@@ -3681,13 +3679,13 @@
       <c r="B37" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="81">
+      <c r="C37" s="79">
         <v>1.42</v>
       </c>
-      <c r="D37" s="81">
+      <c r="D37" s="79">
         <v>0.9</v>
       </c>
-      <c r="E37" s="81">
+      <c r="E37" s="79">
         <v>3.42</v>
       </c>
       <c r="G37" s="55"/>
@@ -3703,13 +3701,13 @@
       <c r="B38" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C38" s="81">
+      <c r="C38" s="79">
         <v>2.14</v>
       </c>
-      <c r="D38" s="81">
+      <c r="D38" s="79">
         <v>1.39</v>
       </c>
-      <c r="E38" s="81">
+      <c r="E38" s="79">
         <v>3.58</v>
       </c>
       <c r="G38" s="55"/>
@@ -3725,13 +3723,13 @@
       <c r="B39" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="81">
+      <c r="C39" s="79">
         <v>0.66</v>
       </c>
-      <c r="D39" s="81">
+      <c r="D39" s="79">
         <v>0.51</v>
       </c>
-      <c r="E39" s="81">
+      <c r="E39" s="79">
         <v>0.94</v>
       </c>
       <c r="G39" s="55"/>
@@ -3780,23 +3778,18 @@
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A43" s="57" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="67"/>
-      <c r="H43" s="67"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="55"/>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44" s="68"/>
-      <c r="B44" s="68"/>
+        <v>132</v>
+      </c>
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+    </row>
+    <row r="44" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A44" s="67"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="58" t="s">
         <v>30</v>
       </c>
@@ -3806,244 +3799,231 @@
       <c r="E44" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="F44" s="67"/>
-      <c r="G44" s="67"/>
-      <c r="H44" s="67"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="55"/>
-    </row>
-    <row r="45" spans="1:14">
-      <c r="A45" s="68"/>
-      <c r="B45" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="69">
-        <v>0.4</v>
-      </c>
-      <c r="D45" s="69">
-        <v>0.3</v>
-      </c>
-      <c r="E45" s="69">
-        <v>0.5</v>
-      </c>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
-      <c r="H45" s="67"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="55"/>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46" s="56"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="67"/>
-      <c r="I46" s="38"/>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="A47" s="56"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="38"/>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="A48" s="56"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="2" t="s">
+    </row>
+    <row r="45" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A45" s="67"/>
+      <c r="B45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="83">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D45" s="83">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E45" s="83">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A46" s="67"/>
+      <c r="B46" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="83">
+        <v>0.15</v>
+      </c>
+      <c r="D46" s="83">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E46" s="83">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A47" s="67"/>
+      <c r="B47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="D47" s="83">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E47" s="83">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A48" s="67"/>
+      <c r="B48" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="83">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D48" s="83">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E48" s="83">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A49" s="67"/>
+      <c r="B49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="83">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="D49" s="83">
+        <v>0.05</v>
+      </c>
+      <c r="E49" s="83">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A50" s="67"/>
+      <c r="B50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="83">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="D50" s="83">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E50" s="83">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A51" s="67"/>
+      <c r="B51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="83">
+        <v>0.09</v>
+      </c>
+      <c r="D51" s="83">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E51" s="83">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A52" s="67"/>
+      <c r="B52" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="83">
+        <v>0.111</v>
+      </c>
+      <c r="D52" s="83">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E52" s="83">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A53" s="84"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+    </row>
+    <row r="54" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A54" s="84"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+    </row>
+    <row r="55" spans="1:9" s="82" customFormat="1" ht="15" customHeight="1">
+      <c r="A55" s="84"/>
+      <c r="B55" s="84"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
-      <c r="C50" s="7" t="s">
+    <row r="57" spans="1:9">
+      <c r="C57" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E57" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="B51" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="51">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D51" s="51">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E51" s="51">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="B52" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="51">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D52" s="51">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E52" s="51">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="B53" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="51">
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="D53" s="51">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="E53" s="51">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="B54" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="51">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="D54" s="51">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E54" s="51">
-        <v>1.01E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="B55" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="51">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="D55" s="51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E55" s="51">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="38"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="B56" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="51">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="D56" s="51">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="E56" s="51">
-        <v>0.432</v>
-      </c>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="38"/>
-      <c r="I56" s="38"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="B57" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C57" s="51">
-        <v>0.23</v>
-      </c>
-      <c r="D57" s="51">
-        <v>0.15</v>
-      </c>
-      <c r="E57" s="51">
-        <v>0.3</v>
-      </c>
-      <c r="F57" s="38"/>
-      <c r="G57" s="38"/>
-      <c r="H57" s="38"/>
-      <c r="I57" s="38"/>
     </row>
     <row r="58" spans="1:9">
       <c r="B58" s="3" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C58" s="51">
-        <v>2.17</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="D58" s="51">
-        <v>1.27</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="E58" s="51">
-        <v>3.71</v>
-      </c>
-      <c r="F58" s="38"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
+        <v>4.4000000000000003E-3</v>
+      </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="38"/>
-      <c r="B59" s="52"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
+      <c r="B59" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="51">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D59" s="51">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E59" s="51">
+        <v>4.4000000000000003E-3</v>
+      </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="38"/>
-      <c r="B60" s="52"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="38"/>
+      <c r="B60" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="51">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D60" s="51">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E60" s="51">
+        <v>7.1000000000000004E-3</v>
+      </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="38"/>
-      <c r="B61" s="52"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
-      <c r="I61" s="38"/>
+      <c r="B61" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="51">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D61" s="51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E61" s="51">
+        <v>1.01E-2</v>
+      </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="2" t="s">
-        <v>110</v>
+      <c r="B62" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="51">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D62" s="51">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E62" s="51">
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F62" s="38"/>
       <c r="G62" s="38"/>
@@ -4051,14 +4031,17 @@
       <c r="I62" s="38"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="C63" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>28</v>
+      <c r="B63" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="51">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D63" s="51">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E63" s="51">
+        <v>0.432</v>
       </c>
       <c r="F63" s="38"/>
       <c r="G63" s="38"/>
@@ -4067,139 +4050,109 @@
     </row>
     <row r="64" spans="1:9">
       <c r="B64" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C64" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="D64" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="E64" s="45">
-        <v>0.98</v>
+        <v>108</v>
+      </c>
+      <c r="C64" s="51">
+        <v>0.23</v>
+      </c>
+      <c r="D64" s="51">
+        <v>0.15</v>
+      </c>
+      <c r="E64" s="51">
+        <v>0.3</v>
       </c>
       <c r="F64" s="38"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="54"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
     </row>
     <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="45">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D65" s="45">
-        <v>0.47</v>
-      </c>
-      <c r="E65" s="45">
-        <v>0.67</v>
+        <v>109</v>
+      </c>
+      <c r="C65" s="51">
+        <v>2.17</v>
+      </c>
+      <c r="D65" s="51">
+        <v>1.27</v>
+      </c>
+      <c r="E65" s="51">
+        <v>3.71</v>
       </c>
       <c r="F65" s="38"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
     </row>
     <row r="66" spans="1:9">
-      <c r="B66" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C66" s="45">
-        <v>0</v>
-      </c>
-      <c r="D66" s="45">
-        <v>0</v>
-      </c>
-      <c r="E66" s="45">
-        <v>0.68</v>
-      </c>
+      <c r="A66" s="38"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
       <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="B67" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C67" s="45">
-        <v>2.65</v>
-      </c>
-      <c r="D67" s="45">
-        <v>1.35</v>
-      </c>
-      <c r="E67" s="45">
-        <v>5.19</v>
-      </c>
+      <c r="A67" s="38"/>
+      <c r="B67" s="52"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
       <c r="F67" s="38"/>
-      <c r="G67" s="54"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="54"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="B68" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C68" s="45">
-        <v>0.54</v>
-      </c>
-      <c r="D68" s="45">
-        <v>0.33</v>
-      </c>
-      <c r="E68" s="45">
-        <v>0.68</v>
-      </c>
+      <c r="A68" s="38"/>
+      <c r="B68" s="52"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
       <c r="F68" s="38"/>
-      <c r="G68" s="54"/>
-      <c r="H68" s="54"/>
-      <c r="I68" s="54"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="B69" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C69" s="45">
-        <v>0.9</v>
-      </c>
-      <c r="D69" s="45">
-        <v>0.82</v>
-      </c>
-      <c r="E69" s="45">
-        <v>0.93</v>
+      <c r="A69" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="F69" s="38"/>
-      <c r="G69" s="54"/>
-      <c r="H69" s="54"/>
-      <c r="I69" s="54"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="B70" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C70" s="45">
-        <v>0.73</v>
-      </c>
-      <c r="D70" s="45">
-        <v>0.65</v>
-      </c>
-      <c r="E70" s="45">
-        <v>0.8</v>
+      <c r="C70" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F70" s="38"/>
-      <c r="G70" s="54"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="54"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
     </row>
     <row r="71" spans="1:9">
       <c r="B71" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C71" s="45">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="D71" s="45">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="E71" s="45">
-        <v>0.8</v>
+        <v>0.98</v>
       </c>
       <c r="F71" s="38"/>
       <c r="G71" s="54"/>
@@ -4208,223 +4161,346 @@
     </row>
     <row r="72" spans="1:9">
       <c r="B72" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" s="45">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D72" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="E72" s="45">
+        <v>0.67</v>
+      </c>
+      <c r="F72" s="38"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="54"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="B73" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C73" s="45">
+        <v>0</v>
+      </c>
+      <c r="D73" s="45">
+        <v>0</v>
+      </c>
+      <c r="E73" s="45">
+        <v>0.68</v>
+      </c>
+      <c r="F73" s="38"/>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="B74" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74" s="45">
+        <v>2.65</v>
+      </c>
+      <c r="D74" s="45">
+        <v>1.35</v>
+      </c>
+      <c r="E74" s="45">
+        <v>5.19</v>
+      </c>
+      <c r="F74" s="38"/>
+      <c r="G74" s="54"/>
+      <c r="H74" s="54"/>
+      <c r="I74" s="54"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="B75" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C75" s="45">
+        <v>0.54</v>
+      </c>
+      <c r="D75" s="45">
+        <v>0.33</v>
+      </c>
+      <c r="E75" s="45">
+        <v>0.68</v>
+      </c>
+      <c r="F75" s="38"/>
+      <c r="G75" s="54"/>
+      <c r="H75" s="54"/>
+      <c r="I75" s="54"/>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="B76" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C76" s="45">
+        <v>0.9</v>
+      </c>
+      <c r="D76" s="45">
+        <v>0.82</v>
+      </c>
+      <c r="E76" s="45">
+        <v>0.93</v>
+      </c>
+      <c r="F76" s="38"/>
+      <c r="G76" s="54"/>
+      <c r="H76" s="54"/>
+      <c r="I76" s="54"/>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="B77" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77" s="45">
+        <v>0.73</v>
+      </c>
+      <c r="D77" s="45">
+        <v>0.65</v>
+      </c>
+      <c r="E77" s="45">
+        <v>0.8</v>
+      </c>
+      <c r="F77" s="38"/>
+      <c r="G77" s="54"/>
+      <c r="H77" s="54"/>
+      <c r="I77" s="54"/>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="B78" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="D78" s="45">
+        <v>0.3</v>
+      </c>
+      <c r="E78" s="45">
+        <v>0.8</v>
+      </c>
+      <c r="F78" s="38"/>
+      <c r="G78" s="54"/>
+      <c r="H78" s="54"/>
+      <c r="I78" s="54"/>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="B79" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C72" s="45">
+      <c r="C79" s="45">
         <v>0.92</v>
       </c>
-      <c r="D72" s="45">
+      <c r="D79" s="45">
         <v>0.8</v>
       </c>
-      <c r="E72" s="45">
+      <c r="E79" s="45">
         <v>0.95</v>
       </c>
-      <c r="F72" s="38"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="38"/>
-      <c r="I72" s="38"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="38"/>
-      <c r="B73" s="52"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="F73" s="38"/>
-      <c r="G73" s="38"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="38"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="60"/>
-      <c r="B74" s="61"/>
-      <c r="C74" s="67"/>
-      <c r="D74" s="67"/>
-      <c r="E74" s="67"/>
-      <c r="F74" s="67"/>
-      <c r="G74" s="67"/>
-      <c r="H74" s="67"/>
-      <c r="I74" s="38"/>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="67"/>
-      <c r="B75" s="61"/>
-      <c r="C75" s="62"/>
-      <c r="D75" s="62"/>
-      <c r="E75" s="62"/>
-      <c r="F75" s="67"/>
-      <c r="G75" s="67"/>
-      <c r="H75" s="67"/>
-      <c r="I75" s="38"/>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="63" t="s">
+      <c r="F79" s="38"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="38"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="59"/>
+      <c r="B81" s="60"/>
+      <c r="C81" s="66"/>
+      <c r="D81" s="66"/>
+      <c r="E81" s="66"/>
+      <c r="F81" s="66"/>
+      <c r="G81" s="66"/>
+      <c r="H81" s="66"/>
+      <c r="I81" s="38"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="66"/>
+      <c r="B82" s="60"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
+      <c r="E82" s="61"/>
+      <c r="F82" s="66"/>
+      <c r="G82" s="66"/>
+      <c r="H82" s="66"/>
+      <c r="I82" s="38"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="B76" s="56"/>
-      <c r="C76" s="56"/>
-      <c r="D76" s="56"/>
-      <c r="E76" s="56"/>
-      <c r="F76" s="56"/>
-      <c r="G76" s="56"/>
-      <c r="H76" s="56"/>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="56"/>
-      <c r="B77" s="56"/>
-      <c r="C77" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D77" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="E77" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="F77" s="56"/>
-      <c r="G77" s="56"/>
-      <c r="H77" s="56"/>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="56"/>
-      <c r="B78" s="65" t="s">
-        <v>121</v>
-      </c>
-      <c r="C78" s="66">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D78" s="66">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E78" s="66">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="F78" s="56"/>
-      <c r="G78" s="56"/>
-      <c r="H78" s="56"/>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="56"/>
-      <c r="B79" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="C79" s="66">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D79" s="66">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E79" s="66">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F79" s="56"/>
-      <c r="G79" s="56"/>
-      <c r="H79" s="56"/>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="56"/>
-      <c r="B80" s="65" t="s">
-        <v>123</v>
-      </c>
-      <c r="C80" s="66">
-        <v>0.02</v>
-      </c>
-      <c r="D80" s="66">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E80" s="66">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F80" s="56"/>
-      <c r="G80" s="56"/>
-      <c r="H80" s="56"/>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="56"/>
-      <c r="B81" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="C81" s="66">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D81" s="66">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="E81" s="66">
-        <v>9.4E-2</v>
-      </c>
-      <c r="F81" s="56"/>
-      <c r="G81" s="56"/>
-      <c r="H81" s="56"/>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="56"/>
-      <c r="B82" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="C82" s="66">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D82" s="66">
-        <v>0.114</v>
-      </c>
-      <c r="E82" s="66">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="F82" s="56"/>
-      <c r="G82" s="56"/>
-      <c r="H82" s="56"/>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="56"/>
-      <c r="B83" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="C83" s="66">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="D83" s="66">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="E83" s="66">
-        <v>0.71499999999999997</v>
-      </c>
+      <c r="B83" s="56"/>
+      <c r="C83" s="56"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="56"/>
       <c r="F83" s="56"/>
       <c r="G83" s="56"/>
       <c r="H83" s="56"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:9">
       <c r="A84" s="56"/>
-      <c r="B84" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="C84" s="66">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D84" s="66">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="E84" s="66">
-        <v>7.9000000000000001E-2</v>
+      <c r="B84" s="56"/>
+      <c r="C84" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="E84" s="63" t="s">
+        <v>28</v>
       </c>
       <c r="F84" s="56"/>
       <c r="G84" s="56"/>
       <c r="H84" s="56"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:9">
+      <c r="A85" s="56"/>
+      <c r="B85" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C85" s="65">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D85" s="65">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E85" s="65">
+        <v>0.20499999999999999</v>
+      </c>
       <c r="F85" s="56"/>
       <c r="G85" s="56"/>
       <c r="H85" s="56"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:9">
+      <c r="A86" s="56"/>
+      <c r="B86" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C86" s="65">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D86" s="65">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E86" s="65">
+        <v>1.0999999999999999E-2</v>
+      </c>
       <c r="F86" s="56"/>
       <c r="G86" s="56"/>
       <c r="H86" s="56"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:9">
+      <c r="A87" s="56"/>
+      <c r="B87" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C87" s="65">
+        <v>0.02</v>
+      </c>
+      <c r="D87" s="65">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E87" s="65">
+        <v>2.9000000000000001E-2</v>
+      </c>
       <c r="F87" s="56"/>
       <c r="G87" s="56"/>
       <c r="H87" s="56"/>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="56"/>
+      <c r="B88" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C88" s="65">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D88" s="65">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E88" s="65">
+        <v>9.4E-2</v>
+      </c>
+      <c r="F88" s="56"/>
+      <c r="G88" s="56"/>
+      <c r="H88" s="56"/>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="56"/>
+      <c r="B89" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" s="65">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D89" s="65">
+        <v>0.114</v>
+      </c>
+      <c r="E89" s="65">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="F89" s="56"/>
+      <c r="G89" s="56"/>
+      <c r="H89" s="56"/>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="56"/>
+      <c r="B90" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C90" s="65">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D90" s="65">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E90" s="65">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F90" s="56"/>
+      <c r="G90" s="56"/>
+      <c r="H90" s="56"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="56"/>
+      <c r="B91" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C91" s="65">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D91" s="65">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E91" s="65">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F91" s="56"/>
+      <c r="G91" s="56"/>
+      <c r="H91" s="56"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="F92" s="56"/>
+      <c r="G92" s="56"/>
+      <c r="H92" s="56"/>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="F93" s="56"/>
+      <c r="G93" s="56"/>
+      <c r="H93" s="56"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="F94" s="56"/>
+      <c r="G94" s="56"/>
+      <c r="H94" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -10011,185 +10087,185 @@
       <c r="Y56" s="32"/>
     </row>
     <row r="60" spans="1:35">
-      <c r="A60" s="71" t="s">
-        <v>129</v>
-      </c>
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="70"/>
-      <c r="G60" s="70"/>
-      <c r="H60" s="70"/>
-      <c r="I60" s="70"/>
-      <c r="J60" s="70"/>
-      <c r="K60" s="70"/>
-      <c r="L60" s="70"/>
-      <c r="M60" s="70"/>
-      <c r="N60" s="70"/>
-      <c r="O60" s="70"/>
-      <c r="P60" s="70"/>
-      <c r="Q60" s="70"/>
-      <c r="R60" s="70"/>
-      <c r="S60" s="70"/>
-      <c r="T60" s="70"/>
-      <c r="U60" s="70"/>
-      <c r="V60" s="70"/>
-      <c r="W60" s="70"/>
-      <c r="X60" s="70"/>
-      <c r="Y60" s="70"/>
-      <c r="Z60" s="70"/>
-      <c r="AA60" s="70"/>
-      <c r="AB60" s="70"/>
-      <c r="AC60" s="70"/>
-      <c r="AD60" s="70"/>
-      <c r="AE60" s="70"/>
-      <c r="AF60" s="70"/>
-      <c r="AG60" s="70"/>
-      <c r="AH60" s="70"/>
-      <c r="AI60" s="70"/>
+      <c r="A60" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" s="68"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="68"/>
+      <c r="F60" s="68"/>
+      <c r="G60" s="68"/>
+      <c r="H60" s="68"/>
+      <c r="I60" s="68"/>
+      <c r="J60" s="68"/>
+      <c r="K60" s="68"/>
+      <c r="L60" s="68"/>
+      <c r="M60" s="68"/>
+      <c r="N60" s="68"/>
+      <c r="O60" s="68"/>
+      <c r="P60" s="68"/>
+      <c r="Q60" s="68"/>
+      <c r="R60" s="68"/>
+      <c r="S60" s="68"/>
+      <c r="T60" s="68"/>
+      <c r="U60" s="68"/>
+      <c r="V60" s="68"/>
+      <c r="W60" s="68"/>
+      <c r="X60" s="68"/>
+      <c r="Y60" s="68"/>
+      <c r="Z60" s="68"/>
+      <c r="AA60" s="68"/>
+      <c r="AB60" s="68"/>
+      <c r="AC60" s="68"/>
+      <c r="AD60" s="68"/>
+      <c r="AE60" s="68"/>
+      <c r="AF60" s="68"/>
+      <c r="AG60" s="68"/>
+      <c r="AH60" s="68"/>
+      <c r="AI60" s="68"/>
     </row>
     <row r="61" spans="1:35">
-      <c r="A61" s="70"/>
-      <c r="B61" s="70"/>
-      <c r="C61" s="72">
+      <c r="A61" s="68"/>
+      <c r="B61" s="68"/>
+      <c r="C61" s="70">
         <v>2000</v>
       </c>
-      <c r="D61" s="72">
+      <c r="D61" s="70">
         <v>2001</v>
       </c>
-      <c r="E61" s="72">
+      <c r="E61" s="70">
         <v>2002</v>
       </c>
-      <c r="F61" s="72">
+      <c r="F61" s="70">
         <v>2003</v>
       </c>
-      <c r="G61" s="72">
+      <c r="G61" s="70">
         <v>2004</v>
       </c>
-      <c r="H61" s="72">
+      <c r="H61" s="70">
         <v>2005</v>
       </c>
-      <c r="I61" s="72">
+      <c r="I61" s="70">
         <v>2006</v>
       </c>
-      <c r="J61" s="72">
+      <c r="J61" s="70">
         <v>2007</v>
       </c>
-      <c r="K61" s="72">
+      <c r="K61" s="70">
         <v>2008</v>
       </c>
-      <c r="L61" s="72">
+      <c r="L61" s="70">
         <v>2009</v>
       </c>
-      <c r="M61" s="72">
+      <c r="M61" s="70">
         <v>2010</v>
       </c>
-      <c r="N61" s="72">
+      <c r="N61" s="70">
         <v>2011</v>
       </c>
-      <c r="O61" s="72">
+      <c r="O61" s="70">
         <v>2012</v>
       </c>
-      <c r="P61" s="72">
+      <c r="P61" s="70">
         <v>2013</v>
       </c>
-      <c r="Q61" s="72">
+      <c r="Q61" s="70">
         <v>2014</v>
       </c>
-      <c r="R61" s="72">
+      <c r="R61" s="70">
         <v>2015</v>
       </c>
-      <c r="S61" s="72">
+      <c r="S61" s="70">
         <v>2016</v>
       </c>
-      <c r="T61" s="72">
+      <c r="T61" s="70">
         <v>2017</v>
       </c>
-      <c r="U61" s="72">
+      <c r="U61" s="70">
         <v>2018</v>
       </c>
-      <c r="V61" s="72">
+      <c r="V61" s="70">
         <v>2019</v>
       </c>
-      <c r="W61" s="72">
+      <c r="W61" s="70">
         <v>2020</v>
       </c>
-      <c r="X61" s="72">
+      <c r="X61" s="70">
         <v>2021</v>
       </c>
-      <c r="Y61" s="72">
+      <c r="Y61" s="70">
         <v>2022</v>
       </c>
-      <c r="Z61" s="72">
+      <c r="Z61" s="70">
         <v>2023</v>
       </c>
-      <c r="AA61" s="72">
+      <c r="AA61" s="70">
         <v>2024</v>
       </c>
-      <c r="AB61" s="72">
+      <c r="AB61" s="70">
         <v>2025</v>
       </c>
-      <c r="AC61" s="72">
+      <c r="AC61" s="70">
         <v>2026</v>
       </c>
-      <c r="AD61" s="72">
+      <c r="AD61" s="70">
         <v>2027</v>
       </c>
-      <c r="AE61" s="72">
+      <c r="AE61" s="70">
         <v>2028</v>
       </c>
-      <c r="AF61" s="72">
+      <c r="AF61" s="70">
         <v>2029</v>
       </c>
-      <c r="AG61" s="72">
+      <c r="AG61" s="70">
         <v>2030</v>
       </c>
-      <c r="AH61" s="70"/>
-      <c r="AI61" s="72" t="s">
+      <c r="AH61" s="68"/>
+      <c r="AI61" s="70" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:35">
-      <c r="A62" s="70"/>
-      <c r="B62" s="72" t="s">
+      <c r="A62" s="68"/>
+      <c r="B62" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="73"/>
-      <c r="I62" s="73"/>
-      <c r="J62" s="73"/>
-      <c r="K62" s="73"/>
-      <c r="L62" s="73"/>
-      <c r="M62" s="73"/>
-      <c r="N62" s="73"/>
-      <c r="O62" s="73"/>
-      <c r="P62" s="73"/>
-      <c r="Q62" s="73"/>
-      <c r="R62" s="73"/>
-      <c r="S62" s="73"/>
-      <c r="T62" s="73"/>
-      <c r="U62" s="73"/>
-      <c r="V62" s="73"/>
-      <c r="W62" s="73"/>
-      <c r="X62" s="73"/>
-      <c r="Y62" s="73"/>
-      <c r="Z62" s="73"/>
-      <c r="AA62" s="73"/>
-      <c r="AB62" s="73"/>
-      <c r="AC62" s="73"/>
-      <c r="AD62" s="73"/>
-      <c r="AE62" s="73"/>
-      <c r="AF62" s="73"/>
-      <c r="AG62" s="73"/>
-      <c r="AH62" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI62" s="73">
+      <c r="C62" s="71"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="71"/>
+      <c r="F62" s="71"/>
+      <c r="G62" s="71"/>
+      <c r="H62" s="71"/>
+      <c r="I62" s="71"/>
+      <c r="J62" s="71"/>
+      <c r="K62" s="71"/>
+      <c r="L62" s="71"/>
+      <c r="M62" s="71"/>
+      <c r="N62" s="71"/>
+      <c r="O62" s="71"/>
+      <c r="P62" s="71"/>
+      <c r="Q62" s="71"/>
+      <c r="R62" s="71"/>
+      <c r="S62" s="71"/>
+      <c r="T62" s="71"/>
+      <c r="U62" s="71"/>
+      <c r="V62" s="71"/>
+      <c r="W62" s="71"/>
+      <c r="X62" s="71"/>
+      <c r="Y62" s="71"/>
+      <c r="Z62" s="71"/>
+      <c r="AA62" s="71"/>
+      <c r="AB62" s="71"/>
+      <c r="AC62" s="71"/>
+      <c r="AD62" s="71"/>
+      <c r="AE62" s="71"/>
+      <c r="AF62" s="71"/>
+      <c r="AG62" s="71"/>
+      <c r="AH62" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI62" s="71">
         <v>0.85</v>
       </c>
     </row>
@@ -10216,7 +10292,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -10318,7 +10394,7 @@
       <c r="X3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="81">
+      <c r="Y3" s="79">
         <v>3</v>
       </c>
     </row>
@@ -10352,7 +10428,7 @@
       <c r="X4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y4" s="81">
+      <c r="Y4" s="79">
         <v>3</v>
       </c>
     </row>
@@ -10385,7 +10461,7 @@
       <c r="X5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y5" s="81">
+      <c r="Y5" s="79">
         <v>3</v>
       </c>
     </row>
@@ -10417,7 +10493,7 @@
       <c r="X6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y6" s="81">
+      <c r="Y6" s="79">
         <v>3</v>
       </c>
     </row>
@@ -10451,7 +10527,7 @@
       <c r="X7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y7" s="81">
+      <c r="Y7" s="79">
         <v>3</v>
       </c>
     </row>
@@ -10485,7 +10561,7 @@
       <c r="X8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y8" s="81">
+      <c r="Y8" s="79">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
triumphantly remove off-art compartment
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="131">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -327,9 +327,6 @@
     <t>PLHIV in care on treatment (%)</t>
   </si>
   <si>
-    <t>Percentage of people who receive ART in the year who stop taking ART (%/year)</t>
-  </si>
-  <si>
     <t>Percentage of people in care who are lost to follow-up per year (%/year)</t>
   </si>
   <si>
@@ -337,9 +334,6 @@
   </si>
   <si>
     <t>Viral load monitoring (number/year)</t>
-  </si>
-  <si>
-    <t>Rate of ART re-initiation (%/year)</t>
   </si>
   <si>
     <t>Average number of acts with regular partners per person per year</t>
@@ -783,7 +777,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -913,6 +907,8 @@
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1142,7 +1138,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="163">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1171,6 +1167,7 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1284,6 +1281,7 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -1865,7 +1863,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -2135,7 +2133,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2405,7 +2403,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2531,7 +2529,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2646,7 +2644,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2761,7 +2759,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2866,7 +2864,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2971,7 +2969,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3026,7 +3024,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3129,7 +3127,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3251,8 +3249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3262,7 +3260,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="75" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3285,7 +3283,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="73"/>
       <c r="B3" s="76" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="77">
         <v>4.0000000000000002E-4</v>
@@ -3300,7 +3298,7 @@
     <row r="4" spans="1:5">
       <c r="A4" s="73"/>
       <c r="B4" s="76" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" s="77">
         <v>8.0000000000000004E-4</v>
@@ -3315,7 +3313,7 @@
     <row r="5" spans="1:5">
       <c r="A5" s="73"/>
       <c r="B5" s="76" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="77">
         <v>1.1000000000000001E-3</v>
@@ -3330,7 +3328,7 @@
     <row r="6" spans="1:5">
       <c r="A6" s="73"/>
       <c r="B6" s="76" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="77">
         <v>1.38E-2</v>
@@ -3345,7 +3343,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="73"/>
       <c r="B7" s="76" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" s="77">
         <v>8.0000000000000002E-3</v>
@@ -3360,7 +3358,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="73"/>
       <c r="B8" s="76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="77">
         <v>0.36699999999999999</v>
@@ -3375,7 +3373,7 @@
     <row r="9" spans="1:5">
       <c r="A9" s="73"/>
       <c r="B9" s="76" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" s="77">
         <v>0.20499999999999999</v>
@@ -3410,7 +3408,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3426,7 +3424,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C15" s="78">
         <v>5.6</v>
@@ -3440,7 +3438,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" s="53">
         <v>1</v>
@@ -3454,7 +3452,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="B17" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" s="53">
         <v>1</v>
@@ -3468,7 +3466,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" s="53">
         <v>1</v>
@@ -3482,7 +3480,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C19" s="53">
         <v>3.49</v>
@@ -3496,7 +3494,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C20" s="53">
         <v>7.17</v>
@@ -3531,7 +3529,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3547,7 +3545,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" s="79">
         <v>0.24</v>
@@ -3561,7 +3559,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C27" s="79">
         <v>0.95</v>
@@ -3576,7 +3574,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C28" s="79">
         <v>3</v>
@@ -3590,7 +3588,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C29" s="79">
         <v>3.74</v>
@@ -3604,7 +3602,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" s="79">
         <v>1.5</v>
@@ -3639,7 +3637,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -3655,7 +3653,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="B36" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C36" s="79">
         <v>2.2000000000000002</v>
@@ -3677,7 +3675,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="B37" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C37" s="79">
         <v>1.42</v>
@@ -3699,7 +3697,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="B38" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C38" s="79">
         <v>2.14</v>
@@ -3721,7 +3719,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="B39" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C39" s="79">
         <v>0.66</v>
@@ -3780,7 +3778,7 @@
     </row>
     <row r="43" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A43" s="57" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B43" s="67"/>
       <c r="C43" s="67"/>
@@ -3803,7 +3801,7 @@
     <row r="45" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A45" s="67"/>
       <c r="B45" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C45" s="83">
         <v>2.5999999999999999E-2</v>
@@ -3818,7 +3816,7 @@
     <row r="46" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A46" s="67"/>
       <c r="B46" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C46" s="83">
         <v>0.15</v>
@@ -3833,7 +3831,7 @@
     <row r="47" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A47" s="67"/>
       <c r="B47" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47" s="83">
         <v>0.1</v>
@@ -3848,7 +3846,7 @@
     <row r="48" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A48" s="67"/>
       <c r="B48" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C48" s="83">
         <v>5.2999999999999999E-2</v>
@@ -3863,7 +3861,7 @@
     <row r="49" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A49" s="67"/>
       <c r="B49" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C49" s="83">
         <v>0.16200000000000001</v>
@@ -3878,7 +3876,7 @@
     <row r="50" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A50" s="67"/>
       <c r="B50" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C50" s="83">
         <v>0.11700000000000001</v>
@@ -3893,7 +3891,7 @@
     <row r="51" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A51" s="67"/>
       <c r="B51" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="83">
         <v>0.09</v>
@@ -3908,7 +3906,7 @@
     <row r="52" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
       <c r="A52" s="67"/>
       <c r="B52" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C52" s="83">
         <v>0.111</v>
@@ -3942,7 +3940,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3958,7 +3956,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="B58" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C58" s="51">
         <v>3.5999999999999999E-3</v>
@@ -3972,7 +3970,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="B59" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C59" s="51">
         <v>3.5999999999999999E-3</v>
@@ -3986,7 +3984,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="B60" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C60" s="51">
         <v>5.7999999999999996E-3</v>
@@ -4000,7 +3998,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="B61" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C61" s="51">
         <v>8.8000000000000005E-3</v>
@@ -4014,7 +4012,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="B62" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C62" s="51">
         <v>5.8999999999999997E-2</v>
@@ -4032,7 +4030,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="B63" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C63" s="51">
         <v>0.32300000000000001</v>
@@ -4050,7 +4048,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="B64" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" s="51">
         <v>0.23</v>
@@ -4068,7 +4066,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C65" s="51">
         <v>2.17</v>
@@ -4119,7 +4117,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F69" s="38"/>
       <c r="G69" s="38"/>
@@ -4143,7 +4141,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="B71" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C71" s="45">
         <v>0.95</v>
@@ -4161,7 +4159,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="B72" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C72" s="45">
         <v>0.57999999999999996</v>
@@ -4179,7 +4177,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="B73" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C73" s="45">
         <v>0</v>
@@ -4194,7 +4192,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="B74" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C74" s="45">
         <v>2.65</v>
@@ -4212,7 +4210,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="B75" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C75" s="45">
         <v>0.54</v>
@@ -4230,7 +4228,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="B76" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C76" s="45">
         <v>0.9</v>
@@ -4248,7 +4246,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="B77" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C77" s="45">
         <v>0.73</v>
@@ -4266,7 +4264,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="B78" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C78" s="45">
         <v>0.5</v>
@@ -4284,7 +4282,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="B79" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C79" s="45">
         <v>0.92</v>
@@ -4335,7 +4333,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B83" s="56"/>
       <c r="C83" s="56"/>
@@ -4364,7 +4362,7 @@
     <row r="85" spans="1:9">
       <c r="A85" s="56"/>
       <c r="B85" s="64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C85" s="65">
         <v>0.14599999999999999</v>
@@ -4382,7 +4380,7 @@
     <row r="86" spans="1:9">
       <c r="A86" s="56"/>
       <c r="B86" s="64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C86" s="65">
         <v>8.0000000000000002E-3</v>
@@ -4400,7 +4398,7 @@
     <row r="87" spans="1:9">
       <c r="A87" s="56"/>
       <c r="B87" s="64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C87" s="65">
         <v>0.02</v>
@@ -4418,7 +4416,7 @@
     <row r="88" spans="1:9">
       <c r="A88" s="56"/>
       <c r="B88" s="64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C88" s="65">
         <v>7.0000000000000007E-2</v>
@@ -4436,7 +4434,7 @@
     <row r="89" spans="1:9">
       <c r="A89" s="56"/>
       <c r="B89" s="64" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C89" s="65">
         <v>0.26500000000000001</v>
@@ -4454,7 +4452,7 @@
     <row r="90" spans="1:9">
       <c r="A90" s="56"/>
       <c r="B90" s="64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C90" s="65">
         <v>0.54700000000000004</v>
@@ -4472,7 +4470,7 @@
     <row r="91" spans="1:9">
       <c r="A91" s="56"/>
       <c r="B91" s="64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C91" s="65">
         <v>5.2999999999999999E-2</v>
@@ -10088,7 +10086,7 @@
     </row>
     <row r="60" spans="1:35">
       <c r="A60" s="69" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B60" s="68"/>
       <c r="C60" s="68"/>
@@ -10282,17 +10280,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y48"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -10842,669 +10840,266 @@
       <c r="A23" s="29" t="s">
         <v>61</v>
       </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="C24" s="7">
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31">
         <v>2000</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="31">
         <v>2001</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="31">
         <v>2002</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="31">
         <v>2003</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="31">
         <v>2004</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="31">
         <v>2005</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="31">
         <v>2006</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="31">
         <v>2007</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="31">
         <v>2008</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="31">
         <v>2009</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="31">
         <v>2010</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="31">
         <v>2011</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="31">
         <v>2012</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24" s="31">
         <v>2013</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="Q24" s="31">
         <v>2014</v>
       </c>
-      <c r="R24" s="7">
+      <c r="R24" s="31">
         <v>2015</v>
       </c>
-      <c r="S24" s="7">
+      <c r="S24" s="31">
         <v>2016</v>
       </c>
-      <c r="T24" s="7">
+      <c r="T24" s="31">
         <v>2017</v>
       </c>
-      <c r="U24" s="7">
+      <c r="U24" s="31">
         <v>2018</v>
       </c>
-      <c r="V24" s="7">
+      <c r="V24" s="31">
         <v>2019</v>
       </c>
-      <c r="W24" s="7">
+      <c r="W24" s="31">
         <v>2020</v>
       </c>
-      <c r="Y24" s="7" t="s">
+      <c r="X24" s="30"/>
+      <c r="Y24" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:25">
-      <c r="B25" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>FSW</v>
-      </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="45"/>
-      <c r="W25" s="45"/>
-      <c r="X25" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y25" s="45">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
-      <c r="B26" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>Clients</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="45"/>
-      <c r="X26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y26" s="45">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
-      <c r="B27" s="7" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
-      </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45"/>
-      <c r="V27" s="45"/>
-      <c r="W27" s="45"/>
-      <c r="X27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y27" s="45">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
-      <c r="B28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="45"/>
-      <c r="W28" s="45"/>
-      <c r="X28" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y28" s="45">
-        <v>0.8</v>
+      <c r="A25" s="30"/>
+      <c r="B25" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y25" s="32">
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:25">
-      <c r="B29" s="7" t="str">
-        <f>Populations!$C$7</f>
-        <v>M 15+</v>
-      </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="45"/>
-      <c r="V29" s="45"/>
-      <c r="W29" s="45"/>
-      <c r="X29" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y29" s="45">
-        <v>0.8</v>
-      </c>
+      <c r="A29" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+      <c r="X29" s="30"/>
+      <c r="Y29" s="30"/>
     </row>
     <row r="30" spans="1:25">
-      <c r="B30" s="7" t="str">
-        <f>Populations!$C$8</f>
-        <v>F 15+</v>
-      </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="45"/>
-      <c r="U30" s="45"/>
-      <c r="V30" s="45"/>
-      <c r="W30" s="45"/>
-      <c r="X30" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y30" s="45">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25">
-      <c r="A34" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="30"/>
-    </row>
-    <row r="35" spans="1:25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31">
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31">
         <v>2000</v>
       </c>
-      <c r="D35" s="31">
+      <c r="D30" s="31">
         <v>2001</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E30" s="31">
         <v>2002</v>
       </c>
-      <c r="F35" s="31">
+      <c r="F30" s="31">
         <v>2003</v>
       </c>
-      <c r="G35" s="31">
+      <c r="G30" s="31">
         <v>2004</v>
       </c>
-      <c r="H35" s="31">
+      <c r="H30" s="31">
         <v>2005</v>
       </c>
-      <c r="I35" s="31">
+      <c r="I30" s="31">
         <v>2006</v>
       </c>
-      <c r="J35" s="31">
+      <c r="J30" s="31">
         <v>2007</v>
       </c>
-      <c r="K35" s="31">
+      <c r="K30" s="31">
         <v>2008</v>
       </c>
-      <c r="L35" s="31">
+      <c r="L30" s="31">
         <v>2009</v>
       </c>
-      <c r="M35" s="31">
+      <c r="M30" s="31">
         <v>2010</v>
       </c>
-      <c r="N35" s="31">
+      <c r="N30" s="31">
         <v>2011</v>
       </c>
-      <c r="O35" s="31">
+      <c r="O30" s="31">
         <v>2012</v>
       </c>
-      <c r="P35" s="31">
+      <c r="P30" s="31">
         <v>2013</v>
       </c>
-      <c r="Q35" s="31">
+      <c r="Q30" s="31">
         <v>2014</v>
       </c>
-      <c r="R35" s="31">
+      <c r="R30" s="31">
         <v>2015</v>
       </c>
-      <c r="S35" s="31">
+      <c r="S30" s="31">
         <v>2016</v>
       </c>
-      <c r="T35" s="31">
+      <c r="T30" s="31">
         <v>2017</v>
       </c>
-      <c r="U35" s="31">
+      <c r="U30" s="31">
         <v>2018</v>
       </c>
-      <c r="V35" s="31">
+      <c r="V30" s="31">
         <v>2019</v>
       </c>
-      <c r="W35" s="31">
+      <c r="W30" s="31">
         <v>2020</v>
       </c>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="31" t="s">
+      <c r="X30" s="30"/>
+      <c r="Y30" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31" t="s">
+    <row r="31" spans="1:25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="32"/>
-      <c r="R36" s="32"/>
-      <c r="S36" s="32"/>
-      <c r="T36" s="32"/>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="32"/>
-      <c r="X36" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y36" s="32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25">
-      <c r="A40" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="30"/>
-      <c r="S40" s="30"/>
-      <c r="T40" s="30"/>
-      <c r="U40" s="30"/>
-      <c r="V40" s="30"/>
-      <c r="W40" s="30"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-    </row>
-    <row r="41" spans="1:25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31">
-        <v>2000</v>
-      </c>
-      <c r="D41" s="31">
-        <v>2001</v>
-      </c>
-      <c r="E41" s="31">
-        <v>2002</v>
-      </c>
-      <c r="F41" s="31">
-        <v>2003</v>
-      </c>
-      <c r="G41" s="31">
-        <v>2004</v>
-      </c>
-      <c r="H41" s="31">
-        <v>2005</v>
-      </c>
-      <c r="I41" s="31">
-        <v>2006</v>
-      </c>
-      <c r="J41" s="31">
-        <v>2007</v>
-      </c>
-      <c r="K41" s="31">
-        <v>2008</v>
-      </c>
-      <c r="L41" s="31">
-        <v>2009</v>
-      </c>
-      <c r="M41" s="31">
-        <v>2010</v>
-      </c>
-      <c r="N41" s="31">
-        <v>2011</v>
-      </c>
-      <c r="O41" s="31">
-        <v>2012</v>
-      </c>
-      <c r="P41" s="31">
-        <v>2013</v>
-      </c>
-      <c r="Q41" s="31">
-        <v>2014</v>
-      </c>
-      <c r="R41" s="31">
-        <v>2015</v>
-      </c>
-      <c r="S41" s="31">
-        <v>2016</v>
-      </c>
-      <c r="T41" s="31">
-        <v>2017</v>
-      </c>
-      <c r="U41" s="31">
-        <v>2018</v>
-      </c>
-      <c r="V41" s="31">
-        <v>2019</v>
-      </c>
-      <c r="W41" s="31">
-        <v>2020</v>
-      </c>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="46"/>
-      <c r="N42" s="46"/>
-      <c r="O42" s="46"/>
-      <c r="P42" s="46"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="46"/>
-      <c r="S42" s="46"/>
-      <c r="T42" s="46"/>
-      <c r="U42" s="46"/>
-      <c r="V42" s="46"/>
-      <c r="W42" s="46"/>
-      <c r="X42" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y42" s="47">
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="46"/>
+      <c r="V31" s="46"/>
+      <c r="W31" s="46"/>
+      <c r="X31" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y31" s="47">
         <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25">
-      <c r="A46" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30"/>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="30"/>
-      <c r="S46" s="30"/>
-      <c r="T46" s="30"/>
-      <c r="U46" s="30"/>
-      <c r="V46" s="30"/>
-      <c r="W46" s="30"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="30"/>
-    </row>
-    <row r="47" spans="1:25">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="31">
-        <v>2000</v>
-      </c>
-      <c r="D47" s="31">
-        <v>2001</v>
-      </c>
-      <c r="E47" s="31">
-        <v>2002</v>
-      </c>
-      <c r="F47" s="31">
-        <v>2003</v>
-      </c>
-      <c r="G47" s="31">
-        <v>2004</v>
-      </c>
-      <c r="H47" s="31">
-        <v>2005</v>
-      </c>
-      <c r="I47" s="31">
-        <v>2006</v>
-      </c>
-      <c r="J47" s="31">
-        <v>2007</v>
-      </c>
-      <c r="K47" s="31">
-        <v>2008</v>
-      </c>
-      <c r="L47" s="31">
-        <v>2009</v>
-      </c>
-      <c r="M47" s="31">
-        <v>2010</v>
-      </c>
-      <c r="N47" s="31">
-        <v>2011</v>
-      </c>
-      <c r="O47" s="31">
-        <v>2012</v>
-      </c>
-      <c r="P47" s="31">
-        <v>2013</v>
-      </c>
-      <c r="Q47" s="31">
-        <v>2014</v>
-      </c>
-      <c r="R47" s="31">
-        <v>2015</v>
-      </c>
-      <c r="S47" s="31">
-        <v>2016</v>
-      </c>
-      <c r="T47" s="31">
-        <v>2017</v>
-      </c>
-      <c r="U47" s="31">
-        <v>2018</v>
-      </c>
-      <c r="V47" s="31">
-        <v>2019</v>
-      </c>
-      <c r="W47" s="31">
-        <v>2020</v>
-      </c>
-      <c r="X47" s="30"/>
-      <c r="Y47" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="32"/>
-      <c r="R48" s="32"/>
-      <c r="S48" s="32"/>
-      <c r="T48" s="32"/>
-      <c r="U48" s="32"/>
-      <c r="V48" s="32"/>
-      <c r="W48" s="32"/>
-      <c r="X48" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y48" s="32">
-        <v>0.95</v>
       </c>
     </row>
   </sheetData>
@@ -11530,7 +11125,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -11800,7 +11395,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -12070,7 +11665,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -12340,7 +11935,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -12610,7 +12205,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -12892,7 +12487,7 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:25">
@@ -13166,7 +12761,7 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:25">
@@ -13370,7 +12965,7 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:25">

</xml_diff>

<commit_message>
make viral suppression a constant
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="131">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>Percentage of HIV-positive women who breastfeed</t>
-  </si>
-  <si>
-    <t>Viral suppression when initiating ART (%)</t>
   </si>
   <si>
     <t>Number of HIV tests per year</t>
@@ -539,6 +536,9 @@
   <si>
     <t>CD4 change due to non-suppressive ART (% per year)</t>
   </si>
+  <si>
+    <t>Average time from initiating ART to achieving viral suppression (years)</t>
+  </si>
 </sst>
 </file>
 
@@ -777,7 +777,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -941,8 +941,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1129,16 +1135,21 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="12" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="169">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1168,6 +1179,9 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1282,6 +1296,9 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -1811,15 +1828,15 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="81"/>
+      <c r="A2" s="84"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="81"/>
+      <c r="A3" s="84"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
@@ -1863,7 +1880,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -2133,7 +2150,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2403,7 +2420,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2529,7 +2546,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2644,7 +2661,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2759,7 +2776,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2864,7 +2881,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2969,7 +2986,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3024,7 +3041,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3127,7 +3144,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3247,10 +3264,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3260,7 +3277,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3283,7 +3300,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="73"/>
       <c r="B3" s="76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="77">
         <v>4.0000000000000002E-4</v>
@@ -3298,7 +3315,7 @@
     <row r="4" spans="1:5">
       <c r="A4" s="73"/>
       <c r="B4" s="76" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="77">
         <v>8.0000000000000004E-4</v>
@@ -3313,7 +3330,7 @@
     <row r="5" spans="1:5">
       <c r="A5" s="73"/>
       <c r="B5" s="76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="77">
         <v>1.1000000000000001E-3</v>
@@ -3328,7 +3345,7 @@
     <row r="6" spans="1:5">
       <c r="A6" s="73"/>
       <c r="B6" s="76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="77">
         <v>1.38E-2</v>
@@ -3343,7 +3360,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="73"/>
       <c r="B7" s="76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="77">
         <v>8.0000000000000002E-3</v>
@@ -3358,7 +3375,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="73"/>
       <c r="B8" s="76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="77">
         <v>0.36699999999999999</v>
@@ -3373,7 +3390,7 @@
     <row r="9" spans="1:5">
       <c r="A9" s="73"/>
       <c r="B9" s="76" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="77">
         <v>0.20499999999999999</v>
@@ -3408,7 +3425,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3424,7 +3441,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="78">
         <v>5.6</v>
@@ -3438,7 +3455,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="53">
         <v>1</v>
@@ -3452,7 +3469,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="B17" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="53">
         <v>1</v>
@@ -3466,7 +3483,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="53">
         <v>1</v>
@@ -3480,7 +3497,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="53">
         <v>3.49</v>
@@ -3494,7 +3511,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="53">
         <v>7.17</v>
@@ -3529,7 +3546,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3545,7 +3562,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="79">
         <v>0.24</v>
@@ -3559,7 +3576,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" s="79">
         <v>0.95</v>
@@ -3574,7 +3591,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="79">
         <v>3</v>
@@ -3588,7 +3605,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="79">
         <v>3.74</v>
@@ -3602,7 +3619,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="79">
         <v>1.5</v>
@@ -3637,7 +3654,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -3653,7 +3670,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="B36" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" s="79">
         <v>2.2000000000000002</v>
@@ -3675,7 +3692,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="B37" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="79">
         <v>1.42</v>
@@ -3697,7 +3714,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="B38" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" s="79">
         <v>2.14</v>
@@ -3719,7 +3736,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="B39" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39" s="79">
         <v>0.66</v>
@@ -3776,7 +3793,7 @@
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
     </row>
-    <row r="43" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+    <row r="43" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A43" s="57" t="s">
         <v>130</v>
       </c>
@@ -3785,7 +3802,7 @@
       <c r="D43" s="67"/>
       <c r="E43" s="67"/>
     </row>
-    <row r="44" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+    <row r="44" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A44" s="67"/>
       <c r="B44" s="67"/>
       <c r="C44" s="58" t="s">
@@ -3798,326 +3815,308 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+    <row r="45" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A45" s="67"/>
       <c r="B45" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="83">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D45" s="83">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E45" s="83">
-        <v>0.27500000000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+        <v>42</v>
+      </c>
+      <c r="C45" s="85">
+        <v>0.2</v>
+      </c>
+      <c r="D45" s="85">
+        <v>0.1</v>
+      </c>
+      <c r="E45" s="85">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A46" s="67"/>
-      <c r="B46" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C46" s="83">
-        <v>0.15</v>
-      </c>
-      <c r="D46" s="83">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="E46" s="83">
-        <v>0.88500000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A47" s="67"/>
-      <c r="B47" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="83">
-        <v>0.1</v>
-      </c>
-      <c r="D47" s="83">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E47" s="83">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" s="82" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A48" s="67"/>
-      <c r="B48" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" s="83">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D48" s="83">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E48" s="83">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A49" s="67"/>
-      <c r="B49" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="83">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="D49" s="83">
-        <v>0.05</v>
-      </c>
-      <c r="E49" s="83">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" s="55" customFormat="1">
+      <c r="A48" s="86"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+    </row>
+    <row r="49" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A49" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" s="67"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+    </row>
+    <row r="50" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A50" s="67"/>
-      <c r="B50" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" s="83">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="D50" s="83">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="E50" s="83">
-        <v>0.68600000000000005</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B50" s="67"/>
+      <c r="C50" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A51" s="67"/>
       <c r="B51" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="83">
-        <v>0.09</v>
-      </c>
-      <c r="D51" s="83">
-        <v>1.9E-2</v>
-      </c>
-      <c r="E51" s="83">
-        <v>0.72299999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
+        <v>91</v>
+      </c>
+      <c r="C51" s="82">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D51" s="82">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E51" s="82">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
       <c r="A52" s="67"/>
       <c r="B52" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="82">
+        <v>0.15</v>
+      </c>
+      <c r="D52" s="82">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E52" s="82">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A53" s="67"/>
+      <c r="B53" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="82">
+        <v>0.1</v>
+      </c>
+      <c r="D53" s="82">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E53" s="82">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A54" s="67"/>
+      <c r="B54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="82">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D54" s="82">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E54" s="82">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A55" s="67"/>
+      <c r="B55" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="82">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="D55" s="82">
+        <v>0.05</v>
+      </c>
+      <c r="E55" s="82">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A56" s="67"/>
+      <c r="B56" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="82">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="D56" s="82">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E56" s="82">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A57" s="67"/>
+      <c r="B57" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="82">
+        <v>0.09</v>
+      </c>
+      <c r="D57" s="82">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E57" s="82">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A58" s="67"/>
+      <c r="B58" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="82">
+        <v>0.111</v>
+      </c>
+      <c r="D58" s="82">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E58" s="82">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A59" s="83"/>
+      <c r="C59" s="83"/>
+      <c r="D59" s="83"/>
+      <c r="E59" s="83"/>
+    </row>
+    <row r="60" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A60" s="83"/>
+      <c r="B60" s="83"/>
+      <c r="C60" s="83"/>
+      <c r="D60" s="83"/>
+      <c r="E60" s="83"/>
+    </row>
+    <row r="61" spans="1:5" s="81" customFormat="1" ht="15" customHeight="1">
+      <c r="A61" s="83"/>
+      <c r="B61" s="83"/>
+      <c r="C61" s="83"/>
+      <c r="D61" s="83"/>
+      <c r="E61" s="83"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="83">
-        <v>0.111</v>
-      </c>
-      <c r="D52" s="83">
-        <v>4.7E-2</v>
-      </c>
-      <c r="E52" s="83">
-        <v>0.56299999999999994</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A53" s="84"/>
-      <c r="C53" s="84"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="84"/>
-    </row>
-    <row r="54" spans="1:9" s="82" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A54" s="84"/>
-      <c r="B54" s="84"/>
-      <c r="C54" s="84"/>
-      <c r="D54" s="84"/>
-      <c r="E54" s="84"/>
-    </row>
-    <row r="55" spans="1:9" s="82" customFormat="1" ht="15" customHeight="1">
-      <c r="A55" s="84"/>
-      <c r="B55" s="84"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="C57" s="7" t="s">
+    </row>
+    <row r="63" spans="1:5">
+      <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D63" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E63" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
-      <c r="B58" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="51">
+    <row r="64" spans="1:5">
+      <c r="B64" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="51">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="D58" s="51">
+      <c r="D64" s="51">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E58" s="51">
+      <c r="E64" s="51">
         <v>4.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="B59" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" s="51">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D59" s="51">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E59" s="51">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="B60" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C60" s="51">
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="D60" s="51">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="E60" s="51">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="B61" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="51">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="D61" s="51">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E61" s="51">
-        <v>1.01E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="B62" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="51">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="D62" s="51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E62" s="51">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F62" s="38"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="38"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="B63" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="51">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="D63" s="51">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="E63" s="51">
-        <v>0.432</v>
-      </c>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="B64" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="51">
-        <v>0.23</v>
-      </c>
-      <c r="D64" s="51">
-        <v>0.15</v>
-      </c>
-      <c r="E64" s="51">
-        <v>0.3</v>
-      </c>
-      <c r="F64" s="38"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
     </row>
     <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C65" s="51">
-        <v>2.17</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="D65" s="51">
-        <v>1.27</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="E65" s="51">
-        <v>3.71</v>
-      </c>
-      <c r="F65" s="38"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
+        <v>4.4000000000000003E-3</v>
+      </c>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="38"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
+      <c r="B66" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="51">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D66" s="51">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E66" s="51">
+        <v>7.1000000000000004E-3</v>
+      </c>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="38"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="38"/>
-      <c r="I67" s="38"/>
+      <c r="B67" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C67" s="51">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D67" s="51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E67" s="51">
+        <v>1.01E-2</v>
+      </c>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="38"/>
-      <c r="B68" s="52"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
+      <c r="B68" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="51">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D68" s="51">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E68" s="51">
+        <v>7.9000000000000001E-2</v>
+      </c>
       <c r="F68" s="38"/>
       <c r="G68" s="38"/>
       <c r="H68" s="38"/>
       <c r="I68" s="38"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="2" t="s">
-        <v>108</v>
+      <c r="B69" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="51">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D69" s="51">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E69" s="51">
+        <v>0.432</v>
       </c>
       <c r="F69" s="38"/>
       <c r="G69" s="38"/>
@@ -4125,14 +4124,17 @@
       <c r="I69" s="38"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="C70" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>28</v>
+      <c r="B70" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" s="51">
+        <v>0.23</v>
+      </c>
+      <c r="D70" s="51">
+        <v>0.15</v>
+      </c>
+      <c r="E70" s="51">
+        <v>0.3</v>
       </c>
       <c r="F70" s="38"/>
       <c r="G70" s="38"/>
@@ -4141,121 +4143,91 @@
     </row>
     <row r="71" spans="1:9">
       <c r="B71" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C71" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="D71" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="E71" s="45">
-        <v>0.98</v>
+        <v>106</v>
+      </c>
+      <c r="C71" s="51">
+        <v>2.17</v>
+      </c>
+      <c r="D71" s="51">
+        <v>1.27</v>
+      </c>
+      <c r="E71" s="51">
+        <v>3.71</v>
       </c>
       <c r="F71" s="38"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="54"/>
-      <c r="I71" s="54"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
     </row>
     <row r="72" spans="1:9">
-      <c r="B72" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="45">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D72" s="45">
-        <v>0.47</v>
-      </c>
-      <c r="E72" s="45">
-        <v>0.67</v>
-      </c>
+      <c r="A72" s="38"/>
+      <c r="B72" s="52"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
       <c r="F72" s="38"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="54"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="B73" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C73" s="45">
-        <v>0</v>
-      </c>
-      <c r="D73" s="45">
-        <v>0</v>
-      </c>
-      <c r="E73" s="45">
-        <v>0.68</v>
-      </c>
+      <c r="A73" s="38"/>
+      <c r="B73" s="52"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
       <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
     </row>
     <row r="74" spans="1:9">
-      <c r="B74" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="45">
-        <v>2.65</v>
-      </c>
-      <c r="D74" s="45">
-        <v>1.35</v>
-      </c>
-      <c r="E74" s="45">
-        <v>5.19</v>
-      </c>
+      <c r="A74" s="38"/>
+      <c r="B74" s="52"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
       <c r="F74" s="38"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
     </row>
     <row r="75" spans="1:9">
-      <c r="B75" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="45">
-        <v>0.54</v>
-      </c>
-      <c r="D75" s="45">
-        <v>0.33</v>
-      </c>
-      <c r="E75" s="45">
-        <v>0.68</v>
+      <c r="A75" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F75" s="38"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="54"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="38"/>
     </row>
     <row r="76" spans="1:9">
-      <c r="B76" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C76" s="45">
-        <v>0.9</v>
-      </c>
-      <c r="D76" s="45">
-        <v>0.82</v>
-      </c>
-      <c r="E76" s="45">
-        <v>0.93</v>
+      <c r="C76" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F76" s="38"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="54"/>
+      <c r="G76" s="38"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
     </row>
     <row r="77" spans="1:9">
       <c r="B77" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C77" s="45">
-        <v>0.73</v>
+        <v>0.95</v>
       </c>
       <c r="D77" s="45">
-        <v>0.65</v>
+        <v>0.8</v>
       </c>
       <c r="E77" s="45">
-        <v>0.8</v>
+        <v>0.98</v>
       </c>
       <c r="F77" s="38"/>
       <c r="G77" s="54"/>
@@ -4264,16 +4236,16 @@
     </row>
     <row r="78" spans="1:9">
       <c r="B78" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C78" s="45">
-        <v>0.5</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D78" s="45">
-        <v>0.3</v>
+        <v>0.47</v>
       </c>
       <c r="E78" s="45">
-        <v>0.8</v>
+        <v>0.67</v>
       </c>
       <c r="F78" s="38"/>
       <c r="G78" s="54"/>
@@ -4282,186 +4254,183 @@
     </row>
     <row r="79" spans="1:9">
       <c r="B79" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="45">
+        <v>0</v>
+      </c>
+      <c r="D79" s="45">
+        <v>0</v>
+      </c>
+      <c r="E79" s="45">
+        <v>0.68</v>
+      </c>
+      <c r="F79" s="38"/>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="B80" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C80" s="45">
+        <v>2.65</v>
+      </c>
+      <c r="D80" s="45">
+        <v>1.35</v>
+      </c>
+      <c r="E80" s="45">
+        <v>5.19</v>
+      </c>
+      <c r="F80" s="38"/>
+      <c r="G80" s="54"/>
+      <c r="H80" s="54"/>
+      <c r="I80" s="54"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="B81" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C81" s="45">
+        <v>0.54</v>
+      </c>
+      <c r="D81" s="45">
+        <v>0.33</v>
+      </c>
+      <c r="E81" s="45">
+        <v>0.68</v>
+      </c>
+      <c r="F81" s="38"/>
+      <c r="G81" s="54"/>
+      <c r="H81" s="54"/>
+      <c r="I81" s="54"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="B82" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C82" s="45">
+        <v>0.9</v>
+      </c>
+      <c r="D82" s="45">
+        <v>0.82</v>
+      </c>
+      <c r="E82" s="45">
+        <v>0.93</v>
+      </c>
+      <c r="F82" s="38"/>
+      <c r="G82" s="54"/>
+      <c r="H82" s="54"/>
+      <c r="I82" s="54"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="B83" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C83" s="45">
+        <v>0.73</v>
+      </c>
+      <c r="D83" s="45">
+        <v>0.65</v>
+      </c>
+      <c r="E83" s="45">
+        <v>0.8</v>
+      </c>
+      <c r="F83" s="38"/>
+      <c r="G83" s="54"/>
+      <c r="H83" s="54"/>
+      <c r="I83" s="54"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="B84" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C84" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="45">
+        <v>0.3</v>
+      </c>
+      <c r="E84" s="45">
+        <v>0.8</v>
+      </c>
+      <c r="F84" s="38"/>
+      <c r="G84" s="54"/>
+      <c r="H84" s="54"/>
+      <c r="I84" s="54"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="B85" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C85" s="45">
+        <v>0.92</v>
+      </c>
+      <c r="D85" s="45">
+        <v>0.8</v>
+      </c>
+      <c r="E85" s="45">
+        <v>0.95</v>
+      </c>
+      <c r="F85" s="38"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="38"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="38"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="38"/>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="59"/>
+      <c r="B87" s="60"/>
+      <c r="C87" s="66"/>
+      <c r="D87" s="66"/>
+      <c r="E87" s="66"/>
+      <c r="F87" s="66"/>
+      <c r="G87" s="66"/>
+      <c r="H87" s="66"/>
+      <c r="I87" s="38"/>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="66"/>
+      <c r="B88" s="60"/>
+      <c r="C88" s="61"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="61"/>
+      <c r="F88" s="66"/>
+      <c r="G88" s="66"/>
+      <c r="H88" s="66"/>
+      <c r="I88" s="38"/>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="C79" s="45">
-        <v>0.92</v>
-      </c>
-      <c r="D79" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="E79" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="F79" s="38"/>
-      <c r="G79" s="38"/>
-      <c r="H79" s="38"/>
-      <c r="I79" s="38"/>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="38"/>
-      <c r="B80" s="52"/>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="38"/>
-      <c r="H80" s="38"/>
-      <c r="I80" s="38"/>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="59"/>
-      <c r="B81" s="60"/>
-      <c r="C81" s="66"/>
-      <c r="D81" s="66"/>
-      <c r="E81" s="66"/>
-      <c r="F81" s="66"/>
-      <c r="G81" s="66"/>
-      <c r="H81" s="66"/>
-      <c r="I81" s="38"/>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="66"/>
-      <c r="B82" s="60"/>
-      <c r="C82" s="61"/>
-      <c r="D82" s="61"/>
-      <c r="E82" s="61"/>
-      <c r="F82" s="66"/>
-      <c r="G82" s="66"/>
-      <c r="H82" s="66"/>
-      <c r="I82" s="38"/>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="B83" s="56"/>
-      <c r="C83" s="56"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="56"/>
-      <c r="F83" s="56"/>
-      <c r="G83" s="56"/>
-      <c r="H83" s="56"/>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="56"/>
-      <c r="B84" s="56"/>
-      <c r="C84" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="D84" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="E84" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="F84" s="56"/>
-      <c r="G84" s="56"/>
-      <c r="H84" s="56"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="56"/>
-      <c r="B85" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="C85" s="65">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D85" s="65">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E85" s="65">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="F85" s="56"/>
-      <c r="G85" s="56"/>
-      <c r="H85" s="56"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="56"/>
-      <c r="B86" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="C86" s="65">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D86" s="65">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E86" s="65">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F86" s="56"/>
-      <c r="G86" s="56"/>
-      <c r="H86" s="56"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="56"/>
-      <c r="B87" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="C87" s="65">
-        <v>0.02</v>
-      </c>
-      <c r="D87" s="65">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E87" s="65">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F87" s="56"/>
-      <c r="G87" s="56"/>
-      <c r="H87" s="56"/>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="56"/>
-      <c r="B88" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="C88" s="65">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D88" s="65">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="E88" s="65">
-        <v>9.4E-2</v>
-      </c>
-      <c r="F88" s="56"/>
-      <c r="G88" s="56"/>
-      <c r="H88" s="56"/>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="56"/>
-      <c r="B89" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" s="65">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D89" s="65">
-        <v>0.114</v>
-      </c>
-      <c r="E89" s="65">
-        <v>0.47399999999999998</v>
-      </c>
+      <c r="B89" s="56"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="56"/>
+      <c r="E89" s="56"/>
       <c r="F89" s="56"/>
       <c r="G89" s="56"/>
       <c r="H89" s="56"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="56"/>
-      <c r="B90" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="C90" s="65">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="D90" s="65">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="E90" s="65">
-        <v>0.71499999999999997</v>
+      <c r="B90" s="56"/>
+      <c r="C90" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D90" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="E90" s="63" t="s">
+        <v>28</v>
       </c>
       <c r="F90" s="56"/>
       <c r="G90" s="56"/>
@@ -4470,35 +4439,143 @@
     <row r="91" spans="1:9">
       <c r="A91" s="56"/>
       <c r="B91" s="64" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C91" s="65">
-        <v>5.2999999999999999E-2</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="D91" s="65">
-        <v>3.4000000000000002E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E91" s="65">
-        <v>7.9000000000000001E-2</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F91" s="56"/>
       <c r="G91" s="56"/>
       <c r="H91" s="56"/>
     </row>
     <row r="92" spans="1:9">
+      <c r="A92" s="56"/>
+      <c r="B92" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C92" s="65">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D92" s="65">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E92" s="65">
+        <v>1.0999999999999999E-2</v>
+      </c>
       <c r="F92" s="56"/>
       <c r="G92" s="56"/>
       <c r="H92" s="56"/>
     </row>
     <row r="93" spans="1:9">
+      <c r="A93" s="56"/>
+      <c r="B93" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="C93" s="65">
+        <v>0.02</v>
+      </c>
+      <c r="D93" s="65">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E93" s="65">
+        <v>2.9000000000000001E-2</v>
+      </c>
       <c r="F93" s="56"/>
       <c r="G93" s="56"/>
       <c r="H93" s="56"/>
     </row>
     <row r="94" spans="1:9">
+      <c r="A94" s="56"/>
+      <c r="B94" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C94" s="65">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D94" s="65">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E94" s="65">
+        <v>9.4E-2</v>
+      </c>
       <c r="F94" s="56"/>
       <c r="G94" s="56"/>
       <c r="H94" s="56"/>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="56"/>
+      <c r="B95" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C95" s="65">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D95" s="65">
+        <v>0.114</v>
+      </c>
+      <c r="E95" s="65">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="F95" s="56"/>
+      <c r="G95" s="56"/>
+      <c r="H95" s="56"/>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="56"/>
+      <c r="B96" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C96" s="65">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D96" s="65">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E96" s="65">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F96" s="56"/>
+      <c r="G96" s="56"/>
+      <c r="H96" s="56"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="56"/>
+      <c r="B97" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" s="65">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D97" s="65">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E97" s="65">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F97" s="56"/>
+      <c r="G97" s="56"/>
+      <c r="H97" s="56"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="F98" s="56"/>
+      <c r="G98" s="56"/>
+      <c r="H98" s="56"/>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="F99" s="56"/>
+      <c r="G99" s="56"/>
+      <c r="H99" s="56"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="F100" s="56"/>
+      <c r="G100" s="56"/>
+      <c r="H100" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7242,10 +7319,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y57"/>
+  <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A55" sqref="A55:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8412,139 +8489,6 @@
         <v>29</v>
       </c>
       <c r="Y51" s="22"/>
-    </row>
-    <row r="55" spans="1:25">
-      <c r="A55" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="30"/>
-      <c r="N55" s="30"/>
-      <c r="O55" s="30"/>
-      <c r="P55" s="30"/>
-      <c r="Q55" s="30"/>
-      <c r="R55" s="30"/>
-      <c r="S55" s="30"/>
-      <c r="T55" s="30"/>
-      <c r="U55" s="30"/>
-      <c r="V55" s="30"/>
-      <c r="W55" s="30"/>
-      <c r="X55" s="30"/>
-      <c r="Y55" s="30"/>
-    </row>
-    <row r="56" spans="1:25">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="31">
-        <v>2000</v>
-      </c>
-      <c r="D56" s="31">
-        <v>2001</v>
-      </c>
-      <c r="E56" s="31">
-        <v>2002</v>
-      </c>
-      <c r="F56" s="31">
-        <v>2003</v>
-      </c>
-      <c r="G56" s="31">
-        <v>2004</v>
-      </c>
-      <c r="H56" s="31">
-        <v>2005</v>
-      </c>
-      <c r="I56" s="31">
-        <v>2006</v>
-      </c>
-      <c r="J56" s="31">
-        <v>2007</v>
-      </c>
-      <c r="K56" s="31">
-        <v>2008</v>
-      </c>
-      <c r="L56" s="31">
-        <v>2009</v>
-      </c>
-      <c r="M56" s="31">
-        <v>2010</v>
-      </c>
-      <c r="N56" s="31">
-        <v>2011</v>
-      </c>
-      <c r="O56" s="31">
-        <v>2012</v>
-      </c>
-      <c r="P56" s="31">
-        <v>2013</v>
-      </c>
-      <c r="Q56" s="31">
-        <v>2014</v>
-      </c>
-      <c r="R56" s="31">
-        <v>2015</v>
-      </c>
-      <c r="S56" s="31">
-        <v>2016</v>
-      </c>
-      <c r="T56" s="31">
-        <v>2017</v>
-      </c>
-      <c r="U56" s="31">
-        <v>2018</v>
-      </c>
-      <c r="V56" s="31">
-        <v>2019</v>
-      </c>
-      <c r="W56" s="31">
-        <v>2020</v>
-      </c>
-      <c r="X56" s="30"/>
-      <c r="Y56" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="32"/>
-      <c r="N57" s="32"/>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
-      <c r="Q57" s="32"/>
-      <c r="R57" s="32"/>
-      <c r="S57" s="32"/>
-      <c r="T57" s="32"/>
-      <c r="U57" s="32"/>
-      <c r="V57" s="32"/>
-      <c r="W57" s="32"/>
-      <c r="X57" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y57" s="32">
-        <v>0.9</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -8569,7 +8513,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -8686,7 +8630,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -8793,7 +8737,7 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -8924,7 +8868,7 @@
     </row>
     <row r="19" spans="1:35">
       <c r="A19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:35">
@@ -9027,7 +8971,7 @@
     </row>
     <row r="25" spans="1:35">
       <c r="A25" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
@@ -9208,7 +9152,7 @@
     </row>
     <row r="30" spans="1:35">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:35">
@@ -9339,7 +9283,7 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:25">
@@ -9531,7 +9475,7 @@
     </row>
     <row r="42" spans="1:25">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -9743,7 +9687,7 @@
     </row>
     <row r="48" spans="1:25">
       <c r="A48" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
@@ -9955,7 +9899,7 @@
     </row>
     <row r="54" spans="1:35">
       <c r="A54" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
@@ -10086,7 +10030,7 @@
     </row>
     <row r="60" spans="1:35">
       <c r="A60" s="69" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="68"/>
       <c r="C60" s="68"/>
@@ -10282,7 +10226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -10290,7 +10234,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -10568,7 +10512,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -10838,7 +10782,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
@@ -10971,7 +10915,7 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="30"/>
@@ -11125,7 +11069,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -11395,7 +11339,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -11665,7 +11609,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -11935,7 +11879,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -12205,7 +12149,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -12487,7 +12431,7 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:25">
@@ -12761,7 +12705,7 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:25">
@@ -12965,7 +12909,7 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:25">

</xml_diff>

<commit_message>
update mortality and remove biofailure
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="132">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -327,9 +327,6 @@
     <t>Percentage of people in care who are lost to follow-up per year (%/year)</t>
   </si>
   <si>
-    <t>Biological failure rate (%/year)</t>
-  </si>
-  <si>
     <t>Viral load monitoring (number/year)</t>
   </si>
   <si>
@@ -462,9 +459,6 @@
     <t>CD4(350-500)</t>
   </si>
   <si>
-    <t>On treatment</t>
-  </si>
-  <si>
     <t>Tuberculosis cofactor</t>
   </si>
   <si>
@@ -531,13 +525,22 @@
     <t>Disease progression (average years to move)</t>
   </si>
   <si>
-    <t>Treatment recovery on suppressive ART (average years to move)</t>
-  </si>
-  <si>
-    <t>CD4 change due to non-suppressive ART (% per year)</t>
-  </si>
-  <si>
-    <t>Average time from initiating ART to achieving viral suppression (years)</t>
+    <t>Relative death rate on suppressive ART</t>
+  </si>
+  <si>
+    <t>Relative death rate on non-suppressive ART</t>
+  </si>
+  <si>
+    <t>Time after initiating ART to achieve viral suppression (years)</t>
+  </si>
+  <si>
+    <t>Treatment recovery due to suppressive ART (average years to move)</t>
+  </si>
+  <si>
+    <t>CD4 change due to non-suppressive ART (%/year)</t>
+  </si>
+  <si>
+    <t>Treatment failure rate</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
     <numFmt numFmtId="170" formatCode="#,##0.0"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -675,11 +678,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -777,7 +775,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -907,48 +905,72 @@
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1077,23 +1099,10 @@
     <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1103,10 +1112,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1"/>
@@ -1127,29 +1132,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="120" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="6" borderId="1" xfId="120" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="10" fontId="7" fillId="7" borderId="1" xfId="124" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="7" fillId="7" borderId="1" xfId="124" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="9" fontId="7" fillId="7" borderId="1" xfId="124" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="18" fillId="7" borderId="1" xfId="124" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="12" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="193">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1182,6 +1187,18 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1299,6 +1316,18 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -1828,15 +1857,15 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="84"/>
+      <c r="A2" s="81"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="84"/>
+      <c r="A3" s="81"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
@@ -1880,7 +1909,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -2150,7 +2179,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2420,7 +2449,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2546,7 +2575,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2661,7 +2690,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2776,7 +2805,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2881,7 +2910,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2986,7 +3015,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3041,7 +3070,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3144,7 +3173,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3264,168 +3293,172 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="51"/>
+    <col min="2" max="2" width="37.6640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.83203125" style="51"/>
+    <col min="10" max="10" width="18.83203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="64"/>
+      <c r="B3" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="74" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="73"/>
-      <c r="B3" s="76" t="s">
+      <c r="C3" s="70">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D3" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="E3" s="70">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="64"/>
+      <c r="B4" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="77">
+      <c r="C4" s="70">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D4" s="70">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E4" s="70">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="64"/>
+      <c r="B5" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="70">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D5" s="70">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D3" s="77">
-        <v>1E-4</v>
-      </c>
-      <c r="E3" s="77">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="73"/>
-      <c r="B4" s="76" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="77">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="D4" s="77">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="E4" s="77">
-        <v>1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="73"/>
-      <c r="B5" s="76" t="s">
+      <c r="E5" s="70">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="64"/>
+      <c r="B6" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="77">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="D5" s="77">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="E5" s="77">
-        <v>2.8E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="73"/>
-      <c r="B6" s="76" t="s">
+      <c r="C6" s="70">
+        <v>1.38E-2</v>
+      </c>
+      <c r="D6" s="70">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="E6" s="70">
+        <v>1.8599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="64"/>
+      <c r="B7" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="77">
-        <v>1.38E-2</v>
-      </c>
-      <c r="D6" s="77">
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="E6" s="77">
-        <v>1.8599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="73"/>
-      <c r="B7" s="76" t="s">
+      <c r="C7" s="70">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D7" s="70">
+        <v>6.3E-3</v>
+      </c>
+      <c r="E7" s="70">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="64"/>
+      <c r="B8" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="77">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D7" s="77">
-        <v>6.3E-3</v>
-      </c>
-      <c r="E7" s="77">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="73"/>
-      <c r="B8" s="76" t="s">
+      <c r="C8" s="70">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="D8" s="70">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="E8" s="70">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="64"/>
+      <c r="B9" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="77">
-        <v>0.36699999999999999</v>
-      </c>
-      <c r="D8" s="77">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="E8" s="77">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="73"/>
-      <c r="B9" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="77">
+      <c r="C9" s="70">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D9" s="77">
+      <c r="D9" s="70">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="70">
         <v>0.27</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="38"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="38"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="38"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3441,112 +3474,112 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="78">
+        <v>88</v>
+      </c>
+      <c r="C15" s="73">
         <v>5.6</v>
       </c>
-      <c r="D15" s="78">
+      <c r="D15" s="73">
         <v>3.3</v>
       </c>
-      <c r="E15" s="78">
+      <c r="E15" s="73">
         <v>9.1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="53">
+        <v>89</v>
+      </c>
+      <c r="C16" s="73">
         <v>1</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="73">
         <v>1</v>
       </c>
-      <c r="E16" s="53">
+      <c r="E16" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="B17" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="53">
+        <v>90</v>
+      </c>
+      <c r="C17" s="73">
         <v>1</v>
       </c>
-      <c r="D17" s="53">
+      <c r="D17" s="73">
         <v>1</v>
       </c>
-      <c r="E17" s="53">
+      <c r="E17" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="53">
+        <v>91</v>
+      </c>
+      <c r="C18" s="73">
         <v>1</v>
       </c>
-      <c r="D18" s="53">
+      <c r="D18" s="73">
         <v>1</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="53">
+        <v>92</v>
+      </c>
+      <c r="C19" s="73">
         <v>3.49</v>
       </c>
-      <c r="D19" s="53">
+      <c r="D19" s="73">
         <v>1.76</v>
       </c>
-      <c r="E19" s="53">
+      <c r="E19" s="73">
         <v>6.92</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="53">
+        <v>93</v>
+      </c>
+      <c r="C20" s="73">
         <v>7.17</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D20" s="73">
         <v>3.9</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="73">
         <v>12.08</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="38"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="38"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="38"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3562,102 +3595,102 @@
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="79">
+        <v>94</v>
+      </c>
+      <c r="C26" s="73">
         <v>0.24</v>
       </c>
-      <c r="D26" s="79">
+      <c r="D26" s="73">
         <v>0.1</v>
       </c>
-      <c r="E26" s="79">
+      <c r="E26" s="73">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="79">
+        <v>90</v>
+      </c>
+      <c r="C27" s="73">
         <v>0.95</v>
       </c>
-      <c r="D27" s="79">
+      <c r="D27" s="73">
         <v>0.62</v>
       </c>
-      <c r="E27" s="79">
+      <c r="E27" s="73">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G27" s="80"/>
+      <c r="G27" s="74"/>
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="79">
+        <v>95</v>
+      </c>
+      <c r="C28" s="73">
         <v>3</v>
       </c>
-      <c r="D28" s="79">
+      <c r="D28" s="73">
         <v>2.83</v>
       </c>
-      <c r="E28" s="79">
+      <c r="E28" s="73">
         <v>3.16</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="79">
+        <v>96</v>
+      </c>
+      <c r="C29" s="73">
         <v>3.74</v>
       </c>
-      <c r="D29" s="79">
+      <c r="D29" s="73">
         <v>3.48</v>
       </c>
-      <c r="E29" s="79">
+      <c r="E29" s="73">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="79">
+        <v>97</v>
+      </c>
+      <c r="C30" s="73">
         <v>1.5</v>
       </c>
-      <c r="D30" s="79">
+      <c r="D30" s="73">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E30" s="79">
+      <c r="E30" s="73">
         <v>2.25</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="38"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
+      <c r="A31" s="71"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="38"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="38"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="A32" s="71"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="71"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="C35" s="7" t="s">
         <v>30</v>
       </c>
@@ -3668,914 +3701,837 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:5">
       <c r="B36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="73">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D36" s="73">
+        <v>1.07</v>
+      </c>
+      <c r="E36" s="73">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="B37" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="79">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D36" s="79">
-        <v>1.07</v>
-      </c>
-      <c r="E36" s="79">
-        <v>7.28</v>
-      </c>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="73">
+        <v>1.42</v>
+      </c>
+      <c r="D37" s="73">
+        <v>0.9</v>
+      </c>
+      <c r="E37" s="73">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="B38" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="79">
-        <v>1.42</v>
-      </c>
-      <c r="D37" s="79">
-        <v>0.9</v>
-      </c>
-      <c r="E37" s="79">
-        <v>3.42</v>
-      </c>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="55"/>
-      <c r="N37" s="55"/>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="73">
+        <v>2.14</v>
+      </c>
+      <c r="D38" s="73">
+        <v>1.39</v>
+      </c>
+      <c r="E38" s="73">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="B39" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="79">
-        <v>2.14</v>
-      </c>
-      <c r="D38" s="79">
-        <v>1.39</v>
-      </c>
-      <c r="E38" s="79">
-        <v>3.58</v>
-      </c>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="55"/>
-      <c r="N38" s="55"/>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="73">
+        <v>0.66</v>
+      </c>
+      <c r="D39" s="73">
+        <v>0.51</v>
+      </c>
+      <c r="E39" s="73">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A40" s="58"/>
+      <c r="B40" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="73">
+        <v>0.2</v>
+      </c>
+      <c r="D40" s="73">
+        <v>0.1</v>
+      </c>
+      <c r="E40" s="73">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="71"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="71"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+    </row>
+    <row r="44" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A44" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
+    </row>
+    <row r="45" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A45" s="58"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A46" s="58"/>
+      <c r="B46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="70">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D46" s="70">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E46" s="70">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A47" s="58"/>
+      <c r="B47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="70">
+        <v>0.15</v>
+      </c>
+      <c r="D47" s="70">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E47" s="70">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A48" s="58"/>
+      <c r="B48" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="70">
+        <v>0.1</v>
+      </c>
+      <c r="D48" s="70">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E48" s="70">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A49" s="58"/>
+      <c r="B49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="70">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D49" s="70">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E49" s="70">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="68" customFormat="1">
+      <c r="A50" s="58"/>
+      <c r="B50" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="70">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="D50" s="70">
+        <v>0.05</v>
+      </c>
+      <c r="E50" s="70">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A51" s="58"/>
+      <c r="B51" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="70">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="D51" s="70">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E51" s="70">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A52" s="58"/>
+      <c r="B52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="70">
+        <v>0.09</v>
+      </c>
+      <c r="D52" s="70">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E52" s="70">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A53" s="58"/>
+      <c r="B53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="70">
+        <v>0.111</v>
+      </c>
+      <c r="D53" s="70">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E53" s="70">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A54" s="58"/>
+      <c r="B54" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="70">
+        <v>0.16</v>
+      </c>
+      <c r="D54" s="70">
+        <v>0.05</v>
+      </c>
+      <c r="E54" s="70">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A55" s="69"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
+    </row>
+    <row r="56" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A56" s="69"/>
+      <c r="B56" s="69"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
+    </row>
+    <row r="57" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A57" s="69"/>
+      <c r="B57" s="69"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="69"/>
+    </row>
+    <row r="58" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A58" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="79">
-        <v>0.66</v>
-      </c>
-      <c r="D39" s="79">
-        <v>0.51</v>
-      </c>
-      <c r="E39" s="79">
-        <v>0.94</v>
-      </c>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="55"/>
-      <c r="M39" s="55"/>
-      <c r="N39" s="55"/>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40" s="38"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="55"/>
-      <c r="N40" s="55"/>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="38"/>
-      <c r="B41" s="52"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="55"/>
-      <c r="M41" s="55"/>
-      <c r="N41" s="55"/>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42" s="38"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-    </row>
-    <row r="43" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A43" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" s="67"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-    </row>
-    <row r="44" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A44" s="67"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="58" t="s">
+    </row>
+    <row r="59" spans="1:6" ht="13.5" customHeight="1">
+      <c r="C59" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D59" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="58" t="s">
+      <c r="E59" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A45" s="67"/>
-      <c r="B45" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="85">
-        <v>0.2</v>
-      </c>
-      <c r="D45" s="85">
-        <v>0.1</v>
-      </c>
-      <c r="E45" s="85">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A46" s="67"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:14" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A47" s="67"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:14" s="55" customFormat="1">
-      <c r="A48" s="86"/>
-      <c r="B48" s="87"/>
-      <c r="C48" s="86"/>
-      <c r="D48" s="86"/>
-      <c r="E48" s="86"/>
-    </row>
-    <row r="49" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A49" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="67"/>
-      <c r="C49" s="67"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
-    </row>
-    <row r="50" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A50" s="67"/>
-      <c r="B50" s="67"/>
-      <c r="C50" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E50" s="58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A51" s="67"/>
-      <c r="B51" s="3" t="s">
+    <row r="60" spans="1:6" ht="13.5" customHeight="1">
+      <c r="B60" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="70">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D60" s="70">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E60" s="70">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="13.5" customHeight="1">
+      <c r="B61" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="70">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D61" s="70">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E61" s="70">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="13.5" customHeight="1">
+      <c r="B62" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="70">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D62" s="70">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E62" s="70">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="13.5" customHeight="1">
+      <c r="B63" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C51" s="82">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D51" s="82">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E51" s="82">
-        <v>0.27500000000000002</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A52" s="67"/>
-      <c r="B52" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="82">
-        <v>0.15</v>
-      </c>
-      <c r="D52" s="82">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="E52" s="82">
-        <v>0.88500000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A53" s="67"/>
-      <c r="B53" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" s="82">
-        <v>0.1</v>
-      </c>
-      <c r="D53" s="82">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E53" s="82">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A54" s="67"/>
-      <c r="B54" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" s="82">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D54" s="82">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E54" s="82">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A55" s="67"/>
-      <c r="B55" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="82">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="D55" s="82">
-        <v>0.05</v>
-      </c>
-      <c r="E55" s="82">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A56" s="67"/>
-      <c r="B56" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C56" s="82">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="D56" s="82">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="E56" s="82">
-        <v>0.68600000000000005</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A57" s="67"/>
-      <c r="B57" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" s="82">
-        <v>0.09</v>
-      </c>
-      <c r="D57" s="82">
-        <v>1.9E-2</v>
-      </c>
-      <c r="E57" s="82">
-        <v>0.72299999999999998</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A58" s="67"/>
-      <c r="B58" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C58" s="82">
-        <v>0.111</v>
-      </c>
-      <c r="D58" s="82">
-        <v>4.7E-2</v>
-      </c>
-      <c r="E58" s="82">
-        <v>0.56299999999999994</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A59" s="83"/>
-      <c r="C59" s="83"/>
-      <c r="D59" s="83"/>
-      <c r="E59" s="83"/>
-    </row>
-    <row r="60" spans="1:5" s="81" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A60" s="83"/>
-      <c r="B60" s="83"/>
-      <c r="C60" s="83"/>
-      <c r="D60" s="83"/>
-      <c r="E60" s="83"/>
-    </row>
-    <row r="61" spans="1:5" s="81" customFormat="1" ht="15" customHeight="1">
-      <c r="A61" s="83"/>
-      <c r="B61" s="83"/>
-      <c r="C61" s="83"/>
-      <c r="D61" s="83"/>
-      <c r="E61" s="83"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="C63" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="C63" s="70">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D63" s="70">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E63" s="70">
+        <v>1.01E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="B64" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="51">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D64" s="51">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E64" s="51">
-        <v>4.4000000000000003E-3</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C64" s="70">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D64" s="70">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E64" s="70">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F64" s="71"/>
     </row>
     <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" s="51">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="D65" s="51">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E65" s="51">
-        <v>4.4000000000000003E-3</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C65" s="70">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D65" s="70">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E65" s="70">
+        <v>0.432</v>
+      </c>
+      <c r="F65" s="71"/>
     </row>
     <row r="66" spans="1:9">
       <c r="B66" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C66" s="51">
-        <v>5.7999999999999996E-3</v>
-      </c>
-      <c r="D66" s="51">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="E66" s="51">
-        <v>7.1000000000000004E-3</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C66" s="70">
+        <v>0.23</v>
+      </c>
+      <c r="D66" s="70">
+        <v>0.15</v>
+      </c>
+      <c r="E66" s="70">
+        <v>0.3</v>
+      </c>
+      <c r="F66" s="71"/>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C67" s="51">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="D67" s="51">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E67" s="51">
-        <v>1.01E-2</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C67" s="70">
+        <v>0.48780000000000001</v>
+      </c>
+      <c r="D67" s="70">
+        <v>0.28349999999999997</v>
+      </c>
+      <c r="E67" s="70">
+        <v>0.8417</v>
+      </c>
+      <c r="F67" s="71"/>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68" s="51">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="D68" s="51">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E68" s="51">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="38"/>
+        <v>104</v>
+      </c>
+      <c r="C68" s="70">
+        <v>2.17</v>
+      </c>
+      <c r="D68" s="70">
+        <v>1.27</v>
+      </c>
+      <c r="E68" s="70">
+        <v>3.71</v>
+      </c>
+      <c r="F68" s="71"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="B69" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="51">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="D69" s="51">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="E69" s="51">
-        <v>0.432</v>
-      </c>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="38"/>
+      <c r="A69" s="71"/>
+      <c r="B69" s="72"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="71"/>
+      <c r="E69" s="71"/>
+      <c r="F69" s="71"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="B70" s="3" t="s">
+      <c r="A70" s="71"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="71"/>
+      <c r="F70" s="71"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="71"/>
+      <c r="I70" s="71"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="71"/>
+      <c r="B71" s="72"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="71"/>
+      <c r="E71" s="71"/>
+      <c r="F71" s="71"/>
+      <c r="G71" s="71"/>
+      <c r="H71" s="71"/>
+      <c r="I71" s="71"/>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C70" s="51">
-        <v>0.23</v>
-      </c>
-      <c r="D70" s="51">
-        <v>0.15</v>
-      </c>
-      <c r="E70" s="51">
-        <v>0.3</v>
-      </c>
-      <c r="F70" s="38"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="38"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="B71" s="3" t="s">
+      <c r="F72" s="71"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="71"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="C73" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F73" s="71"/>
+      <c r="G73" s="71"/>
+      <c r="H73" s="71"/>
+      <c r="I73" s="71"/>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="B74" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C71" s="51">
-        <v>2.17</v>
-      </c>
-      <c r="D71" s="51">
-        <v>1.27</v>
-      </c>
-      <c r="E71" s="51">
-        <v>3.71</v>
-      </c>
-      <c r="F71" s="38"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="38"/>
-      <c r="I71" s="38"/>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="38"/>
-      <c r="B72" s="52"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="38"/>
-      <c r="F72" s="38"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="38"/>
-      <c r="I72" s="38"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="38"/>
-      <c r="B73" s="52"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="F73" s="38"/>
-      <c r="G73" s="38"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="38"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="38"/>
-      <c r="B74" s="52"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="38"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="38"/>
-      <c r="I74" s="38"/>
+      <c r="C74" s="75">
+        <v>0.95</v>
+      </c>
+      <c r="D74" s="75">
+        <v>0.8</v>
+      </c>
+      <c r="E74" s="75">
+        <v>0.98</v>
+      </c>
+      <c r="F74" s="71"/>
+      <c r="G74" s="76"/>
+      <c r="H74" s="76"/>
+      <c r="I74" s="76"/>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="2" t="s">
+      <c r="B75" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="38"/>
+      <c r="C75" s="75">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D75" s="75">
+        <v>0.47</v>
+      </c>
+      <c r="E75" s="75">
+        <v>0.67</v>
+      </c>
+      <c r="F75" s="71"/>
+      <c r="G75" s="76"/>
+      <c r="H75" s="76"/>
+      <c r="I75" s="76"/>
     </row>
     <row r="76" spans="1:9">
-      <c r="C76" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F76" s="38"/>
-      <c r="G76" s="38"/>
-      <c r="H76" s="38"/>
-      <c r="I76" s="38"/>
+      <c r="B76" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" s="75">
+        <v>0</v>
+      </c>
+      <c r="D76" s="75">
+        <v>0</v>
+      </c>
+      <c r="E76" s="75">
+        <v>0.68</v>
+      </c>
+      <c r="F76" s="71"/>
     </row>
     <row r="77" spans="1:9">
       <c r="B77" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C77" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="D77" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="E77" s="45">
-        <v>0.98</v>
-      </c>
-      <c r="F77" s="38"/>
-      <c r="G77" s="54"/>
-      <c r="H77" s="54"/>
-      <c r="I77" s="54"/>
+        <v>109</v>
+      </c>
+      <c r="C77" s="75">
+        <v>2.65</v>
+      </c>
+      <c r="D77" s="75">
+        <v>1.35</v>
+      </c>
+      <c r="E77" s="75">
+        <v>5.19</v>
+      </c>
+      <c r="F77" s="71"/>
+      <c r="G77" s="76"/>
+      <c r="H77" s="76"/>
+      <c r="I77" s="76"/>
     </row>
     <row r="78" spans="1:9">
       <c r="B78" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C78" s="45">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D78" s="45">
-        <v>0.47</v>
-      </c>
-      <c r="E78" s="45">
-        <v>0.67</v>
-      </c>
-      <c r="F78" s="38"/>
-      <c r="G78" s="54"/>
-      <c r="H78" s="54"/>
-      <c r="I78" s="54"/>
+        <v>110</v>
+      </c>
+      <c r="C78" s="75">
+        <v>0.54</v>
+      </c>
+      <c r="D78" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="E78" s="75">
+        <v>0.68</v>
+      </c>
+      <c r="F78" s="71"/>
+      <c r="G78" s="76"/>
+      <c r="H78" s="76"/>
+      <c r="I78" s="76"/>
     </row>
     <row r="79" spans="1:9">
       <c r="B79" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="45">
-        <v>0</v>
-      </c>
-      <c r="D79" s="45">
-        <v>0</v>
-      </c>
-      <c r="E79" s="45">
-        <v>0.68</v>
-      </c>
-      <c r="F79" s="38"/>
+        <v>111</v>
+      </c>
+      <c r="C79" s="75">
+        <v>0.9</v>
+      </c>
+      <c r="D79" s="75">
+        <v>0.82</v>
+      </c>
+      <c r="E79" s="75">
+        <v>0.93</v>
+      </c>
+      <c r="F79" s="71"/>
+      <c r="G79" s="76"/>
+      <c r="H79" s="76"/>
+      <c r="I79" s="76"/>
     </row>
     <row r="80" spans="1:9">
       <c r="B80" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C80" s="45">
-        <v>2.65</v>
-      </c>
-      <c r="D80" s="45">
-        <v>1.35</v>
-      </c>
-      <c r="E80" s="45">
-        <v>5.19</v>
-      </c>
-      <c r="F80" s="38"/>
-      <c r="G80" s="54"/>
-      <c r="H80" s="54"/>
-      <c r="I80" s="54"/>
+        <v>112</v>
+      </c>
+      <c r="C80" s="75">
+        <v>0.73</v>
+      </c>
+      <c r="D80" s="75">
+        <v>0.65</v>
+      </c>
+      <c r="E80" s="75">
+        <v>0.8</v>
+      </c>
+      <c r="F80" s="71"/>
+      <c r="G80" s="76"/>
+      <c r="H80" s="76"/>
+      <c r="I80" s="76"/>
     </row>
     <row r="81" spans="1:9">
       <c r="B81" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C81" s="45">
-        <v>0.54</v>
-      </c>
-      <c r="D81" s="45">
-        <v>0.33</v>
-      </c>
-      <c r="E81" s="45">
-        <v>0.68</v>
-      </c>
-      <c r="F81" s="38"/>
-      <c r="G81" s="54"/>
-      <c r="H81" s="54"/>
-      <c r="I81" s="54"/>
+        <v>113</v>
+      </c>
+      <c r="C81" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="D81" s="75">
+        <v>0.3</v>
+      </c>
+      <c r="E81" s="75">
+        <v>0.8</v>
+      </c>
+      <c r="F81" s="71"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
     </row>
     <row r="82" spans="1:9">
       <c r="B82" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C82" s="45">
-        <v>0.9</v>
-      </c>
-      <c r="D82" s="45">
-        <v>0.82</v>
-      </c>
-      <c r="E82" s="45">
-        <v>0.93</v>
-      </c>
-      <c r="F82" s="38"/>
-      <c r="G82" s="54"/>
-      <c r="H82" s="54"/>
-      <c r="I82" s="54"/>
+        <v>114</v>
+      </c>
+      <c r="C82" s="75">
+        <v>0.92</v>
+      </c>
+      <c r="D82" s="75">
+        <v>0.8</v>
+      </c>
+      <c r="E82" s="75">
+        <v>0.95</v>
+      </c>
+      <c r="F82" s="71"/>
+      <c r="G82" s="71"/>
+      <c r="H82" s="71"/>
+      <c r="I82" s="71"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="B83" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C83" s="45">
-        <v>0.73</v>
-      </c>
-      <c r="D83" s="45">
-        <v>0.65</v>
-      </c>
-      <c r="E83" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="F83" s="38"/>
-      <c r="G83" s="54"/>
-      <c r="H83" s="54"/>
-      <c r="I83" s="54"/>
+      <c r="A83" s="71"/>
+      <c r="B83" s="72"/>
+      <c r="C83" s="71"/>
+      <c r="D83" s="71"/>
+      <c r="E83" s="71"/>
+      <c r="F83" s="71"/>
+      <c r="G83" s="71"/>
+      <c r="H83" s="71"/>
+      <c r="I83" s="71"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="B84" s="3" t="s">
+      <c r="A84" s="77"/>
+      <c r="B84" s="78"/>
+      <c r="C84" s="79"/>
+      <c r="D84" s="79"/>
+      <c r="E84" s="79"/>
+      <c r="F84" s="79"/>
+      <c r="G84" s="79"/>
+      <c r="H84" s="79"/>
+      <c r="I84" s="71"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="79"/>
+      <c r="B85" s="78"/>
+      <c r="C85" s="80"/>
+      <c r="D85" s="80"/>
+      <c r="E85" s="80"/>
+      <c r="F85" s="79"/>
+      <c r="G85" s="79"/>
+      <c r="H85" s="79"/>
+      <c r="I85" s="71"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="D84" s="45">
-        <v>0.3</v>
-      </c>
-      <c r="E84" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="F84" s="38"/>
-      <c r="G84" s="54"/>
-      <c r="H84" s="54"/>
-      <c r="I84" s="54"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="B85" s="3" t="s">
+      <c r="B86" s="52"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
+      <c r="H86" s="52"/>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="52"/>
+      <c r="B87" s="52"/>
+      <c r="C87" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E87" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="F87" s="52"/>
+      <c r="G87" s="52"/>
+      <c r="H87" s="52"/>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="52"/>
+      <c r="B88" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="45">
-        <v>0.92</v>
-      </c>
-      <c r="D85" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="E85" s="45">
-        <v>0.95</v>
-      </c>
-      <c r="F85" s="38"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="38"/>
-      <c r="I85" s="38"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="38"/>
-      <c r="B86" s="52"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="38"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="59"/>
-      <c r="B87" s="60"/>
-      <c r="C87" s="66"/>
-      <c r="D87" s="66"/>
-      <c r="E87" s="66"/>
-      <c r="F87" s="66"/>
-      <c r="G87" s="66"/>
-      <c r="H87" s="66"/>
-      <c r="I87" s="38"/>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="66"/>
-      <c r="B88" s="60"/>
-      <c r="C88" s="61"/>
-      <c r="D88" s="61"/>
-      <c r="E88" s="61"/>
-      <c r="F88" s="66"/>
-      <c r="G88" s="66"/>
-      <c r="H88" s="66"/>
-      <c r="I88" s="38"/>
+      <c r="C88" s="73">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D88" s="73">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E88" s="73">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F88" s="52"/>
+      <c r="G88" s="52"/>
+      <c r="H88" s="52"/>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="62" t="s">
+      <c r="A89" s="52"/>
+      <c r="B89" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="B89" s="56"/>
-      <c r="C89" s="56"/>
-      <c r="D89" s="56"/>
-      <c r="E89" s="56"/>
-      <c r="F89" s="56"/>
-      <c r="G89" s="56"/>
-      <c r="H89" s="56"/>
+      <c r="C89" s="73">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D89" s="73">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E89" s="73">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F89" s="52"/>
+      <c r="G89" s="52"/>
+      <c r="H89" s="52"/>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="56"/>
-      <c r="B90" s="56"/>
-      <c r="C90" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="D90" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="E90" s="63" t="s">
-        <v>28</v>
-      </c>
-      <c r="F90" s="56"/>
-      <c r="G90" s="56"/>
-      <c r="H90" s="56"/>
+      <c r="A90" s="52"/>
+      <c r="B90" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C90" s="73">
+        <v>0.02</v>
+      </c>
+      <c r="D90" s="73">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E90" s="73">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F90" s="52"/>
+      <c r="G90" s="52"/>
+      <c r="H90" s="52"/>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="56"/>
-      <c r="B91" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="C91" s="65">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D91" s="65">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E91" s="65">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="F91" s="56"/>
-      <c r="G91" s="56"/>
-      <c r="H91" s="56"/>
+      <c r="A91" s="52"/>
+      <c r="B91" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C91" s="73">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D91" s="73">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E91" s="73">
+        <v>9.4E-2</v>
+      </c>
+      <c r="F91" s="52"/>
+      <c r="G91" s="52"/>
+      <c r="H91" s="52"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="56"/>
-      <c r="B92" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="C92" s="65">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D92" s="65">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E92" s="65">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F92" s="56"/>
-      <c r="G92" s="56"/>
-      <c r="H92" s="56"/>
+      <c r="A92" s="52"/>
+      <c r="B92" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C92" s="73">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D92" s="73">
+        <v>0.114</v>
+      </c>
+      <c r="E92" s="73">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="F92" s="52"/>
+      <c r="G92" s="52"/>
+      <c r="H92" s="52"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="56"/>
-      <c r="B93" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="C93" s="65">
-        <v>0.02</v>
-      </c>
-      <c r="D93" s="65">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E93" s="65">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F93" s="56"/>
-      <c r="G93" s="56"/>
-      <c r="H93" s="56"/>
+      <c r="A93" s="52"/>
+      <c r="B93" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C93" s="73">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D93" s="73">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E93" s="73">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F93" s="52"/>
+      <c r="G93" s="52"/>
+      <c r="H93" s="52"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="56"/>
-      <c r="B94" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="C94" s="65">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D94" s="65">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="E94" s="65">
-        <v>9.4E-2</v>
-      </c>
-      <c r="F94" s="56"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="56"/>
+      <c r="A94" s="52"/>
+      <c r="B94" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C94" s="73">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D94" s="73">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E94" s="73">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F94" s="52"/>
+      <c r="G94" s="52"/>
+      <c r="H94" s="52"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="56"/>
-      <c r="B95" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="C95" s="65">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D95" s="65">
-        <v>0.114</v>
-      </c>
-      <c r="E95" s="65">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="F95" s="56"/>
-      <c r="G95" s="56"/>
-      <c r="H95" s="56"/>
+      <c r="F95" s="52"/>
+      <c r="G95" s="52"/>
+      <c r="H95" s="52"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="56"/>
-      <c r="B96" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C96" s="65">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="D96" s="65">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="E96" s="65">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="F96" s="56"/>
-      <c r="G96" s="56"/>
-      <c r="H96" s="56"/>
-    </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="56"/>
-      <c r="B97" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="C97" s="65">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D97" s="65">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="E97" s="65">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F97" s="56"/>
-      <c r="G97" s="56"/>
-      <c r="H97" s="56"/>
-    </row>
-    <row r="98" spans="1:8">
-      <c r="F98" s="56"/>
-      <c r="G98" s="56"/>
-      <c r="H98" s="56"/>
-    </row>
-    <row r="99" spans="1:8">
-      <c r="F99" s="56"/>
-      <c r="G99" s="56"/>
-      <c r="H99" s="56"/>
-    </row>
-    <row r="100" spans="1:8">
-      <c r="F100" s="56"/>
-      <c r="G100" s="56"/>
-      <c r="H100" s="56"/>
+      <c r="F96" s="52"/>
+      <c r="G96" s="52"/>
+      <c r="H96" s="52"/>
+    </row>
+    <row r="97" spans="6:8">
+      <c r="F97" s="52"/>
+      <c r="G97" s="52"/>
+      <c r="H97" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7321,7 +7277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A55" sqref="A55:XFD59"/>
     </sheetView>
   </sheetViews>
@@ -8505,8 +8461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="P12" workbookViewId="0">
+      <selection activeCell="AF39" sqref="AF39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8866,12 +8822,12 @@
       </c>
       <c r="Y15" s="27"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:25">
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:25">
       <c r="C20" s="7">
         <v>2000</v>
       </c>
@@ -8939,7 +8895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:25">
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
@@ -8969,7 +8925,7 @@
       </c>
       <c r="Y21" s="37"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:25">
       <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
@@ -8997,18 +8953,8 @@
       <c r="W25" s="38"/>
       <c r="X25" s="38"/>
       <c r="Y25" s="38"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="38"/>
-      <c r="AC25" s="38"/>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="38"/>
-      <c r="AF25" s="38"/>
-      <c r="AG25" s="38"/>
-      <c r="AH25" s="38"/>
-      <c r="AI25" s="38"/>
-    </row>
-    <row r="26" spans="1:35">
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" s="38"/>
       <c r="B26" s="38"/>
       <c r="C26" s="39">
@@ -9074,42 +9020,12 @@
       <c r="W26" s="39">
         <v>2020</v>
       </c>
-      <c r="X26" s="39">
-        <v>2021</v>
-      </c>
-      <c r="Y26" s="39">
-        <v>2022</v>
-      </c>
-      <c r="Z26" s="39">
-        <v>2023</v>
-      </c>
-      <c r="AA26" s="39">
-        <v>2024</v>
-      </c>
-      <c r="AB26" s="39">
-        <v>2025</v>
-      </c>
-      <c r="AC26" s="39">
-        <v>2026</v>
-      </c>
-      <c r="AD26" s="39">
-        <v>2027</v>
-      </c>
-      <c r="AE26" s="39">
-        <v>2028</v>
-      </c>
-      <c r="AF26" s="39">
-        <v>2029</v>
-      </c>
-      <c r="AG26" s="39">
-        <v>2030</v>
-      </c>
-      <c r="AH26" s="38"/>
-      <c r="AI26" s="39" t="s">
+      <c r="X26" s="38"/>
+      <c r="Y26" s="39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:25">
       <c r="A27" s="38"/>
       <c r="B27" s="39" t="s">
         <v>44</v>
@@ -9135,27 +9051,17 @@
       <c r="U27" s="40"/>
       <c r="V27" s="40"/>
       <c r="W27" s="40"/>
-      <c r="X27" s="40"/>
+      <c r="X27" s="41" t="s">
+        <v>29</v>
+      </c>
       <c r="Y27" s="40"/>
-      <c r="Z27" s="40"/>
-      <c r="AA27" s="40"/>
-      <c r="AB27" s="40"/>
-      <c r="AC27" s="40"/>
-      <c r="AD27" s="40"/>
-      <c r="AE27" s="40"/>
-      <c r="AF27" s="40"/>
-      <c r="AG27" s="40"/>
-      <c r="AH27" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI27" s="40"/>
-    </row>
-    <row r="30" spans="1:35">
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:25">
       <c r="C31" s="7">
         <v>2000</v>
       </c>
@@ -9223,7 +9129,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:25">
       <c r="B32" s="7" t="s">
         <v>44</v>
       </c>
@@ -10029,185 +9935,185 @@
       <c r="Y56" s="32"/>
     </row>
     <row r="60" spans="1:35">
-      <c r="A60" s="69" t="s">
-        <v>125</v>
-      </c>
-      <c r="B60" s="68"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="68"/>
-      <c r="F60" s="68"/>
-      <c r="G60" s="68"/>
-      <c r="H60" s="68"/>
-      <c r="I60" s="68"/>
-      <c r="J60" s="68"/>
-      <c r="K60" s="68"/>
-      <c r="L60" s="68"/>
-      <c r="M60" s="68"/>
-      <c r="N60" s="68"/>
-      <c r="O60" s="68"/>
-      <c r="P60" s="68"/>
-      <c r="Q60" s="68"/>
-      <c r="R60" s="68"/>
-      <c r="S60" s="68"/>
-      <c r="T60" s="68"/>
-      <c r="U60" s="68"/>
-      <c r="V60" s="68"/>
-      <c r="W60" s="68"/>
-      <c r="X60" s="68"/>
-      <c r="Y60" s="68"/>
-      <c r="Z60" s="68"/>
-      <c r="AA60" s="68"/>
-      <c r="AB60" s="68"/>
-      <c r="AC60" s="68"/>
-      <c r="AD60" s="68"/>
-      <c r="AE60" s="68"/>
-      <c r="AF60" s="68"/>
-      <c r="AG60" s="68"/>
-      <c r="AH60" s="68"/>
-      <c r="AI60" s="68"/>
+      <c r="A60" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="59"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="59"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="59"/>
+      <c r="N60" s="59"/>
+      <c r="O60" s="59"/>
+      <c r="P60" s="59"/>
+      <c r="Q60" s="59"/>
+      <c r="R60" s="59"/>
+      <c r="S60" s="59"/>
+      <c r="T60" s="59"/>
+      <c r="U60" s="59"/>
+      <c r="V60" s="59"/>
+      <c r="W60" s="59"/>
+      <c r="X60" s="59"/>
+      <c r="Y60" s="59"/>
+      <c r="Z60" s="59"/>
+      <c r="AA60" s="59"/>
+      <c r="AB60" s="59"/>
+      <c r="AC60" s="59"/>
+      <c r="AD60" s="59"/>
+      <c r="AE60" s="59"/>
+      <c r="AF60" s="59"/>
+      <c r="AG60" s="59"/>
+      <c r="AH60" s="59"/>
+      <c r="AI60" s="59"/>
     </row>
     <row r="61" spans="1:35">
-      <c r="A61" s="68"/>
-      <c r="B61" s="68"/>
-      <c r="C61" s="70">
+      <c r="A61" s="59"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="61">
         <v>2000</v>
       </c>
-      <c r="D61" s="70">
+      <c r="D61" s="61">
         <v>2001</v>
       </c>
-      <c r="E61" s="70">
+      <c r="E61" s="61">
         <v>2002</v>
       </c>
-      <c r="F61" s="70">
+      <c r="F61" s="61">
         <v>2003</v>
       </c>
-      <c r="G61" s="70">
+      <c r="G61" s="61">
         <v>2004</v>
       </c>
-      <c r="H61" s="70">
+      <c r="H61" s="61">
         <v>2005</v>
       </c>
-      <c r="I61" s="70">
+      <c r="I61" s="61">
         <v>2006</v>
       </c>
-      <c r="J61" s="70">
+      <c r="J61" s="61">
         <v>2007</v>
       </c>
-      <c r="K61" s="70">
+      <c r="K61" s="61">
         <v>2008</v>
       </c>
-      <c r="L61" s="70">
+      <c r="L61" s="61">
         <v>2009</v>
       </c>
-      <c r="M61" s="70">
+      <c r="M61" s="61">
         <v>2010</v>
       </c>
-      <c r="N61" s="70">
+      <c r="N61" s="61">
         <v>2011</v>
       </c>
-      <c r="O61" s="70">
+      <c r="O61" s="61">
         <v>2012</v>
       </c>
-      <c r="P61" s="70">
+      <c r="P61" s="61">
         <v>2013</v>
       </c>
-      <c r="Q61" s="70">
+      <c r="Q61" s="61">
         <v>2014</v>
       </c>
-      <c r="R61" s="70">
+      <c r="R61" s="61">
         <v>2015</v>
       </c>
-      <c r="S61" s="70">
+      <c r="S61" s="61">
         <v>2016</v>
       </c>
-      <c r="T61" s="70">
+      <c r="T61" s="61">
         <v>2017</v>
       </c>
-      <c r="U61" s="70">
+      <c r="U61" s="61">
         <v>2018</v>
       </c>
-      <c r="V61" s="70">
+      <c r="V61" s="61">
         <v>2019</v>
       </c>
-      <c r="W61" s="70">
+      <c r="W61" s="61">
         <v>2020</v>
       </c>
-      <c r="X61" s="70">
+      <c r="X61" s="61">
         <v>2021</v>
       </c>
-      <c r="Y61" s="70">
+      <c r="Y61" s="61">
         <v>2022</v>
       </c>
-      <c r="Z61" s="70">
+      <c r="Z61" s="61">
         <v>2023</v>
       </c>
-      <c r="AA61" s="70">
+      <c r="AA61" s="61">
         <v>2024</v>
       </c>
-      <c r="AB61" s="70">
+      <c r="AB61" s="61">
         <v>2025</v>
       </c>
-      <c r="AC61" s="70">
+      <c r="AC61" s="61">
         <v>2026</v>
       </c>
-      <c r="AD61" s="70">
+      <c r="AD61" s="61">
         <v>2027</v>
       </c>
-      <c r="AE61" s="70">
+      <c r="AE61" s="61">
         <v>2028</v>
       </c>
-      <c r="AF61" s="70">
+      <c r="AF61" s="61">
         <v>2029</v>
       </c>
-      <c r="AG61" s="70">
+      <c r="AG61" s="61">
         <v>2030</v>
       </c>
-      <c r="AH61" s="68"/>
-      <c r="AI61" s="70" t="s">
+      <c r="AH61" s="59"/>
+      <c r="AI61" s="61" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:35">
-      <c r="A62" s="68"/>
-      <c r="B62" s="70" t="s">
+      <c r="A62" s="59"/>
+      <c r="B62" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C62" s="71"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="71"/>
-      <c r="F62" s="71"/>
-      <c r="G62" s="71"/>
-      <c r="H62" s="71"/>
-      <c r="I62" s="71"/>
-      <c r="J62" s="71"/>
-      <c r="K62" s="71"/>
-      <c r="L62" s="71"/>
-      <c r="M62" s="71"/>
-      <c r="N62" s="71"/>
-      <c r="O62" s="71"/>
-      <c r="P62" s="71"/>
-      <c r="Q62" s="71"/>
-      <c r="R62" s="71"/>
-      <c r="S62" s="71"/>
-      <c r="T62" s="71"/>
-      <c r="U62" s="71"/>
-      <c r="V62" s="71"/>
-      <c r="W62" s="71"/>
-      <c r="X62" s="71"/>
-      <c r="Y62" s="71"/>
-      <c r="Z62" s="71"/>
-      <c r="AA62" s="71"/>
-      <c r="AB62" s="71"/>
-      <c r="AC62" s="71"/>
-      <c r="AD62" s="71"/>
-      <c r="AE62" s="71"/>
-      <c r="AF62" s="71"/>
-      <c r="AG62" s="71"/>
-      <c r="AH62" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI62" s="71">
+      <c r="C62" s="62"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="62"/>
+      <c r="G62" s="62"/>
+      <c r="H62" s="62"/>
+      <c r="I62" s="62"/>
+      <c r="J62" s="62"/>
+      <c r="K62" s="62"/>
+      <c r="L62" s="62"/>
+      <c r="M62" s="62"/>
+      <c r="N62" s="62"/>
+      <c r="O62" s="62"/>
+      <c r="P62" s="62"/>
+      <c r="Q62" s="62"/>
+      <c r="R62" s="62"/>
+      <c r="S62" s="62"/>
+      <c r="T62" s="62"/>
+      <c r="U62" s="62"/>
+      <c r="V62" s="62"/>
+      <c r="W62" s="62"/>
+      <c r="X62" s="62"/>
+      <c r="Y62" s="62"/>
+      <c r="Z62" s="62"/>
+      <c r="AA62" s="62"/>
+      <c r="AB62" s="62"/>
+      <c r="AC62" s="62"/>
+      <c r="AD62" s="62"/>
+      <c r="AE62" s="62"/>
+      <c r="AF62" s="62"/>
+      <c r="AG62" s="62"/>
+      <c r="AH62" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI62" s="62">
         <v>0.85</v>
       </c>
     </row>
@@ -10224,17 +10130,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD38"/>
+      <selection activeCell="Y3" sqref="Y3:Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -10312,31 +10218,31 @@
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
       <c r="X3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="79">
+      <c r="Y3" s="82">
         <v>3</v>
       </c>
     </row>
@@ -10346,31 +10252,31 @@
         <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
       <c r="X4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y4" s="79">
+      <c r="Y4" s="82">
         <v>3</v>
       </c>
     </row>
@@ -10379,31 +10285,31 @@
         <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
       <c r="X5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y5" s="79">
+      <c r="Y5" s="82">
         <v>3</v>
       </c>
     </row>
@@ -10411,31 +10317,31 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
       <c r="X6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y6" s="79">
+      <c r="Y6" s="82">
         <v>3</v>
       </c>
     </row>
@@ -10445,31 +10351,31 @@
         <f>Populations!$C$7</f>
         <v>M 15+</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
       <c r="X7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y7" s="79">
+      <c r="Y7" s="82">
         <v>3</v>
       </c>
     </row>
@@ -10479,31 +10385,31 @@
         <f>Populations!$C$8</f>
         <v>F 15+</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
       <c r="X8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y8" s="79">
+      <c r="Y8" s="82">
         <v>3</v>
       </c>
     </row>
@@ -10885,164 +10791,31 @@
       <c r="B25" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="32"/>
-      <c r="S25" s="32"/>
-      <c r="T25" s="32"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="32"/>
-      <c r="W25" s="32"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="46"/>
+      <c r="U25" s="46"/>
+      <c r="V25" s="46"/>
+      <c r="W25" s="46"/>
       <c r="X25" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="Y25" s="32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
-      <c r="V29" s="30"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="30"/>
-    </row>
-    <row r="30" spans="1:25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31">
-        <v>2000</v>
-      </c>
-      <c r="D30" s="31">
-        <v>2001</v>
-      </c>
-      <c r="E30" s="31">
-        <v>2002</v>
-      </c>
-      <c r="F30" s="31">
-        <v>2003</v>
-      </c>
-      <c r="G30" s="31">
-        <v>2004</v>
-      </c>
-      <c r="H30" s="31">
-        <v>2005</v>
-      </c>
-      <c r="I30" s="31">
-        <v>2006</v>
-      </c>
-      <c r="J30" s="31">
-        <v>2007</v>
-      </c>
-      <c r="K30" s="31">
-        <v>2008</v>
-      </c>
-      <c r="L30" s="31">
-        <v>2009</v>
-      </c>
-      <c r="M30" s="31">
-        <v>2010</v>
-      </c>
-      <c r="N30" s="31">
-        <v>2011</v>
-      </c>
-      <c r="O30" s="31">
-        <v>2012</v>
-      </c>
-      <c r="P30" s="31">
-        <v>2013</v>
-      </c>
-      <c r="Q30" s="31">
-        <v>2014</v>
-      </c>
-      <c r="R30" s="31">
-        <v>2015</v>
-      </c>
-      <c r="S30" s="31">
-        <v>2016</v>
-      </c>
-      <c r="T30" s="31">
-        <v>2017</v>
-      </c>
-      <c r="U30" s="31">
-        <v>2018</v>
-      </c>
-      <c r="V30" s="31">
-        <v>2019</v>
-      </c>
-      <c r="W30" s="31">
-        <v>2020</v>
-      </c>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="46"/>
-      <c r="S31" s="46"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="46"/>
-      <c r="V31" s="46"/>
-      <c r="W31" s="46"/>
-      <c r="X31" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y31" s="47">
+      <c r="Y25" s="47">
         <v>1</v>
       </c>
     </row>
@@ -11069,7 +10842,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -11339,7 +11112,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -11609,7 +11382,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -11879,7 +11652,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -12149,7 +11922,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -12431,7 +12204,7 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:25">
@@ -12705,7 +12478,7 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:25">
@@ -12909,7 +12682,7 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:25">

</xml_diff>

<commit_message>
ok, need data entry as well
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12580" tabRatio="805" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12585" tabRatio="805" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="137">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>Average time taken to be linked to care (years)</t>
+  </si>
+  <si>
+    <t>Pregnant women and mothers on PMTCT (%)</t>
   </si>
 </sst>
 </file>
@@ -1765,31 +1768,31 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1">
+    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="406">
+    <row r="5" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="140">
+    <row r="7" spans="1:1" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1816,14 +1819,14 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -1924,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -1957,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -1990,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -2022,7 +2025,7 @@
       </c>
       <c r="Y6" s="8"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2055,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2088,12 +2091,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2194,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2227,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2260,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -2292,7 +2295,7 @@
       </c>
       <c r="Y17" s="22"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2325,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2358,12 +2361,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>42</v>
       </c>
@@ -2482,14 +2485,14 @@
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2515,7 +2518,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2527,7 +2530,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2543,7 +2546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2557,7 +2560,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2571,7 +2574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2587,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2599,12 +2602,12 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2630,7 +2633,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2642,7 +2645,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2658,7 +2661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2672,7 +2675,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2686,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2702,7 +2705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2714,12 +2717,12 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2745,7 +2748,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2757,7 +2760,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2771,7 +2774,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2783,7 +2786,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2795,7 +2798,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2807,7 +2810,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2819,12 +2822,12 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2850,7 +2853,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2862,7 +2865,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2874,7 +2877,7 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2886,7 +2889,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2900,7 +2903,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2912,7 +2915,7 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2924,12 +2927,12 @@
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2955,7 +2958,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2967,7 +2970,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2979,12 +2982,12 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3010,7 +3013,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3022,7 +3025,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3034,7 +3037,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3046,7 +3049,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3058,7 +3061,7 @@
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3070,7 +3073,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3082,12 +3085,12 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3113,7 +3116,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="65" spans="2:8">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3127,7 +3130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:8">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3141,7 +3144,7 @@
       </c>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="2:8">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3155,7 +3158,7 @@
       </c>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="2:8">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3167,7 +3170,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="2:8">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3179,7 +3182,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="2:8">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3210,9 +3213,9 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>83</v>
       </c>
@@ -3221,7 +3224,7 @@
       <c r="D1" s="75"/>
       <c r="E1" s="75"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="75"/>
       <c r="B2" s="75"/>
       <c r="C2" s="76" t="s">
@@ -3234,7 +3237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="75"/>
       <c r="B3" s="78" t="s">
         <v>84</v>
@@ -3249,7 +3252,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="75"/>
       <c r="B4" s="78" t="s">
         <v>85</v>
@@ -3264,7 +3267,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="75"/>
       <c r="B5" s="78" t="s">
         <v>86</v>
@@ -3279,7 +3282,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="75"/>
       <c r="B6" s="78" t="s">
         <v>87</v>
@@ -3294,7 +3297,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="75"/>
       <c r="B7" s="78" t="s">
         <v>88</v>
@@ -3309,7 +3312,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="75"/>
       <c r="B8" s="78" t="s">
         <v>89</v>
@@ -3324,7 +3327,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="75"/>
       <c r="B9" s="78" t="s">
         <v>90</v>
@@ -3339,33 +3342,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
       <c r="B10" s="52"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
       <c r="B11" s="52"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="52"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>92</v>
       </c>
@@ -3390,7 +3393,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>93</v>
       </c>
@@ -3404,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>94</v>
       </c>
@@ -3418,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>95</v>
       </c>
@@ -3432,7 +3435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>96</v>
       </c>
@@ -3446,7 +3449,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>97</v>
       </c>
@@ -3460,33 +3463,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="52"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="38"/>
       <c r="B22" s="52"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="38"/>
       <c r="B23" s="52"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="7" t="s">
         <v>30</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>99</v>
       </c>
@@ -3511,7 +3514,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>94</v>
       </c>
@@ -3525,7 +3528,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>100</v>
       </c>
@@ -3539,7 +3542,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>101</v>
       </c>
@@ -3553,7 +3556,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>102</v>
       </c>
@@ -3567,33 +3570,33 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="38"/>
       <c r="B31" s="52"/>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="38"/>
       <c r="B32" s="52"/>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
       <c r="E32" s="38"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="38"/>
       <c r="B33" s="52"/>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" s="7" t="s">
         <v>30</v>
       </c>
@@ -3604,7 +3607,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>104</v>
       </c>
@@ -3618,7 +3621,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>105</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>106</v>
       </c>
@@ -3646,7 +3649,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>107</v>
       </c>
@@ -3660,33 +3663,33 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="38"/>
       <c r="B40" s="52"/>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="38"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="38"/>
       <c r="B41" s="52"/>
       <c r="C41" s="38"/>
       <c r="D41" s="38"/>
       <c r="E41" s="38"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="38"/>
       <c r="B42" s="52"/>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" s="7" t="s">
         <v>30</v>
       </c>
@@ -3697,7 +3700,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>92</v>
       </c>
@@ -3711,7 +3714,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>93</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>109</v>
       </c>
@@ -3739,7 +3742,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>95</v>
       </c>
@@ -3753,7 +3756,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>96</v>
       </c>
@@ -3771,7 +3774,7 @@
       <c r="H49" s="38"/>
       <c r="I49" s="38"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>97</v>
       </c>
@@ -3789,7 +3792,7 @@
       <c r="H50" s="38"/>
       <c r="I50" s="38"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>110</v>
       </c>
@@ -3807,7 +3810,7 @@
       <c r="H51" s="38"/>
       <c r="I51" s="38"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>111</v>
       </c>
@@ -3825,7 +3828,7 @@
       <c r="H52" s="38"/>
       <c r="I52" s="38"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="38"/>
       <c r="B53" s="52"/>
       <c r="C53" s="38"/>
@@ -3836,7 +3839,7 @@
       <c r="H53" s="38"/>
       <c r="I53" s="38"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="38"/>
       <c r="B54" s="52"/>
       <c r="C54" s="38"/>
@@ -3847,7 +3850,7 @@
       <c r="H54" s="38"/>
       <c r="I54" s="38"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="38"/>
       <c r="B55" s="52"/>
       <c r="C55" s="38"/>
@@ -3858,7 +3861,7 @@
       <c r="H55" s="38"/>
       <c r="I55" s="38"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -3867,7 +3870,7 @@
       <c r="H56" s="38"/>
       <c r="I56" s="38"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C57" s="7" t="s">
         <v>30</v>
       </c>
@@ -3882,7 +3885,7 @@
       <c r="H57" s="38"/>
       <c r="I57" s="38"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>113</v>
       </c>
@@ -3900,7 +3903,7 @@
       <c r="H58" s="54"/>
       <c r="I58" s="54"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>114</v>
       </c>
@@ -3918,7 +3921,7 @@
       <c r="H59" s="54"/>
       <c r="I59" s="54"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>115</v>
       </c>
@@ -3933,7 +3936,7 @@
       </c>
       <c r="F60" s="38"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>116</v>
       </c>
@@ -3951,7 +3954,7 @@
       <c r="H61" s="54"/>
       <c r="I61" s="54"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>117</v>
       </c>
@@ -3969,7 +3972,7 @@
       <c r="H62" s="54"/>
       <c r="I62" s="54"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>118</v>
       </c>
@@ -3987,7 +3990,7 @@
       <c r="H63" s="54"/>
       <c r="I63" s="54"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>119</v>
       </c>
@@ -4005,7 +4008,7 @@
       <c r="H64" s="54"/>
       <c r="I64" s="54"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>120</v>
       </c>
@@ -4023,7 +4026,7 @@
       <c r="H65" s="54"/>
       <c r="I65" s="54"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>121</v>
       </c>
@@ -4041,7 +4044,7 @@
       <c r="H66" s="38"/>
       <c r="I66" s="38"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="38"/>
       <c r="B67" s="52"/>
       <c r="C67" s="38"/>
@@ -4052,7 +4055,7 @@
       <c r="H67" s="38"/>
       <c r="I67" s="38"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="60"/>
       <c r="B68" s="61"/>
       <c r="C68" s="67"/>
@@ -4063,7 +4066,7 @@
       <c r="H68" s="67"/>
       <c r="I68" s="38"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="67"/>
       <c r="B69" s="61"/>
       <c r="C69" s="62"/>
@@ -4074,7 +4077,7 @@
       <c r="H69" s="67"/>
       <c r="I69" s="38"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="57" t="s">
         <v>130</v>
       </c>
@@ -4088,7 +4091,7 @@
       <c r="I70" s="38"/>
       <c r="J70" s="55"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="68"/>
       <c r="B71" s="68"/>
       <c r="C71" s="58" t="s">
@@ -4106,7 +4109,7 @@
       <c r="I71" s="38"/>
       <c r="J71" s="55"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="68"/>
       <c r="B72" s="59" t="s">
         <v>131</v>
@@ -4126,7 +4129,7 @@
       <c r="I72" s="38"/>
       <c r="J72" s="55"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="68"/>
       <c r="B73" s="59" t="s">
         <v>132</v>
@@ -4145,7 +4148,7 @@
       <c r="H73" s="67"/>
       <c r="I73" s="38"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="68"/>
       <c r="B74" s="59" t="s">
         <v>133</v>
@@ -4164,7 +4167,7 @@
       <c r="H74" s="67"/>
       <c r="I74" s="38"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="56"/>
       <c r="B75" s="56"/>
       <c r="C75" s="56"/>
@@ -4175,7 +4178,7 @@
       <c r="H75" s="67"/>
       <c r="I75" s="38"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="56"/>
       <c r="B76" s="56"/>
       <c r="C76" s="56"/>
@@ -4186,7 +4189,7 @@
       <c r="H76" s="67"/>
       <c r="I76" s="38"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="56"/>
       <c r="B77" s="56"/>
       <c r="C77" s="56"/>
@@ -4196,7 +4199,7 @@
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="63" t="s">
         <v>122</v>
       </c>
@@ -4208,7 +4211,7 @@
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="56"/>
       <c r="B79" s="56"/>
       <c r="C79" s="64" t="s">
@@ -4224,7 +4227,7 @@
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="56"/>
       <c r="B80" s="65" t="s">
         <v>123</v>
@@ -4242,7 +4245,7 @@
       <c r="G80" s="56"/>
       <c r="H80" s="56"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="56"/>
       <c r="B81" s="65" t="s">
         <v>124</v>
@@ -4260,7 +4263,7 @@
       <c r="G81" s="56"/>
       <c r="H81" s="56"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="56"/>
       <c r="B82" s="65" t="s">
         <v>125</v>
@@ -4278,7 +4281,7 @@
       <c r="G82" s="56"/>
       <c r="H82" s="56"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="56"/>
       <c r="B83" s="65" t="s">
         <v>126</v>
@@ -4296,7 +4299,7 @@
       <c r="G83" s="56"/>
       <c r="H83" s="56"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="56"/>
       <c r="B84" s="65" t="s">
         <v>127</v>
@@ -4314,7 +4317,7 @@
       <c r="G84" s="56"/>
       <c r="H84" s="56"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="56"/>
       <c r="B85" s="65" t="s">
         <v>128</v>
@@ -4332,7 +4335,7 @@
       <c r="G85" s="56"/>
       <c r="H85" s="56"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="56"/>
       <c r="B86" s="65" t="s">
         <v>129</v>
@@ -4350,17 +4353,17 @@
       <c r="G86" s="56"/>
       <c r="H86" s="56"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F87" s="56"/>
       <c r="G87" s="56"/>
       <c r="H87" s="56"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F88" s="56"/>
       <c r="G88" s="56"/>
       <c r="H88" s="56"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F89" s="56"/>
       <c r="G89" s="56"/>
       <c r="H89" s="56"/>
@@ -4384,14 +4387,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -4417,7 +4420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -4446,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -4475,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -4504,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -4562,7 +4565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -4610,15 +4613,15 @@
       <selection activeCell="Z2" sqref="Z2:Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4686,7 +4689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4720,7 +4723,7 @@
       </c>
       <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4776,7 +4779,7 @@
       </c>
       <c r="Z4" s="11"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4810,7 +4813,7 @@
       </c>
       <c r="Z5" s="11"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4844,7 +4847,7 @@
       </c>
       <c r="Z7" s="11"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4900,7 +4903,7 @@
       </c>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4934,7 +4937,7 @@
       </c>
       <c r="Z9" s="11"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -4968,7 +4971,7 @@
       </c>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5024,7 +5027,7 @@
       </c>
       <c r="Z12" s="11"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5058,7 +5061,7 @@
       </c>
       <c r="Z13" s="11"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -5071,7 +5074,7 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
@@ -5104,7 +5107,7 @@
       </c>
       <c r="Z15" s="11"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
@@ -5159,7 +5162,7 @@
       </c>
       <c r="Z16" s="11"/>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -5192,7 +5195,7 @@
       </c>
       <c r="Z17" s="11"/>
     </row>
-    <row r="18" spans="2:26">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -5205,7 +5208,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5239,7 +5242,7 @@
       </c>
       <c r="Z19" s="11"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5295,7 +5298,7 @@
       </c>
       <c r="Z20" s="11"/>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5329,7 +5332,7 @@
       </c>
       <c r="Z21" s="11"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5363,7 +5366,7 @@
       </c>
       <c r="Z23" s="11"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5419,7 +5422,7 @@
       </c>
       <c r="Z24" s="11"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5453,7 +5456,7 @@
       </c>
       <c r="Z25" s="11"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
         <v>32</v>
       </c>
@@ -5462,7 +5465,7 @@
         <v>21773583.295806497</v>
       </c>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
         <v>33</v>
       </c>
@@ -5478,7 +5481,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="N29">
         <f>3529/'Population size'!N28*100</f>
         <v>7.0468319579830743</v>
@@ -5506,14 +5509,14 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -5581,7 +5584,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5621,7 +5624,7 @@
       </c>
       <c r="Z3" s="19"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5661,7 +5664,7 @@
       </c>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5701,7 +5704,7 @@
       </c>
       <c r="Z5" s="19"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5735,7 +5738,7 @@
       </c>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5771,7 +5774,7 @@
       </c>
       <c r="Z8" s="19"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5805,7 +5808,7 @@
       </c>
       <c r="Z9" s="19"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5841,7 +5844,7 @@
       </c>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5883,7 +5886,7 @@
       </c>
       <c r="Z12" s="19"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5919,7 +5922,7 @@
       </c>
       <c r="Z13" s="19"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
@@ -5954,7 +5957,7 @@
       </c>
       <c r="Z15" s="19"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
@@ -5995,7 +5998,7 @@
       </c>
       <c r="Z16" s="19"/>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -6030,7 +6033,7 @@
       </c>
       <c r="Z17" s="19"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6064,7 +6067,7 @@
       </c>
       <c r="Z19" s="19"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6112,7 +6115,7 @@
       </c>
       <c r="Z20" s="19"/>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6146,7 +6149,7 @@
       </c>
       <c r="Z21" s="19"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6180,7 +6183,7 @@
       </c>
       <c r="Z23" s="19"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6228,7 +6231,7 @@
       </c>
       <c r="Z24" s="19"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6282,14 +6285,14 @@
       <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -6357,7 +6360,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6390,7 +6393,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6423,7 +6426,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6456,7 +6459,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -6488,7 +6491,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6521,7 +6524,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6554,12 +6557,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -6627,7 +6630,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6660,7 +6663,7 @@
       </c>
       <c r="Y14" s="19"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6693,7 +6696,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6726,7 +6729,7 @@
       </c>
       <c r="Y16" s="19"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -6758,7 +6761,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6791,7 +6794,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6824,12 +6827,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -6897,7 +6900,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6930,7 +6933,7 @@
       </c>
       <c r="Y25" s="19"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6963,7 +6966,7 @@
       </c>
       <c r="Y26" s="19"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6996,7 +6999,7 @@
       </c>
       <c r="Y27" s="19"/>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -7028,7 +7031,7 @@
       </c>
       <c r="Y28" s="19"/>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7061,7 +7064,7 @@
       </c>
       <c r="Y29" s="19"/>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7113,14 +7116,14 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -7188,7 +7191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7223,7 +7226,7 @@
       </c>
       <c r="Y3" s="22"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7260,7 +7263,7 @@
       </c>
       <c r="Y4" s="22"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7293,7 +7296,7 @@
       </c>
       <c r="Y5" s="22"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -7325,7 +7328,7 @@
       </c>
       <c r="Y6" s="22"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7358,7 +7361,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7391,12 +7394,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -7464,7 +7467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>42</v>
       </c>
@@ -7496,12 +7499,12 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" s="7">
         <v>2000</v>
       </c>
@@ -7569,7 +7572,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
@@ -7617,12 +7620,12 @@
       </c>
       <c r="Y20" s="8"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -7690,7 +7693,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7723,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7756,7 +7759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7789,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>20</v>
       </c>
@@ -7821,7 +7824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7854,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7887,12 +7890,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C37" s="7">
         <v>2000</v>
       </c>
@@ -7960,7 +7963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>44</v>
       </c>
@@ -7994,12 +7997,12 @@
       </c>
       <c r="Y38" s="8"/>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C43" s="7">
         <v>2000</v>
       </c>
@@ -8067,7 +8070,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8120,7 +8123,7 @@
       </c>
       <c r="Y44" s="27"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -8173,12 +8176,12 @@
       </c>
       <c r="Y45" s="27"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C50" s="7">
         <v>2000</v>
       </c>
@@ -8246,7 +8249,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
         <v>44</v>
       </c>
@@ -8278,7 +8281,7 @@
       </c>
       <c r="Y51" s="22"/>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>49</v>
       </c>
@@ -8307,7 +8310,7 @@
       <c r="X55" s="30"/>
       <c r="Y55" s="30"/>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="31">
@@ -8378,7 +8381,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
       <c r="B57" s="31" t="s">
         <v>42</v>
@@ -8424,20 +8427,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI62"/>
+  <dimension ref="A1:AI68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
+      <selection activeCell="V64" sqref="V64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -8505,7 +8508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>44</v>
       </c>
@@ -8549,12 +8552,12 @@
       </c>
       <c r="Y3" s="27"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C8" s="7">
         <v>2000</v>
       </c>
@@ -8622,7 +8625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>44</v>
       </c>
@@ -8656,12 +8659,12 @@
       </c>
       <c r="Y9" s="27"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C14" s="7">
         <v>2000</v>
       </c>
@@ -8729,7 +8732,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
@@ -8787,12 +8790,12 @@
       </c>
       <c r="Y15" s="27"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C20" s="7">
         <v>2000</v>
       </c>
@@ -8860,7 +8863,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
@@ -8890,7 +8893,7 @@
       </c>
       <c r="Y21" s="37"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>54</v>
       </c>
@@ -8929,7 +8932,7 @@
       <c r="AH25" s="38"/>
       <c r="AI25" s="38"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="38"/>
       <c r="B26" s="38"/>
       <c r="C26" s="39">
@@ -9030,7 +9033,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="38"/>
       <c r="B27" s="39" t="s">
         <v>44</v>
@@ -9071,12 +9074,12 @@
       </c>
       <c r="AI27" s="40"/>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C31" s="7">
         <v>2000</v>
       </c>
@@ -9144,7 +9147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>44</v>
       </c>
@@ -9202,12 +9205,12 @@
       </c>
       <c r="Y32" s="27"/>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C37" s="7">
         <v>2000</v>
       </c>
@@ -9275,7 +9278,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>44</v>
       </c>
@@ -9313,7 +9316,7 @@
       </c>
       <c r="Y38" s="27"/>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="42"/>
       <c r="B39" s="42"/>
       <c r="C39" s="42"/>
@@ -9340,7 +9343,7 @@
       <c r="X39" s="42"/>
       <c r="Y39" s="42"/>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="42"/>
       <c r="B40" s="42"/>
       <c r="C40" s="42"/>
@@ -9367,7 +9370,7 @@
       <c r="X40" s="42"/>
       <c r="Y40" s="42"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="42"/>
       <c r="B41" s="42"/>
       <c r="C41" s="42"/>
@@ -9394,7 +9397,7 @@
       <c r="X41" s="42"/>
       <c r="Y41" s="42"/>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>57</v>
       </c>
@@ -9423,7 +9426,7 @@
       <c r="X42" s="42"/>
       <c r="Y42" s="42"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="42"/>
       <c r="B43" s="42"/>
       <c r="C43" s="7">
@@ -9494,7 +9497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="42"/>
       <c r="B44" s="7" t="s">
         <v>42</v>
@@ -9525,7 +9528,7 @@
       </c>
       <c r="Y44" s="43"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="42"/>
       <c r="B45" s="42"/>
       <c r="C45" s="42"/>
@@ -9552,7 +9555,7 @@
       <c r="X45" s="42"/>
       <c r="Y45" s="42"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="42"/>
       <c r="B46" s="42"/>
       <c r="C46" s="42"/>
@@ -9579,7 +9582,7 @@
       <c r="X46" s="42"/>
       <c r="Y46" s="42"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="42"/>
       <c r="B47" s="42"/>
       <c r="C47" s="42"/>
@@ -9606,7 +9609,7 @@
       <c r="X47" s="42"/>
       <c r="Y47" s="42"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
         <v>58</v>
       </c>
@@ -9635,7 +9638,7 @@
       <c r="X48" s="30"/>
       <c r="Y48" s="30"/>
     </row>
-    <row r="49" spans="1:35">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="30"/>
       <c r="B49" s="30"/>
       <c r="C49" s="31">
@@ -9706,7 +9709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:35">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
         <v>42</v>
@@ -9737,7 +9740,7 @@
       </c>
       <c r="Y50" s="32"/>
     </row>
-    <row r="51" spans="1:35">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="38"/>
       <c r="B51" s="38"/>
       <c r="C51" s="38"/>
@@ -9764,7 +9767,7 @@
       <c r="X51" s="38"/>
       <c r="Y51" s="38"/>
     </row>
-    <row r="52" spans="1:35">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="38"/>
       <c r="B52" s="38"/>
       <c r="C52" s="38"/>
@@ -9791,7 +9794,7 @@
       <c r="X52" s="38"/>
       <c r="Y52" s="38"/>
     </row>
-    <row r="53" spans="1:35">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="38"/>
       <c r="B53" s="38"/>
       <c r="C53" s="38"/>
@@ -9818,7 +9821,7 @@
       <c r="X53" s="38"/>
       <c r="Y53" s="38"/>
     </row>
-    <row r="54" spans="1:35">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
         <v>59</v>
       </c>
@@ -9847,7 +9850,7 @@
       <c r="X54" s="30"/>
       <c r="Y54" s="30"/>
     </row>
-    <row r="55" spans="1:35">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="30"/>
       <c r="B55" s="30"/>
       <c r="C55" s="31">
@@ -9918,7 +9921,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:35">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" s="31" t="s">
         <v>42</v>
@@ -9949,186 +9952,252 @@
       </c>
       <c r="Y56" s="32"/>
     </row>
-    <row r="60" spans="1:35">
-      <c r="A60" s="71" t="s">
+    <row r="60" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D61" s="7">
+        <v>2001</v>
+      </c>
+      <c r="E61" s="7">
+        <v>2002</v>
+      </c>
+      <c r="F61" s="7">
+        <v>2003</v>
+      </c>
+      <c r="G61" s="7">
+        <v>2004</v>
+      </c>
+      <c r="H61" s="7">
+        <v>2005</v>
+      </c>
+      <c r="I61" s="7">
+        <v>2006</v>
+      </c>
+      <c r="J61" s="7">
+        <v>2007</v>
+      </c>
+      <c r="K61" s="7">
+        <v>2008</v>
+      </c>
+      <c r="L61" s="7">
+        <v>2009</v>
+      </c>
+      <c r="M61" s="7">
+        <v>2010</v>
+      </c>
+      <c r="N61" s="7">
+        <v>2011</v>
+      </c>
+      <c r="O61" s="7">
+        <v>2012</v>
+      </c>
+      <c r="P61" s="7">
+        <v>2013</v>
+      </c>
+      <c r="Q61" s="7">
+        <v>2014</v>
+      </c>
+      <c r="R61" s="7">
+        <v>2015</v>
+      </c>
+      <c r="S61" s="7">
+        <v>2016</v>
+      </c>
+      <c r="T61" s="7">
+        <v>2017</v>
+      </c>
+      <c r="U61" s="7">
+        <v>2018</v>
+      </c>
+      <c r="V61" s="7">
+        <v>2019</v>
+      </c>
+      <c r="W61" s="7">
+        <v>2020</v>
+      </c>
+      <c r="Y61" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="45"/>
+      <c r="L62" s="45"/>
+      <c r="M62" s="45"/>
+      <c r="N62" s="45"/>
+      <c r="O62" s="45"/>
+      <c r="P62" s="45"/>
+      <c r="Q62" s="45"/>
+      <c r="R62" s="45"/>
+      <c r="S62" s="45"/>
+      <c r="T62" s="45"/>
+      <c r="U62" s="45"/>
+      <c r="V62" s="45"/>
+      <c r="W62" s="45"/>
+      <c r="X62" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y62" s="45"/>
+    </row>
+    <row r="63" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:35" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A66" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="70"/>
-      <c r="G60" s="70"/>
-      <c r="H60" s="70"/>
-      <c r="I60" s="70"/>
-      <c r="J60" s="70"/>
-      <c r="K60" s="70"/>
-      <c r="L60" s="70"/>
-      <c r="M60" s="70"/>
-      <c r="N60" s="70"/>
-      <c r="O60" s="70"/>
-      <c r="P60" s="70"/>
-      <c r="Q60" s="70"/>
-      <c r="R60" s="70"/>
-      <c r="S60" s="70"/>
-      <c r="T60" s="70"/>
-      <c r="U60" s="70"/>
-      <c r="V60" s="70"/>
-      <c r="W60" s="70"/>
-      <c r="X60" s="70"/>
-      <c r="Y60" s="70"/>
-      <c r="Z60" s="70"/>
-      <c r="AA60" s="70"/>
-      <c r="AB60" s="70"/>
-      <c r="AC60" s="70"/>
-      <c r="AD60" s="70"/>
-      <c r="AE60" s="70"/>
-      <c r="AF60" s="70"/>
-      <c r="AG60" s="70"/>
-      <c r="AH60" s="70"/>
-      <c r="AI60" s="70"/>
-    </row>
-    <row r="61" spans="1:35">
-      <c r="A61" s="70"/>
-      <c r="B61" s="70"/>
-      <c r="C61" s="72">
+      <c r="B66" s="70"/>
+      <c r="C66" s="70"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="70"/>
+      <c r="G66" s="70"/>
+      <c r="H66" s="70"/>
+      <c r="I66" s="70"/>
+      <c r="J66" s="70"/>
+      <c r="K66" s="70"/>
+      <c r="L66" s="70"/>
+      <c r="M66" s="70"/>
+      <c r="N66" s="70"/>
+      <c r="O66" s="70"/>
+      <c r="P66" s="70"/>
+      <c r="Q66" s="70"/>
+      <c r="R66" s="70"/>
+      <c r="S66" s="70"/>
+      <c r="T66" s="70"/>
+      <c r="U66" s="70"/>
+      <c r="V66" s="70"/>
+      <c r="W66" s="70"/>
+      <c r="X66" s="70"/>
+      <c r="Y66" s="70"/>
+      <c r="Z66" s="70"/>
+      <c r="AA66" s="70"/>
+      <c r="AB66" s="70"/>
+      <c r="AC66" s="70"/>
+      <c r="AD66" s="70"/>
+      <c r="AE66" s="70"/>
+      <c r="AF66" s="70"/>
+      <c r="AG66" s="70"/>
+      <c r="AH66" s="70"/>
+      <c r="AI66" s="70"/>
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A67" s="70"/>
+      <c r="B67" s="70"/>
+      <c r="C67" s="72">
         <v>2000</v>
       </c>
-      <c r="D61" s="72">
+      <c r="D67" s="72">
         <v>2001</v>
       </c>
-      <c r="E61" s="72">
+      <c r="E67" s="72">
         <v>2002</v>
       </c>
-      <c r="F61" s="72">
+      <c r="F67" s="72">
         <v>2003</v>
       </c>
-      <c r="G61" s="72">
+      <c r="G67" s="72">
         <v>2004</v>
       </c>
-      <c r="H61" s="72">
+      <c r="H67" s="72">
         <v>2005</v>
       </c>
-      <c r="I61" s="72">
+      <c r="I67" s="72">
         <v>2006</v>
       </c>
-      <c r="J61" s="72">
+      <c r="J67" s="72">
         <v>2007</v>
       </c>
-      <c r="K61" s="72">
+      <c r="K67" s="72">
         <v>2008</v>
       </c>
-      <c r="L61" s="72">
+      <c r="L67" s="72">
         <v>2009</v>
       </c>
-      <c r="M61" s="72">
+      <c r="M67" s="72">
         <v>2010</v>
       </c>
-      <c r="N61" s="72">
+      <c r="N67" s="72">
         <v>2011</v>
       </c>
-      <c r="O61" s="72">
+      <c r="O67" s="72">
         <v>2012</v>
       </c>
-      <c r="P61" s="72">
+      <c r="P67" s="72">
         <v>2013</v>
       </c>
-      <c r="Q61" s="72">
+      <c r="Q67" s="72">
         <v>2014</v>
       </c>
-      <c r="R61" s="72">
+      <c r="R67" s="72">
         <v>2015</v>
       </c>
-      <c r="S61" s="72">
+      <c r="S67" s="72">
         <v>2016</v>
       </c>
-      <c r="T61" s="72">
+      <c r="T67" s="72">
         <v>2017</v>
       </c>
-      <c r="U61" s="72">
+      <c r="U67" s="72">
         <v>2018</v>
       </c>
-      <c r="V61" s="72">
+      <c r="V67" s="72">
         <v>2019</v>
       </c>
-      <c r="W61" s="72">
+      <c r="W67" s="72">
         <v>2020</v>
       </c>
-      <c r="X61" s="72">
-        <v>2021</v>
-      </c>
-      <c r="Y61" s="72">
-        <v>2022</v>
-      </c>
-      <c r="Z61" s="72">
-        <v>2023</v>
-      </c>
-      <c r="AA61" s="72">
-        <v>2024</v>
-      </c>
-      <c r="AB61" s="72">
-        <v>2025</v>
-      </c>
-      <c r="AC61" s="72">
-        <v>2026</v>
-      </c>
-      <c r="AD61" s="72">
-        <v>2027</v>
-      </c>
-      <c r="AE61" s="72">
-        <v>2028</v>
-      </c>
-      <c r="AF61" s="72">
-        <v>2029</v>
-      </c>
-      <c r="AG61" s="72">
-        <v>2030</v>
-      </c>
-      <c r="AH61" s="70"/>
-      <c r="AI61" s="72" t="s">
+      <c r="X67" s="70"/>
+      <c r="Y67" s="72" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:35">
-      <c r="A62" s="70"/>
-      <c r="B62" s="72" t="s">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A68" s="70"/>
+      <c r="B68" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="73"/>
-      <c r="I62" s="73"/>
-      <c r="J62" s="73"/>
-      <c r="K62" s="73"/>
-      <c r="L62" s="73"/>
-      <c r="M62" s="73"/>
-      <c r="N62" s="73"/>
-      <c r="O62" s="73"/>
-      <c r="P62" s="73"/>
-      <c r="Q62" s="73"/>
-      <c r="R62" s="73"/>
-      <c r="S62" s="73"/>
-      <c r="T62" s="73"/>
-      <c r="U62" s="73"/>
-      <c r="V62" s="73"/>
-      <c r="W62" s="73"/>
-      <c r="X62" s="73"/>
-      <c r="Y62" s="73"/>
-      <c r="Z62" s="73"/>
-      <c r="AA62" s="73"/>
-      <c r="AB62" s="73"/>
-      <c r="AC62" s="73"/>
-      <c r="AD62" s="73"/>
-      <c r="AE62" s="73"/>
-      <c r="AF62" s="73"/>
-      <c r="AG62" s="73"/>
-      <c r="AH62" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI62" s="73">
+      <c r="C68" s="73"/>
+      <c r="D68" s="73"/>
+      <c r="E68" s="73"/>
+      <c r="F68" s="73"/>
+      <c r="G68" s="73"/>
+      <c r="H68" s="73"/>
+      <c r="I68" s="73"/>
+      <c r="J68" s="73"/>
+      <c r="K68" s="73"/>
+      <c r="L68" s="73"/>
+      <c r="M68" s="73"/>
+      <c r="N68" s="73"/>
+      <c r="O68" s="73"/>
+      <c r="P68" s="73"/>
+      <c r="Q68" s="73"/>
+      <c r="R68" s="73"/>
+      <c r="S68" s="73"/>
+      <c r="T68" s="73"/>
+      <c r="U68" s="73"/>
+      <c r="V68" s="73"/>
+      <c r="W68" s="73"/>
+      <c r="X68" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y68" s="73">
         <v>0.85</v>
       </c>
     </row>
@@ -10147,18 +10216,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="Y3" sqref="Y3:Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="C2" s="7">
         <v>2000</v>
@@ -10227,7 +10296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -10261,7 +10330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -10295,7 +10364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10328,7 +10397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -10360,7 +10429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
@@ -10394,7 +10463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
@@ -10428,15 +10497,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -10504,7 +10573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10537,7 +10606,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10570,7 +10639,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10603,7 +10672,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -10635,7 +10704,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10668,7 +10737,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10701,12 +10770,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -10774,7 +10843,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10807,7 +10876,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10840,7 +10909,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10873,7 +10942,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -10905,7 +10974,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10938,7 +11007,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10971,7 +11040,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
         <v>62</v>
       </c>
@@ -11000,7 +11069,7 @@
       <c r="X34" s="30"/>
       <c r="Y34" s="30"/>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="31">
@@ -11071,7 +11140,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
       <c r="B36" s="31" t="s">
         <v>42</v>
@@ -11104,7 +11173,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>63</v>
       </c>
@@ -11133,7 +11202,7 @@
       <c r="X40" s="30"/>
       <c r="Y40" s="30"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="31">
@@ -11204,7 +11273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
         <v>42</v>
@@ -11237,7 +11306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>64</v>
       </c>
@@ -11266,7 +11335,7 @@
       <c r="X46" s="30"/>
       <c r="Y46" s="30"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="30"/>
       <c r="C47" s="31">
@@ -11337,7 +11406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="31" t="s">
         <v>42</v>
@@ -11389,14 +11458,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -11464,7 +11533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11497,7 +11566,7 @@
       </c>
       <c r="Y3" s="8"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11530,7 +11599,7 @@
       </c>
       <c r="Y4" s="8"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11563,7 +11632,7 @@
       </c>
       <c r="Y5" s="8"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -11595,7 +11664,7 @@
       </c>
       <c r="Y6" s="8"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11628,7 +11697,7 @@
       </c>
       <c r="Y7" s="8"/>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11661,12 +11730,12 @@
       </c>
       <c r="Y8" s="8"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -11734,7 +11803,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11767,7 +11836,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11800,7 +11869,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11833,7 +11902,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -11865,7 +11934,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11898,7 +11967,7 @@
       </c>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11931,12 +12000,12 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -12004,7 +12073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12037,7 +12106,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12070,7 +12139,7 @@
       </c>
       <c r="Y26" s="8"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12103,7 +12172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -12135,7 +12204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12168,7 +12237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12201,12 +12270,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C35" s="7">
         <v>2000</v>
       </c>
@@ -12274,7 +12343,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12307,7 +12376,7 @@
       </c>
       <c r="Y36" s="22"/>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12340,7 +12409,7 @@
       </c>
       <c r="Y37" s="22"/>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12373,7 +12442,7 @@
       </c>
       <c r="Y38" s="22"/>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>20</v>
       </c>
@@ -12405,7 +12474,7 @@
       </c>
       <c r="Y39" s="22"/>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12438,7 +12507,7 @@
       </c>
       <c r="Y40" s="22"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12471,12 +12540,12 @@
       </c>
       <c r="Y41" s="22"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C46" s="7">
         <v>2000</v>
       </c>
@@ -12544,7 +12613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12577,7 +12646,7 @@
       </c>
       <c r="Y47" s="22"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12614,7 +12683,7 @@
       </c>
       <c r="Y48" s="22"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12647,7 +12716,7 @@
       </c>
       <c r="Y49" s="22"/>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
         <v>20</v>
       </c>
@@ -12679,7 +12748,7 @@
       </c>
       <c r="Y50" s="22"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12716,7 +12785,7 @@
       </c>
       <c r="Y51" s="22"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12753,12 +12822,12 @@
       </c>
       <c r="Y52" s="22"/>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C57" s="7">
         <v>2000</v>
       </c>
@@ -12826,7 +12895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12861,7 +12930,7 @@
       </c>
       <c r="Y58" s="22"/>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12896,7 +12965,7 @@
       </c>
       <c r="Y59" s="22"/>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12929,7 +12998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B61" s="7" t="s">
         <v>20</v>
       </c>
@@ -12961,7 +13030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12994,7 +13063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -13027,12 +13096,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C68" s="7">
         <v>2000</v>
       </c>
@@ -13100,7 +13169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13133,7 +13202,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -13166,7 +13235,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B71" s="7" t="s">
         <v>20</v>
       </c>
@@ -13198,7 +13267,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -13231,12 +13300,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C77" s="7">
         <v>2000</v>
       </c>
@@ -13304,7 +13373,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13337,7 +13406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -13370,7 +13439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
         <v>20</v>
       </c>
@@ -13402,7 +13471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:25">
+    <row r="81" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B81" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>

</xml_diff>

<commit_message>
make pwid neither male nor female
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12585" tabRatio="805" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="12580" tabRatio="805" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="137">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -795,7 +795,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -925,6 +925,8 @@
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1126,7 +1128,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="137">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1142,6 +1144,7 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1242,6 +1245,7 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -1768,31 +1772,31 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="82"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="82"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="406">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="140">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1819,14 +1823,14 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -1894,7 +1898,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -1927,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -1960,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -1993,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -2025,7 +2029,7 @@
       </c>
       <c r="Y6" s="8"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2058,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2091,12 +2095,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -2164,7 +2168,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2197,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2230,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2263,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -2295,7 +2299,7 @@
       </c>
       <c r="Y17" s="22"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2328,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2361,12 +2365,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -2434,7 +2438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="B25" s="7" t="s">
         <v>42</v>
       </c>
@@ -2481,18 +2485,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2518,7 +2522,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2530,7 +2534,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2546,7 +2550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2560,7 +2564,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="B6" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2574,7 +2578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2590,7 +2594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2602,12 +2606,12 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="C13" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2633,7 +2637,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2645,7 +2649,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2661,7 +2665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2675,7 +2679,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2689,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2705,7 +2709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2717,12 +2721,12 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="C24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2748,7 +2752,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2760,7 +2764,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2774,7 +2778,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2786,7 +2790,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="B28" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2798,7 +2802,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2810,7 +2814,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2822,12 +2826,12 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="C35" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2853,7 +2857,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="B36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2865,7 +2869,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2877,7 +2881,7 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2889,7 +2893,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2903,7 +2907,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="B40" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2915,7 +2919,7 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="B41" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2927,12 +2931,12 @@
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="C46" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2958,7 +2962,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="B47" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2970,7 +2974,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="B48" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2982,12 +2986,12 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="C53" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3013,7 +3017,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="B54" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3025,7 +3029,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="B55" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3037,7 +3041,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="B56" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3049,7 +3053,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="B57" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3061,7 +3065,7 @@
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="B58" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3073,7 +3077,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="B59" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3085,12 +3089,12 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="C64" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3116,7 +3120,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8">
       <c r="B65" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3130,7 +3134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8">
       <c r="B66" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3144,7 +3148,7 @@
       </c>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8">
       <c r="B67" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3158,7 +3162,7 @@
       </c>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8">
       <c r="B68" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3170,7 +3174,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8">
       <c r="B69" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3182,7 +3186,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8">
       <c r="B70" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3213,9 +3217,9 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="77" t="s">
         <v>83</v>
       </c>
@@ -3224,7 +3228,7 @@
       <c r="D1" s="75"/>
       <c r="E1" s="75"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="75"/>
       <c r="B2" s="75"/>
       <c r="C2" s="76" t="s">
@@ -3237,7 +3241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="75"/>
       <c r="B3" s="78" t="s">
         <v>84</v>
@@ -3252,7 +3256,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="75"/>
       <c r="B4" s="78" t="s">
         <v>85</v>
@@ -3267,7 +3271,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="75"/>
       <c r="B5" s="78" t="s">
         <v>86</v>
@@ -3282,7 +3286,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="75"/>
       <c r="B6" s="78" t="s">
         <v>87</v>
@@ -3297,7 +3301,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="75"/>
       <c r="B7" s="78" t="s">
         <v>88</v>
@@ -3312,7 +3316,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="75"/>
       <c r="B8" s="78" t="s">
         <v>89</v>
@@ -3327,7 +3331,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="75"/>
       <c r="B9" s="78" t="s">
         <v>90</v>
@@ -3342,33 +3346,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="38"/>
       <c r="B10" s="52"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="38"/>
       <c r="B11" s="52"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="38"/>
       <c r="B12" s="52"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
@@ -3379,7 +3383,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="B15" s="3" t="s">
         <v>92</v>
       </c>
@@ -3393,7 +3397,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
         <v>93</v>
       </c>
@@ -3407,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="B17" s="3" t="s">
         <v>94</v>
       </c>
@@ -3421,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="B18" s="3" t="s">
         <v>95</v>
       </c>
@@ -3435,7 +3439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="B19" s="3" t="s">
         <v>96</v>
       </c>
@@ -3449,7 +3453,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="B20" s="3" t="s">
         <v>97</v>
       </c>
@@ -3463,33 +3467,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="38"/>
       <c r="B21" s="52"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="38"/>
       <c r="B22" s="52"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="38"/>
       <c r="B23" s="52"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="C25" s="7" t="s">
         <v>30</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="B26" s="3" t="s">
         <v>99</v>
       </c>
@@ -3514,7 +3518,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="B27" s="3" t="s">
         <v>94</v>
       </c>
@@ -3528,7 +3532,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="B28" s="3" t="s">
         <v>100</v>
       </c>
@@ -3542,7 +3546,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="B29" s="3" t="s">
         <v>101</v>
       </c>
@@ -3556,7 +3560,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="B30" s="3" t="s">
         <v>102</v>
       </c>
@@ -3570,33 +3574,33 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="38"/>
       <c r="B31" s="52"/>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="38"/>
       <c r="B32" s="52"/>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
       <c r="E32" s="38"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="38"/>
       <c r="B33" s="52"/>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="C35" s="7" t="s">
         <v>30</v>
       </c>
@@ -3607,7 +3611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="B36" s="3" t="s">
         <v>104</v>
       </c>
@@ -3621,7 +3625,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="B37" s="3" t="s">
         <v>105</v>
       </c>
@@ -3635,7 +3639,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="B38" s="3" t="s">
         <v>106</v>
       </c>
@@ -3649,7 +3653,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="B39" s="3" t="s">
         <v>107</v>
       </c>
@@ -3663,33 +3667,33 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="38"/>
       <c r="B40" s="52"/>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="38"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="38"/>
       <c r="B41" s="52"/>
       <c r="C41" s="38"/>
       <c r="D41" s="38"/>
       <c r="E41" s="38"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="38"/>
       <c r="B42" s="52"/>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="C44" s="7" t="s">
         <v>30</v>
       </c>
@@ -3700,7 +3704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="B45" s="3" t="s">
         <v>92</v>
       </c>
@@ -3714,7 +3718,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="B46" s="3" t="s">
         <v>93</v>
       </c>
@@ -3728,7 +3732,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="B47" s="3" t="s">
         <v>109</v>
       </c>
@@ -3742,7 +3746,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="B48" s="3" t="s">
         <v>95</v>
       </c>
@@ -3756,7 +3760,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="B49" s="3" t="s">
         <v>96</v>
       </c>
@@ -3774,7 +3778,7 @@
       <c r="H49" s="38"/>
       <c r="I49" s="38"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="B50" s="3" t="s">
         <v>97</v>
       </c>
@@ -3792,7 +3796,7 @@
       <c r="H50" s="38"/>
       <c r="I50" s="38"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="B51" s="3" t="s">
         <v>110</v>
       </c>
@@ -3810,7 +3814,7 @@
       <c r="H51" s="38"/>
       <c r="I51" s="38"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="B52" s="3" t="s">
         <v>111</v>
       </c>
@@ -3828,7 +3832,7 @@
       <c r="H52" s="38"/>
       <c r="I52" s="38"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="38"/>
       <c r="B53" s="52"/>
       <c r="C53" s="38"/>
@@ -3839,7 +3843,7 @@
       <c r="H53" s="38"/>
       <c r="I53" s="38"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="38"/>
       <c r="B54" s="52"/>
       <c r="C54" s="38"/>
@@ -3850,7 +3854,7 @@
       <c r="H54" s="38"/>
       <c r="I54" s="38"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="38"/>
       <c r="B55" s="52"/>
       <c r="C55" s="38"/>
@@ -3861,7 +3865,7 @@
       <c r="H55" s="38"/>
       <c r="I55" s="38"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -3870,7 +3874,7 @@
       <c r="H56" s="38"/>
       <c r="I56" s="38"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="C57" s="7" t="s">
         <v>30</v>
       </c>
@@ -3885,7 +3889,7 @@
       <c r="H57" s="38"/>
       <c r="I57" s="38"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="B58" s="3" t="s">
         <v>113</v>
       </c>
@@ -3903,7 +3907,7 @@
       <c r="H58" s="54"/>
       <c r="I58" s="54"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="B59" s="3" t="s">
         <v>114</v>
       </c>
@@ -3921,7 +3925,7 @@
       <c r="H59" s="54"/>
       <c r="I59" s="54"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="B60" s="3" t="s">
         <v>115</v>
       </c>
@@ -3936,7 +3940,7 @@
       </c>
       <c r="F60" s="38"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="B61" s="3" t="s">
         <v>116</v>
       </c>
@@ -3954,7 +3958,7 @@
       <c r="H61" s="54"/>
       <c r="I61" s="54"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="B62" s="3" t="s">
         <v>117</v>
       </c>
@@ -3972,7 +3976,7 @@
       <c r="H62" s="54"/>
       <c r="I62" s="54"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="B63" s="3" t="s">
         <v>118</v>
       </c>
@@ -3990,7 +3994,7 @@
       <c r="H63" s="54"/>
       <c r="I63" s="54"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="B64" s="3" t="s">
         <v>119</v>
       </c>
@@ -4008,7 +4012,7 @@
       <c r="H64" s="54"/>
       <c r="I64" s="54"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="B65" s="3" t="s">
         <v>120</v>
       </c>
@@ -4026,7 +4030,7 @@
       <c r="H65" s="54"/>
       <c r="I65" s="54"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="B66" s="3" t="s">
         <v>121</v>
       </c>
@@ -4044,7 +4048,7 @@
       <c r="H66" s="38"/>
       <c r="I66" s="38"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="38"/>
       <c r="B67" s="52"/>
       <c r="C67" s="38"/>
@@ -4055,7 +4059,7 @@
       <c r="H67" s="38"/>
       <c r="I67" s="38"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="60"/>
       <c r="B68" s="61"/>
       <c r="C68" s="67"/>
@@ -4066,7 +4070,7 @@
       <c r="H68" s="67"/>
       <c r="I68" s="38"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="67"/>
       <c r="B69" s="61"/>
       <c r="C69" s="62"/>
@@ -4077,7 +4081,7 @@
       <c r="H69" s="67"/>
       <c r="I69" s="38"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="57" t="s">
         <v>130</v>
       </c>
@@ -4091,7 +4095,7 @@
       <c r="I70" s="38"/>
       <c r="J70" s="55"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="68"/>
       <c r="B71" s="68"/>
       <c r="C71" s="58" t="s">
@@ -4109,7 +4113,7 @@
       <c r="I71" s="38"/>
       <c r="J71" s="55"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="68"/>
       <c r="B72" s="59" t="s">
         <v>131</v>
@@ -4129,7 +4133,7 @@
       <c r="I72" s="38"/>
       <c r="J72" s="55"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="68"/>
       <c r="B73" s="59" t="s">
         <v>132</v>
@@ -4148,7 +4152,7 @@
       <c r="H73" s="67"/>
       <c r="I73" s="38"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="68"/>
       <c r="B74" s="59" t="s">
         <v>133</v>
@@ -4167,7 +4171,7 @@
       <c r="H74" s="67"/>
       <c r="I74" s="38"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="56"/>
       <c r="B75" s="56"/>
       <c r="C75" s="56"/>
@@ -4178,7 +4182,7 @@
       <c r="H75" s="67"/>
       <c r="I75" s="38"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="56"/>
       <c r="B76" s="56"/>
       <c r="C76" s="56"/>
@@ -4189,7 +4193,7 @@
       <c r="H76" s="67"/>
       <c r="I76" s="38"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="56"/>
       <c r="B77" s="56"/>
       <c r="C77" s="56"/>
@@ -4199,7 +4203,7 @@
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="63" t="s">
         <v>122</v>
       </c>
@@ -4211,7 +4215,7 @@
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="56"/>
       <c r="B79" s="56"/>
       <c r="C79" s="64" t="s">
@@ -4227,7 +4231,7 @@
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="56"/>
       <c r="B80" s="65" t="s">
         <v>123</v>
@@ -4245,7 +4249,7 @@
       <c r="G80" s="56"/>
       <c r="H80" s="56"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81" s="56"/>
       <c r="B81" s="65" t="s">
         <v>124</v>
@@ -4263,7 +4267,7 @@
       <c r="G81" s="56"/>
       <c r="H81" s="56"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82" s="56"/>
       <c r="B82" s="65" t="s">
         <v>125</v>
@@ -4281,7 +4285,7 @@
       <c r="G82" s="56"/>
       <c r="H82" s="56"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="56"/>
       <c r="B83" s="65" t="s">
         <v>126</v>
@@ -4299,7 +4303,7 @@
       <c r="G83" s="56"/>
       <c r="H83" s="56"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84" s="56"/>
       <c r="B84" s="65" t="s">
         <v>127</v>
@@ -4317,7 +4321,7 @@
       <c r="G84" s="56"/>
       <c r="H84" s="56"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="56"/>
       <c r="B85" s="65" t="s">
         <v>128</v>
@@ -4335,7 +4339,7 @@
       <c r="G85" s="56"/>
       <c r="H85" s="56"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="56"/>
       <c r="B86" s="65" t="s">
         <v>129</v>
@@ -4353,17 +4357,17 @@
       <c r="G86" s="56"/>
       <c r="H86" s="56"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8">
       <c r="F87" s="56"/>
       <c r="G87" s="56"/>
       <c r="H87" s="56"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8">
       <c r="F88" s="56"/>
       <c r="G88" s="56"/>
       <c r="H88" s="56"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="F89" s="56"/>
       <c r="G89" s="56"/>
       <c r="H89" s="56"/>
@@ -4384,17 +4388,17 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -4420,7 +4424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -4449,7 +4453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -4478,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -4507,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -4518,7 +4522,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>14</v>
@@ -4536,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -4565,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -4596,7 +4600,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4613,15 +4617,15 @@
       <selection activeCell="Z2" sqref="Z2:Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4689,7 +4693,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4723,7 +4727,7 @@
       </c>
       <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4779,7 +4783,7 @@
       </c>
       <c r="Z4" s="11"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4813,7 +4817,7 @@
       </c>
       <c r="Z5" s="11"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4847,7 +4851,7 @@
       </c>
       <c r="Z7" s="11"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4903,7 +4907,7 @@
       </c>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -4937,7 +4941,7 @@
       </c>
       <c r="Z9" s="11"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -4971,7 +4975,7 @@
       </c>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="B12" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5027,7 +5031,7 @@
       </c>
       <c r="Z12" s="11"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="B13" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5061,7 +5065,7 @@
       </c>
       <c r="Z13" s="11"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -5074,7 +5078,7 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
@@ -5107,7 +5111,7 @@
       </c>
       <c r="Z15" s="11"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
@@ -5162,7 +5166,7 @@
       </c>
       <c r="Z16" s="11"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -5195,7 +5199,7 @@
       </c>
       <c r="Z17" s="11"/>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26">
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -5208,7 +5212,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5242,7 +5246,7 @@
       </c>
       <c r="Z19" s="11"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26">
       <c r="B20" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5298,7 +5302,7 @@
       </c>
       <c r="Z20" s="11"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26">
       <c r="B21" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5332,7 +5336,7 @@
       </c>
       <c r="Z21" s="11"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5366,7 +5370,7 @@
       </c>
       <c r="Z23" s="11"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5422,7 +5426,7 @@
       </c>
       <c r="Z24" s="11"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5456,7 +5460,7 @@
       </c>
       <c r="Z25" s="11"/>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26">
       <c r="M27" t="s">
         <v>32</v>
       </c>
@@ -5465,7 +5469,7 @@
         <v>21773583.295806497</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26">
       <c r="M28" t="s">
         <v>33</v>
       </c>
@@ -5481,7 +5485,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26">
       <c r="N29">
         <f>3529/'Population size'!N28*100</f>
         <v>7.0468319579830743</v>
@@ -5509,14 +5513,14 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -5584,7 +5588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5624,7 +5628,7 @@
       </c>
       <c r="Z3" s="19"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5664,7 +5668,7 @@
       </c>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5704,7 +5708,7 @@
       </c>
       <c r="Z5" s="19"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5738,7 +5742,7 @@
       </c>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5774,7 +5778,7 @@
       </c>
       <c r="Z8" s="19"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5808,7 +5812,7 @@
       </c>
       <c r="Z9" s="19"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5844,7 +5848,7 @@
       </c>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="B12" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5886,7 +5890,7 @@
       </c>
       <c r="Z12" s="19"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="B13" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5922,7 +5926,7 @@
       </c>
       <c r="Z13" s="19"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
@@ -5957,7 +5961,7 @@
       </c>
       <c r="Z15" s="19"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
@@ -5998,7 +6002,7 @@
       </c>
       <c r="Z16" s="19"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -6033,7 +6037,7 @@
       </c>
       <c r="Z17" s="19"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6067,7 +6071,7 @@
       </c>
       <c r="Z19" s="19"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26">
       <c r="B20" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6115,7 +6119,7 @@
       </c>
       <c r="Z20" s="19"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26">
       <c r="B21" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6149,7 +6153,7 @@
       </c>
       <c r="Z21" s="19"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6183,7 +6187,7 @@
       </c>
       <c r="Z23" s="19"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6231,7 +6235,7 @@
       </c>
       <c r="Z24" s="19"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6285,14 +6289,14 @@
       <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -6360,7 +6364,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6393,7 +6397,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6426,7 +6430,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6459,7 +6463,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -6491,7 +6495,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6524,7 +6528,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6557,12 +6561,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -6630,7 +6634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6663,7 +6667,7 @@
       </c>
       <c r="Y14" s="19"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6696,7 +6700,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6729,7 +6733,7 @@
       </c>
       <c r="Y16" s="19"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -6761,7 +6765,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6794,7 +6798,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6827,12 +6831,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -6900,7 +6904,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6933,7 +6937,7 @@
       </c>
       <c r="Y25" s="19"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6966,7 +6970,7 @@
       </c>
       <c r="Y26" s="19"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6999,7 +7003,7 @@
       </c>
       <c r="Y27" s="19"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -7031,7 +7035,7 @@
       </c>
       <c r="Y28" s="19"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7064,7 +7068,7 @@
       </c>
       <c r="Y29" s="19"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7112,18 +7116,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -7191,7 +7195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7226,7 +7230,7 @@
       </c>
       <c r="Y3" s="22"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7263,7 +7267,7 @@
       </c>
       <c r="Y4" s="22"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7296,7 +7300,7 @@
       </c>
       <c r="Y5" s="22"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -7328,7 +7332,7 @@
       </c>
       <c r="Y6" s="22"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7361,7 +7365,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7394,12 +7398,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -7467,7 +7471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="7" t="s">
         <v>42</v>
       </c>
@@ -7499,12 +7503,12 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="A18" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="C19" s="7">
         <v>2000</v>
       </c>
@@ -7572,7 +7576,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
@@ -7620,12 +7624,12 @@
       </c>
       <c r="Y20" s="8"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -7693,7 +7697,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7726,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="B28" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7759,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7792,7 +7796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="B30" s="7" t="s">
         <v>20</v>
       </c>
@@ -7824,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7857,7 +7861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7890,12 +7894,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="C37" s="7">
         <v>2000</v>
       </c>
@@ -7963,7 +7967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25">
       <c r="B38" s="7" t="s">
         <v>44</v>
       </c>
@@ -7997,12 +8001,12 @@
       </c>
       <c r="Y38" s="8"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25">
       <c r="C43" s="7">
         <v>2000</v>
       </c>
@@ -8070,7 +8074,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25">
       <c r="B44" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8123,7 +8127,7 @@
       </c>
       <c r="Y44" s="27"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -8176,12 +8180,12 @@
       </c>
       <c r="Y45" s="27"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25">
       <c r="C50" s="7">
         <v>2000</v>
       </c>
@@ -8249,7 +8253,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="B51" s="7" t="s">
         <v>44</v>
       </c>
@@ -8281,7 +8285,7 @@
       </c>
       <c r="Y51" s="22"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25">
       <c r="A55" s="29" t="s">
         <v>49</v>
       </c>
@@ -8310,7 +8314,7 @@
       <c r="X55" s="30"/>
       <c r="Y55" s="30"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="31">
@@ -8381,7 +8385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25">
       <c r="A57" s="30"/>
       <c r="B57" s="31" t="s">
         <v>42</v>
@@ -8429,18 +8433,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
+    <sheetView topLeftCell="F31" workbookViewId="0">
       <selection activeCell="V64" sqref="V64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -8508,7 +8512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="7" t="s">
         <v>44</v>
       </c>
@@ -8552,12 +8556,12 @@
       </c>
       <c r="Y3" s="27"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="C8" s="7">
         <v>2000</v>
       </c>
@@ -8625,7 +8629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" s="7" t="s">
         <v>44</v>
       </c>
@@ -8659,12 +8663,12 @@
       </c>
       <c r="Y9" s="27"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="C14" s="7">
         <v>2000</v>
       </c>
@@ -8732,7 +8736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
@@ -8790,12 +8794,12 @@
       </c>
       <c r="Y15" s="27"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35">
       <c r="C20" s="7">
         <v>2000</v>
       </c>
@@ -8863,7 +8867,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35">
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
@@ -8893,7 +8897,7 @@
       </c>
       <c r="Y21" s="37"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35">
       <c r="A25" s="24" t="s">
         <v>54</v>
       </c>
@@ -8932,7 +8936,7 @@
       <c r="AH25" s="38"/>
       <c r="AI25" s="38"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35">
       <c r="A26" s="38"/>
       <c r="B26" s="38"/>
       <c r="C26" s="39">
@@ -9033,7 +9037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35">
       <c r="A27" s="38"/>
       <c r="B27" s="39" t="s">
         <v>44</v>
@@ -9074,12 +9078,12 @@
       </c>
       <c r="AI27" s="40"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35">
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35">
       <c r="C31" s="7">
         <v>2000</v>
       </c>
@@ -9147,7 +9151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35">
       <c r="B32" s="7" t="s">
         <v>44</v>
       </c>
@@ -9205,12 +9209,12 @@
       </c>
       <c r="Y32" s="27"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="A36" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="C37" s="7">
         <v>2000</v>
       </c>
@@ -9278,7 +9282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25">
       <c r="B38" s="7" t="s">
         <v>44</v>
       </c>
@@ -9316,7 +9320,7 @@
       </c>
       <c r="Y38" s="27"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25">
       <c r="A39" s="42"/>
       <c r="B39" s="42"/>
       <c r="C39" s="42"/>
@@ -9343,7 +9347,7 @@
       <c r="X39" s="42"/>
       <c r="Y39" s="42"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25">
       <c r="A40" s="42"/>
       <c r="B40" s="42"/>
       <c r="C40" s="42"/>
@@ -9370,7 +9374,7 @@
       <c r="X40" s="42"/>
       <c r="Y40" s="42"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25">
       <c r="A41" s="42"/>
       <c r="B41" s="42"/>
       <c r="C41" s="42"/>
@@ -9397,7 +9401,7 @@
       <c r="X41" s="42"/>
       <c r="Y41" s="42"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25">
       <c r="A42" s="2" t="s">
         <v>57</v>
       </c>
@@ -9426,7 +9430,7 @@
       <c r="X42" s="42"/>
       <c r="Y42" s="42"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25">
       <c r="A43" s="42"/>
       <c r="B43" s="42"/>
       <c r="C43" s="7">
@@ -9497,7 +9501,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25">
       <c r="A44" s="42"/>
       <c r="B44" s="7" t="s">
         <v>42</v>
@@ -9528,7 +9532,7 @@
       </c>
       <c r="Y44" s="43"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25">
       <c r="A45" s="42"/>
       <c r="B45" s="42"/>
       <c r="C45" s="42"/>
@@ -9555,7 +9559,7 @@
       <c r="X45" s="42"/>
       <c r="Y45" s="42"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25">
       <c r="A46" s="42"/>
       <c r="B46" s="42"/>
       <c r="C46" s="42"/>
@@ -9582,7 +9586,7 @@
       <c r="X46" s="42"/>
       <c r="Y46" s="42"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25">
       <c r="A47" s="42"/>
       <c r="B47" s="42"/>
       <c r="C47" s="42"/>
@@ -9609,7 +9613,7 @@
       <c r="X47" s="42"/>
       <c r="Y47" s="42"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25">
       <c r="A48" s="29" t="s">
         <v>58</v>
       </c>
@@ -9638,7 +9642,7 @@
       <c r="X48" s="30"/>
       <c r="Y48" s="30"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25">
       <c r="A49" s="30"/>
       <c r="B49" s="30"/>
       <c r="C49" s="31">
@@ -9709,7 +9713,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
         <v>42</v>
@@ -9740,7 +9744,7 @@
       </c>
       <c r="Y50" s="32"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="A51" s="38"/>
       <c r="B51" s="38"/>
       <c r="C51" s="38"/>
@@ -9767,7 +9771,7 @@
       <c r="X51" s="38"/>
       <c r="Y51" s="38"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25">
       <c r="A52" s="38"/>
       <c r="B52" s="38"/>
       <c r="C52" s="38"/>
@@ -9794,7 +9798,7 @@
       <c r="X52" s="38"/>
       <c r="Y52" s="38"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25">
       <c r="A53" s="38"/>
       <c r="B53" s="38"/>
       <c r="C53" s="38"/>
@@ -9821,7 +9825,7 @@
       <c r="X53" s="38"/>
       <c r="Y53" s="38"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25">
       <c r="A54" s="29" t="s">
         <v>59</v>
       </c>
@@ -9850,7 +9854,7 @@
       <c r="X54" s="30"/>
       <c r="Y54" s="30"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25">
       <c r="A55" s="30"/>
       <c r="B55" s="30"/>
       <c r="C55" s="31">
@@ -9921,7 +9925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25">
       <c r="A56" s="30"/>
       <c r="B56" s="31" t="s">
         <v>42</v>
@@ -9952,12 +9956,12 @@
       </c>
       <c r="Y56" s="32"/>
     </row>
-    <row r="60" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1">
       <c r="C61" s="7">
         <v>2000</v>
       </c>
@@ -10025,7 +10029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" s="55" customFormat="1" ht="15" customHeight="1">
       <c r="B62" s="7" t="s">
         <v>42</v>
       </c>
@@ -10055,10 +10059,10 @@
       </c>
       <c r="Y62" s="45"/>
     </row>
-    <row r="63" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:35" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" s="55" customFormat="1"/>
+    <row r="64" spans="1:25" s="55" customFormat="1"/>
+    <row r="65" spans="1:35" s="55" customFormat="1"/>
+    <row r="66" spans="1:35">
       <c r="A66" s="71" t="s">
         <v>134</v>
       </c>
@@ -10097,7 +10101,7 @@
       <c r="AH66" s="70"/>
       <c r="AI66" s="70"/>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:35">
       <c r="A67" s="70"/>
       <c r="B67" s="70"/>
       <c r="C67" s="72">
@@ -10168,7 +10172,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:35">
       <c r="A68" s="70"/>
       <c r="B68" s="72" t="s">
         <v>42</v>
@@ -10220,14 +10224,14 @@
       <selection activeCell="Y3" sqref="Y3:Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="A2" s="30"/>
       <c r="C2" s="7">
         <v>2000</v>
@@ -10296,7 +10300,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="A3" s="30"/>
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -10330,7 +10334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="A4" s="30"/>
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -10364,7 +10368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10397,7 +10401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -10429,7 +10433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" s="30"/>
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
@@ -10463,7 +10467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="A8" s="30"/>
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
@@ -10497,15 +10501,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="A9" s="30"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -10573,7 +10577,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10606,7 +10610,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10639,7 +10643,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10672,7 +10676,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -10704,7 +10708,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10737,7 +10741,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10770,12 +10774,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -10843,7 +10847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10876,7 +10880,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10909,7 +10913,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10942,7 +10946,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -10974,7 +10978,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11007,7 +11011,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11040,7 +11044,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25">
       <c r="A34" s="29" t="s">
         <v>62</v>
       </c>
@@ -11069,7 +11073,7 @@
       <c r="X34" s="30"/>
       <c r="Y34" s="30"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="31">
@@ -11140,7 +11144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="A36" s="30"/>
       <c r="B36" s="31" t="s">
         <v>42</v>
@@ -11173,7 +11177,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25">
       <c r="A40" s="29" t="s">
         <v>63</v>
       </c>
@@ -11202,7 +11206,7 @@
       <c r="X40" s="30"/>
       <c r="Y40" s="30"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="31">
@@ -11273,7 +11277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
         <v>42</v>
@@ -11306,7 +11310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25">
       <c r="A46" s="29" t="s">
         <v>64</v>
       </c>
@@ -11335,7 +11339,7 @@
       <c r="X46" s="30"/>
       <c r="Y46" s="30"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25">
       <c r="A47" s="30"/>
       <c r="B47" s="30"/>
       <c r="C47" s="31">
@@ -11406,7 +11410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25">
       <c r="A48" s="30"/>
       <c r="B48" s="31" t="s">
         <v>42</v>
@@ -11452,20 +11456,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y81"/>
+  <dimension ref="A1:Y79"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -11533,7 +11537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11566,7 +11570,7 @@
       </c>
       <c r="Y3" s="8"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11599,7 +11603,7 @@
       </c>
       <c r="Y4" s="8"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11632,7 +11636,7 @@
       </c>
       <c r="Y5" s="8"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -11664,7 +11668,7 @@
       </c>
       <c r="Y6" s="8"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11697,7 +11701,7 @@
       </c>
       <c r="Y7" s="8"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11730,12 +11734,12 @@
       </c>
       <c r="Y8" s="8"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -11803,7 +11807,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11836,7 +11840,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11869,7 +11873,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11902,7 +11906,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -11934,7 +11938,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11967,7 +11971,7 @@
       </c>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12000,12 +12004,12 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -12073,7 +12077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12106,7 +12110,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12139,7 +12143,7 @@
       </c>
       <c r="Y26" s="8"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12172,7 +12176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -12204,7 +12208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12237,7 +12241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12270,12 +12274,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25">
       <c r="C35" s="7">
         <v>2000</v>
       </c>
@@ -12343,7 +12347,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="B36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12376,7 +12380,7 @@
       </c>
       <c r="Y36" s="22"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12409,7 +12413,7 @@
       </c>
       <c r="Y37" s="22"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12442,7 +12446,7 @@
       </c>
       <c r="Y38" s="22"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25">
       <c r="B39" s="7" t="s">
         <v>20</v>
       </c>
@@ -12474,7 +12478,7 @@
       </c>
       <c r="Y39" s="22"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25">
       <c r="B40" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12507,7 +12511,7 @@
       </c>
       <c r="Y40" s="22"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25">
       <c r="B41" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12540,12 +12544,12 @@
       </c>
       <c r="Y41" s="22"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25">
       <c r="A45" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25">
       <c r="C46" s="7">
         <v>2000</v>
       </c>
@@ -12613,7 +12617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25">
       <c r="B47" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12646,7 +12650,7 @@
       </c>
       <c r="Y47" s="22"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25">
       <c r="B48" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12683,7 +12687,7 @@
       </c>
       <c r="Y48" s="22"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25">
       <c r="B49" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12716,7 +12720,7 @@
       </c>
       <c r="Y49" s="22"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25">
       <c r="B50" s="7" t="s">
         <v>20</v>
       </c>
@@ -12748,7 +12752,7 @@
       </c>
       <c r="Y50" s="22"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="B51" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12785,7 +12789,7 @@
       </c>
       <c r="Y51" s="22"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25">
       <c r="B52" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12822,12 +12826,12 @@
       </c>
       <c r="Y52" s="22"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25">
       <c r="A56" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25">
       <c r="C57" s="7">
         <v>2000</v>
       </c>
@@ -12895,7 +12899,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25">
       <c r="B58" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12930,7 +12934,7 @@
       </c>
       <c r="Y58" s="22"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25">
       <c r="B59" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12965,7 +12969,7 @@
       </c>
       <c r="Y59" s="22"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25">
       <c r="B60" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12998,7 +13002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25">
       <c r="B61" s="7" t="s">
         <v>20</v>
       </c>
@@ -13030,7 +13034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25">
       <c r="B62" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -13063,7 +13067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25">
       <c r="B63" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -13096,12 +13100,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25">
       <c r="C68" s="7">
         <v>2000</v>
       </c>
@@ -13169,7 +13173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25">
       <c r="B69" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13202,10 +13206,9 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B70" s="7" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
+    <row r="70" spans="1:25">
+      <c r="B70" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
@@ -13235,9 +13238,10 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B71" s="7" t="s">
-        <v>20</v>
+    <row r="71" spans="1:25">
+      <c r="B71" s="7" t="str">
+        <f>Populations!$C$7</f>
+        <v>M 15+</v>
       </c>
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
@@ -13267,116 +13271,116 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B72" s="7" t="str">
-        <f>Populations!$C$7</f>
-        <v>M 15+</v>
-      </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-      <c r="G72" s="22"/>
-      <c r="H72" s="22"/>
-      <c r="I72" s="22"/>
-      <c r="J72" s="22"/>
-      <c r="K72" s="22"/>
-      <c r="L72" s="22"/>
-      <c r="M72" s="22"/>
-      <c r="N72" s="22"/>
-      <c r="O72" s="22"/>
-      <c r="P72" s="22"/>
-      <c r="Q72" s="22"/>
-      <c r="R72" s="22"/>
-      <c r="S72" s="22"/>
-      <c r="T72" s="22"/>
-      <c r="U72" s="22"/>
-      <c r="V72" s="22"/>
-      <c r="W72" s="22"/>
-      <c r="X72" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y72" s="22">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A76" s="24" t="s">
+    <row r="75" spans="1:25">
+      <c r="A75" s="24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C77" s="7">
+    <row r="76" spans="1:25">
+      <c r="C76" s="7">
         <v>2000</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D76" s="7">
         <v>2001</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E76" s="7">
         <v>2002</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F76" s="7">
         <v>2003</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G76" s="7">
         <v>2004</v>
       </c>
-      <c r="H77" s="7">
+      <c r="H76" s="7">
         <v>2005</v>
       </c>
-      <c r="I77" s="7">
+      <c r="I76" s="7">
         <v>2006</v>
       </c>
-      <c r="J77" s="7">
+      <c r="J76" s="7">
         <v>2007</v>
       </c>
-      <c r="K77" s="7">
+      <c r="K76" s="7">
         <v>2008</v>
       </c>
-      <c r="L77" s="7">
+      <c r="L76" s="7">
         <v>2009</v>
       </c>
-      <c r="M77" s="7">
+      <c r="M76" s="7">
         <v>2010</v>
       </c>
-      <c r="N77" s="7">
+      <c r="N76" s="7">
         <v>2011</v>
       </c>
-      <c r="O77" s="7">
+      <c r="O76" s="7">
         <v>2012</v>
       </c>
-      <c r="P77" s="7">
+      <c r="P76" s="7">
         <v>2013</v>
       </c>
-      <c r="Q77" s="7">
+      <c r="Q76" s="7">
         <v>2014</v>
       </c>
-      <c r="R77" s="7">
+      <c r="R76" s="7">
         <v>2015</v>
       </c>
-      <c r="S77" s="7">
+      <c r="S76" s="7">
         <v>2016</v>
       </c>
-      <c r="T77" s="7">
+      <c r="T76" s="7">
         <v>2017</v>
       </c>
-      <c r="U77" s="7">
+      <c r="U76" s="7">
         <v>2018</v>
       </c>
-      <c r="V77" s="7">
+      <c r="V76" s="7">
         <v>2019</v>
       </c>
-      <c r="W77" s="7">
+      <c r="W76" s="7">
         <v>2020</v>
       </c>
-      <c r="Y77" s="7" t="s">
+      <c r="Y76" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B78" s="7" t="str">
+    <row r="77" spans="1:25">
+      <c r="B77" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
+      </c>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
+      <c r="K77" s="22"/>
+      <c r="L77" s="22"/>
+      <c r="M77" s="22"/>
+      <c r="N77" s="22"/>
+      <c r="O77" s="22"/>
+      <c r="P77" s="22"/>
+      <c r="Q77" s="22"/>
+      <c r="R77" s="22"/>
+      <c r="S77" s="22"/>
+      <c r="T77" s="22"/>
+      <c r="U77" s="22"/>
+      <c r="V77" s="22"/>
+      <c r="W77" s="22"/>
+      <c r="X77" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y77" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25">
+      <c r="B78" s="7" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="22"/>
@@ -13406,10 +13410,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25">
       <c r="B79" s="7" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
+        <f>Populations!$C$7</f>
+        <v>M 15+</v>
       </c>
       <c r="C79" s="22"/>
       <c r="D79" s="22"/>
@@ -13439,71 +13443,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B80" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22"/>
-      <c r="J80" s="22"/>
-      <c r="K80" s="22"/>
-      <c r="L80" s="22"/>
-      <c r="M80" s="22"/>
-      <c r="N80" s="22"/>
-      <c r="O80" s="22"/>
-      <c r="P80" s="22"/>
-      <c r="Q80" s="22"/>
-      <c r="R80" s="22"/>
-      <c r="S80" s="22"/>
-      <c r="T80" s="22"/>
-      <c r="U80" s="22"/>
-      <c r="V80" s="22"/>
-      <c r="W80" s="22"/>
-      <c r="X80" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y80" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B81" s="7" t="str">
-        <f>Populations!$C$7</f>
-        <v>M 15+</v>
-      </c>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="22"/>
-      <c r="G81" s="22"/>
-      <c r="H81" s="22"/>
-      <c r="I81" s="22"/>
-      <c r="J81" s="22"/>
-      <c r="K81" s="22"/>
-      <c r="L81" s="22"/>
-      <c r="M81" s="22"/>
-      <c r="N81" s="22"/>
-      <c r="O81" s="22"/>
-      <c r="P81" s="22"/>
-      <c r="Q81" s="22"/>
-      <c r="R81" s="22"/>
-      <c r="S81" s="22"/>
-      <c r="T81" s="22"/>
-      <c r="U81" s="22"/>
-      <c r="V81" s="22"/>
-      <c r="W81" s="22"/>
-      <c r="X81" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y81" s="22">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
recalibrated concentrated, and removed some dubious transitions
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28575" windowHeight="15975" tabRatio="805" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1865,31 +1865,31 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1">
+    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="406">
+    <row r="5" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="140">
+    <row r="7" spans="1:1" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1916,14 +1916,14 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2024,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="Y6" s="8"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2155,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2188,12 +2188,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2360,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="Y17" s="22"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2458,12 +2458,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>42</v>
       </c>
@@ -2578,18 +2578,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2615,7 +2615,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2627,7 +2627,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2643,7 +2643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2657,7 +2657,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2671,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2687,7 +2687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2699,12 +2699,12 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2730,7 +2730,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2742,7 +2742,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2758,7 +2758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2772,7 +2772,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2786,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2802,7 +2802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2814,12 +2814,12 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2845,7 +2845,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2857,7 +2857,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2871,7 +2871,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2883,7 +2883,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2895,7 +2895,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2907,7 +2907,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2919,12 +2919,12 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2950,7 +2950,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2962,7 +2962,7 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2974,7 +2974,7 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2986,7 +2986,7 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3000,7 +3000,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3012,7 +3012,7 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3024,12 +3024,12 @@
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3055,7 +3055,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3067,7 +3067,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3079,12 +3079,12 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3110,7 +3110,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3122,7 +3122,7 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3134,7 +3134,7 @@
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3146,7 +3146,7 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3158,7 +3158,7 @@
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3170,7 +3170,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3182,12 +3182,12 @@
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3213,7 +3213,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="65" spans="2:8">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3224,10 +3224,10 @@
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3236,12 +3236,10 @@
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="8">
-        <v>15</v>
-      </c>
+      <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="2:8">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3250,12 +3248,10 @@
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
-      <c r="G67" s="8">
-        <v>15</v>
-      </c>
+      <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="2:8">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3267,7 +3263,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="2:8">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3279,7 +3275,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
     </row>
-    <row r="70" spans="2:8">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3310,16 +3306,16 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="51"/>
-    <col min="2" max="2" width="37.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="8.83203125" style="51"/>
-    <col min="10" max="10" width="18.83203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="51"/>
+    <col min="1" max="1" width="8.85546875" style="51"/>
+    <col min="2" max="2" width="37.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.85546875" style="51"/>
+    <col min="10" max="10" width="18.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
         <v>79</v>
       </c>
@@ -3328,7 +3324,7 @@
       <c r="D1" s="64"/>
       <c r="E1" s="64"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="64"/>
       <c r="B2" s="64"/>
       <c r="C2" s="65" t="s">
@@ -3341,7 +3337,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="64"/>
       <c r="B3" s="67" t="s">
         <v>80</v>
@@ -3356,7 +3352,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="64"/>
       <c r="B4" s="67" t="s">
         <v>81</v>
@@ -3371,7 +3367,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="64"/>
       <c r="B5" s="67" t="s">
         <v>82</v>
@@ -3386,7 +3382,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="64"/>
       <c r="B6" s="67" t="s">
         <v>83</v>
@@ -3401,7 +3397,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="67" t="s">
         <v>84</v>
@@ -3416,7 +3412,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="64"/>
       <c r="B8" s="67" t="s">
         <v>85</v>
@@ -3431,7 +3427,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="64"/>
       <c r="B9" s="67" t="s">
         <v>86</v>
@@ -3446,33 +3442,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="71"/>
       <c r="B10" s="72"/>
       <c r="C10" s="71"/>
       <c r="D10" s="71"/>
       <c r="E10" s="71"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="71"/>
       <c r="B11" s="72"/>
       <c r="C11" s="71"/>
       <c r="D11" s="71"/>
       <c r="E11" s="71"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
       <c r="B12" s="72"/>
       <c r="C12" s="71"/>
       <c r="D12" s="71"/>
       <c r="E12" s="71"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
@@ -3483,7 +3479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>88</v>
       </c>
@@ -3497,7 +3493,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>89</v>
       </c>
@@ -3511,7 +3507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>90</v>
       </c>
@@ -3525,7 +3521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>91</v>
       </c>
@@ -3539,7 +3535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>92</v>
       </c>
@@ -3553,7 +3549,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>93</v>
       </c>
@@ -3567,33 +3563,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="71"/>
       <c r="B21" s="72"/>
       <c r="C21" s="71"/>
       <c r="D21" s="71"/>
       <c r="E21" s="71"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="71"/>
       <c r="B22" s="72"/>
       <c r="C22" s="71"/>
       <c r="D22" s="71"/>
       <c r="E22" s="71"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="71"/>
       <c r="B23" s="72"/>
       <c r="C23" s="71"/>
       <c r="D23" s="71"/>
       <c r="E23" s="71"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7" t="s">
         <v>30</v>
       </c>
@@ -3604,7 +3600,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>94</v>
       </c>
@@ -3618,7 +3614,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>90</v>
       </c>
@@ -3633,7 +3629,7 @@
       </c>
       <c r="G27" s="74"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>95</v>
       </c>
@@ -3647,7 +3643,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>96</v>
       </c>
@@ -3661,7 +3657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>97</v>
       </c>
@@ -3675,33 +3671,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="71"/>
       <c r="B31" s="72"/>
       <c r="C31" s="71"/>
       <c r="D31" s="71"/>
       <c r="E31" s="71"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="71"/>
       <c r="B32" s="72"/>
       <c r="C32" s="71"/>
       <c r="D32" s="71"/>
       <c r="E32" s="71"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="71"/>
       <c r="B33" s="72"/>
       <c r="C33" s="71"/>
       <c r="D33" s="71"/>
       <c r="E33" s="71"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" s="7" t="s">
         <v>30</v>
       </c>
@@ -3712,7 +3708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>98</v>
       </c>
@@ -3726,7 +3722,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>99</v>
       </c>
@@ -3740,7 +3736,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>100</v>
       </c>
@@ -3754,7 +3750,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>101</v>
       </c>
@@ -3768,7 +3764,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="40" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="58"/>
       <c r="B40" s="3" t="s">
         <v>128</v>
@@ -3783,28 +3779,28 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="71"/>
       <c r="B41" s="72"/>
       <c r="C41" s="71"/>
       <c r="D41" s="71"/>
       <c r="E41" s="71"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="71"/>
       <c r="B42" s="72"/>
       <c r="C42" s="71"/>
       <c r="D42" s="71"/>
       <c r="E42" s="71"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="71"/>
       <c r="B43" s="72"/>
       <c r="C43" s="71"/>
       <c r="D43" s="71"/>
       <c r="E43" s="71"/>
     </row>
-    <row r="44" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="44" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="53" t="s">
         <v>130</v>
       </c>
@@ -3813,7 +3809,7 @@
       <c r="D44" s="58"/>
       <c r="E44" s="58"/>
     </row>
-    <row r="45" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="45" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="58"/>
       <c r="B45" s="58"/>
       <c r="C45" s="54" t="s">
@@ -3826,7 +3822,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="46" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="58"/>
       <c r="B46" s="3" t="s">
         <v>90</v>
@@ -3841,7 +3837,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="47" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="58"/>
       <c r="B47" s="3" t="s">
         <v>98</v>
@@ -3856,7 +3852,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="48" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="58"/>
       <c r="B48" s="3" t="s">
         <v>95</v>
@@ -3871,7 +3867,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="49" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="58"/>
       <c r="B49" s="3" t="s">
         <v>99</v>
@@ -3886,7 +3882,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="68" customFormat="1">
+    <row r="50" spans="1:6" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="58"/>
       <c r="B50" s="3" t="s">
         <v>96</v>
@@ -3901,7 +3897,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="51" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="58"/>
       <c r="B51" s="3" t="s">
         <v>100</v>
@@ -3916,7 +3912,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="52" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="58"/>
       <c r="B52" s="3" t="s">
         <v>97</v>
@@ -3931,7 +3927,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="53" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="58"/>
       <c r="B53" s="3" t="s">
         <v>101</v>
@@ -3946,7 +3942,7 @@
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="54" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="58"/>
       <c r="B54" s="3" t="s">
         <v>131</v>
@@ -3961,33 +3957,33 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="55" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="69"/>
       <c r="B55" s="69"/>
       <c r="C55" s="69"/>
       <c r="D55" s="69"/>
       <c r="E55" s="69"/>
     </row>
-    <row r="56" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="56" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="69"/>
       <c r="B56" s="69"/>
       <c r="C56" s="69"/>
       <c r="D56" s="69"/>
       <c r="E56" s="69"/>
     </row>
-    <row r="57" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
+    <row r="57" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="69"/>
       <c r="B57" s="69"/>
       <c r="C57" s="69"/>
       <c r="D57" s="69"/>
       <c r="E57" s="69"/>
     </row>
-    <row r="58" spans="1:6" ht="13.5" customHeight="1">
+    <row r="58" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="13.5" customHeight="1">
+    <row r="59" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="7" t="s">
         <v>30</v>
       </c>
@@ -3998,7 +3994,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="13.5" customHeight="1">
+    <row r="60" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>88</v>
       </c>
@@ -4012,7 +4008,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="13.5" customHeight="1">
+    <row r="61" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>89</v>
       </c>
@@ -4026,7 +4022,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="13.5" customHeight="1">
+    <row r="62" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>103</v>
       </c>
@@ -4040,7 +4036,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="13.5" customHeight="1">
+    <row r="63" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>91</v>
       </c>
@@ -4054,7 +4050,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1">
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>92</v>
       </c>
@@ -4069,7 +4065,7 @@
       </c>
       <c r="F64" s="71"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>93</v>
       </c>
@@ -4084,7 +4080,7 @@
       </c>
       <c r="F65" s="71"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>126</v>
       </c>
@@ -4099,7 +4095,7 @@
       </c>
       <c r="F66" s="71"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>127</v>
       </c>
@@ -4114,7 +4110,7 @@
       </c>
       <c r="F67" s="71"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>104</v>
       </c>
@@ -4129,7 +4125,7 @@
       </c>
       <c r="F68" s="71"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="71"/>
       <c r="B69" s="72"/>
       <c r="C69" s="71"/>
@@ -4137,7 +4133,7 @@
       <c r="E69" s="71"/>
       <c r="F69" s="71"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="71"/>
       <c r="B70" s="72"/>
       <c r="C70" s="71"/>
@@ -4148,7 +4144,7 @@
       <c r="H70" s="71"/>
       <c r="I70" s="71"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="71"/>
       <c r="B71" s="72"/>
       <c r="C71" s="71"/>
@@ -4159,7 +4155,7 @@
       <c r="H71" s="71"/>
       <c r="I71" s="71"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>105</v>
       </c>
@@ -4168,7 +4164,7 @@
       <c r="H72" s="71"/>
       <c r="I72" s="71"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C73" s="7" t="s">
         <v>30</v>
       </c>
@@ -4183,7 +4179,7 @@
       <c r="H73" s="71"/>
       <c r="I73" s="71"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>106</v>
       </c>
@@ -4201,7 +4197,7 @@
       <c r="H74" s="76"/>
       <c r="I74" s="76"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>107</v>
       </c>
@@ -4219,7 +4215,7 @@
       <c r="H75" s="76"/>
       <c r="I75" s="76"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>108</v>
       </c>
@@ -4234,7 +4230,7 @@
       </c>
       <c r="F76" s="71"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>109</v>
       </c>
@@ -4252,7 +4248,7 @@
       <c r="H77" s="76"/>
       <c r="I77" s="76"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>110</v>
       </c>
@@ -4270,7 +4266,7 @@
       <c r="H78" s="76"/>
       <c r="I78" s="76"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
         <v>111</v>
       </c>
@@ -4288,7 +4284,7 @@
       <c r="H79" s="76"/>
       <c r="I79" s="76"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
         <v>112</v>
       </c>
@@ -4306,7 +4302,7 @@
       <c r="H80" s="76"/>
       <c r="I80" s="76"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>113</v>
       </c>
@@ -4324,7 +4320,7 @@
       <c r="H81" s="76"/>
       <c r="I81" s="76"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>114</v>
       </c>
@@ -4342,7 +4338,7 @@
       <c r="H82" s="71"/>
       <c r="I82" s="71"/>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="71"/>
       <c r="B83" s="72"/>
       <c r="C83" s="71"/>
@@ -4353,7 +4349,7 @@
       <c r="H83" s="71"/>
       <c r="I83" s="71"/>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="77"/>
       <c r="B84" s="78"/>
       <c r="C84" s="79"/>
@@ -4364,7 +4360,7 @@
       <c r="H84" s="79"/>
       <c r="I84" s="71"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="79"/>
       <c r="B85" s="78"/>
       <c r="C85" s="80"/>
@@ -4375,7 +4371,7 @@
       <c r="H85" s="79"/>
       <c r="I85" s="71"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="55" t="s">
         <v>115</v>
       </c>
@@ -4387,7 +4383,7 @@
       <c r="G86" s="52"/>
       <c r="H86" s="52"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="52"/>
       <c r="B87" s="52"/>
       <c r="C87" s="56" t="s">
@@ -4403,7 +4399,7 @@
       <c r="G87" s="52"/>
       <c r="H87" s="52"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="52"/>
       <c r="B88" s="57" t="s">
         <v>116</v>
@@ -4421,7 +4417,7 @@
       <c r="G88" s="52"/>
       <c r="H88" s="52"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="52"/>
       <c r="B89" s="57" t="s">
         <v>117</v>
@@ -4439,7 +4435,7 @@
       <c r="G89" s="52"/>
       <c r="H89" s="52"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="52"/>
       <c r="B90" s="57" t="s">
         <v>118</v>
@@ -4457,7 +4453,7 @@
       <c r="G90" s="52"/>
       <c r="H90" s="52"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="52"/>
       <c r="B91" s="57" t="s">
         <v>119</v>
@@ -4475,7 +4471,7 @@
       <c r="G91" s="52"/>
       <c r="H91" s="52"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="52"/>
       <c r="B92" s="57" t="s">
         <v>120</v>
@@ -4493,7 +4489,7 @@
       <c r="G92" s="52"/>
       <c r="H92" s="52"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="52"/>
       <c r="B93" s="57" t="s">
         <v>121</v>
@@ -4511,7 +4507,7 @@
       <c r="G93" s="52"/>
       <c r="H93" s="52"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="52"/>
       <c r="B94" s="57" t="s">
         <v>122</v>
@@ -4529,17 +4525,17 @@
       <c r="G94" s="52"/>
       <c r="H94" s="52"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F95" s="52"/>
       <c r="G95" s="52"/>
       <c r="H95" s="52"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F96" s="52"/>
       <c r="G96" s="52"/>
       <c r="H96" s="52"/>
     </row>
-    <row r="97" spans="6:8">
+    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F97" s="52"/>
       <c r="G97" s="52"/>
       <c r="H97" s="52"/>
@@ -4563,14 +4559,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -4596,7 +4592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -4625,7 +4621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -4654,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -4683,7 +4679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -4712,7 +4708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -4741,7 +4737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -4789,15 +4785,15 @@
       <selection activeCell="Z2" sqref="Z2:Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -4865,7 +4861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4899,7 +4895,7 @@
       </c>
       <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4955,7 +4951,7 @@
       </c>
       <c r="Z4" s="11"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4989,7 +4985,7 @@
       </c>
       <c r="Z5" s="11"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5023,7 +5019,7 @@
       </c>
       <c r="Z7" s="11"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5079,7 +5075,7 @@
       </c>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5113,7 +5109,7 @@
       </c>
       <c r="Z9" s="11"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5147,7 +5143,7 @@
       </c>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5203,7 +5199,7 @@
       </c>
       <c r="Z12" s="11"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5237,7 +5233,7 @@
       </c>
       <c r="Z13" s="11"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -5250,7 +5246,7 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
@@ -5283,7 +5279,7 @@
       </c>
       <c r="Z15" s="11"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
@@ -5338,7 +5334,7 @@
       </c>
       <c r="Z16" s="11"/>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -5371,7 +5367,7 @@
       </c>
       <c r="Z17" s="11"/>
     </row>
-    <row r="18" spans="2:26">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -5384,7 +5380,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5418,7 +5414,7 @@
       </c>
       <c r="Z19" s="11"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5474,7 +5470,7 @@
       </c>
       <c r="Z20" s="11"/>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5508,7 +5504,7 @@
       </c>
       <c r="Z21" s="11"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5542,7 +5538,7 @@
       </c>
       <c r="Z23" s="11"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5598,7 +5594,7 @@
       </c>
       <c r="Z24" s="11"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5632,7 +5628,7 @@
       </c>
       <c r="Z25" s="11"/>
     </row>
-    <row r="27" spans="2:26">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
         <v>32</v>
       </c>
@@ -5641,7 +5637,7 @@
         <v>21773583.295806497</v>
       </c>
     </row>
-    <row r="28" spans="2:26">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
         <v>33</v>
       </c>
@@ -5657,7 +5653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:26">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="N29">
         <f>3529/'Population size'!N28*100</f>
         <v>7.0468319579830743</v>
@@ -5685,14 +5681,14 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="7">
         <v>2000</v>
       </c>
@@ -5760,7 +5756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5800,7 +5796,7 @@
       </c>
       <c r="Z3" s="19"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5840,7 +5836,7 @@
       </c>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5880,7 +5876,7 @@
       </c>
       <c r="Z5" s="19"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5914,7 +5910,7 @@
       </c>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5950,7 +5946,7 @@
       </c>
       <c r="Z8" s="19"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5984,7 +5980,7 @@
       </c>
       <c r="Z9" s="19"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6020,7 +6016,7 @@
       </c>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6062,7 +6058,7 @@
       </c>
       <c r="Z12" s="19"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6098,7 +6094,7 @@
       </c>
       <c r="Z13" s="19"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
@@ -6133,7 +6129,7 @@
       </c>
       <c r="Z15" s="19"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
@@ -6174,7 +6170,7 @@
       </c>
       <c r="Z16" s="19"/>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -6209,7 +6205,7 @@
       </c>
       <c r="Z17" s="19"/>
     </row>
-    <row r="19" spans="2:26">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6243,7 +6239,7 @@
       </c>
       <c r="Z19" s="19"/>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6291,7 +6287,7 @@
       </c>
       <c r="Z20" s="19"/>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6325,7 +6321,7 @@
       </c>
       <c r="Z21" s="19"/>
     </row>
-    <row r="23" spans="2:26">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6359,7 +6355,7 @@
       </c>
       <c r="Z23" s="19"/>
     </row>
-    <row r="24" spans="2:26">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6407,7 +6403,7 @@
       </c>
       <c r="Z24" s="19"/>
     </row>
-    <row r="25" spans="2:26">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6461,14 +6457,14 @@
       <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -6536,7 +6532,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6569,7 +6565,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6602,7 +6598,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6635,7 +6631,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -6667,7 +6663,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6700,7 +6696,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6733,12 +6729,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -6806,7 +6802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6839,7 +6835,7 @@
       </c>
       <c r="Y14" s="19"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6872,7 +6868,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6905,7 +6901,7 @@
       </c>
       <c r="Y16" s="19"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -6937,7 +6933,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6970,7 +6966,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7003,12 +6999,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -7076,7 +7072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7109,7 +7105,7 @@
       </c>
       <c r="Y25" s="19"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7142,7 +7138,7 @@
       </c>
       <c r="Y26" s="19"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7175,7 +7171,7 @@
       </c>
       <c r="Y27" s="19"/>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -7207,7 +7203,7 @@
       </c>
       <c r="Y28" s="19"/>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7240,7 +7236,7 @@
       </c>
       <c r="Y29" s="19"/>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7292,14 +7288,14 @@
       <selection activeCell="A55" sqref="A55:XFD59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -7367,7 +7363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7402,7 +7398,7 @@
       </c>
       <c r="Y3" s="22"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7439,7 +7435,7 @@
       </c>
       <c r="Y4" s="22"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7472,7 +7468,7 @@
       </c>
       <c r="Y5" s="22"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -7504,7 +7500,7 @@
       </c>
       <c r="Y6" s="22"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7537,7 +7533,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7570,12 +7566,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -7643,7 +7639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>42</v>
       </c>
@@ -7675,12 +7671,12 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" s="7">
         <v>2000</v>
       </c>
@@ -7748,7 +7744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
@@ -7796,12 +7792,12 @@
       </c>
       <c r="Y20" s="8"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C26" s="7">
         <v>2000</v>
       </c>
@@ -7869,7 +7865,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7902,7 +7898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7935,7 +7931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7968,7 +7964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>20</v>
       </c>
@@ -8000,7 +7996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -8033,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -8066,12 +8062,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C37" s="7">
         <v>2000</v>
       </c>
@@ -8139,7 +8135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>44</v>
       </c>
@@ -8173,12 +8169,12 @@
       </c>
       <c r="Y38" s="8"/>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C43" s="7">
         <v>2000</v>
       </c>
@@ -8246,7 +8242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8299,7 +8295,7 @@
       </c>
       <c r="Y44" s="27"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -8352,12 +8348,12 @@
       </c>
       <c r="Y45" s="27"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C50" s="7">
         <v>2000</v>
       </c>
@@ -8425,7 +8421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
         <v>44</v>
       </c>
@@ -8472,18 +8468,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C45" sqref="C45:G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -8551,7 +8547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>44</v>
       </c>
@@ -8595,12 +8591,12 @@
       </c>
       <c r="Y3" s="27"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C8" s="7">
         <v>2000</v>
       </c>
@@ -8668,7 +8664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>44</v>
       </c>
@@ -8702,12 +8698,12 @@
       </c>
       <c r="Y9" s="27"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C14" s="7">
         <v>2000</v>
       </c>
@@ -8775,7 +8771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
@@ -8833,12 +8829,12 @@
       </c>
       <c r="Y15" s="27"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C20" s="7">
         <v>2000</v>
       </c>
@@ -8906,7 +8902,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
@@ -8936,7 +8932,7 @@
       </c>
       <c r="Y21" s="37"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
@@ -8965,7 +8961,7 @@
       <c r="X25" s="38"/>
       <c r="Y25" s="38"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="38"/>
       <c r="B26" s="38"/>
       <c r="C26" s="39">
@@ -9036,7 +9032,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="38"/>
       <c r="B27" s="39" t="s">
         <v>44</v>
@@ -9067,13 +9063,13 @@
       </c>
       <c r="Y27" s="40"/>
     </row>
-    <row r="29" spans="1:25" s="51" customFormat="1"/>
-    <row r="31" spans="1:25">
+    <row r="29" spans="1:25" s="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C32" s="7">
         <v>2000</v>
       </c>
@@ -9141,7 +9137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>44</v>
       </c>
@@ -9199,12 +9195,12 @@
       </c>
       <c r="Y33" s="27"/>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C38" s="7">
         <v>2000</v>
       </c>
@@ -9272,7 +9268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>44</v>
       </c>
@@ -9310,7 +9306,7 @@
       </c>
       <c r="Y39" s="27"/>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="42"/>
       <c r="B40" s="42"/>
       <c r="C40" s="42"/>
@@ -9337,7 +9333,7 @@
       <c r="X40" s="42"/>
       <c r="Y40" s="42"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="42"/>
       <c r="B41" s="42"/>
       <c r="C41" s="42"/>
@@ -9364,7 +9360,7 @@
       <c r="X41" s="42"/>
       <c r="Y41" s="42"/>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="42"/>
       <c r="B42" s="42"/>
       <c r="C42" s="42"/>
@@ -9391,7 +9387,7 @@
       <c r="X42" s="42"/>
       <c r="Y42" s="42"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>56</v>
       </c>
@@ -9420,7 +9416,7 @@
       <c r="X43" s="42"/>
       <c r="Y43" s="42"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="42"/>
       <c r="B44" s="42"/>
       <c r="C44" s="7">
@@ -9491,7 +9487,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="42"/>
       <c r="B45" s="7" t="s">
         <v>42</v>
@@ -9522,7 +9518,7 @@
       </c>
       <c r="Y45" s="43"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="42"/>
       <c r="B46" s="42"/>
       <c r="C46" s="42"/>
@@ -9549,7 +9545,7 @@
       <c r="X46" s="42"/>
       <c r="Y46" s="42"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="42"/>
       <c r="B47" s="42"/>
       <c r="C47" s="42"/>
@@ -9576,7 +9572,7 @@
       <c r="X47" s="42"/>
       <c r="Y47" s="42"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="42"/>
       <c r="B48" s="42"/>
       <c r="C48" s="42"/>
@@ -9603,7 +9599,7 @@
       <c r="X48" s="42"/>
       <c r="Y48" s="42"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
         <v>57</v>
       </c>
@@ -9632,7 +9628,7 @@
       <c r="X49" s="30"/>
       <c r="Y49" s="30"/>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="30"/>
       <c r="C50" s="31">
@@ -9703,7 +9699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="30"/>
       <c r="B51" s="31" t="s">
         <v>42</v>
@@ -9734,7 +9730,7 @@
       </c>
       <c r="Y51" s="32"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="38"/>
       <c r="B52" s="38"/>
       <c r="C52" s="38"/>
@@ -9761,7 +9757,7 @@
       <c r="X52" s="38"/>
       <c r="Y52" s="38"/>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="38"/>
       <c r="B53" s="38"/>
       <c r="C53" s="38"/>
@@ -9788,7 +9784,7 @@
       <c r="X53" s="38"/>
       <c r="Y53" s="38"/>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="38"/>
       <c r="B54" s="38"/>
       <c r="C54" s="38"/>
@@ -9815,7 +9811,7 @@
       <c r="X54" s="38"/>
       <c r="Y54" s="38"/>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>58</v>
       </c>
@@ -9844,7 +9840,7 @@
       <c r="X55" s="30"/>
       <c r="Y55" s="30"/>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="31">
@@ -9915,7 +9911,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
       <c r="B57" s="31" t="s">
         <v>42</v>
@@ -9946,12 +9942,12 @@
       </c>
       <c r="Y57" s="32"/>
     </row>
-    <row r="61" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="61" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="62" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="7">
         <v>2000</v>
       </c>
@@ -10019,7 +10015,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1">
+    <row r="63" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="7" t="s">
         <v>42</v>
       </c>
@@ -10049,10 +10045,10 @@
       </c>
       <c r="Y63" s="45"/>
     </row>
-    <row r="64" spans="1:25" s="51" customFormat="1"/>
-    <row r="65" spans="1:25" s="51" customFormat="1"/>
-    <row r="66" spans="1:25" s="51" customFormat="1"/>
-    <row r="67" spans="1:25">
+    <row r="64" spans="1:25" s="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:25" s="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:25" s="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="60" t="s">
         <v>123</v>
       </c>
@@ -10081,7 +10077,7 @@
       <c r="X67" s="59"/>
       <c r="Y67" s="59"/>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="59"/>
       <c r="B68" s="59"/>
       <c r="C68" s="61">
@@ -10152,7 +10148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="59"/>
       <c r="B69" s="61" t="s">
         <v>42</v>
@@ -10204,14 +10200,14 @@
       <selection activeCell="Y3" sqref="Y3:Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="C2" s="7">
         <v>2000</v>
@@ -10280,7 +10276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
@@ -10314,7 +10310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
@@ -10348,7 +10344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10381,7 +10377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -10413,7 +10409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
@@ -10447,7 +10443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
@@ -10481,15 +10477,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -10557,7 +10553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10590,7 +10586,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10623,7 +10619,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10656,7 +10652,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -10688,7 +10684,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10721,7 +10717,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10754,7 +10750,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>60</v>
       </c>
@@ -10783,7 +10779,7 @@
       <c r="X23" s="30"/>
       <c r="Y23" s="30"/>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
       <c r="B24" s="30"/>
       <c r="C24" s="31">
@@ -10854,7 +10850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="30"/>
       <c r="B25" s="31" t="s">
         <v>42</v>
@@ -10906,14 +10902,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="7">
         <v>2000</v>
       </c>
@@ -10981,7 +10977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11014,7 +11010,7 @@
       </c>
       <c r="Y3" s="8"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11047,7 +11043,7 @@
       </c>
       <c r="Y4" s="8"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11080,7 +11076,7 @@
       </c>
       <c r="Y5" s="8"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
@@ -11112,7 +11108,7 @@
       </c>
       <c r="Y6" s="8"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11145,7 +11141,7 @@
       </c>
       <c r="Y7" s="8"/>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11178,12 +11174,12 @@
       </c>
       <c r="Y8" s="8"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>2000</v>
       </c>
@@ -11251,7 +11247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11284,7 +11280,7 @@
       </c>
       <c r="Y14" s="8"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11317,7 +11313,7 @@
       </c>
       <c r="Y15" s="8"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11350,7 +11346,7 @@
       </c>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
@@ -11382,7 +11378,7 @@
       </c>
       <c r="Y17" s="8"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11415,7 +11411,7 @@
       </c>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11448,12 +11444,12 @@
       </c>
       <c r="Y19" s="8"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="7">
         <v>2000</v>
       </c>
@@ -11521,7 +11517,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11554,7 +11550,7 @@
       </c>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11587,7 +11583,7 @@
       </c>
       <c r="Y26" s="8"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11620,7 +11616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>20</v>
       </c>
@@ -11652,7 +11648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11685,7 +11681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11718,12 +11714,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C35" s="7">
         <v>2000</v>
       </c>
@@ -11791,7 +11787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11824,7 +11820,7 @@
       </c>
       <c r="Y36" s="22"/>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11857,7 +11853,7 @@
       </c>
       <c r="Y37" s="22"/>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11890,7 +11886,7 @@
       </c>
       <c r="Y38" s="22"/>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>20</v>
       </c>
@@ -11922,7 +11918,7 @@
       </c>
       <c r="Y39" s="22"/>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11955,7 +11951,7 @@
       </c>
       <c r="Y40" s="22"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11988,12 +11984,12 @@
       </c>
       <c r="Y41" s="22"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C46" s="7">
         <v>2000</v>
       </c>
@@ -12061,7 +12057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12094,7 +12090,7 @@
       </c>
       <c r="Y47" s="22"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12131,7 +12127,7 @@
       </c>
       <c r="Y48" s="22"/>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12164,7 +12160,7 @@
       </c>
       <c r="Y49" s="22"/>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
         <v>20</v>
       </c>
@@ -12196,7 +12192,7 @@
       </c>
       <c r="Y50" s="22"/>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12233,7 +12229,7 @@
       </c>
       <c r="Y51" s="22"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12270,12 +12266,12 @@
       </c>
       <c r="Y52" s="22"/>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C57" s="7">
         <v>2000</v>
       </c>
@@ -12343,7 +12339,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12378,7 +12374,7 @@
       </c>
       <c r="Y58" s="22"/>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12413,7 +12409,7 @@
       </c>
       <c r="Y59" s="22"/>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12446,7 +12442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B61" s="7" t="s">
         <v>20</v>
       </c>
@@ -12478,7 +12474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12511,7 +12507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="7" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12544,12 +12540,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C68" s="7">
         <v>2000</v>
       </c>
@@ -12617,7 +12613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12650,7 +12646,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12683,7 +12679,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B71" s="7" t="s">
         <v>20</v>
       </c>
@@ -12715,7 +12711,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12748,12 +12744,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C77" s="7">
         <v>2000</v>
       </c>
@@ -12821,7 +12817,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12854,7 +12850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12887,7 +12883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
         <v>20</v>
       </c>
@@ -12919,7 +12915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:25">
+    <row r="81" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B81" s="7" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>

</xml_diff>

<commit_message>
changed some numbers around
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28575" windowHeight="15975" tabRatio="805" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28575" windowHeight="15975" tabRatio="805" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -2578,7 +2578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
@@ -7284,8 +7284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7780,8 +7780,12 @@
       <c r="P20" s="8">
         <v>33080</v>
       </c>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
+      <c r="Q20" s="8">
+        <v>48100</v>
+      </c>
+      <c r="R20" s="8">
+        <v>61430</v>
+      </c>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
@@ -10196,8 +10200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10307,7 +10311,7 @@
         <v>29</v>
       </c>
       <c r="Y3" s="81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -10341,7 +10345,7 @@
         <v>29</v>
       </c>
       <c r="Y4" s="81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -10374,7 +10378,7 @@
         <v>29</v>
       </c>
       <c r="Y5" s="81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -10406,7 +10410,7 @@
         <v>29</v>
       </c>
       <c r="Y6" s="81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -10440,7 +10444,7 @@
         <v>29</v>
       </c>
       <c r="Y7" s="81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -10474,7 +10478,7 @@
         <v>29</v>
       </c>
       <c r="Y8" s="81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -10583,7 +10587,7 @@
         <v>29</v>
       </c>
       <c r="Y14" s="45">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -10616,7 +10620,7 @@
         <v>29</v>
       </c>
       <c r="Y15" s="45">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -10649,7 +10653,7 @@
         <v>29</v>
       </c>
       <c r="Y16" s="45">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -10681,7 +10685,7 @@
         <v>29</v>
       </c>
       <c r="Y17" s="45">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -10714,7 +10718,7 @@
         <v>29</v>
       </c>
       <c r="Y18" s="45">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -10747,7 +10751,7 @@
         <v>29</v>
       </c>
       <c r="Y19" s="45">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
made concentrated treatment a little more reasonable
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28575" windowHeight="15975" tabRatio="805" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28575" windowHeight="15975" tabRatio="805" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -7284,8 +7284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7783,9 +7783,7 @@
       <c r="Q20" s="8">
         <v>48100</v>
       </c>
-      <c r="R20" s="8">
-        <v>61430</v>
-      </c>
+      <c r="R20" s="8"/>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
@@ -10200,8 +10198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove proppars from spreadsheet
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="128">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -315,15 +315,6 @@
     <t>Number of people initiating ART each year</t>
   </si>
   <si>
-    <t>PLHIV aware of their status (%)</t>
-  </si>
-  <si>
-    <t>Diagnosed PLHIV in care (%)</t>
-  </si>
-  <si>
-    <t>PLHIV in care on treatment (%)</t>
-  </si>
-  <si>
     <t>Percentage of people in care who are lost to follow-up per year (%/year)</t>
   </si>
   <si>
@@ -516,9 +507,6 @@
     <t>Treated HIV</t>
   </si>
   <si>
-    <t>People on ART with viral suppression (%)</t>
-  </si>
-  <si>
     <t>Average time taken to be linked to care (years)</t>
   </si>
   <si>
@@ -541,9 +529,6 @@
   </si>
   <si>
     <t>Treatment failure rate</t>
-  </si>
-  <si>
-    <t>Pregnant women and mothers on PMTCT (%)</t>
   </si>
 </sst>
 </file>
@@ -741,7 +726,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -753,19 +738,6 @@
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
@@ -977,7 +949,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1054,9 +1026,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1079,13 +1048,6 @@
     <xf numFmtId="4" fontId="0" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1120,17 +1082,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="120"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="120" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1868,15 +1819,15 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="82"/>
+      <c r="A2" s="73"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="82"/>
+      <c r="A3" s="73"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
@@ -1920,7 +1871,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -2190,7 +2141,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2460,7 +2411,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2578,15 +2529,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2701,7 +2652,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2816,7 +2767,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2921,7 +2872,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -3026,7 +2977,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3081,7 +3032,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3184,7 +3135,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3224,7 +3175,7 @@
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
       <c r="H65" s="8">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="2:8">
@@ -3236,9 +3187,7 @@
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="8">
-        <v>15</v>
-      </c>
+      <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
     <row r="67" spans="2:8">
@@ -3250,9 +3199,7 @@
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
-      <c r="G67" s="8">
-        <v>15</v>
-      </c>
+      <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
     <row r="68" spans="2:8">
@@ -3312,164 +3259,164 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="51"/>
-    <col min="2" max="2" width="37.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="8.83203125" style="51"/>
-    <col min="10" max="10" width="18.83203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="51"/>
+    <col min="1" max="1" width="8.83203125" style="47"/>
+    <col min="2" max="2" width="37.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.83203125" style="47"/>
+    <col min="10" max="10" width="18.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="55"/>
+      <c r="B3" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="61">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D3" s="61">
+        <v>1E-4</v>
+      </c>
+      <c r="E3" s="61">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="55"/>
+      <c r="B4" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="61">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D4" s="61">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E4" s="61">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="65" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="64"/>
-      <c r="B3" s="67" t="s">
+      <c r="C5" s="61">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D5" s="61">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E5" s="61">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="70">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="D3" s="70">
-        <v>1E-4</v>
-      </c>
-      <c r="E3" s="70">
-        <v>1.4E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="64"/>
-      <c r="B4" s="67" t="s">
+      <c r="C6" s="61">
+        <v>1.38E-2</v>
+      </c>
+      <c r="D6" s="61">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="E6" s="61">
+        <v>1.8599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="70">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="D4" s="70">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="E4" s="70">
-        <v>1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="64"/>
-      <c r="B5" s="67" t="s">
+      <c r="C7" s="61">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D7" s="61">
+        <v>6.3E-3</v>
+      </c>
+      <c r="E7" s="61">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="55"/>
+      <c r="B8" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="70">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="D5" s="70">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="E5" s="70">
-        <v>2.8E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="64"/>
-      <c r="B6" s="67" t="s">
+      <c r="C8" s="61">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="D8" s="61">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="E8" s="61">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="55"/>
+      <c r="B9" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="70">
-        <v>1.38E-2</v>
-      </c>
-      <c r="D6" s="70">
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="E6" s="70">
-        <v>1.8599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="64"/>
-      <c r="B7" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="70">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D7" s="70">
-        <v>6.3E-3</v>
-      </c>
-      <c r="E7" s="70">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="64"/>
-      <c r="B8" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="70">
-        <v>0.36699999999999999</v>
-      </c>
-      <c r="D8" s="70">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="E8" s="70">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="64"/>
-      <c r="B9" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="70">
+      <c r="C9" s="61">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="61">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="61">
         <v>0.27</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="71"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3485,112 +3432,112 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" s="73">
+        <v>85</v>
+      </c>
+      <c r="C15" s="64">
         <v>5.6</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D15" s="64">
         <v>3.3</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="64">
         <v>9.1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="73">
+        <v>86</v>
+      </c>
+      <c r="C16" s="64">
         <v>1</v>
       </c>
-      <c r="D16" s="73">
+      <c r="D16" s="64">
         <v>1</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="64">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="B17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="73">
+        <v>87</v>
+      </c>
+      <c r="C17" s="64">
         <v>1</v>
       </c>
-      <c r="D17" s="73">
+      <c r="D17" s="64">
         <v>1</v>
       </c>
-      <c r="E17" s="73">
+      <c r="E17" s="64">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="73">
+        <v>88</v>
+      </c>
+      <c r="C18" s="64">
         <v>1</v>
       </c>
-      <c r="D18" s="73">
+      <c r="D18" s="64">
         <v>1</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="64">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="73">
+        <v>89</v>
+      </c>
+      <c r="C19" s="64">
         <v>3.49</v>
       </c>
-      <c r="D19" s="73">
+      <c r="D19" s="64">
         <v>1.76</v>
       </c>
-      <c r="E19" s="73">
+      <c r="E19" s="64">
         <v>6.92</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="73">
+        <v>90</v>
+      </c>
+      <c r="C20" s="64">
         <v>7.17</v>
       </c>
-      <c r="D20" s="73">
+      <c r="D20" s="64">
         <v>3.9</v>
       </c>
-      <c r="E20" s="73">
+      <c r="E20" s="64">
         <v>12.08</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="71"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="71"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3606,99 +3553,99 @@
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="73">
+        <v>91</v>
+      </c>
+      <c r="C26" s="64">
         <v>0.24</v>
       </c>
-      <c r="D26" s="73">
+      <c r="D26" s="64">
         <v>0.1</v>
       </c>
-      <c r="E26" s="73">
+      <c r="E26" s="64">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="73">
+        <v>87</v>
+      </c>
+      <c r="C27" s="64">
         <v>0.95</v>
       </c>
-      <c r="D27" s="73">
+      <c r="D27" s="64">
         <v>0.62</v>
       </c>
-      <c r="E27" s="73">
+      <c r="E27" s="64">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G27" s="74"/>
+      <c r="G27" s="65"/>
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="73">
+        <v>92</v>
+      </c>
+      <c r="C28" s="64">
         <v>3</v>
       </c>
-      <c r="D28" s="73">
+      <c r="D28" s="64">
         <v>2.83</v>
       </c>
-      <c r="E28" s="73">
+      <c r="E28" s="64">
         <v>3.16</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="73">
+        <v>93</v>
+      </c>
+      <c r="C29" s="64">
         <v>3.74</v>
       </c>
-      <c r="D29" s="73">
+      <c r="D29" s="64">
         <v>3.48</v>
       </c>
-      <c r="E29" s="73">
+      <c r="E29" s="64">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="73">
+        <v>94</v>
+      </c>
+      <c r="C30" s="64">
         <v>1.5</v>
       </c>
-      <c r="D30" s="73">
+      <c r="D30" s="64">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E30" s="73">
+      <c r="E30" s="64">
         <v>2.25</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="71"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="71"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="71"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3714,277 +3661,277 @@
     </row>
     <row r="36" spans="1:5">
       <c r="B36" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="73">
+        <v>95</v>
+      </c>
+      <c r="C36" s="64">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D36" s="73">
+      <c r="D36" s="64">
         <v>1.07</v>
       </c>
-      <c r="E36" s="73">
+      <c r="E36" s="64">
         <v>7.28</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="73">
+        <v>96</v>
+      </c>
+      <c r="C37" s="64">
         <v>1.42</v>
       </c>
-      <c r="D37" s="73">
+      <c r="D37" s="64">
         <v>0.9</v>
       </c>
-      <c r="E37" s="73">
+      <c r="E37" s="64">
         <v>3.42</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="73">
+        <v>97</v>
+      </c>
+      <c r="C38" s="64">
         <v>2.14</v>
       </c>
-      <c r="D38" s="73">
+      <c r="D38" s="64">
         <v>1.39</v>
       </c>
-      <c r="E38" s="73">
+      <c r="E38" s="64">
         <v>3.58</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="B39" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="73">
+        <v>98</v>
+      </c>
+      <c r="C39" s="64">
         <v>0.66</v>
       </c>
-      <c r="D39" s="73">
+      <c r="D39" s="64">
         <v>0.51</v>
       </c>
-      <c r="E39" s="73">
+      <c r="E39" s="64">
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A40" s="58"/>
+    <row r="40" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A40" s="54"/>
       <c r="B40" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="73">
+        <v>124</v>
+      </c>
+      <c r="C40" s="64">
         <v>0.2</v>
       </c>
-      <c r="D40" s="73">
+      <c r="D40" s="64">
         <v>0.1</v>
       </c>
-      <c r="E40" s="73">
+      <c r="E40" s="64">
         <v>0.3</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="71"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
+      <c r="A41" s="62"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="71"/>
-      <c r="B42" s="72"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-    </row>
-    <row r="44" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A44" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-    </row>
-    <row r="45" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A45" s="58"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="54" t="s">
+      <c r="A43" s="62"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+    </row>
+    <row r="44" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A44" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+    </row>
+    <row r="45" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A45" s="54"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="54" t="s">
+      <c r="D45" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="54" t="s">
+      <c r="E45" s="50" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A46" s="58"/>
+    <row r="46" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A46" s="54"/>
       <c r="B46" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="70">
+        <v>87</v>
+      </c>
+      <c r="C46" s="61">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="D46" s="70">
+      <c r="D46" s="61">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E46" s="70">
+      <c r="E46" s="61">
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A47" s="58"/>
+    <row r="47" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A47" s="54"/>
       <c r="B47" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="61">
+        <v>0.15</v>
+      </c>
+      <c r="D47" s="61">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E47" s="61">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A48" s="54"/>
+      <c r="B48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="61">
+        <v>0.1</v>
+      </c>
+      <c r="D48" s="61">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E48" s="61">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A49" s="54"/>
+      <c r="B49" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="61">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D49" s="61">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E49" s="61">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="59" customFormat="1">
+      <c r="A50" s="54"/>
+      <c r="B50" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="61">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="D50" s="61">
+        <v>0.05</v>
+      </c>
+      <c r="E50" s="61">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A51" s="54"/>
+      <c r="B51" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="61">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="D51" s="61">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E51" s="61">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A52" s="54"/>
+      <c r="B52" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="61">
+        <v>0.09</v>
+      </c>
+      <c r="D52" s="61">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E52" s="61">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A53" s="54"/>
+      <c r="B53" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="70">
-        <v>0.15</v>
-      </c>
-      <c r="D47" s="70">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="E47" s="70">
-        <v>0.88500000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A48" s="58"/>
-      <c r="B48" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="70">
-        <v>0.1</v>
-      </c>
-      <c r="D48" s="70">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E48" s="70">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A49" s="58"/>
-      <c r="B49" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="70">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D49" s="70">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E49" s="70">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="68" customFormat="1">
-      <c r="A50" s="58"/>
-      <c r="B50" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="70">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="D50" s="70">
+      <c r="C53" s="61">
+        <v>0.111</v>
+      </c>
+      <c r="D53" s="61">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E53" s="61">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A54" s="54"/>
+      <c r="B54" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="61">
+        <v>0.16</v>
+      </c>
+      <c r="D54" s="61">
         <v>0.05</v>
       </c>
-      <c r="E50" s="70">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A51" s="58"/>
-      <c r="B51" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="70">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="D51" s="70">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="E51" s="70">
-        <v>0.68600000000000005</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A52" s="58"/>
-      <c r="B52" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="70">
-        <v>0.09</v>
-      </c>
-      <c r="D52" s="70">
-        <v>1.9E-2</v>
-      </c>
-      <c r="E52" s="70">
-        <v>0.72299999999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A53" s="58"/>
-      <c r="B53" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C53" s="70">
-        <v>0.111</v>
-      </c>
-      <c r="D53" s="70">
-        <v>4.7E-2</v>
-      </c>
-      <c r="E53" s="70">
-        <v>0.56299999999999994</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A54" s="58"/>
-      <c r="B54" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" s="70">
-        <v>0.16</v>
-      </c>
-      <c r="D54" s="70">
-        <v>0.05</v>
-      </c>
-      <c r="E54" s="70">
+      <c r="E54" s="61">
         <v>0.26</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A55" s="69"/>
-      <c r="B55" s="69"/>
-      <c r="C55" s="69"/>
-      <c r="D55" s="69"/>
-      <c r="E55" s="69"/>
-    </row>
-    <row r="56" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A56" s="69"/>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-    </row>
-    <row r="57" spans="1:6" s="68" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A57" s="69"/>
-      <c r="B57" s="69"/>
-      <c r="C57" s="69"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="69"/>
+    <row r="55" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A55" s="60"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
+    </row>
+    <row r="56" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A56" s="60"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+    </row>
+    <row r="57" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A57" s="60"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
     </row>
     <row r="58" spans="1:6" ht="13.5" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="13.5" customHeight="1">
@@ -4000,173 +3947,173 @@
     </row>
     <row r="60" spans="1:6" ht="13.5" customHeight="1">
       <c r="B60" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" s="70">
+        <v>85</v>
+      </c>
+      <c r="C60" s="61">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="D60" s="70">
+      <c r="D60" s="61">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E60" s="70">
+      <c r="E60" s="61">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="13.5" customHeight="1">
       <c r="B61" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="70">
+        <v>86</v>
+      </c>
+      <c r="C61" s="61">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="D61" s="70">
+      <c r="D61" s="61">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E61" s="70">
+      <c r="E61" s="61">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="13.5" customHeight="1">
       <c r="B62" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" s="70">
+        <v>100</v>
+      </c>
+      <c r="C62" s="61">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D62" s="70">
+      <c r="D62" s="61">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="E62" s="70">
+      <c r="E62" s="61">
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="13.5" customHeight="1">
       <c r="B63" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C63" s="70">
+        <v>88</v>
+      </c>
+      <c r="C63" s="61">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="D63" s="70">
+      <c r="D63" s="61">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="E63" s="70">
+      <c r="E63" s="61">
         <v>1.01E-2</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="B64" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C64" s="70">
+        <v>89</v>
+      </c>
+      <c r="C64" s="61">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D64" s="70">
+      <c r="D64" s="61">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E64" s="70">
+      <c r="E64" s="61">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F64" s="71"/>
+      <c r="F64" s="62"/>
     </row>
     <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C65" s="70">
+        <v>90</v>
+      </c>
+      <c r="C65" s="61">
         <v>0.32300000000000001</v>
       </c>
-      <c r="D65" s="70">
+      <c r="D65" s="61">
         <v>0.29599999999999999</v>
       </c>
-      <c r="E65" s="70">
+      <c r="E65" s="61">
         <v>0.432</v>
       </c>
-      <c r="F65" s="71"/>
+      <c r="F65" s="62"/>
     </row>
     <row r="66" spans="1:9">
       <c r="B66" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C66" s="70">
+        <v>122</v>
+      </c>
+      <c r="C66" s="61">
         <v>0.23</v>
       </c>
-      <c r="D66" s="70">
+      <c r="D66" s="61">
         <v>0.15</v>
       </c>
-      <c r="E66" s="70">
+      <c r="E66" s="61">
         <v>0.3</v>
       </c>
-      <c r="F66" s="71"/>
+      <c r="F66" s="62"/>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C67" s="70">
+        <v>123</v>
+      </c>
+      <c r="C67" s="61">
         <v>0.48780000000000001</v>
       </c>
-      <c r="D67" s="70">
+      <c r="D67" s="61">
         <v>0.28349999999999997</v>
       </c>
-      <c r="E67" s="70">
+      <c r="E67" s="61">
         <v>0.8417</v>
       </c>
-      <c r="F67" s="71"/>
+      <c r="F67" s="62"/>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C68" s="70">
+        <v>101</v>
+      </c>
+      <c r="C68" s="61">
         <v>2.17</v>
       </c>
-      <c r="D68" s="70">
+      <c r="D68" s="61">
         <v>1.27</v>
       </c>
-      <c r="E68" s="70">
+      <c r="E68" s="61">
         <v>3.71</v>
       </c>
-      <c r="F68" s="71"/>
+      <c r="F68" s="62"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="71"/>
-      <c r="B69" s="72"/>
-      <c r="C69" s="71"/>
-      <c r="D69" s="71"/>
-      <c r="E69" s="71"/>
-      <c r="F69" s="71"/>
+      <c r="A69" s="62"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="71"/>
-      <c r="B70" s="72"/>
-      <c r="C70" s="71"/>
-      <c r="D70" s="71"/>
-      <c r="E70" s="71"/>
-      <c r="F70" s="71"/>
-      <c r="G70" s="71"/>
-      <c r="H70" s="71"/>
-      <c r="I70" s="71"/>
+      <c r="A70" s="62"/>
+      <c r="B70" s="63"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="62"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="62"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="62"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="71"/>
-      <c r="B71" s="72"/>
-      <c r="C71" s="71"/>
-      <c r="D71" s="71"/>
-      <c r="E71" s="71"/>
-      <c r="F71" s="71"/>
-      <c r="G71" s="71"/>
-      <c r="H71" s="71"/>
-      <c r="I71" s="71"/>
+      <c r="A71" s="62"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="62"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="62"/>
+      <c r="G71" s="62"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="62"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F72" s="71"/>
-      <c r="G72" s="71"/>
-      <c r="H72" s="71"/>
-      <c r="I72" s="71"/>
+        <v>102</v>
+      </c>
+      <c r="F72" s="62"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
+      <c r="I72" s="62"/>
     </row>
     <row r="73" spans="1:9">
       <c r="C73" s="7" t="s">
@@ -4178,371 +4125,371 @@
       <c r="E73" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F73" s="71"/>
-      <c r="G73" s="71"/>
-      <c r="H73" s="71"/>
-      <c r="I73" s="71"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="62"/>
     </row>
     <row r="74" spans="1:9">
       <c r="B74" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C74" s="75">
+        <v>103</v>
+      </c>
+      <c r="C74" s="66">
         <v>0.95</v>
       </c>
-      <c r="D74" s="75">
+      <c r="D74" s="66">
         <v>0.8</v>
       </c>
-      <c r="E74" s="75">
+      <c r="E74" s="66">
         <v>0.98</v>
       </c>
-      <c r="F74" s="71"/>
-      <c r="G74" s="76"/>
-      <c r="H74" s="76"/>
-      <c r="I74" s="76"/>
+      <c r="F74" s="62"/>
+      <c r="G74" s="67"/>
+      <c r="H74" s="67"/>
+      <c r="I74" s="67"/>
     </row>
     <row r="75" spans="1:9">
       <c r="B75" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C75" s="75">
+        <v>104</v>
+      </c>
+      <c r="C75" s="66">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D75" s="75">
+      <c r="D75" s="66">
         <v>0.47</v>
       </c>
-      <c r="E75" s="75">
+      <c r="E75" s="66">
         <v>0.67</v>
       </c>
-      <c r="F75" s="71"/>
-      <c r="G75" s="76"/>
-      <c r="H75" s="76"/>
-      <c r="I75" s="76"/>
+      <c r="F75" s="62"/>
+      <c r="G75" s="67"/>
+      <c r="H75" s="67"/>
+      <c r="I75" s="67"/>
     </row>
     <row r="76" spans="1:9">
       <c r="B76" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C76" s="75">
+        <v>105</v>
+      </c>
+      <c r="C76" s="66">
         <v>0</v>
       </c>
-      <c r="D76" s="75">
+      <c r="D76" s="66">
         <v>0</v>
       </c>
-      <c r="E76" s="75">
+      <c r="E76" s="66">
         <v>0.68</v>
       </c>
-      <c r="F76" s="71"/>
+      <c r="F76" s="62"/>
     </row>
     <row r="77" spans="1:9">
       <c r="B77" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" s="75">
+        <v>106</v>
+      </c>
+      <c r="C77" s="66">
         <v>2.65</v>
       </c>
-      <c r="D77" s="75">
+      <c r="D77" s="66">
         <v>1.35</v>
       </c>
-      <c r="E77" s="75">
+      <c r="E77" s="66">
         <v>5.19</v>
       </c>
-      <c r="F77" s="71"/>
-      <c r="G77" s="76"/>
-      <c r="H77" s="76"/>
-      <c r="I77" s="76"/>
+      <c r="F77" s="62"/>
+      <c r="G77" s="67"/>
+      <c r="H77" s="67"/>
+      <c r="I77" s="67"/>
     </row>
     <row r="78" spans="1:9">
       <c r="B78" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C78" s="75">
+        <v>107</v>
+      </c>
+      <c r="C78" s="66">
         <v>0.54</v>
       </c>
-      <c r="D78" s="75">
+      <c r="D78" s="66">
         <v>0.33</v>
       </c>
-      <c r="E78" s="75">
+      <c r="E78" s="66">
         <v>0.68</v>
       </c>
-      <c r="F78" s="71"/>
-      <c r="G78" s="76"/>
-      <c r="H78" s="76"/>
-      <c r="I78" s="76"/>
+      <c r="F78" s="62"/>
+      <c r="G78" s="67"/>
+      <c r="H78" s="67"/>
+      <c r="I78" s="67"/>
     </row>
     <row r="79" spans="1:9">
       <c r="B79" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C79" s="75">
+        <v>108</v>
+      </c>
+      <c r="C79" s="66">
         <v>0.9</v>
       </c>
-      <c r="D79" s="75">
+      <c r="D79" s="66">
         <v>0.82</v>
       </c>
-      <c r="E79" s="75">
+      <c r="E79" s="66">
         <v>0.93</v>
       </c>
-      <c r="F79" s="71"/>
-      <c r="G79" s="76"/>
-      <c r="H79" s="76"/>
-      <c r="I79" s="76"/>
+      <c r="F79" s="62"/>
+      <c r="G79" s="67"/>
+      <c r="H79" s="67"/>
+      <c r="I79" s="67"/>
     </row>
     <row r="80" spans="1:9">
       <c r="B80" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C80" s="75">
+        <v>109</v>
+      </c>
+      <c r="C80" s="66">
         <v>0.73</v>
       </c>
-      <c r="D80" s="75">
+      <c r="D80" s="66">
         <v>0.65</v>
       </c>
-      <c r="E80" s="75">
+      <c r="E80" s="66">
         <v>0.8</v>
       </c>
-      <c r="F80" s="71"/>
-      <c r="G80" s="76"/>
-      <c r="H80" s="76"/>
-      <c r="I80" s="76"/>
+      <c r="F80" s="62"/>
+      <c r="G80" s="67"/>
+      <c r="H80" s="67"/>
+      <c r="I80" s="67"/>
     </row>
     <row r="81" spans="1:9">
       <c r="B81" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C81" s="75">
+        <v>110</v>
+      </c>
+      <c r="C81" s="66">
         <v>0.5</v>
       </c>
-      <c r="D81" s="75">
+      <c r="D81" s="66">
         <v>0.3</v>
       </c>
-      <c r="E81" s="75">
+      <c r="E81" s="66">
         <v>0.8</v>
       </c>
-      <c r="F81" s="71"/>
-      <c r="G81" s="76"/>
-      <c r="H81" s="76"/>
-      <c r="I81" s="76"/>
+      <c r="F81" s="62"/>
+      <c r="G81" s="67"/>
+      <c r="H81" s="67"/>
+      <c r="I81" s="67"/>
     </row>
     <row r="82" spans="1:9">
       <c r="B82" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C82" s="66">
+        <v>0.92</v>
+      </c>
+      <c r="D82" s="66">
+        <v>0.8</v>
+      </c>
+      <c r="E82" s="66">
+        <v>0.95</v>
+      </c>
+      <c r="F82" s="62"/>
+      <c r="G82" s="62"/>
+      <c r="H82" s="62"/>
+      <c r="I82" s="62"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="62"/>
+      <c r="B83" s="63"/>
+      <c r="C83" s="62"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="62"/>
+      <c r="F83" s="62"/>
+      <c r="G83" s="62"/>
+      <c r="H83" s="62"/>
+      <c r="I83" s="62"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="68"/>
+      <c r="B84" s="69"/>
+      <c r="C84" s="70"/>
+      <c r="D84" s="70"/>
+      <c r="E84" s="70"/>
+      <c r="F84" s="70"/>
+      <c r="G84" s="70"/>
+      <c r="H84" s="70"/>
+      <c r="I84" s="62"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="70"/>
+      <c r="B85" s="69"/>
+      <c r="C85" s="71"/>
+      <c r="D85" s="71"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="70"/>
+      <c r="G85" s="70"/>
+      <c r="H85" s="70"/>
+      <c r="I85" s="62"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="48"/>
+      <c r="C86" s="48"/>
+      <c r="D86" s="48"/>
+      <c r="E86" s="48"/>
+      <c r="F86" s="48"/>
+      <c r="G86" s="48"/>
+      <c r="H86" s="48"/>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="48"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E87" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="F87" s="48"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="48"/>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="48"/>
+      <c r="B88" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C88" s="64">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D88" s="64">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E88" s="64">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F88" s="48"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="48"/>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="48"/>
+      <c r="B89" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C82" s="75">
-        <v>0.92</v>
-      </c>
-      <c r="D82" s="75">
-        <v>0.8</v>
-      </c>
-      <c r="E82" s="75">
-        <v>0.95</v>
-      </c>
-      <c r="F82" s="71"/>
-      <c r="G82" s="71"/>
-      <c r="H82" s="71"/>
-      <c r="I82" s="71"/>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="71"/>
-      <c r="B83" s="72"/>
-      <c r="C83" s="71"/>
-      <c r="D83" s="71"/>
-      <c r="E83" s="71"/>
-      <c r="F83" s="71"/>
-      <c r="G83" s="71"/>
-      <c r="H83" s="71"/>
-      <c r="I83" s="71"/>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="77"/>
-      <c r="B84" s="78"/>
-      <c r="C84" s="79"/>
-      <c r="D84" s="79"/>
-      <c r="E84" s="79"/>
-      <c r="F84" s="79"/>
-      <c r="G84" s="79"/>
-      <c r="H84" s="79"/>
-      <c r="I84" s="71"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="79"/>
-      <c r="B85" s="78"/>
-      <c r="C85" s="80"/>
-      <c r="D85" s="80"/>
-      <c r="E85" s="80"/>
-      <c r="F85" s="79"/>
-      <c r="G85" s="79"/>
-      <c r="H85" s="79"/>
-      <c r="I85" s="71"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="55" t="s">
+      <c r="C89" s="64">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D89" s="64">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E89" s="64">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F89" s="48"/>
+      <c r="G89" s="48"/>
+      <c r="H89" s="48"/>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="48"/>
+      <c r="B90" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="B86" s="52"/>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
-      <c r="E86" s="52"/>
-      <c r="F86" s="52"/>
-      <c r="G86" s="52"/>
-      <c r="H86" s="52"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="52"/>
-      <c r="B87" s="52"/>
-      <c r="C87" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="D87" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="E87" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="F87" s="52"/>
-      <c r="G87" s="52"/>
-      <c r="H87" s="52"/>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="52"/>
-      <c r="B88" s="57" t="s">
+      <c r="C90" s="64">
+        <v>0.02</v>
+      </c>
+      <c r="D90" s="64">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E90" s="64">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F90" s="48"/>
+      <c r="G90" s="48"/>
+      <c r="H90" s="48"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="48"/>
+      <c r="B91" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="C88" s="73">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D88" s="73">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E88" s="73">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="F88" s="52"/>
-      <c r="G88" s="52"/>
-      <c r="H88" s="52"/>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="52"/>
-      <c r="B89" s="57" t="s">
+      <c r="C91" s="64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D91" s="64">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E91" s="64">
+        <v>9.4E-2</v>
+      </c>
+      <c r="F91" s="48"/>
+      <c r="G91" s="48"/>
+      <c r="H91" s="48"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="48"/>
+      <c r="B92" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="C89" s="73">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D89" s="73">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E89" s="73">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F89" s="52"/>
-      <c r="G89" s="52"/>
-      <c r="H89" s="52"/>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="52"/>
-      <c r="B90" s="57" t="s">
+      <c r="C92" s="64">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D92" s="64">
+        <v>0.114</v>
+      </c>
+      <c r="E92" s="64">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="F92" s="48"/>
+      <c r="G92" s="48"/>
+      <c r="H92" s="48"/>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="48"/>
+      <c r="B93" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="C90" s="73">
-        <v>0.02</v>
-      </c>
-      <c r="D90" s="73">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E90" s="73">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F90" s="52"/>
-      <c r="G90" s="52"/>
-      <c r="H90" s="52"/>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="52"/>
-      <c r="B91" s="57" t="s">
+      <c r="C93" s="64">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D93" s="64">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E93" s="64">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="F93" s="48"/>
+      <c r="G93" s="48"/>
+      <c r="H93" s="48"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="48"/>
+      <c r="B94" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C91" s="73">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D91" s="73">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="E91" s="73">
-        <v>9.4E-2</v>
-      </c>
-      <c r="F91" s="52"/>
-      <c r="G91" s="52"/>
-      <c r="H91" s="52"/>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="52"/>
-      <c r="B92" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C92" s="73">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D92" s="73">
-        <v>0.114</v>
-      </c>
-      <c r="E92" s="73">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="F92" s="52"/>
-      <c r="G92" s="52"/>
-      <c r="H92" s="52"/>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="52"/>
-      <c r="B93" s="57" t="s">
-        <v>121</v>
-      </c>
-      <c r="C93" s="73">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="D93" s="73">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="E93" s="73">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="F93" s="52"/>
-      <c r="G93" s="52"/>
-      <c r="H93" s="52"/>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="52"/>
-      <c r="B94" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="C94" s="73">
+      <c r="C94" s="64">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D94" s="73">
+      <c r="D94" s="64">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E94" s="73">
+      <c r="E94" s="64">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F94" s="52"/>
-      <c r="G94" s="52"/>
-      <c r="H94" s="52"/>
+      <c r="F94" s="48"/>
+      <c r="G94" s="48"/>
+      <c r="H94" s="48"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="F95" s="52"/>
-      <c r="G95" s="52"/>
-      <c r="H95" s="52"/>
+      <c r="F95" s="48"/>
+      <c r="G95" s="48"/>
+      <c r="H95" s="48"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="F96" s="52"/>
-      <c r="G96" s="52"/>
-      <c r="H96" s="52"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="48"/>
+      <c r="H96" s="48"/>
     </row>
     <row r="97" spans="6:8">
-      <c r="F97" s="52"/>
-      <c r="G97" s="52"/>
-      <c r="H97" s="52"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="48"/>
+      <c r="H97" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7288,8 +7235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7784,7 +7731,9 @@
       <c r="P20" s="8">
         <v>33080</v>
       </c>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="8">
+        <v>48100</v>
+      </c>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
@@ -8470,10 +8419,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y69"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45:G45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8562,25 +8511,25 @@
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
-      <c r="J3" s="34">
+      <c r="J3" s="33">
         <v>4910000</v>
       </c>
-      <c r="K3" s="34">
+      <c r="K3" s="33">
         <v>6852184.8953114701</v>
       </c>
-      <c r="L3" s="34">
+      <c r="L3" s="33">
         <v>8794369.7906229403</v>
       </c>
-      <c r="M3" s="34">
+      <c r="M3" s="33">
         <v>9345777.3429672103</v>
       </c>
-      <c r="N3" s="34">
+      <c r="N3" s="33">
         <v>9897184.8953114692</v>
       </c>
-      <c r="O3" s="34">
+      <c r="O3" s="33">
         <v>10448592.4476557</v>
       </c>
-      <c r="P3" s="34">
+      <c r="P3" s="33">
         <v>11000000</v>
       </c>
       <c r="Q3" s="27"/>
@@ -8687,7 +8636,7 @@
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
       <c r="O9" s="27"/>
-      <c r="P9" s="34">
+      <c r="P9" s="33">
         <v>3535</v>
       </c>
       <c r="Q9" s="27"/>
@@ -8779,46 +8728,46 @@
       <c r="B15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="33">
         <v>3121.27</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="33">
         <v>3721.45</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="33">
         <v>3923.85</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="33">
         <v>4279.33</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="33">
         <v>4533.55</v>
       </c>
-      <c r="H15" s="34">
+      <c r="H15" s="33">
         <v>4685.01</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="33">
         <v>4700.13</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="33">
         <v>4808.6400000000003</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="33">
         <v>4994.5</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L15" s="33">
         <v>5208.76</v>
       </c>
-      <c r="M15" s="34">
+      <c r="M15" s="33">
         <v>5323.27</v>
       </c>
-      <c r="N15" s="34">
+      <c r="N15" s="33">
         <v>5703.88</v>
       </c>
-      <c r="O15" s="34">
+      <c r="O15" s="33">
         <v>5196.3500000000004</v>
       </c>
-      <c r="P15" s="34">
+      <c r="P15" s="33">
         <v>5204.3599999999997</v>
       </c>
       <c r="Q15" s="27"/>
@@ -8910,164 +8859,164 @@
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
-      <c r="X21" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y21" s="37"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y21" s="36"/>
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="37"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="39">
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38">
         <v>2000</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="38">
         <v>2001</v>
       </c>
-      <c r="E26" s="39">
+      <c r="E26" s="38">
         <v>2002</v>
       </c>
-      <c r="F26" s="39">
+      <c r="F26" s="38">
         <v>2003</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="38">
         <v>2004</v>
       </c>
-      <c r="H26" s="39">
+      <c r="H26" s="38">
         <v>2005</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26" s="38">
         <v>2006</v>
       </c>
-      <c r="J26" s="39">
+      <c r="J26" s="38">
         <v>2007</v>
       </c>
-      <c r="K26" s="39">
+      <c r="K26" s="38">
         <v>2008</v>
       </c>
-      <c r="L26" s="39">
+      <c r="L26" s="38">
         <v>2009</v>
       </c>
-      <c r="M26" s="39">
+      <c r="M26" s="38">
         <v>2010</v>
       </c>
-      <c r="N26" s="39">
+      <c r="N26" s="38">
         <v>2011</v>
       </c>
-      <c r="O26" s="39">
+      <c r="O26" s="38">
         <v>2012</v>
       </c>
-      <c r="P26" s="39">
+      <c r="P26" s="38">
         <v>2013</v>
       </c>
-      <c r="Q26" s="39">
+      <c r="Q26" s="38">
         <v>2014</v>
       </c>
-      <c r="R26" s="39">
+      <c r="R26" s="38">
         <v>2015</v>
       </c>
-      <c r="S26" s="39">
+      <c r="S26" s="38">
         <v>2016</v>
       </c>
-      <c r="T26" s="39">
+      <c r="T26" s="38">
         <v>2017</v>
       </c>
-      <c r="U26" s="39">
+      <c r="U26" s="38">
         <v>2018</v>
       </c>
-      <c r="V26" s="39">
+      <c r="V26" s="38">
         <v>2019</v>
       </c>
-      <c r="W26" s="39">
+      <c r="W26" s="38">
         <v>2020</v>
       </c>
-      <c r="X26" s="38"/>
-      <c r="Y26" s="39" t="s">
+      <c r="X26" s="37"/>
+      <c r="Y26" s="38" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="39" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="40"/>
-      <c r="U27" s="40"/>
-      <c r="V27" s="40"/>
-      <c r="W27" s="40"/>
-      <c r="X27" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y27" s="40"/>
-    </row>
-    <row r="29" spans="1:25" s="51" customFormat="1"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
+      <c r="T27" s="39"/>
+      <c r="U27" s="39"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y27" s="39"/>
+    </row>
+    <row r="29" spans="1:25" s="47" customFormat="1"/>
     <row r="31" spans="1:25">
       <c r="A31" s="2" t="s">
         <v>54</v>
@@ -9145,46 +9094,46 @@
       <c r="B33" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="34">
+      <c r="C33" s="33">
         <v>714</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="33">
         <v>857</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="33">
         <v>1020</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="33">
         <v>1199</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="33">
         <v>1396</v>
       </c>
-      <c r="H33" s="34">
+      <c r="H33" s="33">
         <v>1607</v>
       </c>
-      <c r="I33" s="34">
+      <c r="I33" s="33">
         <v>1831</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="33">
         <v>2060</v>
       </c>
-      <c r="K33" s="34">
+      <c r="K33" s="33">
         <v>2233</v>
       </c>
-      <c r="L33" s="34">
+      <c r="L33" s="33">
         <v>2089</v>
       </c>
-      <c r="M33" s="34">
+      <c r="M33" s="33">
         <v>2197</v>
       </c>
-      <c r="N33" s="34">
+      <c r="N33" s="33">
         <v>2583</v>
       </c>
-      <c r="O33" s="34">
+      <c r="O33" s="33">
         <v>2858</v>
       </c>
-      <c r="P33" s="34">
+      <c r="P33" s="33">
         <v>3101</v>
       </c>
       <c r="Q33" s="27"/>
@@ -9309,881 +9258,6 @@
         <v>29</v>
       </c>
       <c r="Y39" s="27"/>
-    </row>
-    <row r="40" spans="1:25">
-      <c r="A40" s="42"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
-      <c r="Q40" s="42"/>
-      <c r="R40" s="42"/>
-      <c r="S40" s="42"/>
-      <c r="T40" s="42"/>
-      <c r="U40" s="42"/>
-      <c r="V40" s="42"/>
-      <c r="W40" s="42"/>
-      <c r="X40" s="42"/>
-      <c r="Y40" s="42"/>
-    </row>
-    <row r="41" spans="1:25">
-      <c r="A41" s="42"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="42"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="42"/>
-      <c r="R41" s="42"/>
-      <c r="S41" s="42"/>
-      <c r="T41" s="42"/>
-      <c r="U41" s="42"/>
-      <c r="V41" s="42"/>
-      <c r="W41" s="42"/>
-      <c r="X41" s="42"/>
-      <c r="Y41" s="42"/>
-    </row>
-    <row r="42" spans="1:25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="42"/>
-      <c r="Q42" s="42"/>
-      <c r="R42" s="42"/>
-      <c r="S42" s="42"/>
-      <c r="T42" s="42"/>
-      <c r="U42" s="42"/>
-      <c r="V42" s="42"/>
-      <c r="W42" s="42"/>
-      <c r="X42" s="42"/>
-      <c r="Y42" s="42"/>
-    </row>
-    <row r="43" spans="1:25">
-      <c r="A43" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="42"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="42"/>
-      <c r="S43" s="42"/>
-      <c r="T43" s="42"/>
-      <c r="U43" s="42"/>
-      <c r="V43" s="42"/>
-      <c r="W43" s="42"/>
-      <c r="X43" s="42"/>
-      <c r="Y43" s="42"/>
-    </row>
-    <row r="44" spans="1:25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D44" s="7">
-        <v>2001</v>
-      </c>
-      <c r="E44" s="7">
-        <v>2002</v>
-      </c>
-      <c r="F44" s="7">
-        <v>2003</v>
-      </c>
-      <c r="G44" s="7">
-        <v>2004</v>
-      </c>
-      <c r="H44" s="7">
-        <v>2005</v>
-      </c>
-      <c r="I44" s="7">
-        <v>2006</v>
-      </c>
-      <c r="J44" s="7">
-        <v>2007</v>
-      </c>
-      <c r="K44" s="7">
-        <v>2008</v>
-      </c>
-      <c r="L44" s="7">
-        <v>2009</v>
-      </c>
-      <c r="M44" s="7">
-        <v>2010</v>
-      </c>
-      <c r="N44" s="7">
-        <v>2011</v>
-      </c>
-      <c r="O44" s="7">
-        <v>2012</v>
-      </c>
-      <c r="P44" s="7">
-        <v>2013</v>
-      </c>
-      <c r="Q44" s="7">
-        <v>2014</v>
-      </c>
-      <c r="R44" s="7">
-        <v>2015</v>
-      </c>
-      <c r="S44" s="7">
-        <v>2016</v>
-      </c>
-      <c r="T44" s="7">
-        <v>2017</v>
-      </c>
-      <c r="U44" s="7">
-        <v>2018</v>
-      </c>
-      <c r="V44" s="7">
-        <v>2019</v>
-      </c>
-      <c r="W44" s="7">
-        <v>2020</v>
-      </c>
-      <c r="X44" s="42"/>
-      <c r="Y44" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25">
-      <c r="A45" s="42"/>
-      <c r="B45" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-      <c r="O45" s="44"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
-      <c r="T45" s="44"/>
-      <c r="U45" s="44"/>
-      <c r="V45" s="44"/>
-      <c r="W45" s="44"/>
-      <c r="X45" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y45" s="43"/>
-    </row>
-    <row r="46" spans="1:25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="42"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="42"/>
-      <c r="O46" s="42"/>
-      <c r="P46" s="42"/>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="42"/>
-      <c r="S46" s="42"/>
-      <c r="T46" s="42"/>
-      <c r="U46" s="42"/>
-      <c r="V46" s="42"/>
-      <c r="W46" s="42"/>
-      <c r="X46" s="42"/>
-      <c r="Y46" s="42"/>
-    </row>
-    <row r="47" spans="1:25">
-      <c r="A47" s="42"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="42"/>
-      <c r="L47" s="42"/>
-      <c r="M47" s="42"/>
-      <c r="N47" s="42"/>
-      <c r="O47" s="42"/>
-      <c r="P47" s="42"/>
-      <c r="Q47" s="42"/>
-      <c r="R47" s="42"/>
-      <c r="S47" s="42"/>
-      <c r="T47" s="42"/>
-      <c r="U47" s="42"/>
-      <c r="V47" s="42"/>
-      <c r="W47" s="42"/>
-      <c r="X47" s="42"/>
-      <c r="Y47" s="42"/>
-    </row>
-    <row r="48" spans="1:25">
-      <c r="A48" s="42"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
-      <c r="N48" s="42"/>
-      <c r="O48" s="42"/>
-      <c r="P48" s="42"/>
-      <c r="Q48" s="42"/>
-      <c r="R48" s="42"/>
-      <c r="S48" s="42"/>
-      <c r="T48" s="42"/>
-      <c r="U48" s="42"/>
-      <c r="V48" s="42"/>
-      <c r="W48" s="42"/>
-      <c r="X48" s="42"/>
-      <c r="Y48" s="42"/>
-    </row>
-    <row r="49" spans="1:25">
-      <c r="A49" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="30"/>
-      <c r="O49" s="30"/>
-      <c r="P49" s="30"/>
-      <c r="Q49" s="30"/>
-      <c r="R49" s="30"/>
-      <c r="S49" s="30"/>
-      <c r="T49" s="30"/>
-      <c r="U49" s="30"/>
-      <c r="V49" s="30"/>
-      <c r="W49" s="30"/>
-      <c r="X49" s="30"/>
-      <c r="Y49" s="30"/>
-    </row>
-    <row r="50" spans="1:25">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="31">
-        <v>2000</v>
-      </c>
-      <c r="D50" s="31">
-        <v>2001</v>
-      </c>
-      <c r="E50" s="31">
-        <v>2002</v>
-      </c>
-      <c r="F50" s="31">
-        <v>2003</v>
-      </c>
-      <c r="G50" s="31">
-        <v>2004</v>
-      </c>
-      <c r="H50" s="31">
-        <v>2005</v>
-      </c>
-      <c r="I50" s="31">
-        <v>2006</v>
-      </c>
-      <c r="J50" s="31">
-        <v>2007</v>
-      </c>
-      <c r="K50" s="31">
-        <v>2008</v>
-      </c>
-      <c r="L50" s="31">
-        <v>2009</v>
-      </c>
-      <c r="M50" s="31">
-        <v>2010</v>
-      </c>
-      <c r="N50" s="31">
-        <v>2011</v>
-      </c>
-      <c r="O50" s="31">
-        <v>2012</v>
-      </c>
-      <c r="P50" s="31">
-        <v>2013</v>
-      </c>
-      <c r="Q50" s="31">
-        <v>2014</v>
-      </c>
-      <c r="R50" s="31">
-        <v>2015</v>
-      </c>
-      <c r="S50" s="31">
-        <v>2016</v>
-      </c>
-      <c r="T50" s="31">
-        <v>2017</v>
-      </c>
-      <c r="U50" s="31">
-        <v>2018</v>
-      </c>
-      <c r="V50" s="31">
-        <v>2019</v>
-      </c>
-      <c r="W50" s="31">
-        <v>2020</v>
-      </c>
-      <c r="X50" s="30"/>
-      <c r="Y50" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25">
-      <c r="A51" s="30"/>
-      <c r="B51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="32"/>
-      <c r="R51" s="32"/>
-      <c r="S51" s="32"/>
-      <c r="T51" s="32"/>
-      <c r="U51" s="32"/>
-      <c r="V51" s="32"/>
-      <c r="W51" s="32"/>
-      <c r="X51" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y51" s="32"/>
-    </row>
-    <row r="52" spans="1:25">
-      <c r="A52" s="38"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="38"/>
-      <c r="M52" s="38"/>
-      <c r="N52" s="38"/>
-      <c r="O52" s="38"/>
-      <c r="P52" s="38"/>
-      <c r="Q52" s="38"/>
-      <c r="R52" s="38"/>
-      <c r="S52" s="38"/>
-      <c r="T52" s="38"/>
-      <c r="U52" s="38"/>
-      <c r="V52" s="38"/>
-      <c r="W52" s="38"/>
-      <c r="X52" s="38"/>
-      <c r="Y52" s="38"/>
-    </row>
-    <row r="53" spans="1:25">
-      <c r="A53" s="38"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="38"/>
-      <c r="L53" s="38"/>
-      <c r="M53" s="38"/>
-      <c r="N53" s="38"/>
-      <c r="O53" s="38"/>
-      <c r="P53" s="38"/>
-      <c r="Q53" s="38"/>
-      <c r="R53" s="38"/>
-      <c r="S53" s="38"/>
-      <c r="T53" s="38"/>
-      <c r="U53" s="38"/>
-      <c r="V53" s="38"/>
-      <c r="W53" s="38"/>
-      <c r="X53" s="38"/>
-      <c r="Y53" s="38"/>
-    </row>
-    <row r="54" spans="1:25">
-      <c r="A54" s="38"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
-      <c r="K54" s="38"/>
-      <c r="L54" s="38"/>
-      <c r="M54" s="38"/>
-      <c r="N54" s="38"/>
-      <c r="O54" s="38"/>
-      <c r="P54" s="38"/>
-      <c r="Q54" s="38"/>
-      <c r="R54" s="38"/>
-      <c r="S54" s="38"/>
-      <c r="T54" s="38"/>
-      <c r="U54" s="38"/>
-      <c r="V54" s="38"/>
-      <c r="W54" s="38"/>
-      <c r="X54" s="38"/>
-      <c r="Y54" s="38"/>
-    </row>
-    <row r="55" spans="1:25">
-      <c r="A55" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="30"/>
-      <c r="N55" s="30"/>
-      <c r="O55" s="30"/>
-      <c r="P55" s="30"/>
-      <c r="Q55" s="30"/>
-      <c r="R55" s="30"/>
-      <c r="S55" s="30"/>
-      <c r="T55" s="30"/>
-      <c r="U55" s="30"/>
-      <c r="V55" s="30"/>
-      <c r="W55" s="30"/>
-      <c r="X55" s="30"/>
-      <c r="Y55" s="30"/>
-    </row>
-    <row r="56" spans="1:25">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="31">
-        <v>2000</v>
-      </c>
-      <c r="D56" s="31">
-        <v>2001</v>
-      </c>
-      <c r="E56" s="31">
-        <v>2002</v>
-      </c>
-      <c r="F56" s="31">
-        <v>2003</v>
-      </c>
-      <c r="G56" s="31">
-        <v>2004</v>
-      </c>
-      <c r="H56" s="31">
-        <v>2005</v>
-      </c>
-      <c r="I56" s="31">
-        <v>2006</v>
-      </c>
-      <c r="J56" s="31">
-        <v>2007</v>
-      </c>
-      <c r="K56" s="31">
-        <v>2008</v>
-      </c>
-      <c r="L56" s="31">
-        <v>2009</v>
-      </c>
-      <c r="M56" s="31">
-        <v>2010</v>
-      </c>
-      <c r="N56" s="31">
-        <v>2011</v>
-      </c>
-      <c r="O56" s="31">
-        <v>2012</v>
-      </c>
-      <c r="P56" s="31">
-        <v>2013</v>
-      </c>
-      <c r="Q56" s="31">
-        <v>2014</v>
-      </c>
-      <c r="R56" s="31">
-        <v>2015</v>
-      </c>
-      <c r="S56" s="31">
-        <v>2016</v>
-      </c>
-      <c r="T56" s="31">
-        <v>2017</v>
-      </c>
-      <c r="U56" s="31">
-        <v>2018</v>
-      </c>
-      <c r="V56" s="31">
-        <v>2019</v>
-      </c>
-      <c r="W56" s="31">
-        <v>2020</v>
-      </c>
-      <c r="X56" s="30"/>
-      <c r="Y56" s="31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="32"/>
-      <c r="N57" s="32"/>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
-      <c r="Q57" s="32"/>
-      <c r="R57" s="32"/>
-      <c r="S57" s="32"/>
-      <c r="T57" s="32"/>
-      <c r="U57" s="32"/>
-      <c r="V57" s="32"/>
-      <c r="W57" s="32"/>
-      <c r="X57" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y57" s="32"/>
-    </row>
-    <row r="61" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1">
-      <c r="A61" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1">
-      <c r="C62" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D62" s="7">
-        <v>2001</v>
-      </c>
-      <c r="E62" s="7">
-        <v>2002</v>
-      </c>
-      <c r="F62" s="7">
-        <v>2003</v>
-      </c>
-      <c r="G62" s="7">
-        <v>2004</v>
-      </c>
-      <c r="H62" s="7">
-        <v>2005</v>
-      </c>
-      <c r="I62" s="7">
-        <v>2006</v>
-      </c>
-      <c r="J62" s="7">
-        <v>2007</v>
-      </c>
-      <c r="K62" s="7">
-        <v>2008</v>
-      </c>
-      <c r="L62" s="7">
-        <v>2009</v>
-      </c>
-      <c r="M62" s="7">
-        <v>2010</v>
-      </c>
-      <c r="N62" s="7">
-        <v>2011</v>
-      </c>
-      <c r="O62" s="7">
-        <v>2012</v>
-      </c>
-      <c r="P62" s="7">
-        <v>2013</v>
-      </c>
-      <c r="Q62" s="7">
-        <v>2014</v>
-      </c>
-      <c r="R62" s="7">
-        <v>2015</v>
-      </c>
-      <c r="S62" s="7">
-        <v>2016</v>
-      </c>
-      <c r="T62" s="7">
-        <v>2017</v>
-      </c>
-      <c r="U62" s="7">
-        <v>2018</v>
-      </c>
-      <c r="V62" s="7">
-        <v>2019</v>
-      </c>
-      <c r="W62" s="7">
-        <v>2020</v>
-      </c>
-      <c r="Y62" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" s="51" customFormat="1" ht="15" customHeight="1">
-      <c r="B63" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="45"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="45"/>
-      <c r="L63" s="45"/>
-      <c r="M63" s="45"/>
-      <c r="N63" s="45"/>
-      <c r="O63" s="45"/>
-      <c r="P63" s="45"/>
-      <c r="Q63" s="45"/>
-      <c r="R63" s="45"/>
-      <c r="S63" s="45"/>
-      <c r="T63" s="45"/>
-      <c r="U63" s="45"/>
-      <c r="V63" s="45"/>
-      <c r="W63" s="45"/>
-      <c r="X63" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y63" s="45"/>
-    </row>
-    <row r="64" spans="1:25" s="51" customFormat="1"/>
-    <row r="65" spans="1:25" s="51" customFormat="1"/>
-    <row r="66" spans="1:25" s="51" customFormat="1"/>
-    <row r="67" spans="1:25">
-      <c r="A67" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="B67" s="59"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="59"/>
-      <c r="E67" s="59"/>
-      <c r="F67" s="59"/>
-      <c r="G67" s="59"/>
-      <c r="H67" s="59"/>
-      <c r="I67" s="59"/>
-      <c r="J67" s="59"/>
-      <c r="K67" s="59"/>
-      <c r="L67" s="59"/>
-      <c r="M67" s="59"/>
-      <c r="N67" s="59"/>
-      <c r="O67" s="59"/>
-      <c r="P67" s="59"/>
-      <c r="Q67" s="59"/>
-      <c r="R67" s="59"/>
-      <c r="S67" s="59"/>
-      <c r="T67" s="59"/>
-      <c r="U67" s="59"/>
-      <c r="V67" s="59"/>
-      <c r="W67" s="59"/>
-      <c r="X67" s="59"/>
-      <c r="Y67" s="59"/>
-    </row>
-    <row r="68" spans="1:25">
-      <c r="A68" s="59"/>
-      <c r="B68" s="59"/>
-      <c r="C68" s="61">
-        <v>2000</v>
-      </c>
-      <c r="D68" s="61">
-        <v>2001</v>
-      </c>
-      <c r="E68" s="61">
-        <v>2002</v>
-      </c>
-      <c r="F68" s="61">
-        <v>2003</v>
-      </c>
-      <c r="G68" s="61">
-        <v>2004</v>
-      </c>
-      <c r="H68" s="61">
-        <v>2005</v>
-      </c>
-      <c r="I68" s="61">
-        <v>2006</v>
-      </c>
-      <c r="J68" s="61">
-        <v>2007</v>
-      </c>
-      <c r="K68" s="61">
-        <v>2008</v>
-      </c>
-      <c r="L68" s="61">
-        <v>2009</v>
-      </c>
-      <c r="M68" s="61">
-        <v>2010</v>
-      </c>
-      <c r="N68" s="61">
-        <v>2011</v>
-      </c>
-      <c r="O68" s="61">
-        <v>2012</v>
-      </c>
-      <c r="P68" s="61">
-        <v>2013</v>
-      </c>
-      <c r="Q68" s="61">
-        <v>2014</v>
-      </c>
-      <c r="R68" s="61">
-        <v>2015</v>
-      </c>
-      <c r="S68" s="61">
-        <v>2016</v>
-      </c>
-      <c r="T68" s="61">
-        <v>2017</v>
-      </c>
-      <c r="U68" s="61">
-        <v>2018</v>
-      </c>
-      <c r="V68" s="61">
-        <v>2019</v>
-      </c>
-      <c r="W68" s="61">
-        <v>2020</v>
-      </c>
-      <c r="X68" s="59"/>
-      <c r="Y68" s="61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:25">
-      <c r="A69" s="59"/>
-      <c r="B69" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="C69" s="62"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="62"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="62"/>
-      <c r="I69" s="62"/>
-      <c r="J69" s="62"/>
-      <c r="K69" s="62"/>
-      <c r="L69" s="62"/>
-      <c r="M69" s="62"/>
-      <c r="N69" s="62"/>
-      <c r="O69" s="62"/>
-      <c r="P69" s="62"/>
-      <c r="Q69" s="62"/>
-      <c r="R69" s="62"/>
-      <c r="S69" s="62"/>
-      <c r="T69" s="62"/>
-      <c r="U69" s="62"/>
-      <c r="V69" s="62"/>
-      <c r="W69" s="62"/>
-      <c r="X69" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y69" s="62">
-        <v>0.85</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -10201,14 +9275,14 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y8"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -10310,8 +9384,8 @@
       <c r="X3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="81">
-        <v>3</v>
+      <c r="Y3" s="72">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -10344,8 +9418,8 @@
       <c r="X4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y4" s="81">
-        <v>3</v>
+      <c r="Y4" s="72">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -10377,8 +9451,8 @@
       <c r="X5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y5" s="81">
-        <v>3</v>
+      <c r="Y5" s="72">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -10409,8 +9483,8 @@
       <c r="X6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y6" s="81">
-        <v>3</v>
+      <c r="Y6" s="72">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -10443,8 +9517,8 @@
       <c r="X7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y7" s="81">
-        <v>3</v>
+      <c r="Y7" s="72">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -10477,8 +9551,8 @@
       <c r="X8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y8" s="81">
-        <v>3</v>
+      <c r="Y8" s="72">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -10486,7 +9560,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -10562,32 +9636,32 @@
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
       <c r="X14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y14" s="45">
-        <v>0.8</v>
+      <c r="Y14" s="41">
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -10595,32 +9669,32 @@
         <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="45"/>
-      <c r="W15" s="45"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="41"/>
+      <c r="W15" s="41"/>
       <c r="X15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y15" s="45">
-        <v>0.8</v>
+      <c r="Y15" s="41">
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -10628,64 +9702,64 @@
         <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
       <c r="X16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="45">
-        <v>0.8</v>
+      <c r="Y16" s="41">
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:25">
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
       <c r="X17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y17" s="45">
-        <v>0.8</v>
+      <c r="Y17" s="41">
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -10693,32 +9767,32 @@
         <f>Populations!$C$7</f>
         <v>M 15+</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="45"/>
-      <c r="W18" s="45"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
       <c r="X18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y18" s="45">
-        <v>0.8</v>
+      <c r="Y18" s="41">
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -10726,37 +9800,37 @@
         <f>Populations!$C$8</f>
         <v>F 15+</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="45"/>
-      <c r="W19" s="45"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
       <c r="X19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y19" s="45">
-        <v>0.8</v>
+      <c r="Y19" s="41">
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
@@ -10859,31 +9933,31 @@
       <c r="B25" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="46"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="46"/>
-      <c r="W25" s="46"/>
-      <c r="X25" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y25" s="47">
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="42"/>
+      <c r="X25" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y25" s="43">
         <v>1</v>
       </c>
     </row>
@@ -10910,7 +9984,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -11180,7 +10254,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -11450,7 +10524,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -11720,7 +10794,7 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -11907,7 +10981,7 @@
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
-      <c r="P39" s="48">
+      <c r="P39" s="44">
         <v>1E-3</v>
       </c>
       <c r="Q39" s="22"/>
@@ -11990,7 +11064,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -12075,10 +11149,10 @@
       <c r="I47" s="22"/>
       <c r="J47" s="22"/>
       <c r="K47" s="22"/>
-      <c r="L47" s="49">
+      <c r="L47" s="45">
         <v>0.8</v>
       </c>
-      <c r="M47" s="49"/>
+      <c r="M47" s="45"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
       <c r="P47" s="22"/>
@@ -12177,8 +11251,8 @@
       <c r="I50" s="22"/>
       <c r="J50" s="22"/>
       <c r="K50" s="22"/>
-      <c r="L50" s="50"/>
-      <c r="M50" s="50"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="46"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
       <c r="P50" s="22">
@@ -12272,7 +11346,7 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:25">
@@ -12546,7 +11620,7 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:25">
@@ -12750,7 +11824,7 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:25">

</xml_diff>

<commit_message>
add props back to spreadsheet and add to plots
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="133">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -529,6 +529,21 @@
   </si>
   <si>
     <t>Treatment failure rate</t>
+  </si>
+  <si>
+    <t>PLHIV aware of their status (%)</t>
+  </si>
+  <si>
+    <t>Diagnosed PLHIV in care (%)</t>
+  </si>
+  <si>
+    <t>PLHIV in care on treatment (%)</t>
+  </si>
+  <si>
+    <t>Pregnant women on PMTCT (%)</t>
+  </si>
+  <si>
+    <t>People on ART with viral suppression (%)</t>
   </si>
 </sst>
 </file>
@@ -546,7 +561,7 @@
     <numFmt numFmtId="170" formatCode="#,##0.0"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -681,8 +696,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,6 +748,12 @@
         <bgColor rgb="FF18C1FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF18C1FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -750,7 +779,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="199">
+  <cellStyleXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -950,8 +979,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1051,7 +1086,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1111,11 +1145,21 @@
     <xf numFmtId="4" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="199">
+  <cellStyles count="205">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1163,6 +1207,9 @@
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1295,6 +1342,9 @@
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -1824,15 +1874,15 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="74"/>
+      <c r="A2" s="77"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="74"/>
+      <c r="A3" s="77"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
@@ -2534,7 +2584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
@@ -3264,160 +3314,160 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="48"/>
-    <col min="2" max="2" width="37.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="8.83203125" style="48"/>
-    <col min="10" max="10" width="18.83203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="48"/>
+    <col min="1" max="1" width="8.83203125" style="47"/>
+    <col min="2" max="2" width="37.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.83203125" style="47"/>
+    <col min="10" max="10" width="18.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="56" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="56"/>
-      <c r="B3" s="59" t="s">
+      <c r="A3" s="55"/>
+      <c r="B3" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="62">
+      <c r="C3" s="61">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D3" s="62">
+      <c r="D3" s="61">
         <v>1E-4</v>
       </c>
-      <c r="E3" s="62">
+      <c r="E3" s="61">
         <v>1.4E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="56"/>
-      <c r="B4" s="59" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="62">
+      <c r="C4" s="61">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="D4" s="62">
+      <c r="D4" s="61">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E4" s="62">
+      <c r="E4" s="61">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="56"/>
-      <c r="B5" s="59" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="62">
+      <c r="C5" s="61">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="61">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="E5" s="62">
+      <c r="E5" s="61">
         <v>2.8E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="56"/>
-      <c r="B6" s="59" t="s">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="61">
         <v>1.38E-2</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="61">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="E6" s="62">
+      <c r="E6" s="61">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="56"/>
-      <c r="B7" s="59" t="s">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="62">
+      <c r="C7" s="61">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="61">
         <v>6.3E-3</v>
       </c>
-      <c r="E7" s="62">
+      <c r="E7" s="61">
         <v>2.4E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="56"/>
-      <c r="B8" s="59" t="s">
+      <c r="A8" s="55"/>
+      <c r="B8" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="62">
+      <c r="C8" s="61">
         <v>0.36699999999999999</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="61">
         <v>0.29399999999999998</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="61">
         <v>0.44</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="56"/>
-      <c r="B9" s="59" t="s">
+      <c r="A9" s="55"/>
+      <c r="B9" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="62">
+      <c r="C9" s="61">
         <v>0.20499999999999999</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="61">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E9" s="62">
+      <c r="E9" s="61">
         <v>0.27</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="63"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="63"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
@@ -3439,13 +3489,13 @@
       <c r="B15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="64">
         <v>5.6</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="64">
         <v>3.3</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="64">
         <v>9.1</v>
       </c>
     </row>
@@ -3453,13 +3503,13 @@
       <c r="B16" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="64">
         <v>1</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="64">
         <v>1</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="64">
         <v>1</v>
       </c>
     </row>
@@ -3467,13 +3517,13 @@
       <c r="B17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="65">
+      <c r="C17" s="64">
         <v>1</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="64">
         <v>1</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="64">
         <v>1</v>
       </c>
     </row>
@@ -3481,13 +3531,13 @@
       <c r="B18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="65">
+      <c r="C18" s="64">
         <v>1</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="64">
         <v>1</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="64">
         <v>1</v>
       </c>
     </row>
@@ -3495,13 +3545,13 @@
       <c r="B19" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="65">
+      <c r="C19" s="64">
         <v>3.49</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="64">
         <v>1.76</v>
       </c>
-      <c r="E19" s="65">
+      <c r="E19" s="64">
         <v>6.92</v>
       </c>
     </row>
@@ -3509,36 +3559,36 @@
       <c r="B20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="65">
+      <c r="C20" s="64">
         <v>7.17</v>
       </c>
-      <c r="D20" s="65">
+      <c r="D20" s="64">
         <v>3.9</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="64">
         <v>12.08</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="63"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="63"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
@@ -3560,13 +3610,13 @@
       <c r="B26" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="65">
+      <c r="C26" s="64">
         <v>0.24</v>
       </c>
-      <c r="D26" s="65">
+      <c r="D26" s="64">
         <v>0.1</v>
       </c>
-      <c r="E26" s="65">
+      <c r="E26" s="64">
         <v>0.5</v>
       </c>
     </row>
@@ -3574,28 +3624,28 @@
       <c r="B27" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="65">
+      <c r="C27" s="64">
         <v>0.95</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="64">
         <v>0.62</v>
       </c>
-      <c r="E27" s="65">
+      <c r="E27" s="64">
         <v>1.1599999999999999</v>
       </c>
-      <c r="G27" s="66"/>
+      <c r="G27" s="65"/>
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="65">
+      <c r="C28" s="64">
         <v>3</v>
       </c>
-      <c r="D28" s="65">
+      <c r="D28" s="64">
         <v>2.83</v>
       </c>
-      <c r="E28" s="65">
+      <c r="E28" s="64">
         <v>3.16</v>
       </c>
     </row>
@@ -3603,13 +3653,13 @@
       <c r="B29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="65">
+      <c r="C29" s="64">
         <v>3.74</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="64">
         <v>3.48</v>
       </c>
-      <c r="E29" s="65">
+      <c r="E29" s="64">
         <v>4</v>
       </c>
     </row>
@@ -3617,36 +3667,36 @@
       <c r="B30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="65">
+      <c r="C30" s="64">
         <v>1.5</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="64">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E30" s="65">
+      <c r="E30" s="64">
         <v>2.25</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="63"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="63"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="63"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
@@ -3668,13 +3718,13 @@
       <c r="B36" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="65">
+      <c r="C36" s="64">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="64">
         <v>1.07</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="64">
         <v>7.28</v>
       </c>
     </row>
@@ -3682,13 +3732,13 @@
       <c r="B37" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="65">
+      <c r="C37" s="64">
         <v>1.42</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="64">
         <v>0.9</v>
       </c>
-      <c r="E37" s="65">
+      <c r="E37" s="64">
         <v>3.42</v>
       </c>
     </row>
@@ -3696,13 +3746,13 @@
       <c r="B38" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="65">
+      <c r="C38" s="64">
         <v>2.14</v>
       </c>
-      <c r="D38" s="65">
+      <c r="D38" s="64">
         <v>1.39</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="64">
         <v>3.58</v>
       </c>
     </row>
@@ -3710,229 +3760,229 @@
       <c r="B39" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="65">
+      <c r="C39" s="64">
         <v>0.66</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="64">
         <v>0.51</v>
       </c>
-      <c r="E39" s="65">
+      <c r="E39" s="64">
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A40" s="55"/>
+    <row r="40" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A40" s="54"/>
       <c r="B40" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="65">
+      <c r="C40" s="64">
         <v>0.2</v>
       </c>
-      <c r="D40" s="65">
+      <c r="D40" s="64">
         <v>0.1</v>
       </c>
-      <c r="E40" s="65">
+      <c r="E40" s="64">
         <v>0.3</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="63"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
+      <c r="A41" s="62"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="63"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="63"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-    </row>
-    <row r="44" spans="1:5" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A44" s="50" t="s">
+      <c r="A43" s="62"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+    </row>
+    <row r="44" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A44" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-    </row>
-    <row r="45" spans="1:5" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A45" s="55"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="51" t="s">
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+    </row>
+    <row r="45" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A45" s="54"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="51" t="s">
+      <c r="D45" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="50" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A46" s="55"/>
+    <row r="46" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A46" s="54"/>
       <c r="B46" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="62">
+      <c r="C46" s="61">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="61">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E46" s="62">
+      <c r="E46" s="61">
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A47" s="55"/>
+    <row r="47" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A47" s="54"/>
       <c r="B47" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="62">
+      <c r="C47" s="61">
         <v>0.15</v>
       </c>
-      <c r="D47" s="62">
+      <c r="D47" s="61">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="E47" s="62">
+      <c r="E47" s="61">
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A48" s="55"/>
+    <row r="48" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A48" s="54"/>
       <c r="B48" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="62">
+      <c r="C48" s="61">
         <v>0.1</v>
       </c>
-      <c r="D48" s="62">
+      <c r="D48" s="61">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E48" s="62">
+      <c r="E48" s="61">
         <v>0.87</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A49" s="55"/>
+    <row r="49" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A49" s="54"/>
       <c r="B49" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="62">
+      <c r="C49" s="61">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D49" s="62">
+      <c r="D49" s="61">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E49" s="62">
+      <c r="E49" s="61">
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="60" customFormat="1">
-      <c r="A50" s="55"/>
+    <row r="50" spans="1:6" s="59" customFormat="1">
+      <c r="A50" s="54"/>
       <c r="B50" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="62">
+      <c r="C50" s="61">
         <v>0.16200000000000001</v>
       </c>
-      <c r="D50" s="62">
+      <c r="D50" s="61">
         <v>0.05</v>
       </c>
-      <c r="E50" s="62">
+      <c r="E50" s="61">
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A51" s="55"/>
+    <row r="51" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A51" s="54"/>
       <c r="B51" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="62">
+      <c r="C51" s="61">
         <v>0.11700000000000001</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D51" s="61">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E51" s="62">
+      <c r="E51" s="61">
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A52" s="55"/>
+    <row r="52" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A52" s="54"/>
       <c r="B52" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="62">
+      <c r="C52" s="61">
         <v>0.09</v>
       </c>
-      <c r="D52" s="62">
+      <c r="D52" s="61">
         <v>1.9E-2</v>
       </c>
-      <c r="E52" s="62">
+      <c r="E52" s="61">
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A53" s="55"/>
+    <row r="53" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A53" s="54"/>
       <c r="B53" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C53" s="62">
+      <c r="C53" s="61">
         <v>0.111</v>
       </c>
-      <c r="D53" s="62">
+      <c r="D53" s="61">
         <v>4.7E-2</v>
       </c>
-      <c r="E53" s="62">
+      <c r="E53" s="61">
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A54" s="55"/>
+    <row r="54" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A54" s="54"/>
       <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C54" s="62">
+      <c r="C54" s="61">
         <v>0.16</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="61">
         <v>0.05</v>
       </c>
-      <c r="E54" s="62">
+      <c r="E54" s="61">
         <v>0.26</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A55" s="61"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="61"/>
-      <c r="E55" s="61"/>
-    </row>
-    <row r="56" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A56" s="61"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="61"/>
-    </row>
-    <row r="57" spans="1:6" s="60" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A57" s="61"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
+    <row r="55" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A55" s="60"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
+    </row>
+    <row r="56" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A56" s="60"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+    </row>
+    <row r="57" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A57" s="60"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
     </row>
     <row r="58" spans="1:6" ht="13.5" customHeight="1">
       <c r="A58" s="2" t="s">
@@ -3954,13 +4004,13 @@
       <c r="B60" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="62">
+      <c r="C60" s="61">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="61">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E60" s="62">
+      <c r="E60" s="61">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
@@ -3968,13 +4018,13 @@
       <c r="B61" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="62">
+      <c r="C61" s="61">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="D61" s="62">
+      <c r="D61" s="61">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="E61" s="62">
+      <c r="E61" s="61">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
@@ -3982,13 +4032,13 @@
       <c r="B62" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="62">
+      <c r="C62" s="61">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D62" s="62">
+      <c r="D62" s="61">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="E62" s="62">
+      <c r="E62" s="61">
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
@@ -3996,13 +4046,13 @@
       <c r="B63" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="62">
+      <c r="C63" s="61">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="D63" s="62">
+      <c r="D63" s="61">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="E63" s="62">
+      <c r="E63" s="61">
         <v>1.01E-2</v>
       </c>
     </row>
@@ -4010,115 +4060,115 @@
       <c r="B64" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C64" s="62">
+      <c r="C64" s="61">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D64" s="62">
+      <c r="D64" s="61">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E64" s="62">
+      <c r="E64" s="61">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F64" s="63"/>
+      <c r="F64" s="62"/>
     </row>
     <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C65" s="62">
+      <c r="C65" s="61">
         <v>0.32300000000000001</v>
       </c>
-      <c r="D65" s="62">
+      <c r="D65" s="61">
         <v>0.29599999999999999</v>
       </c>
-      <c r="E65" s="62">
+      <c r="E65" s="61">
         <v>0.432</v>
       </c>
-      <c r="F65" s="63"/>
+      <c r="F65" s="62"/>
     </row>
     <row r="66" spans="1:9">
       <c r="B66" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="62">
+      <c r="C66" s="61">
         <v>0.23</v>
       </c>
-      <c r="D66" s="62">
+      <c r="D66" s="61">
         <v>0.15</v>
       </c>
-      <c r="E66" s="62">
+      <c r="E66" s="61">
         <v>0.3</v>
       </c>
-      <c r="F66" s="63"/>
+      <c r="F66" s="62"/>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C67" s="62">
+      <c r="C67" s="61">
         <v>0.48780000000000001</v>
       </c>
-      <c r="D67" s="62">
+      <c r="D67" s="61">
         <v>0.28349999999999997</v>
       </c>
-      <c r="E67" s="62">
+      <c r="E67" s="61">
         <v>0.8417</v>
       </c>
-      <c r="F67" s="63"/>
+      <c r="F67" s="62"/>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C68" s="62">
+      <c r="C68" s="61">
         <v>2.17</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="61">
         <v>1.27</v>
       </c>
-      <c r="E68" s="62">
+      <c r="E68" s="61">
         <v>3.71</v>
       </c>
-      <c r="F68" s="63"/>
+      <c r="F68" s="62"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="63"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="63"/>
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
-      <c r="F69" s="63"/>
+      <c r="A69" s="62"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="63"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="63"/>
-      <c r="D70" s="63"/>
-      <c r="E70" s="63"/>
-      <c r="F70" s="63"/>
-      <c r="G70" s="63"/>
-      <c r="H70" s="63"/>
-      <c r="I70" s="63"/>
+      <c r="A70" s="62"/>
+      <c r="B70" s="63"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="62"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="62"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="62"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="63"/>
-      <c r="B71" s="64"/>
-      <c r="C71" s="63"/>
-      <c r="D71" s="63"/>
-      <c r="E71" s="63"/>
-      <c r="F71" s="63"/>
-      <c r="G71" s="63"/>
-      <c r="H71" s="63"/>
-      <c r="I71" s="63"/>
+      <c r="A71" s="62"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="62"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="62"/>
+      <c r="G71" s="62"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="62"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F72" s="63"/>
-      <c r="G72" s="63"/>
-      <c r="H72" s="63"/>
-      <c r="I72" s="63"/>
+      <c r="F72" s="62"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="62"/>
+      <c r="I72" s="62"/>
     </row>
     <row r="73" spans="1:9">
       <c r="C73" s="7" t="s">
@@ -4130,371 +4180,371 @@
       <c r="E73" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F73" s="63"/>
-      <c r="G73" s="63"/>
-      <c r="H73" s="63"/>
-      <c r="I73" s="63"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="62"/>
     </row>
     <row r="74" spans="1:9">
       <c r="B74" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C74" s="67">
+      <c r="C74" s="66">
         <v>0.95</v>
       </c>
-      <c r="D74" s="67">
+      <c r="D74" s="66">
         <v>0.8</v>
       </c>
-      <c r="E74" s="67">
+      <c r="E74" s="66">
         <v>0.98</v>
       </c>
-      <c r="F74" s="63"/>
-      <c r="G74" s="68"/>
-      <c r="H74" s="68"/>
-      <c r="I74" s="68"/>
+      <c r="F74" s="62"/>
+      <c r="G74" s="67"/>
+      <c r="H74" s="67"/>
+      <c r="I74" s="67"/>
     </row>
     <row r="75" spans="1:9">
       <c r="B75" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C75" s="67">
+      <c r="C75" s="66">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D75" s="67">
+      <c r="D75" s="66">
         <v>0.47</v>
       </c>
-      <c r="E75" s="67">
+      <c r="E75" s="66">
         <v>0.67</v>
       </c>
-      <c r="F75" s="63"/>
-      <c r="G75" s="68"/>
-      <c r="H75" s="68"/>
-      <c r="I75" s="68"/>
+      <c r="F75" s="62"/>
+      <c r="G75" s="67"/>
+      <c r="H75" s="67"/>
+      <c r="I75" s="67"/>
     </row>
     <row r="76" spans="1:9">
       <c r="B76" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C76" s="67">
+      <c r="C76" s="66">
         <v>0</v>
       </c>
-      <c r="D76" s="67">
+      <c r="D76" s="66">
         <v>0</v>
       </c>
-      <c r="E76" s="67">
+      <c r="E76" s="66">
         <v>0.68</v>
       </c>
-      <c r="F76" s="63"/>
+      <c r="F76" s="62"/>
     </row>
     <row r="77" spans="1:9">
       <c r="B77" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C77" s="67">
+      <c r="C77" s="66">
         <v>2.65</v>
       </c>
-      <c r="D77" s="67">
+      <c r="D77" s="66">
         <v>1.35</v>
       </c>
-      <c r="E77" s="67">
+      <c r="E77" s="66">
         <v>5.19</v>
       </c>
-      <c r="F77" s="63"/>
-      <c r="G77" s="68"/>
-      <c r="H77" s="68"/>
-      <c r="I77" s="68"/>
+      <c r="F77" s="62"/>
+      <c r="G77" s="67"/>
+      <c r="H77" s="67"/>
+      <c r="I77" s="67"/>
     </row>
     <row r="78" spans="1:9">
       <c r="B78" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C78" s="67">
+      <c r="C78" s="66">
         <v>0.54</v>
       </c>
-      <c r="D78" s="67">
+      <c r="D78" s="66">
         <v>0.33</v>
       </c>
-      <c r="E78" s="67">
+      <c r="E78" s="66">
         <v>0.68</v>
       </c>
-      <c r="F78" s="63"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="68"/>
-      <c r="I78" s="68"/>
+      <c r="F78" s="62"/>
+      <c r="G78" s="67"/>
+      <c r="H78" s="67"/>
+      <c r="I78" s="67"/>
     </row>
     <row r="79" spans="1:9">
       <c r="B79" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C79" s="67">
+      <c r="C79" s="66">
         <v>0.9</v>
       </c>
-      <c r="D79" s="67">
+      <c r="D79" s="66">
         <v>0.82</v>
       </c>
-      <c r="E79" s="67">
+      <c r="E79" s="66">
         <v>0.93</v>
       </c>
-      <c r="F79" s="63"/>
-      <c r="G79" s="68"/>
-      <c r="H79" s="68"/>
-      <c r="I79" s="68"/>
+      <c r="F79" s="62"/>
+      <c r="G79" s="67"/>
+      <c r="H79" s="67"/>
+      <c r="I79" s="67"/>
     </row>
     <row r="80" spans="1:9">
       <c r="B80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="67">
+      <c r="C80" s="66">
         <v>0.73</v>
       </c>
-      <c r="D80" s="67">
+      <c r="D80" s="66">
         <v>0.65</v>
       </c>
-      <c r="E80" s="67">
+      <c r="E80" s="66">
         <v>0.8</v>
       </c>
-      <c r="F80" s="63"/>
-      <c r="G80" s="68"/>
-      <c r="H80" s="68"/>
-      <c r="I80" s="68"/>
+      <c r="F80" s="62"/>
+      <c r="G80" s="67"/>
+      <c r="H80" s="67"/>
+      <c r="I80" s="67"/>
     </row>
     <row r="81" spans="1:9">
       <c r="B81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="67">
+      <c r="C81" s="66">
         <v>0.5</v>
       </c>
-      <c r="D81" s="67">
+      <c r="D81" s="66">
         <v>0.3</v>
       </c>
-      <c r="E81" s="67">
+      <c r="E81" s="66">
         <v>0.8</v>
       </c>
-      <c r="F81" s="63"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
-      <c r="I81" s="68"/>
+      <c r="F81" s="62"/>
+      <c r="G81" s="67"/>
+      <c r="H81" s="67"/>
+      <c r="I81" s="67"/>
     </row>
     <row r="82" spans="1:9">
       <c r="B82" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C82" s="67">
+      <c r="C82" s="66">
         <v>0.92</v>
       </c>
-      <c r="D82" s="67">
+      <c r="D82" s="66">
         <v>0.8</v>
       </c>
-      <c r="E82" s="67">
+      <c r="E82" s="66">
         <v>0.95</v>
       </c>
-      <c r="F82" s="63"/>
-      <c r="G82" s="63"/>
-      <c r="H82" s="63"/>
-      <c r="I82" s="63"/>
+      <c r="F82" s="62"/>
+      <c r="G82" s="62"/>
+      <c r="H82" s="62"/>
+      <c r="I82" s="62"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="63"/>
-      <c r="B83" s="64"/>
-      <c r="C83" s="63"/>
-      <c r="D83" s="63"/>
-      <c r="E83" s="63"/>
-      <c r="F83" s="63"/>
-      <c r="G83" s="63"/>
-      <c r="H83" s="63"/>
-      <c r="I83" s="63"/>
+      <c r="A83" s="62"/>
+      <c r="B83" s="63"/>
+      <c r="C83" s="62"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="62"/>
+      <c r="F83" s="62"/>
+      <c r="G83" s="62"/>
+      <c r="H83" s="62"/>
+      <c r="I83" s="62"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="69"/>
-      <c r="B84" s="70"/>
-      <c r="C84" s="71"/>
-      <c r="D84" s="71"/>
-      <c r="E84" s="71"/>
-      <c r="F84" s="71"/>
-      <c r="G84" s="71"/>
-      <c r="H84" s="71"/>
-      <c r="I84" s="63"/>
+      <c r="A84" s="68"/>
+      <c r="B84" s="69"/>
+      <c r="C84" s="70"/>
+      <c r="D84" s="70"/>
+      <c r="E84" s="70"/>
+      <c r="F84" s="70"/>
+      <c r="G84" s="70"/>
+      <c r="H84" s="70"/>
+      <c r="I84" s="62"/>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="71"/>
-      <c r="B85" s="70"/>
-      <c r="C85" s="72"/>
-      <c r="D85" s="72"/>
-      <c r="E85" s="72"/>
-      <c r="F85" s="71"/>
-      <c r="G85" s="71"/>
-      <c r="H85" s="71"/>
-      <c r="I85" s="63"/>
+      <c r="A85" s="70"/>
+      <c r="B85" s="69"/>
+      <c r="C85" s="71"/>
+      <c r="D85" s="71"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="70"/>
+      <c r="G85" s="70"/>
+      <c r="H85" s="70"/>
+      <c r="I85" s="62"/>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="52" t="s">
+      <c r="A86" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="B86" s="49"/>
-      <c r="C86" s="49"/>
-      <c r="D86" s="49"/>
-      <c r="E86" s="49"/>
-      <c r="F86" s="49"/>
-      <c r="G86" s="49"/>
-      <c r="H86" s="49"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="48"/>
+      <c r="D86" s="48"/>
+      <c r="E86" s="48"/>
+      <c r="F86" s="48"/>
+      <c r="G86" s="48"/>
+      <c r="H86" s="48"/>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="49"/>
-      <c r="B87" s="49"/>
-      <c r="C87" s="53" t="s">
+      <c r="A87" s="48"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="53" t="s">
+      <c r="D87" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E87" s="53" t="s">
+      <c r="E87" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F87" s="49"/>
-      <c r="G87" s="49"/>
-      <c r="H87" s="49"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="48"/>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="49"/>
-      <c r="B88" s="54" t="s">
+      <c r="A88" s="48"/>
+      <c r="B88" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="C88" s="65">
+      <c r="C88" s="64">
         <v>0.14599999999999999</v>
       </c>
-      <c r="D88" s="65">
+      <c r="D88" s="64">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="E88" s="65">
+      <c r="E88" s="64">
         <v>0.20499999999999999</v>
       </c>
-      <c r="F88" s="49"/>
-      <c r="G88" s="49"/>
-      <c r="H88" s="49"/>
+      <c r="F88" s="48"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="48"/>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="49"/>
-      <c r="B89" s="54" t="s">
+      <c r="A89" s="48"/>
+      <c r="B89" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C89" s="65">
+      <c r="C89" s="64">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D89" s="65">
+      <c r="D89" s="64">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E89" s="65">
+      <c r="E89" s="64">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F89" s="49"/>
-      <c r="G89" s="49"/>
-      <c r="H89" s="49"/>
+      <c r="F89" s="48"/>
+      <c r="G89" s="48"/>
+      <c r="H89" s="48"/>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="49"/>
-      <c r="B90" s="54" t="s">
+      <c r="A90" s="48"/>
+      <c r="B90" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="C90" s="65">
+      <c r="C90" s="64">
         <v>0.02</v>
       </c>
-      <c r="D90" s="65">
+      <c r="D90" s="64">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E90" s="65">
+      <c r="E90" s="64">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F90" s="49"/>
-      <c r="G90" s="49"/>
-      <c r="H90" s="49"/>
+      <c r="F90" s="48"/>
+      <c r="G90" s="48"/>
+      <c r="H90" s="48"/>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="49"/>
-      <c r="B91" s="54" t="s">
+      <c r="A91" s="48"/>
+      <c r="B91" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="C91" s="65">
+      <c r="C91" s="64">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D91" s="65">
+      <c r="D91" s="64">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E91" s="65">
+      <c r="E91" s="64">
         <v>9.4E-2</v>
       </c>
-      <c r="F91" s="49"/>
-      <c r="G91" s="49"/>
-      <c r="H91" s="49"/>
+      <c r="F91" s="48"/>
+      <c r="G91" s="48"/>
+      <c r="H91" s="48"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="49"/>
-      <c r="B92" s="54" t="s">
+      <c r="A92" s="48"/>
+      <c r="B92" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="C92" s="65">
+      <c r="C92" s="64">
         <v>0.26500000000000001</v>
       </c>
-      <c r="D92" s="65">
+      <c r="D92" s="64">
         <v>0.114</v>
       </c>
-      <c r="E92" s="65">
+      <c r="E92" s="64">
         <v>0.47399999999999998</v>
       </c>
-      <c r="F92" s="49"/>
-      <c r="G92" s="49"/>
-      <c r="H92" s="49"/>
+      <c r="F92" s="48"/>
+      <c r="G92" s="48"/>
+      <c r="H92" s="48"/>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="49"/>
-      <c r="B93" s="54" t="s">
+      <c r="A93" s="48"/>
+      <c r="B93" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="C93" s="65">
+      <c r="C93" s="64">
         <v>0.54700000000000004</v>
       </c>
-      <c r="D93" s="65">
+      <c r="D93" s="64">
         <v>0.38200000000000001</v>
       </c>
-      <c r="E93" s="65">
+      <c r="E93" s="64">
         <v>0.71499999999999997</v>
       </c>
-      <c r="F93" s="49"/>
-      <c r="G93" s="49"/>
-      <c r="H93" s="49"/>
+      <c r="F93" s="48"/>
+      <c r="G93" s="48"/>
+      <c r="H93" s="48"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="49"/>
-      <c r="B94" s="54" t="s">
+      <c r="A94" s="48"/>
+      <c r="B94" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C94" s="65">
+      <c r="C94" s="64">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D94" s="65">
+      <c r="D94" s="64">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E94" s="65">
+      <c r="E94" s="64">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F94" s="49"/>
-      <c r="G94" s="49"/>
-      <c r="H94" s="49"/>
+      <c r="F94" s="48"/>
+      <c r="G94" s="48"/>
+      <c r="H94" s="48"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="F95" s="49"/>
-      <c r="G95" s="49"/>
-      <c r="H95" s="49"/>
+      <c r="F95" s="48"/>
+      <c r="G95" s="48"/>
+      <c r="H95" s="48"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="F96" s="49"/>
-      <c r="G96" s="49"/>
-      <c r="H96" s="49"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="48"/>
+      <c r="H96" s="48"/>
     </row>
     <row r="97" spans="6:8">
-      <c r="F97" s="49"/>
-      <c r="G97" s="49"/>
-      <c r="H97" s="49"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="48"/>
+      <c r="H97" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -8434,10 +8484,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD71"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="O69" sqref="O69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9031,7 +9081,7 @@
       </c>
       <c r="Y27" s="39"/>
     </row>
-    <row r="29" spans="1:25" s="48" customFormat="1"/>
+    <row r="29" spans="1:25" s="47" customFormat="1"/>
     <row r="31" spans="1:25">
       <c r="A31" s="2" t="s">
         <v>54</v>
@@ -9274,32 +9324,545 @@
       </c>
       <c r="Y39" s="27"/>
     </row>
-    <row r="40" spans="1:25">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="41"/>
-      <c r="M40" s="41"/>
-      <c r="N40" s="41"/>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="41"/>
-      <c r="S40" s="41"/>
-      <c r="T40" s="41"/>
-      <c r="U40" s="41"/>
-      <c r="V40" s="41"/>
-      <c r="W40" s="41"/>
-      <c r="X40" s="41"/>
-      <c r="Y40" s="41"/>
+    <row r="40" spans="1:25" s="47" customFormat="1"/>
+    <row r="41" spans="1:25" s="47" customFormat="1"/>
+    <row r="42" spans="1:25" s="47" customFormat="1"/>
+    <row r="43" spans="1:25" s="47" customFormat="1">
+      <c r="A43" s="73" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" s="47" customFormat="1">
+      <c r="C44" s="74">
+        <v>2000</v>
+      </c>
+      <c r="D44" s="74">
+        <v>2001</v>
+      </c>
+      <c r="E44" s="74">
+        <v>2002</v>
+      </c>
+      <c r="F44" s="74">
+        <v>2003</v>
+      </c>
+      <c r="G44" s="74">
+        <v>2004</v>
+      </c>
+      <c r="H44" s="74">
+        <v>2005</v>
+      </c>
+      <c r="I44" s="74">
+        <v>2006</v>
+      </c>
+      <c r="J44" s="74">
+        <v>2007</v>
+      </c>
+      <c r="K44" s="74">
+        <v>2008</v>
+      </c>
+      <c r="L44" s="74">
+        <v>2009</v>
+      </c>
+      <c r="M44" s="74">
+        <v>2010</v>
+      </c>
+      <c r="N44" s="74">
+        <v>2011</v>
+      </c>
+      <c r="O44" s="74">
+        <v>2012</v>
+      </c>
+      <c r="P44" s="74">
+        <v>2013</v>
+      </c>
+      <c r="Q44" s="74">
+        <v>2014</v>
+      </c>
+      <c r="R44" s="74">
+        <v>2015</v>
+      </c>
+      <c r="S44" s="74">
+        <v>2016</v>
+      </c>
+      <c r="T44" s="74">
+        <v>2017</v>
+      </c>
+      <c r="U44" s="74">
+        <v>2018</v>
+      </c>
+      <c r="V44" s="74">
+        <v>2019</v>
+      </c>
+      <c r="W44" s="74">
+        <v>2020</v>
+      </c>
+      <c r="Y44" s="74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" s="47" customFormat="1">
+      <c r="B45" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="76">
+        <v>0.62</v>
+      </c>
+      <c r="P45" s="76"/>
+      <c r="Q45" s="76"/>
+      <c r="R45" s="76"/>
+      <c r="S45" s="76"/>
+      <c r="T45" s="76"/>
+      <c r="U45" s="76"/>
+      <c r="V45" s="76"/>
+      <c r="W45" s="76"/>
+      <c r="X45" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y45" s="76"/>
+    </row>
+    <row r="46" spans="1:25" s="47" customFormat="1"/>
+    <row r="47" spans="1:25" s="47" customFormat="1"/>
+    <row r="48" spans="1:25" s="47" customFormat="1"/>
+    <row r="49" spans="1:25" s="47" customFormat="1">
+      <c r="A49" s="73" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" s="47" customFormat="1">
+      <c r="C50" s="74">
+        <v>2000</v>
+      </c>
+      <c r="D50" s="74">
+        <v>2001</v>
+      </c>
+      <c r="E50" s="74">
+        <v>2002</v>
+      </c>
+      <c r="F50" s="74">
+        <v>2003</v>
+      </c>
+      <c r="G50" s="74">
+        <v>2004</v>
+      </c>
+      <c r="H50" s="74">
+        <v>2005</v>
+      </c>
+      <c r="I50" s="74">
+        <v>2006</v>
+      </c>
+      <c r="J50" s="74">
+        <v>2007</v>
+      </c>
+      <c r="K50" s="74">
+        <v>2008</v>
+      </c>
+      <c r="L50" s="74">
+        <v>2009</v>
+      </c>
+      <c r="M50" s="74">
+        <v>2010</v>
+      </c>
+      <c r="N50" s="74">
+        <v>2011</v>
+      </c>
+      <c r="O50" s="74">
+        <v>2012</v>
+      </c>
+      <c r="P50" s="74">
+        <v>2013</v>
+      </c>
+      <c r="Q50" s="74">
+        <v>2014</v>
+      </c>
+      <c r="R50" s="74">
+        <v>2015</v>
+      </c>
+      <c r="S50" s="74">
+        <v>2016</v>
+      </c>
+      <c r="T50" s="74">
+        <v>2017</v>
+      </c>
+      <c r="U50" s="74">
+        <v>2018</v>
+      </c>
+      <c r="V50" s="74">
+        <v>2019</v>
+      </c>
+      <c r="W50" s="74">
+        <v>2020</v>
+      </c>
+      <c r="Y50" s="74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" s="47" customFormat="1">
+      <c r="B51" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="76"/>
+      <c r="M51" s="76"/>
+      <c r="N51" s="76"/>
+      <c r="O51" s="76">
+        <v>0.7</v>
+      </c>
+      <c r="P51" s="76"/>
+      <c r="Q51" s="76"/>
+      <c r="R51" s="76"/>
+      <c r="S51" s="76"/>
+      <c r="T51" s="76"/>
+      <c r="U51" s="76"/>
+      <c r="V51" s="76"/>
+      <c r="W51" s="76"/>
+      <c r="X51" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y51" s="76"/>
+    </row>
+    <row r="52" spans="1:25" s="47" customFormat="1"/>
+    <row r="53" spans="1:25" s="47" customFormat="1"/>
+    <row r="54" spans="1:25" s="47" customFormat="1"/>
+    <row r="55" spans="1:25" s="47" customFormat="1">
+      <c r="A55" s="73" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" s="47" customFormat="1">
+      <c r="C56" s="74">
+        <v>2000</v>
+      </c>
+      <c r="D56" s="74">
+        <v>2001</v>
+      </c>
+      <c r="E56" s="74">
+        <v>2002</v>
+      </c>
+      <c r="F56" s="74">
+        <v>2003</v>
+      </c>
+      <c r="G56" s="74">
+        <v>2004</v>
+      </c>
+      <c r="H56" s="74">
+        <v>2005</v>
+      </c>
+      <c r="I56" s="74">
+        <v>2006</v>
+      </c>
+      <c r="J56" s="74">
+        <v>2007</v>
+      </c>
+      <c r="K56" s="74">
+        <v>2008</v>
+      </c>
+      <c r="L56" s="74">
+        <v>2009</v>
+      </c>
+      <c r="M56" s="74">
+        <v>2010</v>
+      </c>
+      <c r="N56" s="74">
+        <v>2011</v>
+      </c>
+      <c r="O56" s="74">
+        <v>2012</v>
+      </c>
+      <c r="P56" s="74">
+        <v>2013</v>
+      </c>
+      <c r="Q56" s="74">
+        <v>2014</v>
+      </c>
+      <c r="R56" s="74">
+        <v>2015</v>
+      </c>
+      <c r="S56" s="74">
+        <v>2016</v>
+      </c>
+      <c r="T56" s="74">
+        <v>2017</v>
+      </c>
+      <c r="U56" s="74">
+        <v>2018</v>
+      </c>
+      <c r="V56" s="74">
+        <v>2019</v>
+      </c>
+      <c r="W56" s="74">
+        <v>2020</v>
+      </c>
+      <c r="Y56" s="74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" s="47" customFormat="1">
+      <c r="B57" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="76"/>
+      <c r="O57" s="76">
+        <v>0.69</v>
+      </c>
+      <c r="P57" s="76"/>
+      <c r="Q57" s="76"/>
+      <c r="R57" s="76"/>
+      <c r="S57" s="76"/>
+      <c r="T57" s="76"/>
+      <c r="U57" s="76"/>
+      <c r="V57" s="76"/>
+      <c r="W57" s="76"/>
+      <c r="X57" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y57" s="76"/>
+    </row>
+    <row r="58" spans="1:25" s="47" customFormat="1"/>
+    <row r="59" spans="1:25" s="47" customFormat="1"/>
+    <row r="60" spans="1:25" s="47" customFormat="1"/>
+    <row r="61" spans="1:25" s="47" customFormat="1">
+      <c r="A61" s="73" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" s="47" customFormat="1">
+      <c r="C62" s="74">
+        <v>2000</v>
+      </c>
+      <c r="D62" s="74">
+        <v>2001</v>
+      </c>
+      <c r="E62" s="74">
+        <v>2002</v>
+      </c>
+      <c r="F62" s="74">
+        <v>2003</v>
+      </c>
+      <c r="G62" s="74">
+        <v>2004</v>
+      </c>
+      <c r="H62" s="74">
+        <v>2005</v>
+      </c>
+      <c r="I62" s="74">
+        <v>2006</v>
+      </c>
+      <c r="J62" s="74">
+        <v>2007</v>
+      </c>
+      <c r="K62" s="74">
+        <v>2008</v>
+      </c>
+      <c r="L62" s="74">
+        <v>2009</v>
+      </c>
+      <c r="M62" s="74">
+        <v>2010</v>
+      </c>
+      <c r="N62" s="74">
+        <v>2011</v>
+      </c>
+      <c r="O62" s="74">
+        <v>2012</v>
+      </c>
+      <c r="P62" s="74">
+        <v>2013</v>
+      </c>
+      <c r="Q62" s="74">
+        <v>2014</v>
+      </c>
+      <c r="R62" s="74">
+        <v>2015</v>
+      </c>
+      <c r="S62" s="74">
+        <v>2016</v>
+      </c>
+      <c r="T62" s="74">
+        <v>2017</v>
+      </c>
+      <c r="U62" s="74">
+        <v>2018</v>
+      </c>
+      <c r="V62" s="74">
+        <v>2019</v>
+      </c>
+      <c r="W62" s="74">
+        <v>2020</v>
+      </c>
+      <c r="Y62" s="74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" s="47" customFormat="1">
+      <c r="B63" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="76"/>
+      <c r="J63" s="76"/>
+      <c r="K63" s="76"/>
+      <c r="L63" s="76"/>
+      <c r="M63" s="76"/>
+      <c r="N63" s="76"/>
+      <c r="O63" s="76">
+        <v>0.8</v>
+      </c>
+      <c r="P63" s="76"/>
+      <c r="Q63" s="76"/>
+      <c r="R63" s="76"/>
+      <c r="S63" s="76"/>
+      <c r="T63" s="76"/>
+      <c r="U63" s="76"/>
+      <c r="V63" s="76"/>
+      <c r="W63" s="76"/>
+      <c r="X63" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y63" s="76"/>
+    </row>
+    <row r="64" spans="1:25" s="47" customFormat="1"/>
+    <row r="65" spans="1:25" s="47" customFormat="1"/>
+    <row r="66" spans="1:25" s="47" customFormat="1"/>
+    <row r="67" spans="1:25" s="47" customFormat="1">
+      <c r="A67" s="73" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" s="47" customFormat="1">
+      <c r="C68" s="74">
+        <v>2000</v>
+      </c>
+      <c r="D68" s="74">
+        <v>2001</v>
+      </c>
+      <c r="E68" s="74">
+        <v>2002</v>
+      </c>
+      <c r="F68" s="74">
+        <v>2003</v>
+      </c>
+      <c r="G68" s="74">
+        <v>2004</v>
+      </c>
+      <c r="H68" s="74">
+        <v>2005</v>
+      </c>
+      <c r="I68" s="74">
+        <v>2006</v>
+      </c>
+      <c r="J68" s="74">
+        <v>2007</v>
+      </c>
+      <c r="K68" s="74">
+        <v>2008</v>
+      </c>
+      <c r="L68" s="74">
+        <v>2009</v>
+      </c>
+      <c r="M68" s="74">
+        <v>2010</v>
+      </c>
+      <c r="N68" s="74">
+        <v>2011</v>
+      </c>
+      <c r="O68" s="74">
+        <v>2012</v>
+      </c>
+      <c r="P68" s="74">
+        <v>2013</v>
+      </c>
+      <c r="Q68" s="74">
+        <v>2014</v>
+      </c>
+      <c r="R68" s="74">
+        <v>2015</v>
+      </c>
+      <c r="S68" s="74">
+        <v>2016</v>
+      </c>
+      <c r="T68" s="74">
+        <v>2017</v>
+      </c>
+      <c r="U68" s="74">
+        <v>2018</v>
+      </c>
+      <c r="V68" s="74">
+        <v>2019</v>
+      </c>
+      <c r="W68" s="74">
+        <v>2020</v>
+      </c>
+      <c r="Y68" s="74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" s="47" customFormat="1">
+      <c r="B69" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="76"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="76"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="76"/>
+      <c r="L69" s="76"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="76"/>
+      <c r="O69" s="76">
+        <v>0.65</v>
+      </c>
+      <c r="P69" s="76"/>
+      <c r="Q69" s="76"/>
+      <c r="R69" s="76"/>
+      <c r="S69" s="76"/>
+      <c r="T69" s="76"/>
+      <c r="U69" s="76"/>
+      <c r="V69" s="76"/>
+      <c r="W69" s="76"/>
+      <c r="X69" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y69" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -9426,7 +9989,7 @@
       <c r="X3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="73">
+      <c r="Y3" s="72">
         <v>1</v>
       </c>
     </row>
@@ -9460,7 +10023,7 @@
       <c r="X4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y4" s="73">
+      <c r="Y4" s="72">
         <v>1</v>
       </c>
     </row>
@@ -9493,7 +10056,7 @@
       <c r="X5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y5" s="73">
+      <c r="Y5" s="72">
         <v>1</v>
       </c>
     </row>
@@ -9525,7 +10088,7 @@
       <c r="X6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y6" s="73">
+      <c r="Y6" s="72">
         <v>1</v>
       </c>
     </row>
@@ -9559,7 +10122,7 @@
       <c r="X7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y7" s="73">
+      <c r="Y7" s="72">
         <v>1</v>
       </c>
     </row>
@@ -9593,7 +10156,7 @@
       <c r="X8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y8" s="73">
+      <c r="Y8" s="72">
         <v>1</v>
       </c>
     </row>
@@ -9678,31 +10241,31 @@
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="42"/>
-      <c r="V14" s="42"/>
-      <c r="W14" s="42"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
       <c r="X14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y14" s="42">
+      <c r="Y14" s="41">
         <v>0.2</v>
       </c>
     </row>
@@ -9711,31 +10274,31 @@
         <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="42"/>
-      <c r="V15" s="42"/>
-      <c r="W15" s="42"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="41"/>
+      <c r="W15" s="41"/>
       <c r="X15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y15" s="42">
+      <c r="Y15" s="41">
         <v>0.2</v>
       </c>
     </row>
@@ -9744,31 +10307,31 @@
         <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="42"/>
-      <c r="V16" s="42"/>
-      <c r="W16" s="42"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
       <c r="X16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y16" s="42">
+      <c r="Y16" s="41">
         <v>0.2</v>
       </c>
     </row>
@@ -9776,31 +10339,31 @@
       <c r="B17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
-      <c r="U17" s="42"/>
-      <c r="V17" s="42"/>
-      <c r="W17" s="42"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
       <c r="X17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y17" s="42">
+      <c r="Y17" s="41">
         <v>0.2</v>
       </c>
     </row>
@@ -9809,31 +10372,31 @@
         <f>Populations!$C$7</f>
         <v>M 15+</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
-      <c r="U18" s="42"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="42"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
       <c r="X18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y18" s="42">
+      <c r="Y18" s="41">
         <v>0.2</v>
       </c>
     </row>
@@ -9842,31 +10405,31 @@
         <f>Populations!$C$8</f>
         <v>F 15+</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="42"/>
-      <c r="V19" s="42"/>
-      <c r="W19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
       <c r="X19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="Y19" s="42">
+      <c r="Y19" s="41">
         <v>0.2</v>
       </c>
     </row>
@@ -9975,31 +10538,31 @@
       <c r="B25" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="43"/>
-      <c r="T25" s="43"/>
-      <c r="U25" s="43"/>
-      <c r="V25" s="43"/>
-      <c r="W25" s="43"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="42"/>
       <c r="X25" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="Y25" s="44">
+      <c r="Y25" s="43">
         <v>1</v>
       </c>
     </row>
@@ -11023,7 +11586,7 @@
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
-      <c r="P39" s="45">
+      <c r="P39" s="44">
         <v>1E-3</v>
       </c>
       <c r="Q39" s="22"/>
@@ -11191,10 +11754,10 @@
       <c r="I47" s="22"/>
       <c r="J47" s="22"/>
       <c r="K47" s="22"/>
-      <c r="L47" s="46">
+      <c r="L47" s="45">
         <v>0.8</v>
       </c>
-      <c r="M47" s="46"/>
+      <c r="M47" s="45"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
       <c r="P47" s="22"/>
@@ -11293,8 +11856,8 @@
       <c r="I50" s="22"/>
       <c r="J50" s="22"/>
       <c r="K50" s="22"/>
-      <c r="L50" s="47"/>
-      <c r="M50" s="47"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="46"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
       <c r="P50" s="22">

</xml_diff>

<commit_message>
remove numcirc from spreadsheet
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="132">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>Percentage of males who have been circumcised</t>
-  </si>
-  <si>
-    <t>Number of voluntary medical male circumcisions performed</t>
   </si>
   <si>
     <t>Average number of injections per person per year</t>
@@ -1926,7 +1923,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -2196,7 +2193,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2466,7 +2463,7 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2592,7 +2589,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2707,7 +2704,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2822,7 +2819,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2927,7 +2924,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -3032,7 +3029,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3087,7 +3084,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3190,7 +3187,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3323,7 +3320,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
@@ -3346,7 +3343,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="55"/>
       <c r="B3" s="58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="61">
         <v>4.0000000000000002E-4</v>
@@ -3361,7 +3358,7 @@
     <row r="4" spans="1:5">
       <c r="A4" s="55"/>
       <c r="B4" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="61">
         <v>8.0000000000000004E-4</v>
@@ -3376,7 +3373,7 @@
     <row r="5" spans="1:5">
       <c r="A5" s="55"/>
       <c r="B5" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="61">
         <v>1.1000000000000001E-3</v>
@@ -3391,7 +3388,7 @@
     <row r="6" spans="1:5">
       <c r="A6" s="55"/>
       <c r="B6" s="58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="61">
         <v>1.38E-2</v>
@@ -3406,7 +3403,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="55"/>
       <c r="B7" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="61">
         <v>8.0000000000000002E-3</v>
@@ -3421,7 +3418,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="55"/>
       <c r="B8" s="58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="61">
         <v>0.36699999999999999</v>
@@ -3436,7 +3433,7 @@
     <row r="9" spans="1:5">
       <c r="A9" s="55"/>
       <c r="B9" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="61">
         <v>0.20499999999999999</v>
@@ -3471,7 +3468,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3487,7 +3484,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="64">
         <v>5.6</v>
@@ -3501,7 +3498,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="64">
         <v>1</v>
@@ -3515,7 +3512,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="B17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="64">
         <v>1</v>
@@ -3529,7 +3526,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="64">
         <v>1</v>
@@ -3543,7 +3540,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="B19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="64">
         <v>3.49</v>
@@ -3557,7 +3554,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="B20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="64">
         <v>7.17</v>
@@ -3592,7 +3589,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3608,7 +3605,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="64">
         <v>0.24</v>
@@ -3622,7 +3619,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="B27" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="64">
         <v>0.95</v>
@@ -3637,7 +3634,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="B28" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="64">
         <v>3</v>
@@ -3651,7 +3648,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" s="64">
         <v>3.74</v>
@@ -3665,7 +3662,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="B30" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C30" s="64">
         <v>1.5</v>
@@ -3700,7 +3697,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3716,7 +3713,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="B36" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="64">
         <v>2.2000000000000002</v>
@@ -3730,7 +3727,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37" s="64">
         <v>1.42</v>
@@ -3744,7 +3741,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="64">
         <v>2.14</v>
@@ -3758,7 +3755,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="B39" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C39" s="64">
         <v>0.66</v>
@@ -3773,7 +3770,7 @@
     <row r="40" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A40" s="54"/>
       <c r="B40" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" s="64">
         <v>0.2</v>
@@ -3808,7 +3805,7 @@
     </row>
     <row r="44" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A44" s="49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44" s="54"/>
       <c r="C44" s="54"/>
@@ -3831,7 +3828,7 @@
     <row r="46" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A46" s="54"/>
       <c r="B46" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="61">
         <v>2.5999999999999999E-2</v>
@@ -3846,7 +3843,7 @@
     <row r="47" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A47" s="54"/>
       <c r="B47" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47" s="61">
         <v>0.15</v>
@@ -3861,7 +3858,7 @@
     <row r="48" spans="1:5" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A48" s="54"/>
       <c r="B48" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C48" s="61">
         <v>0.1</v>
@@ -3876,7 +3873,7 @@
     <row r="49" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A49" s="54"/>
       <c r="B49" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" s="61">
         <v>5.2999999999999999E-2</v>
@@ -3891,7 +3888,7 @@
     <row r="50" spans="1:6" s="59" customFormat="1">
       <c r="A50" s="54"/>
       <c r="B50" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50" s="61">
         <v>0.16200000000000001</v>
@@ -3906,7 +3903,7 @@
     <row r="51" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A51" s="54"/>
       <c r="B51" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51" s="61">
         <v>0.11700000000000001</v>
@@ -3921,7 +3918,7 @@
     <row r="52" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A52" s="54"/>
       <c r="B52" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C52" s="61">
         <v>0.09</v>
@@ -3936,7 +3933,7 @@
     <row r="53" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A53" s="54"/>
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" s="61">
         <v>0.111</v>
@@ -3951,7 +3948,7 @@
     <row r="54" spans="1:6" s="59" customFormat="1" ht="13.5" customHeight="1">
       <c r="A54" s="54"/>
       <c r="B54" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C54" s="61">
         <v>0.16</v>
@@ -3986,7 +3983,7 @@
     </row>
     <row r="58" spans="1:6" ht="13.5" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="13.5" customHeight="1">
@@ -4002,7 +3999,7 @@
     </row>
     <row r="60" spans="1:6" ht="13.5" customHeight="1">
       <c r="B60" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" s="61">
         <v>3.5999999999999999E-3</v>
@@ -4016,7 +4013,7 @@
     </row>
     <row r="61" spans="1:6" ht="13.5" customHeight="1">
       <c r="B61" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C61" s="61">
         <v>3.5999999999999999E-3</v>
@@ -4030,7 +4027,7 @@
     </row>
     <row r="62" spans="1:6" ht="13.5" customHeight="1">
       <c r="B62" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" s="61">
         <v>5.7999999999999996E-3</v>
@@ -4044,7 +4041,7 @@
     </row>
     <row r="63" spans="1:6" ht="13.5" customHeight="1">
       <c r="B63" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="61">
         <v>8.8000000000000005E-3</v>
@@ -4058,7 +4055,7 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="B64" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C64" s="61">
         <v>5.8999999999999997E-2</v>
@@ -4073,7 +4070,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="B65" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C65" s="61">
         <v>0.32300000000000001</v>
@@ -4088,7 +4085,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C66" s="61">
         <v>0.23</v>
@@ -4103,7 +4100,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="B67" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C67" s="61">
         <v>0.48780000000000001</v>
@@ -4118,7 +4115,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="B68" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C68" s="61">
         <v>2.17</v>
@@ -4163,7 +4160,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F72" s="62"/>
       <c r="G72" s="62"/>
@@ -4187,7 +4184,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="B74" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C74" s="66">
         <v>0.95</v>
@@ -4205,7 +4202,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="B75" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C75" s="66">
         <v>0.57999999999999996</v>
@@ -4223,7 +4220,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="B76" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C76" s="66">
         <v>0</v>
@@ -4238,7 +4235,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="B77" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C77" s="66">
         <v>2.65</v>
@@ -4256,7 +4253,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="B78" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C78" s="66">
         <v>0.54</v>
@@ -4274,7 +4271,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="B79" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C79" s="66">
         <v>0.9</v>
@@ -4292,7 +4289,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="B80" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C80" s="66">
         <v>0.73</v>
@@ -4310,7 +4307,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="B81" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C81" s="66">
         <v>0.5</v>
@@ -4328,7 +4325,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="B82" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C82" s="66">
         <v>0.92</v>
@@ -4379,7 +4376,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86" s="48"/>
       <c r="C86" s="48"/>
@@ -4408,7 +4405,7 @@
     <row r="88" spans="1:9">
       <c r="A88" s="48"/>
       <c r="B88" s="53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C88" s="64">
         <v>0.14599999999999999</v>
@@ -4426,7 +4423,7 @@
     <row r="89" spans="1:9">
       <c r="A89" s="48"/>
       <c r="B89" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C89" s="64">
         <v>8.0000000000000002E-3</v>
@@ -4444,7 +4441,7 @@
     <row r="90" spans="1:9">
       <c r="A90" s="48"/>
       <c r="B90" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C90" s="64">
         <v>0.02</v>
@@ -4462,7 +4459,7 @@
     <row r="91" spans="1:9">
       <c r="A91" s="48"/>
       <c r="B91" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C91" s="64">
         <v>7.0000000000000007E-2</v>
@@ -4480,7 +4477,7 @@
     <row r="92" spans="1:9">
       <c r="A92" s="48"/>
       <c r="B92" s="53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C92" s="64">
         <v>0.26500000000000001</v>
@@ -4498,7 +4495,7 @@
     <row r="93" spans="1:9">
       <c r="A93" s="48"/>
       <c r="B93" s="53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C93" s="64">
         <v>0.54700000000000004</v>
@@ -4516,7 +4513,7 @@
     <row r="94" spans="1:9">
       <c r="A94" s="48"/>
       <c r="B94" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C94" s="64">
         <v>5.2999999999999999E-2</v>
@@ -8486,7 +8483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="O69" sqref="O69"/>
     </sheetView>
   </sheetViews>
@@ -9329,7 +9326,7 @@
     <row r="42" spans="1:25" s="47" customFormat="1"/>
     <row r="43" spans="1:25" s="47" customFormat="1">
       <c r="A43" s="73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:25" s="47" customFormat="1">
@@ -9437,7 +9434,7 @@
     <row r="48" spans="1:25" s="47" customFormat="1"/>
     <row r="49" spans="1:25" s="47" customFormat="1">
       <c r="A49" s="73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:25" s="47" customFormat="1">
@@ -9545,7 +9542,7 @@
     <row r="54" spans="1:25" s="47" customFormat="1"/>
     <row r="55" spans="1:25" s="47" customFormat="1">
       <c r="A55" s="73" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:25" s="47" customFormat="1">
@@ -9653,7 +9650,7 @@
     <row r="60" spans="1:25" s="47" customFormat="1"/>
     <row r="61" spans="1:25" s="47" customFormat="1">
       <c r="A61" s="73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:25" s="47" customFormat="1">
@@ -9761,7 +9758,7 @@
     <row r="66" spans="1:25" s="47" customFormat="1"/>
     <row r="67" spans="1:25" s="47" customFormat="1">
       <c r="A67" s="73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:25" s="47" customFormat="1">
@@ -9887,7 +9884,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -10579,10 +10576,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y80"/>
+  <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:XFD80"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12427,178 +12424,6 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
-      <c r="A76" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="77" spans="1:25">
-      <c r="C77" s="7">
-        <v>2000</v>
-      </c>
-      <c r="D77" s="7">
-        <v>2001</v>
-      </c>
-      <c r="E77" s="7">
-        <v>2002</v>
-      </c>
-      <c r="F77" s="7">
-        <v>2003</v>
-      </c>
-      <c r="G77" s="7">
-        <v>2004</v>
-      </c>
-      <c r="H77" s="7">
-        <v>2005</v>
-      </c>
-      <c r="I77" s="7">
-        <v>2006</v>
-      </c>
-      <c r="J77" s="7">
-        <v>2007</v>
-      </c>
-      <c r="K77" s="7">
-        <v>2008</v>
-      </c>
-      <c r="L77" s="7">
-        <v>2009</v>
-      </c>
-      <c r="M77" s="7">
-        <v>2010</v>
-      </c>
-      <c r="N77" s="7">
-        <v>2011</v>
-      </c>
-      <c r="O77" s="7">
-        <v>2012</v>
-      </c>
-      <c r="P77" s="7">
-        <v>2013</v>
-      </c>
-      <c r="Q77" s="7">
-        <v>2014</v>
-      </c>
-      <c r="R77" s="7">
-        <v>2015</v>
-      </c>
-      <c r="S77" s="7">
-        <v>2016</v>
-      </c>
-      <c r="T77" s="7">
-        <v>2017</v>
-      </c>
-      <c r="U77" s="7">
-        <v>2018</v>
-      </c>
-      <c r="V77" s="7">
-        <v>2019</v>
-      </c>
-      <c r="W77" s="7">
-        <v>2020</v>
-      </c>
-      <c r="Y77" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="78" spans="1:25">
-      <c r="B78" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>Clients</v>
-      </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="22"/>
-      <c r="H78" s="22"/>
-      <c r="I78" s="22"/>
-      <c r="J78" s="22"/>
-      <c r="K78" s="22"/>
-      <c r="L78" s="22"/>
-      <c r="M78" s="22"/>
-      <c r="N78" s="22"/>
-      <c r="O78" s="22"/>
-      <c r="P78" s="22"/>
-      <c r="Q78" s="22"/>
-      <c r="R78" s="22"/>
-      <c r="S78" s="22"/>
-      <c r="T78" s="22"/>
-      <c r="U78" s="22"/>
-      <c r="V78" s="22"/>
-      <c r="W78" s="22"/>
-      <c r="X78" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y78" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:25">
-      <c r="B79" s="7" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
-      </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="22"/>
-      <c r="H79" s="22"/>
-      <c r="I79" s="22"/>
-      <c r="J79" s="22"/>
-      <c r="K79" s="22"/>
-      <c r="L79" s="22"/>
-      <c r="M79" s="22"/>
-      <c r="N79" s="22"/>
-      <c r="O79" s="22"/>
-      <c r="P79" s="22"/>
-      <c r="Q79" s="22"/>
-      <c r="R79" s="22"/>
-      <c r="S79" s="22"/>
-      <c r="T79" s="22"/>
-      <c r="U79" s="22"/>
-      <c r="V79" s="22"/>
-      <c r="W79" s="22"/>
-      <c r="X79" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y79" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:25">
-      <c r="B80" s="7" t="str">
-        <f>Populations!$C$7</f>
-        <v>M 15+</v>
-      </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22"/>
-      <c r="J80" s="22"/>
-      <c r="K80" s="22"/>
-      <c r="L80" s="22"/>
-      <c r="M80" s="22"/>
-      <c r="N80" s="22"/>
-      <c r="O80" s="22"/>
-      <c r="P80" s="22"/>
-      <c r="Q80" s="22"/>
-      <c r="R80" s="22"/>
-      <c r="S80" s="22"/>
-      <c r="T80" s="22"/>
-      <c r="U80" s="22"/>
-      <c r="V80" s="22"/>
-      <c r="W80" s="22"/>
-      <c r="X80" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y80" s="22">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
add aids ltfu rate to spreadsheets
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="131">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -535,6 +535,9 @@
   </si>
   <si>
     <t>People on ART with viral suppression (%)</t>
+  </si>
+  <si>
+    <t>Percentage of people with CD4&lt;200 lost to follow-up (%/year)</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="205">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -976,8 +979,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1145,8 +1156,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="205">
+  <cellStyles count="213">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1197,6 +1211,10 @@
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1332,6 +1350,10 @@
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -7235,8 +7257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8418,7 +8440,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9822,10 +9844,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AI31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10280,7 +10302,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:35">
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
@@ -10309,10 +10331,10 @@
         <v>27</v>
       </c>
       <c r="Y17" s="39">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35">
       <c r="B18" s="6" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10345,7 +10367,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:35">
       <c r="B19" s="6" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10378,136 +10400,349 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
-      <c r="A23" s="27" t="s">
+    <row r="23" spans="1:35" s="45" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" s="45" customFormat="1">
+      <c r="C24" s="6">
+        <v>2000</v>
+      </c>
+      <c r="D24" s="6">
+        <v>2001</v>
+      </c>
+      <c r="E24" s="6">
+        <v>2002</v>
+      </c>
+      <c r="F24" s="6">
+        <v>2003</v>
+      </c>
+      <c r="G24" s="6">
+        <v>2004</v>
+      </c>
+      <c r="H24" s="6">
+        <v>2005</v>
+      </c>
+      <c r="I24" s="6">
+        <v>2006</v>
+      </c>
+      <c r="J24" s="6">
+        <v>2007</v>
+      </c>
+      <c r="K24" s="6">
+        <v>2008</v>
+      </c>
+      <c r="L24" s="6">
+        <v>2009</v>
+      </c>
+      <c r="M24" s="6">
+        <v>2010</v>
+      </c>
+      <c r="N24" s="6">
+        <v>2011</v>
+      </c>
+      <c r="O24" s="6">
+        <v>2012</v>
+      </c>
+      <c r="P24" s="6">
+        <v>2013</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>2014</v>
+      </c>
+      <c r="R24" s="6">
+        <v>2015</v>
+      </c>
+      <c r="S24" s="6">
+        <v>2016</v>
+      </c>
+      <c r="T24" s="6">
+        <v>2017</v>
+      </c>
+      <c r="U24" s="6">
+        <v>2018</v>
+      </c>
+      <c r="V24" s="6">
+        <v>2019</v>
+      </c>
+      <c r="W24" s="6">
+        <v>2020</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" s="45" customFormat="1">
+      <c r="B25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y25" s="76">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" s="45" customFormat="1">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="6"/>
+      <c r="AG26" s="6"/>
+      <c r="AH26" s="6"/>
+      <c r="AI26" s="6"/>
+    </row>
+    <row r="27" spans="1:35" s="45" customFormat="1">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="6"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="6"/>
+    </row>
+    <row r="28" spans="1:35" s="45" customFormat="1">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="6"/>
+      <c r="AG28" s="6"/>
+      <c r="AH28" s="6"/>
+      <c r="AI28" s="6"/>
+    </row>
+    <row r="29" spans="1:35">
+      <c r="A29" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="28"/>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="28"/>
+    </row>
+    <row r="30" spans="1:35">
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29">
         <v>2000</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D30" s="29">
         <v>2001</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E30" s="29">
         <v>2002</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F30" s="29">
         <v>2003</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G30" s="29">
         <v>2004</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H30" s="29">
         <v>2005</v>
       </c>
-      <c r="I24" s="29">
+      <c r="I30" s="29">
         <v>2006</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J30" s="29">
         <v>2007</v>
       </c>
-      <c r="K24" s="29">
+      <c r="K30" s="29">
         <v>2008</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L30" s="29">
         <v>2009</v>
       </c>
-      <c r="M24" s="29">
+      <c r="M30" s="29">
         <v>2010</v>
       </c>
-      <c r="N24" s="29">
+      <c r="N30" s="29">
         <v>2011</v>
       </c>
-      <c r="O24" s="29">
+      <c r="O30" s="29">
         <v>2012</v>
       </c>
-      <c r="P24" s="29">
+      <c r="P30" s="29">
         <v>2013</v>
       </c>
-      <c r="Q24" s="29">
+      <c r="Q30" s="29">
         <v>2014</v>
       </c>
-      <c r="R24" s="29">
+      <c r="R30" s="29">
         <v>2015</v>
       </c>
-      <c r="S24" s="29">
+      <c r="S30" s="29">
         <v>2016</v>
       </c>
-      <c r="T24" s="29">
+      <c r="T30" s="29">
         <v>2017</v>
       </c>
-      <c r="U24" s="29">
+      <c r="U30" s="29">
         <v>2018</v>
       </c>
-      <c r="V24" s="29">
+      <c r="V30" s="29">
         <v>2019</v>
       </c>
-      <c r="W24" s="29">
+      <c r="W30" s="29">
         <v>2020</v>
       </c>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="29" t="s">
+      <c r="X30" s="28"/>
+      <c r="Y30" s="29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29" t="s">
+    <row r="31" spans="1:35">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
-      <c r="S25" s="40"/>
-      <c r="T25" s="40"/>
-      <c r="U25" s="40"/>
-      <c r="V25" s="40"/>
-      <c r="W25" s="40"/>
-      <c r="X25" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y25" s="41">
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="40"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y31" s="41">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add treatment cost and migration
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28575" windowHeight="15975" tabRatio="805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,12 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -140,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="135">
   <si>
     <t>For further details please visit: http://optimamodel.com/file/indicator-guide</t>
   </si>
@@ -542,13 +547,16 @@
   </si>
   <si>
     <t>Date created: 2016-Nov-02 17:07:35</t>
+  </si>
+  <si>
+    <t>Unit cost of treatment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
@@ -558,6 +566,7 @@
     <numFmt numFmtId="169" formatCode="#,##0.000"/>
     <numFmt numFmtId="170" formatCode="#,##0.0"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -784,7 +793,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="220">
+  <cellStyleXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -1005,8 +1014,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1178,8 +1189,11 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="219" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="174" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="220">
+  <cellStyles count="222">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1237,6 +1251,7 @@
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1379,6 +1394,7 @@
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -1902,59 +1918,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="77" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15" customHeight="1">
       <c r="A2" s="77"/>
     </row>
-    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15" customHeight="1">
       <c r="A3" s="77"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="76"/>
     </row>
-    <row r="5" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="56">
       <c r="A5" s="76" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="76"/>
     </row>
-    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="28">
       <c r="A7" s="76" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="76"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="76" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="76"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="76" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="76"/>
     </row>
   </sheetData>
@@ -1963,6 +1979,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1974,14 +1995,14 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2049,7 +2070,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2082,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2115,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2148,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -2180,7 +2201,7 @@
       </c>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2213,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2246,12 +2267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -2319,7 +2340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2352,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2385,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2418,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -2450,7 +2471,7 @@
       </c>
       <c r="Y17" s="19"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2483,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2516,12 +2537,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -2589,7 +2610,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
@@ -2640,14 +2661,14 @@
       <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="C2" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2673,7 +2694,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2685,7 +2706,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2701,7 +2722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2715,7 +2736,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="B6" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2729,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2745,7 +2766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2757,12 +2778,12 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="C13" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2788,7 +2809,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2800,7 +2821,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2816,7 +2837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2830,7 +2851,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="B17" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2844,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2860,7 +2881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2872,12 +2893,12 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="C24" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2903,7 +2924,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2915,7 +2936,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2929,7 +2950,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2941,7 +2962,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="B28" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2953,7 +2974,7 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2965,7 +2986,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2977,12 +2998,12 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="C35" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3008,7 +3029,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="B36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3020,7 +3041,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3032,7 +3053,7 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3044,7 +3065,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="B39" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3058,7 +3079,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="B40" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3070,7 +3091,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="B41" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3082,12 +3103,12 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="C46" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3113,7 +3134,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="B47" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3125,7 +3146,7 @@
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="B48" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3137,12 +3158,12 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="C53" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3168,7 +3189,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="B54" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3180,7 +3201,7 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="B55" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3192,7 +3213,7 @@
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="B56" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3204,7 +3225,7 @@
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="B57" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3216,7 +3237,7 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="B58" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3228,7 +3249,7 @@
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="B59" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3240,12 +3261,12 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="C64" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3271,7 +3292,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8">
       <c r="B65" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3285,7 +3306,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8">
       <c r="B66" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3297,7 +3318,7 @@
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8">
       <c r="B67" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3309,7 +3330,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8">
       <c r="B68" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3321,7 +3342,7 @@
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8">
       <c r="B69" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3333,7 +3354,7 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8">
       <c r="B70" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3364,16 +3385,16 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="44"/>
-    <col min="2" max="2" width="37.7109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="8.85546875" style="44"/>
-    <col min="10" max="10" width="18.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="44"/>
+    <col min="1" max="1" width="8.83203125" style="44"/>
+    <col min="2" max="2" width="37.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.83203125" style="44"/>
+    <col min="10" max="10" width="18.83203125" style="44" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="54" t="s">
         <v>71</v>
       </c>
@@ -3382,7 +3403,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="53" t="s">
@@ -3395,7 +3416,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="52"/>
       <c r="B3" s="55" t="s">
         <v>72</v>
@@ -3410,7 +3431,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="52"/>
       <c r="B4" s="55" t="s">
         <v>73</v>
@@ -3425,7 +3446,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="52"/>
       <c r="B5" s="55" t="s">
         <v>74</v>
@@ -3440,7 +3461,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="52"/>
       <c r="B6" s="55" t="s">
         <v>75</v>
@@ -3455,7 +3476,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="52"/>
       <c r="B7" s="55" t="s">
         <v>76</v>
@@ -3470,7 +3491,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="52"/>
       <c r="B8" s="55" t="s">
         <v>77</v>
@@ -3485,7 +3506,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="52"/>
       <c r="B9" s="55" t="s">
         <v>78</v>
@@ -3500,33 +3521,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="59"/>
       <c r="B10" s="60"/>
       <c r="C10" s="59"/>
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="59"/>
       <c r="B11" s="60"/>
       <c r="C11" s="59"/>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="59"/>
       <c r="B12" s="60"/>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
@@ -3537,7 +3558,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="B15" s="2" t="s">
         <v>80</v>
       </c>
@@ -3551,7 +3572,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="B16" s="2" t="s">
         <v>81</v>
       </c>
@@ -3565,7 +3586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="B17" s="2" t="s">
         <v>82</v>
       </c>
@@ -3579,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="B18" s="2" t="s">
         <v>83</v>
       </c>
@@ -3593,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="B19" s="2" t="s">
         <v>84</v>
       </c>
@@ -3607,7 +3628,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="B20" s="2" t="s">
         <v>85</v>
       </c>
@@ -3621,33 +3642,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="59"/>
       <c r="B21" s="60"/>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="59"/>
       <c r="B22" s="60"/>
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="59"/>
       <c r="B23" s="60"/>
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="C25" s="5" t="s">
         <v>26</v>
       </c>
@@ -3658,7 +3679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="B26" s="2" t="s">
         <v>86</v>
       </c>
@@ -3672,7 +3693,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="B27" s="2" t="s">
         <v>82</v>
       </c>
@@ -3687,7 +3708,7 @@
       </c>
       <c r="G27" s="62"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
@@ -3701,7 +3722,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="B29" s="2" t="s">
         <v>88</v>
       </c>
@@ -3715,7 +3736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="B30" s="2" t="s">
         <v>89</v>
       </c>
@@ -3729,33 +3750,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="59"/>
       <c r="B31" s="60"/>
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="59"/>
       <c r="B32" s="60"/>
       <c r="C32" s="59"/>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="59"/>
       <c r="B33" s="60"/>
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="C35" s="5" t="s">
         <v>26</v>
       </c>
@@ -3766,7 +3787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="B36" s="2" t="s">
         <v>90</v>
       </c>
@@ -3780,7 +3801,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="B37" s="2" t="s">
         <v>91</v>
       </c>
@@ -3794,7 +3815,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
@@ -3808,7 +3829,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="B39" s="2" t="s">
         <v>93</v>
       </c>
@@ -3822,7 +3843,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A40" s="51"/>
       <c r="B40" s="2" t="s">
         <v>119</v>
@@ -3837,28 +3858,28 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="59"/>
       <c r="B41" s="60"/>
       <c r="C41" s="59"/>
       <c r="D41" s="59"/>
       <c r="E41" s="59"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="59"/>
       <c r="B42" s="60"/>
       <c r="C42" s="59"/>
       <c r="D42" s="59"/>
       <c r="E42" s="59"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="59"/>
       <c r="B43" s="60"/>
       <c r="C43" s="59"/>
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
     </row>
-    <row r="44" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A44" s="46" t="s">
         <v>121</v>
       </c>
@@ -3867,7 +3888,7 @@
       <c r="D44" s="51"/>
       <c r="E44" s="51"/>
     </row>
-    <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A45" s="51"/>
       <c r="B45" s="51"/>
       <c r="C45" s="47" t="s">
@@ -3880,7 +3901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A46" s="51"/>
       <c r="B46" s="2" t="s">
         <v>82</v>
@@ -3895,7 +3916,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A47" s="51"/>
       <c r="B47" s="2" t="s">
         <v>90</v>
@@ -3910,7 +3931,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A48" s="51"/>
       <c r="B48" s="2" t="s">
         <v>87</v>
@@ -3925,7 +3946,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A49" s="51"/>
       <c r="B49" s="2" t="s">
         <v>91</v>
@@ -3940,7 +3961,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="56" customFormat="1">
       <c r="A50" s="51"/>
       <c r="B50" s="2" t="s">
         <v>88</v>
@@ -3955,7 +3976,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A51" s="51"/>
       <c r="B51" s="2" t="s">
         <v>92</v>
@@ -3970,7 +3991,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A52" s="51"/>
       <c r="B52" s="2" t="s">
         <v>89</v>
@@ -3985,7 +4006,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A53" s="51"/>
       <c r="B53" s="2" t="s">
         <v>93</v>
@@ -4000,7 +4021,7 @@
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A54" s="51"/>
       <c r="B54" s="2" t="s">
         <v>122</v>
@@ -4015,33 +4036,33 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A55" s="57"/>
       <c r="B55" s="57"/>
       <c r="C55" s="57"/>
       <c r="D55" s="57"/>
       <c r="E55" s="57"/>
     </row>
-    <row r="56" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A56" s="57"/>
       <c r="B56" s="57"/>
       <c r="C56" s="57"/>
       <c r="D56" s="57"/>
       <c r="E56" s="57"/>
     </row>
-    <row r="57" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A57" s="57"/>
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
       <c r="E57" s="57"/>
     </row>
-    <row r="58" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="13.5" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="13.5" customHeight="1">
       <c r="C59" s="5" t="s">
         <v>26</v>
       </c>
@@ -4052,7 +4073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="13.5" customHeight="1">
       <c r="B60" s="2" t="s">
         <v>80</v>
       </c>
@@ -4066,7 +4087,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="13.5" customHeight="1">
       <c r="B61" s="2" t="s">
         <v>81</v>
       </c>
@@ -4080,7 +4101,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="13.5" customHeight="1">
       <c r="B62" s="2" t="s">
         <v>95</v>
       </c>
@@ -4094,7 +4115,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="13.5" customHeight="1">
       <c r="B63" s="2" t="s">
         <v>83</v>
       </c>
@@ -4108,7 +4129,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="B64" s="2" t="s">
         <v>84</v>
       </c>
@@ -4123,7 +4144,7 @@
       </c>
       <c r="F64" s="59"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="B65" s="2" t="s">
         <v>85</v>
       </c>
@@ -4138,7 +4159,7 @@
       </c>
       <c r="F65" s="59"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9">
       <c r="B66" s="2" t="s">
         <v>117</v>
       </c>
@@ -4153,7 +4174,7 @@
       </c>
       <c r="F66" s="59"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9">
       <c r="B67" s="2" t="s">
         <v>118</v>
       </c>
@@ -4168,7 +4189,7 @@
       </c>
       <c r="F67" s="59"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9">
       <c r="B68" s="2" t="s">
         <v>96</v>
       </c>
@@ -4183,7 +4204,7 @@
       </c>
       <c r="F68" s="59"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9">
       <c r="A69" s="59"/>
       <c r="B69" s="60"/>
       <c r="C69" s="59"/>
@@ -4191,7 +4212,7 @@
       <c r="E69" s="59"/>
       <c r="F69" s="59"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9">
       <c r="A70" s="59"/>
       <c r="B70" s="60"/>
       <c r="C70" s="59"/>
@@ -4202,7 +4223,7 @@
       <c r="H70" s="59"/>
       <c r="I70" s="59"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9">
       <c r="A71" s="59"/>
       <c r="B71" s="60"/>
       <c r="C71" s="59"/>
@@ -4213,7 +4234,7 @@
       <c r="H71" s="59"/>
       <c r="I71" s="59"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
         <v>97</v>
       </c>
@@ -4222,7 +4243,7 @@
       <c r="H72" s="59"/>
       <c r="I72" s="59"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9">
       <c r="C73" s="5" t="s">
         <v>26</v>
       </c>
@@ -4237,7 +4258,7 @@
       <c r="H73" s="59"/>
       <c r="I73" s="59"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9">
       <c r="B74" s="2" t="s">
         <v>98</v>
       </c>
@@ -4255,7 +4276,7 @@
       <c r="H74" s="64"/>
       <c r="I74" s="64"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9">
       <c r="B75" s="2" t="s">
         <v>99</v>
       </c>
@@ -4273,7 +4294,7 @@
       <c r="H75" s="64"/>
       <c r="I75" s="64"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9">
       <c r="B76" s="2" t="s">
         <v>100</v>
       </c>
@@ -4288,7 +4309,7 @@
       </c>
       <c r="F76" s="59"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9">
       <c r="B77" s="2" t="s">
         <v>101</v>
       </c>
@@ -4306,7 +4327,7 @@
       <c r="H77" s="64"/>
       <c r="I77" s="64"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9">
       <c r="B78" s="2" t="s">
         <v>102</v>
       </c>
@@ -4324,7 +4345,7 @@
       <c r="H78" s="64"/>
       <c r="I78" s="64"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="B79" s="2" t="s">
         <v>103</v>
       </c>
@@ -4342,7 +4363,7 @@
       <c r="H79" s="64"/>
       <c r="I79" s="64"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="B80" s="2" t="s">
         <v>104</v>
       </c>
@@ -4360,7 +4381,7 @@
       <c r="H80" s="64"/>
       <c r="I80" s="64"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9">
       <c r="B81" s="2" t="s">
         <v>105</v>
       </c>
@@ -4378,7 +4399,7 @@
       <c r="H81" s="64"/>
       <c r="I81" s="64"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9">
       <c r="B82" s="2" t="s">
         <v>106</v>
       </c>
@@ -4396,7 +4417,7 @@
       <c r="H82" s="59"/>
       <c r="I82" s="59"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9">
       <c r="A83" s="59"/>
       <c r="B83" s="60"/>
       <c r="C83" s="59"/>
@@ -4407,7 +4428,7 @@
       <c r="H83" s="59"/>
       <c r="I83" s="59"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9">
       <c r="A84" s="65"/>
       <c r="B84" s="66"/>
       <c r="C84" s="67"/>
@@ -4418,7 +4439,7 @@
       <c r="H84" s="67"/>
       <c r="I84" s="59"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9">
       <c r="A85" s="67"/>
       <c r="B85" s="66"/>
       <c r="C85" s="68"/>
@@ -4429,7 +4450,7 @@
       <c r="H85" s="67"/>
       <c r="I85" s="59"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9">
       <c r="A86" s="48" t="s">
         <v>107</v>
       </c>
@@ -4441,7 +4462,7 @@
       <c r="G86" s="45"/>
       <c r="H86" s="45"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9">
       <c r="A87" s="45"/>
       <c r="B87" s="45"/>
       <c r="C87" s="49" t="s">
@@ -4457,7 +4478,7 @@
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9">
       <c r="A88" s="45"/>
       <c r="B88" s="50" t="s">
         <v>108</v>
@@ -4475,7 +4496,7 @@
       <c r="G88" s="45"/>
       <c r="H88" s="45"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9">
       <c r="A89" s="45"/>
       <c r="B89" s="50" t="s">
         <v>109</v>
@@ -4493,7 +4514,7 @@
       <c r="G89" s="45"/>
       <c r="H89" s="45"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9">
       <c r="A90" s="45"/>
       <c r="B90" s="50" t="s">
         <v>110</v>
@@ -4511,7 +4532,7 @@
       <c r="G90" s="45"/>
       <c r="H90" s="45"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9">
       <c r="A91" s="45"/>
       <c r="B91" s="50" t="s">
         <v>111</v>
@@ -4529,7 +4550,7 @@
       <c r="G91" s="45"/>
       <c r="H91" s="45"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9">
       <c r="A92" s="45"/>
       <c r="B92" s="50" t="s">
         <v>112</v>
@@ -4547,7 +4568,7 @@
       <c r="G92" s="45"/>
       <c r="H92" s="45"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9">
       <c r="A93" s="45"/>
       <c r="B93" s="50" t="s">
         <v>113</v>
@@ -4565,7 +4586,7 @@
       <c r="G93" s="45"/>
       <c r="H93" s="45"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9">
       <c r="A94" s="45"/>
       <c r="B94" s="50" t="s">
         <v>114</v>
@@ -4583,17 +4604,17 @@
       <c r="G94" s="45"/>
       <c r="H94" s="45"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9">
       <c r="F95" s="45"/>
       <c r="G95" s="45"/>
       <c r="H95" s="45"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9">
       <c r="F96" s="45"/>
       <c r="G96" s="45"/>
       <c r="H96" s="45"/>
     </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="6:8">
       <c r="F97" s="45"/>
       <c r="G97" s="45"/>
       <c r="H97" s="45"/>
@@ -4617,14 +4638,14 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4644,7 +4665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4667,7 +4688,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4690,7 +4711,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -4713,7 +4734,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -4736,7 +4757,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -4759,7 +4780,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -4801,15 +4822,15 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4877,7 +4898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4911,7 +4932,7 @@
       </c>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4967,7 +4988,7 @@
       </c>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5001,7 +5022,7 @@
       </c>
       <c r="Z5" s="8"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5035,7 +5056,7 @@
       </c>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5091,7 +5112,7 @@
       </c>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5125,7 +5146,7 @@
       </c>
       <c r="Z9" s="8"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5159,7 +5180,7 @@
       </c>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="B12" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5215,7 +5236,7 @@
       </c>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="B13" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5249,7 +5270,7 @@
       </c>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -5262,7 +5283,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
@@ -5295,7 +5316,7 @@
       </c>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -5350,7 +5371,7 @@
       </c>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -5383,7 +5404,7 @@
       </c>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26">
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -5396,7 +5417,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5430,7 +5451,7 @@
       </c>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5486,7 +5507,7 @@
       </c>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5520,7 +5541,7 @@
       </c>
       <c r="Z21" s="8"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26">
       <c r="B23" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5554,7 +5575,7 @@
       </c>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5610,7 +5631,7 @@
       </c>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5644,7 +5665,7 @@
       </c>
       <c r="Z25" s="8"/>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26">
       <c r="M27" t="s">
         <v>28</v>
       </c>
@@ -5653,7 +5674,7 @@
         <v>21773583.295806497</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26">
       <c r="M28" t="s">
         <v>29</v>
       </c>
@@ -5669,7 +5690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26">
       <c r="N29">
         <f>3529/'Population size'!N28*100</f>
         <v>7.0468319579830743</v>
@@ -5697,14 +5718,14 @@
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -5772,7 +5793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5812,7 +5833,7 @@
       </c>
       <c r="Z3" s="16"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5852,7 +5873,7 @@
       </c>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5892,7 +5913,7 @@
       </c>
       <c r="Z5" s="16"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5926,7 +5947,7 @@
       </c>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5962,7 +5983,7 @@
       </c>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5996,7 +6017,7 @@
       </c>
       <c r="Z9" s="16"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6032,7 +6053,7 @@
       </c>
       <c r="Z11" s="16"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="B12" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6074,7 +6095,7 @@
       </c>
       <c r="Z12" s="16"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="B13" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6110,7 +6131,7 @@
       </c>
       <c r="Z13" s="16"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
@@ -6145,7 +6166,7 @@
       </c>
       <c r="Z15" s="16"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -6186,7 +6207,7 @@
       </c>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -6221,7 +6242,7 @@
       </c>
       <c r="Z17" s="16"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6255,7 +6276,7 @@
       </c>
       <c r="Z19" s="16"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6303,7 +6324,7 @@
       </c>
       <c r="Z20" s="16"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6337,7 +6358,7 @@
       </c>
       <c r="Z21" s="16"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26">
       <c r="B23" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6371,7 +6392,7 @@
       </c>
       <c r="Z23" s="16"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6419,7 +6440,7 @@
       </c>
       <c r="Z24" s="16"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6473,14 +6494,14 @@
       <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -6548,7 +6569,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6581,7 +6602,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6614,7 +6635,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6647,7 +6668,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -6679,7 +6700,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6712,7 +6733,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6745,12 +6766,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -6818,7 +6839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6851,7 +6872,7 @@
       </c>
       <c r="Y14" s="16"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6884,7 +6905,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6917,7 +6938,7 @@
       </c>
       <c r="Y16" s="16"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -6949,7 +6970,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6982,7 +7003,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7015,12 +7036,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -7088,7 +7109,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7121,7 +7142,7 @@
       </c>
       <c r="Y25" s="16"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7154,7 +7175,7 @@
       </c>
       <c r="Y26" s="16"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7187,7 +7208,7 @@
       </c>
       <c r="Y27" s="16"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
@@ -7219,7 +7240,7 @@
       </c>
       <c r="Y28" s="16"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7252,7 +7273,7 @@
       </c>
       <c r="Y29" s="16"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7298,20 +7319,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y51"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -7379,7 +7404,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7414,7 +7439,7 @@
       </c>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7451,7 +7476,7 @@
       </c>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7484,7 +7509,7 @@
       </c>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -7516,7 +7541,7 @@
       </c>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7549,7 +7574,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7582,12 +7607,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -7655,7 +7680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
@@ -7687,12 +7712,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="A18" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="C19" s="5">
         <v>2000</v>
       </c>
@@ -7760,7 +7785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
@@ -7820,247 +7845,195 @@
       </c>
       <c r="Y20" s="6"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="24" spans="1:25" s="44" customFormat="1">
+      <c r="A24" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" s="44" customFormat="1">
+      <c r="C25" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E25" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H25" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I25" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J25" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K25" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L25" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M25" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N25" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O25" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P25" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R25" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S25" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T25" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U25" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V25" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W25" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" s="44" customFormat="1">
+      <c r="B26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="78">
+        <v>500</v>
+      </c>
+      <c r="O26" s="78"/>
+      <c r="P26" s="78">
+        <v>350</v>
+      </c>
+      <c r="Q26" s="78">
+        <v>300</v>
+      </c>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
+      <c r="U26" s="78"/>
+      <c r="V26" s="78"/>
+      <c r="W26" s="78"/>
+      <c r="X26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y26" s="6"/>
+    </row>
+    <row r="27" spans="1:25" s="44" customFormat="1"/>
+    <row r="28" spans="1:25" s="44" customFormat="1"/>
+    <row r="29" spans="1:25" s="44" customFormat="1"/>
+    <row r="30" spans="1:25">
+      <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C26" s="5">
+    <row r="31" spans="1:25">
+      <c r="C31" s="5">
         <v>2000</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D31" s="5">
         <v>2001</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E31" s="5">
         <v>2002</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F31" s="5">
         <v>2003</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G31" s="5">
         <v>2004</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H31" s="5">
         <v>2005</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I31" s="5">
         <v>2006</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J31" s="5">
         <v>2007</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K31" s="5">
         <v>2008</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L31" s="5">
         <v>2009</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M31" s="5">
         <v>2010</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N31" s="5">
         <v>2011</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O31" s="5">
         <v>2012</v>
       </c>
-      <c r="P26" s="5">
+      <c r="P31" s="5">
         <v>2013</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="Q31" s="5">
         <v>2014</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R31" s="5">
         <v>2015</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S31" s="5">
         <v>2016</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T31" s="5">
         <v>2017</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U31" s="5">
         <v>2018</v>
       </c>
-      <c r="V26" s="5">
+      <c r="V31" s="5">
         <v>2019</v>
       </c>
-      <c r="W26" s="5">
+      <c r="W31" s="5">
         <v>2020</v>
       </c>
-      <c r="Y26" s="5" t="s">
+      <c r="Y31" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="str">
+    <row r="32" spans="1:25">
+      <c r="B32" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19"/>
-      <c r="W27" s="19"/>
-      <c r="X27" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y27" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="str">
-        <f>Populations!$C$4</f>
-        <v>Clients</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="19"/>
-      <c r="X28" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y28" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
-      <c r="W29" s="19"/>
-      <c r="X29" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y29" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="19"/>
-      <c r="X30" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y30" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="str">
-        <f>Populations!$C$7</f>
-        <v>M 15+</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="19"/>
-      <c r="X31" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y31" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="str">
-        <f>Populations!$C$8</f>
-        <v>F 15+</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -8090,396 +8063,560 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="33" spans="1:25">
+      <c r="B33" s="5" t="str">
+        <f>Populations!$C$4</f>
+        <v>Clients</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y33" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="B34" s="5" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y34" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="B35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y35" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="B36" s="5" t="str">
+        <f>Populations!$C$7</f>
+        <v>M 15+</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y36" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="B37" s="5" t="str">
+        <f>Populations!$C$8</f>
+        <v>F 15+</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y37" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C37" s="5">
+    <row r="42" spans="1:25">
+      <c r="C42" s="5">
         <v>2000</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D42" s="5">
         <v>2001</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E42" s="5">
         <v>2002</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F42" s="5">
         <v>2003</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G42" s="5">
         <v>2004</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H42" s="5">
         <v>2005</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I42" s="5">
         <v>2006</v>
       </c>
-      <c r="J37" s="5">
+      <c r="J42" s="5">
         <v>2007</v>
       </c>
-      <c r="K37" s="5">
+      <c r="K42" s="5">
         <v>2008</v>
       </c>
-      <c r="L37" s="5">
+      <c r="L42" s="5">
         <v>2009</v>
       </c>
-      <c r="M37" s="5">
+      <c r="M42" s="5">
         <v>2010</v>
       </c>
-      <c r="N37" s="5">
+      <c r="N42" s="5">
         <v>2011</v>
       </c>
-      <c r="O37" s="5">
+      <c r="O42" s="5">
         <v>2012</v>
       </c>
-      <c r="P37" s="5">
+      <c r="P42" s="5">
         <v>2013</v>
       </c>
-      <c r="Q37" s="5">
+      <c r="Q42" s="5">
         <v>2014</v>
       </c>
-      <c r="R37" s="5">
+      <c r="R42" s="5">
         <v>2015</v>
       </c>
-      <c r="S37" s="5">
+      <c r="S42" s="5">
         <v>2016</v>
       </c>
-      <c r="T37" s="5">
+      <c r="T42" s="5">
         <v>2017</v>
       </c>
-      <c r="U37" s="5">
+      <c r="U42" s="5">
         <v>2018</v>
       </c>
-      <c r="V37" s="5">
+      <c r="V42" s="5">
         <v>2019</v>
       </c>
-      <c r="W37" s="5">
+      <c r="W42" s="5">
         <v>2020</v>
       </c>
-      <c r="Y37" s="5" t="s">
+      <c r="Y42" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+    <row r="43" spans="1:25">
+      <c r="B43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="6">
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+      <c r="N43" s="6">
         <v>500</v>
       </c>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6">
+      <c r="O43" s="6"/>
+      <c r="P43" s="6">
         <v>612</v>
       </c>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
-      <c r="V38" s="22"/>
-      <c r="W38" s="22"/>
-      <c r="X38" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y38" s="6"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y43" s="6"/>
+    </row>
+    <row r="47" spans="1:25">
+      <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C43" s="5">
+    <row r="48" spans="1:25">
+      <c r="C48" s="5">
         <v>2000</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D48" s="5">
         <v>2001</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E48" s="5">
         <v>2002</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F48" s="5">
         <v>2003</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G48" s="5">
         <v>2004</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H48" s="5">
         <v>2005</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I48" s="5">
         <v>2006</v>
       </c>
-      <c r="J43" s="5">
+      <c r="J48" s="5">
         <v>2007</v>
       </c>
-      <c r="K43" s="5">
+      <c r="K48" s="5">
         <v>2008</v>
       </c>
-      <c r="L43" s="5">
+      <c r="L48" s="5">
         <v>2009</v>
       </c>
-      <c r="M43" s="5">
+      <c r="M48" s="5">
         <v>2010</v>
       </c>
-      <c r="N43" s="5">
+      <c r="N48" s="5">
         <v>2011</v>
       </c>
-      <c r="O43" s="5">
+      <c r="O48" s="5">
         <v>2012</v>
       </c>
-      <c r="P43" s="5">
+      <c r="P48" s="5">
         <v>2013</v>
       </c>
-      <c r="Q43" s="5">
+      <c r="Q48" s="5">
         <v>2014</v>
       </c>
-      <c r="R43" s="5">
+      <c r="R48" s="5">
         <v>2015</v>
       </c>
-      <c r="S43" s="5">
+      <c r="S48" s="5">
         <v>2016</v>
       </c>
-      <c r="T43" s="5">
+      <c r="T48" s="5">
         <v>2017</v>
       </c>
-      <c r="U43" s="5">
+      <c r="U48" s="5">
         <v>2018</v>
       </c>
-      <c r="V43" s="5">
+      <c r="V48" s="5">
         <v>2019</v>
       </c>
-      <c r="W43" s="5">
+      <c r="W48" s="5">
         <v>2020</v>
       </c>
-      <c r="Y43" s="5" t="s">
+      <c r="Y48" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="str">
+    <row r="49" spans="1:25">
+      <c r="B49" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="C44" s="23">
+      <c r="C49" s="23">
         <v>9.0399361562071207E-2</v>
       </c>
-      <c r="D44" s="23">
+      <c r="D49" s="23">
         <v>9.0352495793761797E-2</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E49" s="23">
         <v>9.03509105055256E-2</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F49" s="23">
         <v>9.0349112944317397E-2</v>
       </c>
-      <c r="G44" s="23">
+      <c r="G49" s="23">
         <v>9.0292047960886607E-2</v>
       </c>
-      <c r="H44" s="23">
+      <c r="H49" s="23">
         <v>8.3642402217548498E-2</v>
       </c>
-      <c r="I44" s="23">
+      <c r="I49" s="23">
         <v>8.3588880435537694E-2</v>
       </c>
-      <c r="J44" s="23">
+      <c r="J49" s="23">
         <v>8.3422244145891195E-2</v>
       </c>
-      <c r="K44" s="23">
+      <c r="K49" s="23">
         <v>8.3179781995007904E-2</v>
       </c>
-      <c r="L44" s="23">
+      <c r="L49" s="23">
         <v>8.2909632807747005E-2</v>
       </c>
-      <c r="M44" s="23">
+      <c r="M49" s="23">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="24"/>
-      <c r="R44" s="24"/>
-      <c r="S44" s="24"/>
-      <c r="T44" s="24"/>
-      <c r="U44" s="24"/>
-      <c r="V44" s="24"/>
-      <c r="W44" s="24"/>
-      <c r="X44" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y44" s="24"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="str">
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="23"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="24"/>
+      <c r="S49" s="24"/>
+      <c r="T49" s="24"/>
+      <c r="U49" s="24"/>
+      <c r="V49" s="24"/>
+      <c r="W49" s="24"/>
+      <c r="X49" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y49" s="24"/>
+    </row>
+    <row r="50" spans="1:25">
+      <c r="B50" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
       </c>
-      <c r="C45" s="23">
+      <c r="C50" s="23">
         <v>9.0399361562071207E-2</v>
       </c>
-      <c r="D45" s="23">
+      <c r="D50" s="23">
         <v>9.0352495793761797E-2</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E50" s="23">
         <v>9.03509105055256E-2</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F50" s="23">
         <v>9.0349112944317397E-2</v>
       </c>
-      <c r="G45" s="23">
+      <c r="G50" s="23">
         <v>9.0292047960886607E-2</v>
       </c>
-      <c r="H45" s="23">
+      <c r="H50" s="23">
         <v>8.3642402217548498E-2</v>
       </c>
-      <c r="I45" s="23">
+      <c r="I50" s="23">
         <v>8.3588880435537694E-2</v>
       </c>
-      <c r="J45" s="23">
+      <c r="J50" s="23">
         <v>8.3422244145891195E-2</v>
       </c>
-      <c r="K45" s="23">
+      <c r="K50" s="23">
         <v>8.3179781995007904E-2</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L50" s="23">
         <v>8.2909632807747005E-2</v>
       </c>
-      <c r="M45" s="23">
+      <c r="M50" s="23">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="24"/>
-      <c r="S45" s="24"/>
-      <c r="T45" s="24"/>
-      <c r="U45" s="24"/>
-      <c r="V45" s="24"/>
-      <c r="W45" s="24"/>
-      <c r="X45" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y45" s="24"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="23"/>
+      <c r="Q50" s="24"/>
+      <c r="R50" s="24"/>
+      <c r="S50" s="24"/>
+      <c r="T50" s="24"/>
+      <c r="U50" s="24"/>
+      <c r="V50" s="24"/>
+      <c r="W50" s="24"/>
+      <c r="X50" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y50" s="24"/>
+    </row>
+    <row r="54" spans="1:25">
+      <c r="A54" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C50" s="5">
+    <row r="55" spans="1:25">
+      <c r="C55" s="5">
         <v>2000</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D55" s="5">
         <v>2001</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E55" s="5">
         <v>2002</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F55" s="5">
         <v>2003</v>
       </c>
-      <c r="G50" s="5">
+      <c r="G55" s="5">
         <v>2004</v>
       </c>
-      <c r="H50" s="5">
+      <c r="H55" s="5">
         <v>2005</v>
       </c>
-      <c r="I50" s="5">
+      <c r="I55" s="5">
         <v>2006</v>
       </c>
-      <c r="J50" s="5">
+      <c r="J55" s="5">
         <v>2007</v>
       </c>
-      <c r="K50" s="5">
+      <c r="K55" s="5">
         <v>2008</v>
       </c>
-      <c r="L50" s="5">
+      <c r="L55" s="5">
         <v>2009</v>
       </c>
-      <c r="M50" s="5">
+      <c r="M55" s="5">
         <v>2010</v>
       </c>
-      <c r="N50" s="5">
+      <c r="N55" s="5">
         <v>2011</v>
       </c>
-      <c r="O50" s="5">
+      <c r="O55" s="5">
         <v>2012</v>
       </c>
-      <c r="P50" s="5">
+      <c r="P55" s="5">
         <v>2013</v>
       </c>
-      <c r="Q50" s="5">
+      <c r="Q55" s="5">
         <v>2014</v>
       </c>
-      <c r="R50" s="5">
+      <c r="R55" s="5">
         <v>2015</v>
       </c>
-      <c r="S50" s="5">
+      <c r="S55" s="5">
         <v>2016</v>
       </c>
-      <c r="T50" s="5">
+      <c r="T55" s="5">
         <v>2017</v>
       </c>
-      <c r="U50" s="5">
+      <c r="U55" s="5">
         <v>2018</v>
       </c>
-      <c r="V50" s="5">
+      <c r="V55" s="5">
         <v>2019</v>
       </c>
-      <c r="W50" s="5">
+      <c r="W55" s="5">
         <v>2020</v>
       </c>
-      <c r="Y50" s="5" t="s">
+      <c r="Y55" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
+    <row r="56" spans="1:25">
+      <c r="B56" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="25">
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="25">
         <v>0.876</v>
       </c>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="19"/>
-      <c r="R51" s="19"/>
-      <c r="S51" s="19"/>
-      <c r="T51" s="19"/>
-      <c r="U51" s="19"/>
-      <c r="V51" s="19"/>
-      <c r="W51" s="19"/>
-      <c r="X51" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y51" s="19"/>
+      <c r="N56" s="19"/>
+      <c r="O56" s="19"/>
+      <c r="P56" s="19"/>
+      <c r="Q56" s="19"/>
+      <c r="R56" s="19"/>
+      <c r="S56" s="19"/>
+      <c r="T56" s="19"/>
+      <c r="U56" s="19"/>
+      <c r="V56" s="19"/>
+      <c r="W56" s="19"/>
+      <c r="X56" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y56" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -8500,14 +8637,14 @@
       <selection activeCell="O69" sqref="O69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8575,7 +8712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="5" t="s">
         <v>40</v>
       </c>
@@ -8619,12 +8756,12 @@
       </c>
       <c r="Y3" s="24"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -8692,7 +8829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
@@ -8726,12 +8863,12 @@
       </c>
       <c r="Y9" s="24"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -8799,7 +8936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="5" t="s">
         <v>40</v>
       </c>
@@ -8857,12 +8994,12 @@
       </c>
       <c r="Y15" s="24"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -8930,7 +9067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25">
       <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
@@ -8960,7 +9097,7 @@
       </c>
       <c r="Y21" s="33"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="A25" s="21" t="s">
         <v>49</v>
       </c>
@@ -8989,7 +9126,7 @@
       <c r="X25" s="34"/>
       <c r="Y25" s="34"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="A26" s="34"/>
       <c r="B26" s="34"/>
       <c r="C26" s="35">
@@ -9060,7 +9197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="A27" s="34"/>
       <c r="B27" s="35" t="s">
         <v>40</v>
@@ -9091,13 +9228,13 @@
       </c>
       <c r="Y27" s="36"/>
     </row>
-    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" s="44" customFormat="1"/>
+    <row r="31" spans="1:25">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -9165,7 +9302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25">
       <c r="B33" s="5" t="s">
         <v>40</v>
       </c>
@@ -9223,12 +9360,12 @@
       </c>
       <c r="Y33" s="24"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -9296,7 +9433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25">
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -9334,15 +9471,15 @@
       </c>
       <c r="Y39" s="24"/>
     </row>
-    <row r="40" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" s="44" customFormat="1"/>
+    <row r="41" spans="1:25" s="44" customFormat="1"/>
+    <row r="42" spans="1:25" s="44" customFormat="1"/>
+    <row r="43" spans="1:25" s="44" customFormat="1">
       <c r="A43" s="70" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" s="44" customFormat="1">
       <c r="C44" s="71">
         <v>2000</v>
       </c>
@@ -9410,7 +9547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" s="44" customFormat="1">
       <c r="B45" s="71" t="s">
         <v>38</v>
       </c>
@@ -9442,15 +9579,15 @@
       </c>
       <c r="Y45" s="73"/>
     </row>
-    <row r="46" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" s="44" customFormat="1"/>
+    <row r="47" spans="1:25" s="44" customFormat="1"/>
+    <row r="48" spans="1:25" s="44" customFormat="1"/>
+    <row r="49" spans="1:25" s="44" customFormat="1">
       <c r="A49" s="70" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" s="44" customFormat="1">
       <c r="C50" s="71">
         <v>2000</v>
       </c>
@@ -9518,7 +9655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" s="44" customFormat="1">
       <c r="B51" s="71" t="s">
         <v>38</v>
       </c>
@@ -9550,15 +9687,15 @@
       </c>
       <c r="Y51" s="73"/>
     </row>
-    <row r="52" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" s="44" customFormat="1"/>
+    <row r="53" spans="1:25" s="44" customFormat="1"/>
+    <row r="54" spans="1:25" s="44" customFormat="1"/>
+    <row r="55" spans="1:25" s="44" customFormat="1">
       <c r="A55" s="70" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" s="44" customFormat="1">
       <c r="C56" s="71">
         <v>2000</v>
       </c>
@@ -9626,7 +9763,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" s="44" customFormat="1">
       <c r="B57" s="71" t="s">
         <v>38</v>
       </c>
@@ -9658,15 +9795,15 @@
       </c>
       <c r="Y57" s="73"/>
     </row>
-    <row r="58" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" s="44" customFormat="1"/>
+    <row r="59" spans="1:25" s="44" customFormat="1"/>
+    <row r="60" spans="1:25" s="44" customFormat="1"/>
+    <row r="61" spans="1:25" s="44" customFormat="1">
       <c r="A61" s="70" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" s="44" customFormat="1">
       <c r="C62" s="71">
         <v>2000</v>
       </c>
@@ -9734,7 +9871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" s="44" customFormat="1">
       <c r="B63" s="71" t="s">
         <v>38</v>
       </c>
@@ -9766,15 +9903,15 @@
       </c>
       <c r="Y63" s="73"/>
     </row>
-    <row r="64" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" s="44" customFormat="1"/>
+    <row r="65" spans="1:25" s="44" customFormat="1"/>
+    <row r="66" spans="1:25" s="44" customFormat="1"/>
+    <row r="67" spans="1:25" s="44" customFormat="1">
       <c r="A67" s="70" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" s="44" customFormat="1">
       <c r="C68" s="71">
         <v>2000</v>
       </c>
@@ -9842,7 +9979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" s="44" customFormat="1">
       <c r="B69" s="71" t="s">
         <v>38</v>
       </c>
@@ -9893,14 +10030,14 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35">
       <c r="A1" s="26" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35">
       <c r="A2" s="27"/>
       <c r="C2" s="5">
         <v>2000</v>
@@ -9969,7 +10106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35">
       <c r="A3" s="27"/>
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
@@ -10003,7 +10140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35">
       <c r="A4" s="27"/>
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
@@ -10037,7 +10174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10070,7 +10207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -10102,7 +10239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35">
       <c r="A7" s="27"/>
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
@@ -10136,7 +10273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35">
       <c r="A8" s="27"/>
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
@@ -10170,15 +10307,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35">
       <c r="A9" s="27"/>
     </row>
-    <row r="12" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" s="44" customFormat="1">
       <c r="A12" s="75" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" s="44" customFormat="1">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -10246,7 +10383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" s="44" customFormat="1">
       <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
@@ -10278,7 +10415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" s="44" customFormat="1">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -10314,7 +10451,7 @@
       <c r="AH15" s="5"/>
       <c r="AI15" s="5"/>
     </row>
-    <row r="16" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" s="44" customFormat="1">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -10350,7 +10487,7 @@
       <c r="AH16" s="5"/>
       <c r="AI16" s="5"/>
     </row>
-    <row r="17" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" s="44" customFormat="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -10386,12 +10523,12 @@
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35">
       <c r="A18" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35">
       <c r="C19" s="5">
         <v>2000</v>
       </c>
@@ -10459,7 +10596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10492,7 +10629,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10525,7 +10662,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35">
       <c r="B22" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10558,7 +10695,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35">
       <c r="B23" s="5" t="s">
         <v>16</v>
       </c>
@@ -10590,7 +10727,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10623,7 +10760,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10656,12 +10793,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" s="44" customFormat="1">
       <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" s="44" customFormat="1">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -10729,7 +10866,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" s="44" customFormat="1">
       <c r="B31" s="5" t="s">
         <v>38</v>
       </c>
@@ -10761,7 +10898,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" s="44" customFormat="1">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -10797,7 +10934,7 @@
       <c r="AH32" s="5"/>
       <c r="AI32" s="5"/>
     </row>
-    <row r="33" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" s="44" customFormat="1">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -10833,7 +10970,7 @@
       <c r="AH33" s="5"/>
       <c r="AI33" s="5"/>
     </row>
-    <row r="34" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" s="44" customFormat="1">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -10869,7 +11006,7 @@
       <c r="AH34" s="5"/>
       <c r="AI34" s="5"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35">
       <c r="A35" s="26" t="s">
         <v>53</v>
       </c>
@@ -10898,7 +11035,7 @@
       <c r="X35" s="27"/>
       <c r="Y35" s="27"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
       <c r="C36" s="28">
@@ -10969,7 +11106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35">
       <c r="A37" s="27"/>
       <c r="B37" s="28" t="s">
         <v>38</v>
@@ -11021,14 +11158,14 @@
       <selection activeCell="A76" sqref="A76:XFD80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -11096,7 +11233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11129,7 +11266,7 @@
       </c>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11162,7 +11299,7 @@
       </c>
       <c r="Y4" s="6"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11195,7 +11332,7 @@
       </c>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -11227,7 +11364,7 @@
       </c>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11260,7 +11397,7 @@
       </c>
       <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11293,12 +11430,12 @@
       </c>
       <c r="Y8" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -11366,7 +11503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11399,7 +11536,7 @@
       </c>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11432,7 +11569,7 @@
       </c>
       <c r="Y15" s="6"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11465,7 +11602,7 @@
       </c>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -11497,7 +11634,7 @@
       </c>
       <c r="Y17" s="6"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11530,7 +11667,7 @@
       </c>
       <c r="Y18" s="6"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11563,12 +11700,12 @@
       </c>
       <c r="Y19" s="6"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -11636,7 +11773,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11669,7 +11806,7 @@
       </c>
       <c r="Y25" s="6"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11702,7 +11839,7 @@
       </c>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11735,7 +11872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25">
       <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
@@ -11767,7 +11904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11800,7 +11937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11833,12 +11970,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25">
       <c r="C35" s="5">
         <v>2000</v>
       </c>
@@ -11906,7 +12043,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25">
       <c r="B36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11939,7 +12076,7 @@
       </c>
       <c r="Y36" s="19"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11972,7 +12109,7 @@
       </c>
       <c r="Y37" s="19"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12005,7 +12142,7 @@
       </c>
       <c r="Y38" s="19"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25">
       <c r="B39" s="5" t="s">
         <v>16</v>
       </c>
@@ -12037,7 +12174,7 @@
       </c>
       <c r="Y39" s="19"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25">
       <c r="B40" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12070,7 +12207,7 @@
       </c>
       <c r="Y40" s="19"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25">
       <c r="B41" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12103,12 +12240,12 @@
       </c>
       <c r="Y41" s="19"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25">
       <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25">
       <c r="C46" s="5">
         <v>2000</v>
       </c>
@@ -12176,7 +12313,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25">
       <c r="B47" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12209,7 +12346,7 @@
       </c>
       <c r="Y47" s="19"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25">
       <c r="B48" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12246,7 +12383,7 @@
       </c>
       <c r="Y48" s="19"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25">
       <c r="B49" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12279,7 +12416,7 @@
       </c>
       <c r="Y49" s="19"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25">
       <c r="B50" s="5" t="s">
         <v>16</v>
       </c>
@@ -12311,7 +12448,7 @@
       </c>
       <c r="Y50" s="19"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25">
       <c r="B51" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12348,7 +12485,7 @@
       </c>
       <c r="Y51" s="19"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25">
       <c r="B52" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12385,12 +12522,12 @@
       </c>
       <c r="Y52" s="19"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25">
       <c r="C57" s="5">
         <v>2000</v>
       </c>
@@ -12458,7 +12595,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25">
       <c r="B58" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12493,7 +12630,7 @@
       </c>
       <c r="Y58" s="19"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25">
       <c r="B59" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12528,7 +12665,7 @@
       </c>
       <c r="Y59" s="19"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25">
       <c r="B60" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12561,7 +12698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25">
       <c r="B61" s="5" t="s">
         <v>16</v>
       </c>
@@ -12593,7 +12730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25">
       <c r="B62" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12626,7 +12763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25">
       <c r="B63" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12659,12 +12796,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25">
       <c r="A67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25">
       <c r="C68" s="5">
         <v>2000</v>
       </c>
@@ -12732,7 +12869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25">
       <c r="B69" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12765,7 +12902,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25">
       <c r="B70" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12798,7 +12935,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25">
       <c r="B71" s="5" t="s">
         <v>16</v>
       </c>
@@ -12830,7 +12967,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25">
       <c r="B72" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>

</xml_diff>

<commit_message>
change vl in concentrated
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -566,7 +566,7 @@
     <numFmt numFmtId="169" formatCode="#,##0.000"/>
     <numFmt numFmtId="170" formatCode="#,##0.0"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1186,11 +1186,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="219" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="219" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="222">
@@ -1928,15 +1928,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1">
-      <c r="A2" s="77"/>
+      <c r="A2" s="78"/>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1">
-      <c r="A3" s="77"/>
+      <c r="A3" s="78"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="76"/>
@@ -7321,8 +7321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7922,33 +7922,33 @@
       <c r="B26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="78">
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77">
         <v>500</v>
       </c>
-      <c r="O26" s="78"/>
-      <c r="P26" s="78">
+      <c r="O26" s="77"/>
+      <c r="P26" s="77">
         <v>350</v>
       </c>
-      <c r="Q26" s="78">
+      <c r="Q26" s="77">
         <v>300</v>
       </c>
-      <c r="R26" s="78"/>
-      <c r="S26" s="78"/>
-      <c r="T26" s="78"/>
-      <c r="U26" s="78"/>
-      <c r="V26" s="78"/>
-      <c r="W26" s="78"/>
+      <c r="R26" s="77"/>
+      <c r="S26" s="77"/>
+      <c r="T26" s="77"/>
+      <c r="U26" s="77"/>
+      <c r="V26" s="77"/>
+      <c r="W26" s="77"/>
       <c r="X26" s="9" t="s">
         <v>25</v>
       </c>
@@ -10026,8 +10026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11125,7 +11125,10 @@
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
       <c r="P37" s="39"/>
-      <c r="Q37" s="39"/>
+      <c r="Q37" s="39">
+        <f>'Testing &amp; treatment'!Q20*0.8</f>
+        <v>38480</v>
+      </c>
       <c r="R37" s="39"/>
       <c r="S37" s="39"/>
       <c r="T37" s="39"/>
@@ -11135,9 +11138,7 @@
       <c r="X37" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="Y37" s="40">
-        <v>1</v>
-      </c>
+      <c r="Y37" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MODEL-INPUT CHANGES for vl, on second thought dont need this
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="135">
   <si>
     <t>For further details please visit: http://optimamodel.com/file/indicator-guide</t>
   </si>
@@ -550,9 +550,6 @@
   </si>
   <si>
     <t>Unit cost of treatment</t>
-  </si>
-  <si>
-    <t>Number of VL tests recommended per person per year</t>
   </si>
 </sst>
 </file>
@@ -796,7 +793,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="224">
+  <cellStyleXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -1021,6 +1018,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1198,7 +1199,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="224">
+  <cellStyles count="228">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1258,6 +1259,8 @@
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1402,6 +1405,8 @@
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -3386,10 +3391,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3867,18 +3872,10 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="59"/>
-      <c r="B41" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C41" s="61">
-        <v>2</v>
-      </c>
-      <c r="D41" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="E41" s="61">
-        <v>2.5</v>
-      </c>
+      <c r="B41" s="60"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="59"/>
@@ -3894,210 +3891,217 @@
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="59"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
+    <row r="44" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A44" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
     </row>
     <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A45" s="46" t="s">
-        <v>121</v>
-      </c>
+      <c r="A45" s="51"/>
       <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
+      <c r="C45" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="47" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A46" s="51"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="47" t="s">
-        <v>24</v>
+      <c r="B46" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="58">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D46" s="58">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E46" s="58">
+        <v>0.27500000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A47" s="51"/>
       <c r="B47" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C47" s="58">
-        <v>2.5999999999999999E-2</v>
+        <v>0.15</v>
       </c>
       <c r="D47" s="58">
-        <v>5.0000000000000001E-3</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E47" s="58">
-        <v>0.27500000000000002</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A48" s="51"/>
       <c r="B48" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C48" s="58">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D48" s="58">
-        <v>3.7999999999999999E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E48" s="58">
-        <v>0.88500000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A49" s="51"/>
       <c r="B49" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C49" s="58">
-        <v>0.1</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D49" s="58">
-        <v>2.1999999999999999E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E49" s="58">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="56" customFormat="1">
       <c r="A50" s="51"/>
       <c r="B50" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C50" s="58">
-        <v>5.2999999999999999E-2</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="D50" s="58">
-        <v>8.0000000000000002E-3</v>
+        <v>0.05</v>
       </c>
       <c r="E50" s="58">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="56" customFormat="1">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A51" s="51"/>
       <c r="B51" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C51" s="58">
-        <v>0.16200000000000001</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="D51" s="58">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="E51" s="58">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A52" s="51"/>
       <c r="B52" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C52" s="58">
-        <v>0.11700000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="D52" s="58">
-        <v>3.2000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="E52" s="58">
-        <v>0.68600000000000005</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A53" s="51"/>
       <c r="B53" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C53" s="58">
-        <v>0.09</v>
+        <v>0.111</v>
       </c>
       <c r="D53" s="58">
-        <v>1.9E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="E53" s="58">
-        <v>0.72299999999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A54" s="51"/>
       <c r="B54" s="2" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="C54" s="58">
-        <v>0.111</v>
+        <v>0.16</v>
       </c>
       <c r="D54" s="58">
-        <v>4.7E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E54" s="58">
-        <v>0.56299999999999994</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A55" s="51"/>
-      <c r="B55" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C55" s="58">
-        <v>0.16</v>
-      </c>
-      <c r="D55" s="58">
-        <v>0.05</v>
-      </c>
-      <c r="E55" s="58">
         <v>0.26</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+    <row r="55" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A55" s="57"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+    </row>
+    <row r="56" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A56" s="57"/>
       <c r="B56" s="57"/>
       <c r="C56" s="57"/>
       <c r="D56" s="57"/>
       <c r="E56" s="57"/>
     </row>
-    <row r="57" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
+    <row r="57" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1">
       <c r="A57" s="57"/>
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
       <c r="E57" s="57"/>
     </row>
-    <row r="58" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A58" s="57"/>
-      <c r="B58" s="57"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="57"/>
-    </row>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A59" s="1" t="s">
+    <row r="58" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A58" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C60" s="5" t="s">
+    <row r="59" spans="1:6" ht="13.5" customHeight="1">
+      <c r="C59" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D59" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1">
+    <row r="60" spans="1:6" ht="13.5" customHeight="1">
+      <c r="B60" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="58">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D60" s="58">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E60" s="58">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="13.5" customHeight="1">
       <c r="B61" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C61" s="58">
         <v>3.5999999999999999E-3</v>
@@ -4109,121 +4113,115 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1">
+    <row r="62" spans="1:6" ht="13.5" customHeight="1">
       <c r="B62" s="2" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C62" s="58">
-        <v>3.5999999999999999E-3</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="D62" s="58">
-        <v>2.8999999999999998E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="E62" s="58">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="13.5" customHeight="1">
       <c r="B63" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C63" s="58">
-        <v>5.7999999999999996E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="D63" s="58">
-        <v>4.7999999999999996E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E63" s="58">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="13.5" customHeight="1">
+        <v>1.01E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="B64" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C64" s="58">
-        <v>8.8000000000000005E-3</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D64" s="58">
-        <v>7.4999999999999997E-3</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="E64" s="58">
-        <v>1.01E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="15" customHeight="1">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F64" s="59"/>
+    </row>
+    <row r="65" spans="1:9">
       <c r="B65" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C65" s="58">
-        <v>5.8999999999999997E-2</v>
+        <v>0.32300000000000001</v>
       </c>
       <c r="D65" s="58">
-        <v>5.3999999999999999E-2</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="E65" s="58">
-        <v>7.9000000000000001E-2</v>
+        <v>0.432</v>
       </c>
       <c r="F65" s="59"/>
     </row>
     <row r="66" spans="1:9">
       <c r="B66" s="2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="C66" s="58">
-        <v>0.32300000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="D66" s="58">
-        <v>0.29599999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="E66" s="58">
-        <v>0.432</v>
+        <v>0.3</v>
       </c>
       <c r="F66" s="59"/>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C67" s="58">
-        <v>0.23</v>
+        <v>0.48780000000000001</v>
       </c>
       <c r="D67" s="58">
-        <v>0.15</v>
+        <v>0.28349999999999997</v>
       </c>
       <c r="E67" s="58">
-        <v>0.3</v>
+        <v>0.8417</v>
       </c>
       <c r="F67" s="59"/>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" s="2" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C68" s="58">
-        <v>0.48780000000000001</v>
+        <v>2.17</v>
       </c>
       <c r="D68" s="58">
-        <v>0.28349999999999997</v>
+        <v>1.27</v>
       </c>
       <c r="E68" s="58">
-        <v>0.8417</v>
+        <v>3.71</v>
       </c>
       <c r="F68" s="59"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="B69" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="58">
-        <v>2.17</v>
-      </c>
-      <c r="D69" s="58">
-        <v>1.27</v>
-      </c>
-      <c r="E69" s="58">
-        <v>3.71</v>
-      </c>
+      <c r="A69" s="59"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
       <c r="F69" s="59"/>
     </row>
     <row r="70" spans="1:9">
@@ -4233,6 +4231,9 @@
       <c r="D70" s="59"/>
       <c r="E70" s="59"/>
       <c r="F70" s="59"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="59"/>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="59"/>
@@ -4246,19 +4247,23 @@
       <c r="I71" s="59"/>
     </row>
     <row r="72" spans="1:9">
-      <c r="A72" s="59"/>
-      <c r="B72" s="60"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="59"/>
+      <c r="A72" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="F72" s="59"/>
       <c r="G72" s="59"/>
       <c r="H72" s="59"/>
       <c r="I72" s="59"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="1" t="s">
-        <v>97</v>
+      <c r="C73" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="F73" s="59"/>
       <c r="G73" s="59"/>
@@ -4266,32 +4271,35 @@
       <c r="I73" s="59"/>
     </row>
     <row r="74" spans="1:9">
-      <c r="C74" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>24</v>
+      <c r="B74" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" s="63">
+        <v>0.95</v>
+      </c>
+      <c r="D74" s="63">
+        <v>0.8</v>
+      </c>
+      <c r="E74" s="63">
+        <v>0.98</v>
       </c>
       <c r="F74" s="59"/>
-      <c r="G74" s="59"/>
-      <c r="H74" s="59"/>
-      <c r="I74" s="59"/>
+      <c r="G74" s="64"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="64"/>
     </row>
     <row r="75" spans="1:9">
       <c r="B75" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C75" s="63">
-        <v>0.95</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D75" s="63">
-        <v>0.8</v>
+        <v>0.47</v>
       </c>
       <c r="E75" s="63">
-        <v>0.98</v>
+        <v>0.67</v>
       </c>
       <c r="F75" s="59"/>
       <c r="G75" s="64"/>
@@ -4300,49 +4308,49 @@
     </row>
     <row r="76" spans="1:9">
       <c r="B76" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C76" s="63">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="D76" s="63">
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="E76" s="63">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="F76" s="59"/>
-      <c r="G76" s="64"/>
-      <c r="H76" s="64"/>
-      <c r="I76" s="64"/>
     </row>
     <row r="77" spans="1:9">
       <c r="B77" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C77" s="63">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="D77" s="63">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E77" s="63">
-        <v>0.68</v>
+        <v>5.19</v>
       </c>
       <c r="F77" s="59"/>
+      <c r="G77" s="64"/>
+      <c r="H77" s="64"/>
+      <c r="I77" s="64"/>
     </row>
     <row r="78" spans="1:9">
       <c r="B78" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C78" s="63">
-        <v>2.65</v>
+        <v>0.54</v>
       </c>
       <c r="D78" s="63">
-        <v>1.35</v>
+        <v>0.33</v>
       </c>
       <c r="E78" s="63">
-        <v>5.19</v>
+        <v>0.68</v>
       </c>
       <c r="F78" s="59"/>
       <c r="G78" s="64"/>
@@ -4351,16 +4359,16 @@
     </row>
     <row r="79" spans="1:9">
       <c r="B79" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C79" s="63">
-        <v>0.54</v>
+        <v>0.9</v>
       </c>
       <c r="D79" s="63">
-        <v>0.33</v>
+        <v>0.82</v>
       </c>
       <c r="E79" s="63">
-        <v>0.68</v>
+        <v>0.93</v>
       </c>
       <c r="F79" s="59"/>
       <c r="G79" s="64"/>
@@ -4369,16 +4377,16 @@
     </row>
     <row r="80" spans="1:9">
       <c r="B80" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C80" s="63">
-        <v>0.9</v>
+        <v>0.73</v>
       </c>
       <c r="D80" s="63">
-        <v>0.82</v>
+        <v>0.65</v>
       </c>
       <c r="E80" s="63">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="F80" s="59"/>
       <c r="G80" s="64"/>
@@ -4387,13 +4395,13 @@
     </row>
     <row r="81" spans="1:9">
       <c r="B81" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C81" s="63">
-        <v>0.73</v>
+        <v>0.5</v>
       </c>
       <c r="D81" s="63">
-        <v>0.65</v>
+        <v>0.3</v>
       </c>
       <c r="E81" s="63">
         <v>0.8</v>
@@ -4405,96 +4413,96 @@
     </row>
     <row r="82" spans="1:9">
       <c r="B82" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C82" s="63">
-        <v>0.5</v>
+        <v>0.92</v>
       </c>
       <c r="D82" s="63">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="E82" s="63">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="F82" s="59"/>
-      <c r="G82" s="64"/>
-      <c r="H82" s="64"/>
-      <c r="I82" s="64"/>
+      <c r="G82" s="59"/>
+      <c r="H82" s="59"/>
+      <c r="I82" s="59"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="B83" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C83" s="63">
-        <v>0.92</v>
-      </c>
-      <c r="D83" s="63">
-        <v>0.8</v>
-      </c>
-      <c r="E83" s="63">
-        <v>0.95</v>
-      </c>
+      <c r="A83" s="59"/>
+      <c r="B83" s="60"/>
+      <c r="C83" s="59"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="59"/>
       <c r="F83" s="59"/>
       <c r="G83" s="59"/>
       <c r="H83" s="59"/>
       <c r="I83" s="59"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="59"/>
-      <c r="B84" s="60"/>
-      <c r="C84" s="59"/>
-      <c r="D84" s="59"/>
-      <c r="E84" s="59"/>
-      <c r="F84" s="59"/>
-      <c r="G84" s="59"/>
-      <c r="H84" s="59"/>
+      <c r="A84" s="65"/>
+      <c r="B84" s="66"/>
+      <c r="C84" s="67"/>
+      <c r="D84" s="67"/>
+      <c r="E84" s="67"/>
+      <c r="F84" s="67"/>
+      <c r="G84" s="67"/>
+      <c r="H84" s="67"/>
       <c r="I84" s="59"/>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="65"/>
+      <c r="A85" s="67"/>
       <c r="B85" s="66"/>
-      <c r="C85" s="67"/>
-      <c r="D85" s="67"/>
-      <c r="E85" s="67"/>
+      <c r="C85" s="68"/>
+      <c r="D85" s="68"/>
+      <c r="E85" s="68"/>
       <c r="F85" s="67"/>
       <c r="G85" s="67"/>
       <c r="H85" s="67"/>
       <c r="I85" s="59"/>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="67"/>
-      <c r="B86" s="66"/>
-      <c r="C86" s="68"/>
-      <c r="D86" s="68"/>
-      <c r="E86" s="68"/>
-      <c r="F86" s="67"/>
-      <c r="G86" s="67"/>
-      <c r="H86" s="67"/>
-      <c r="I86" s="59"/>
+      <c r="A86" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B86" s="45"/>
+      <c r="C86" s="45"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="45"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="45"/>
+      <c r="H86" s="45"/>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="48" t="s">
-        <v>107</v>
-      </c>
+      <c r="A87" s="45"/>
       <c r="B87" s="45"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="45"/>
+      <c r="C87" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D87" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="49" t="s">
+        <v>24</v>
+      </c>
       <c r="F87" s="45"/>
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="45"/>
-      <c r="B88" s="45"/>
-      <c r="C88" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="D88" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="E88" s="49" t="s">
-        <v>24</v>
+      <c r="B88" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C88" s="61">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D88" s="61">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E88" s="61">
+        <v>0.20499999999999999</v>
       </c>
       <c r="F88" s="45"/>
       <c r="G88" s="45"/>
@@ -4503,16 +4511,16 @@
     <row r="89" spans="1:9">
       <c r="A89" s="45"/>
       <c r="B89" s="50" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C89" s="61">
-        <v>0.14599999999999999</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D89" s="61">
-        <v>9.6000000000000002E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E89" s="61">
-        <v>0.20499999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F89" s="45"/>
       <c r="G89" s="45"/>
@@ -4521,16 +4529,16 @@
     <row r="90" spans="1:9">
       <c r="A90" s="45"/>
       <c r="B90" s="50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C90" s="61">
-        <v>8.0000000000000002E-3</v>
+        <v>0.02</v>
       </c>
       <c r="D90" s="61">
-        <v>5.0000000000000001E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="E90" s="61">
-        <v>1.0999999999999999E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F90" s="45"/>
       <c r="G90" s="45"/>
@@ -4539,16 +4547,16 @@
     <row r="91" spans="1:9">
       <c r="A91" s="45"/>
       <c r="B91" s="50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C91" s="61">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D91" s="61">
-        <v>1.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E91" s="61">
-        <v>2.9000000000000001E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="F91" s="45"/>
       <c r="G91" s="45"/>
@@ -4557,16 +4565,16 @@
     <row r="92" spans="1:9">
       <c r="A92" s="45"/>
       <c r="B92" s="50" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C92" s="61">
-        <v>7.0000000000000007E-2</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="D92" s="61">
-        <v>4.8000000000000001E-2</v>
+        <v>0.114</v>
       </c>
       <c r="E92" s="61">
-        <v>9.4E-2</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="F92" s="45"/>
       <c r="G92" s="45"/>
@@ -4575,16 +4583,16 @@
     <row r="93" spans="1:9">
       <c r="A93" s="45"/>
       <c r="B93" s="50" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C93" s="61">
-        <v>0.26500000000000001</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="D93" s="61">
-        <v>0.114</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="E93" s="61">
-        <v>0.47399999999999998</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="F93" s="45"/>
       <c r="G93" s="45"/>
@@ -4593,35 +4601,22 @@
     <row r="94" spans="1:9">
       <c r="A94" s="45"/>
       <c r="B94" s="50" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C94" s="61">
-        <v>0.54700000000000004</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D94" s="61">
-        <v>0.38200000000000001</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E94" s="61">
-        <v>0.71499999999999997</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F94" s="45"/>
       <c r="G94" s="45"/>
       <c r="H94" s="45"/>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="45"/>
-      <c r="B95" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C95" s="61">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D95" s="61">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="E95" s="61">
-        <v>7.9000000000000001E-2</v>
-      </c>
       <c r="F95" s="45"/>
       <c r="G95" s="45"/>
       <c r="H95" s="45"/>
@@ -4635,11 +4630,6 @@
       <c r="F97" s="45"/>
       <c r="G97" s="45"/>
       <c r="H97" s="45"/>
-    </row>
-    <row r="98" spans="6:8">
-      <c r="F98" s="45"/>
-      <c r="G98" s="45"/>
-      <c r="H98" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
hotfix: undo spreadsheet change
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="136">
   <si>
     <t>For further details please visit: http://optimamodel.com/file/indicator-guide</t>
   </si>
@@ -804,7 +804,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="236">
+  <cellStyleXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -1037,10 +1037,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1218,7 +1214,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="236">
+  <cellStyles count="232">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="6"/>
     <cellStyle name="Comma 2 2" xfId="121"/>
@@ -1282,8 +1278,6 @@
     <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink 10" xfId="25"/>
     <cellStyle name="Followed Hyperlink 11" xfId="26"/>
     <cellStyle name="Followed Hyperlink 12" xfId="27"/>
@@ -1432,8 +1426,6 @@
     <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 2 2" xfId="119"/>
@@ -2686,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3405,8 +3397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E20"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3653,10 +3645,18 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="61">
+        <v>7.17</v>
+      </c>
+      <c r="D20" s="61">
+        <v>3.9</v>
+      </c>
+      <c r="E20" s="61">
+        <v>12.08</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="59"/>
@@ -4840,7 +4840,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6502,7 +6502,7 @@
   <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7327,8 +7327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10084,7 +10084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
@@ -11253,8 +11253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y60" sqref="Y60"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
aha, i found a problem
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/optima/tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="15980" tabRatio="805" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28575" windowHeight="15975" tabRatio="805" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -25,11 +20,8 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1953,55 +1945,55 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
     </row>
-    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="78"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="76"/>
     </row>
-    <row r="5" spans="1:1" ht="60" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="76" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="76"/>
     </row>
-    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="76"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="76" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="76"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="76" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="76"/>
     </row>
   </sheetData>
@@ -2021,14 +2013,14 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2096,7 +2088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2129,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2162,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2195,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -2227,7 +2219,7 @@
       </c>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2260,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2293,12 +2285,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -2366,7 +2358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2399,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2432,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2465,7 +2457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -2497,7 +2489,7 @@
       </c>
       <c r="Y17" s="19"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2530,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2563,12 +2555,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -2636,7 +2628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
@@ -2682,14 +2674,14 @@
       <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2715,7 +2707,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2727,7 +2719,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2743,7 +2735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2757,7 +2749,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2771,7 +2763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2787,7 +2779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2799,12 +2791,12 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2830,7 +2822,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2842,7 +2834,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2858,7 +2850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2872,7 +2864,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2886,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2902,7 +2894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2914,12 +2906,12 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2945,7 +2937,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2957,7 +2949,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2971,7 +2963,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2983,7 +2975,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2995,7 +2987,7 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3007,7 +2999,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3019,12 +3011,12 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3050,7 +3042,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3062,7 +3054,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3074,7 +3066,7 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3086,7 +3078,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3100,7 +3092,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3112,7 +3104,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3124,12 +3116,12 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3155,7 +3147,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3167,7 +3159,7 @@
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3179,12 +3171,12 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C53" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3210,7 +3202,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3222,7 +3214,7 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3234,7 +3226,7 @@
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3246,7 +3238,7 @@
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3258,7 +3250,7 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3270,7 +3262,7 @@
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3282,12 +3274,12 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3313,7 +3305,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3327,7 +3319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3339,7 +3331,7 @@
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3351,7 +3343,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3363,7 +3355,7 @@
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3375,7 +3367,7 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3401,16 +3393,16 @@
       <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="44"/>
-    <col min="2" max="2" width="37.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="8.83203125" style="44"/>
-    <col min="10" max="10" width="18.83203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="44"/>
+    <col min="1" max="1" width="8.85546875" style="44"/>
+    <col min="2" max="2" width="37.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.85546875" style="44"/>
+    <col min="10" max="10" width="18.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>71</v>
       </c>
@@ -3419,7 +3411,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="53" t="s">
@@ -3432,7 +3424,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="55" t="s">
         <v>72</v>
@@ -3447,7 +3439,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
       <c r="B4" s="55" t="s">
         <v>73</v>
@@ -3462,7 +3454,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
       <c r="B5" s="55" t="s">
         <v>74</v>
@@ -3477,7 +3469,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="55" t="s">
         <v>75</v>
@@ -3492,7 +3484,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="55" t="s">
         <v>76</v>
@@ -3507,7 +3499,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="55" t="s">
         <v>77</v>
@@ -3522,7 +3514,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="B9" s="55" t="s">
         <v>78</v>
@@ -3537,33 +3529,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="59"/>
       <c r="B10" s="60"/>
       <c r="C10" s="59"/>
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="59"/>
       <c r="B11" s="60"/>
       <c r="C11" s="59"/>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="59"/>
       <c r="B12" s="60"/>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
@@ -3574,7 +3566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>80</v>
       </c>
@@ -3588,7 +3580,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>81</v>
       </c>
@@ -3602,7 +3594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>82</v>
       </c>
@@ -3616,7 +3608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>83</v>
       </c>
@@ -3630,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>84</v>
       </c>
@@ -3644,7 +3636,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>85</v>
       </c>
@@ -3658,33 +3650,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="59"/>
       <c r="B21" s="60"/>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="59"/>
       <c r="B22" s="60"/>
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="59"/>
       <c r="B23" s="60"/>
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
         <v>26</v>
       </c>
@@ -3695,7 +3687,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>86</v>
       </c>
@@ -3709,7 +3701,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>82</v>
       </c>
@@ -3724,7 +3716,7 @@
       </c>
       <c r="G27" s="62"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
@@ -3738,7 +3730,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>88</v>
       </c>
@@ -3752,7 +3744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>89</v>
       </c>
@@ -3766,33 +3758,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="59"/>
       <c r="B31" s="60"/>
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="59"/>
       <c r="B32" s="60"/>
       <c r="C32" s="59"/>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="59"/>
       <c r="B33" s="60"/>
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>26</v>
       </c>
@@ -3803,7 +3795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>90</v>
       </c>
@@ -3817,7 +3809,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>91</v>
       </c>
@@ -3831,7 +3823,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
@@ -3845,7 +3837,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>93</v>
       </c>
@@ -3859,7 +3851,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
       <c r="B40" s="2" t="s">
         <v>119</v>
@@ -3874,7 +3866,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
       <c r="B41" s="2" t="s">
         <v>135</v>
@@ -3889,28 +3881,28 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="59"/>
       <c r="B42" s="60"/>
       <c r="C42" s="59"/>
       <c r="D42" s="59"/>
       <c r="E42" s="59"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="59"/>
       <c r="B43" s="60"/>
       <c r="C43" s="59"/>
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="59"/>
       <c r="B44" s="60"/>
       <c r="C44" s="59"/>
       <c r="D44" s="59"/>
       <c r="E44" s="59"/>
     </row>
-    <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
         <v>121</v>
       </c>
@@ -3919,7 +3911,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="51"/>
     </row>
-    <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
       <c r="B46" s="51"/>
       <c r="C46" s="47" t="s">
@@ -3932,7 +3924,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
       <c r="B47" s="2" t="s">
         <v>82</v>
@@ -3947,7 +3939,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
       <c r="B48" s="2" t="s">
         <v>90</v>
@@ -3962,7 +3954,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
       <c r="B49" s="2" t="s">
         <v>87</v>
@@ -3977,7 +3969,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
       <c r="B50" s="2" t="s">
         <v>91</v>
@@ -3992,7 +3984,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
       <c r="B51" s="2" t="s">
         <v>88</v>
@@ -4007,7 +3999,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
       <c r="B52" s="2" t="s">
         <v>92</v>
@@ -4022,7 +4014,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
       <c r="B53" s="2" t="s">
         <v>89</v>
@@ -4037,7 +4029,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="51"/>
       <c r="B54" s="2" t="s">
         <v>93</v>
@@ -4052,7 +4044,7 @@
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="51"/>
       <c r="B55" s="2" t="s">
         <v>122</v>
@@ -4067,33 +4059,33 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="57"/>
       <c r="B56" s="57"/>
       <c r="C56" s="57"/>
       <c r="D56" s="57"/>
       <c r="E56" s="57"/>
     </row>
-    <row r="57" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="57"/>
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
       <c r="E57" s="57"/>
     </row>
-    <row r="58" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="57"/>
       <c r="B58" s="57"/>
       <c r="C58" s="57"/>
       <c r="D58" s="57"/>
       <c r="E58" s="57"/>
     </row>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="5" t="s">
         <v>26</v>
       </c>
@@ -4104,7 +4096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>80</v>
       </c>
@@ -4118,7 +4110,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>81</v>
       </c>
@@ -4132,7 +4124,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>95</v>
       </c>
@@ -4146,7 +4138,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>83</v>
       </c>
@@ -4160,7 +4152,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>84</v>
       </c>
@@ -4175,7 +4167,7 @@
       </c>
       <c r="F65" s="59"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>85</v>
       </c>
@@ -4190,7 +4182,7 @@
       </c>
       <c r="F66" s="59"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>117</v>
       </c>
@@ -4205,7 +4197,7 @@
       </c>
       <c r="F67" s="59"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>118</v>
       </c>
@@ -4220,7 +4212,7 @@
       </c>
       <c r="F68" s="59"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>96</v>
       </c>
@@ -4235,7 +4227,7 @@
       </c>
       <c r="F69" s="59"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="59"/>
       <c r="B70" s="60"/>
       <c r="C70" s="59"/>
@@ -4243,7 +4235,7 @@
       <c r="E70" s="59"/>
       <c r="F70" s="59"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="59"/>
       <c r="B71" s="60"/>
       <c r="C71" s="59"/>
@@ -4254,7 +4246,7 @@
       <c r="H71" s="59"/>
       <c r="I71" s="59"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="59"/>
       <c r="B72" s="60"/>
       <c r="C72" s="59"/>
@@ -4265,7 +4257,7 @@
       <c r="H72" s="59"/>
       <c r="I72" s="59"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>97</v>
       </c>
@@ -4274,7 +4266,7 @@
       <c r="H73" s="59"/>
       <c r="I73" s="59"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C74" s="5" t="s">
         <v>26</v>
       </c>
@@ -4289,7 +4281,7 @@
       <c r="H74" s="59"/>
       <c r="I74" s="59"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
         <v>98</v>
       </c>
@@ -4307,7 +4299,7 @@
       <c r="H75" s="64"/>
       <c r="I75" s="64"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>99</v>
       </c>
@@ -4325,7 +4317,7 @@
       <c r="H76" s="64"/>
       <c r="I76" s="64"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>100</v>
       </c>
@@ -4340,7 +4332,7 @@
       </c>
       <c r="F77" s="59"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>101</v>
       </c>
@@ -4358,7 +4350,7 @@
       <c r="H78" s="64"/>
       <c r="I78" s="64"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>102</v>
       </c>
@@ -4376,7 +4368,7 @@
       <c r="H79" s="64"/>
       <c r="I79" s="64"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>103</v>
       </c>
@@ -4394,7 +4386,7 @@
       <c r="H80" s="64"/>
       <c r="I80" s="64"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>104</v>
       </c>
@@ -4412,7 +4404,7 @@
       <c r="H81" s="64"/>
       <c r="I81" s="64"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>105</v>
       </c>
@@ -4430,7 +4422,7 @@
       <c r="H82" s="64"/>
       <c r="I82" s="64"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>106</v>
       </c>
@@ -4448,7 +4440,7 @@
       <c r="H83" s="59"/>
       <c r="I83" s="59"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="59"/>
       <c r="B84" s="60"/>
       <c r="C84" s="59"/>
@@ -4459,7 +4451,7 @@
       <c r="H84" s="59"/>
       <c r="I84" s="59"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="65"/>
       <c r="B85" s="66"/>
       <c r="C85" s="67"/>
@@ -4470,7 +4462,7 @@
       <c r="H85" s="67"/>
       <c r="I85" s="59"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="67"/>
       <c r="B86" s="66"/>
       <c r="C86" s="68"/>
@@ -4481,7 +4473,7 @@
       <c r="H86" s="67"/>
       <c r="I86" s="59"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="48" t="s">
         <v>107</v>
       </c>
@@ -4493,7 +4485,7 @@
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="45"/>
       <c r="B88" s="45"/>
       <c r="C88" s="49" t="s">
@@ -4509,7 +4501,7 @@
       <c r="G88" s="45"/>
       <c r="H88" s="45"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="45"/>
       <c r="B89" s="50" t="s">
         <v>108</v>
@@ -4527,7 +4519,7 @@
       <c r="G89" s="45"/>
       <c r="H89" s="45"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="45"/>
       <c r="B90" s="50" t="s">
         <v>109</v>
@@ -4545,7 +4537,7 @@
       <c r="G90" s="45"/>
       <c r="H90" s="45"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="45"/>
       <c r="B91" s="50" t="s">
         <v>110</v>
@@ -4563,7 +4555,7 @@
       <c r="G91" s="45"/>
       <c r="H91" s="45"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="45"/>
       <c r="B92" s="50" t="s">
         <v>111</v>
@@ -4581,7 +4573,7 @@
       <c r="G92" s="45"/>
       <c r="H92" s="45"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="45"/>
       <c r="B93" s="50" t="s">
         <v>112</v>
@@ -4599,7 +4591,7 @@
       <c r="G93" s="45"/>
       <c r="H93" s="45"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="45"/>
       <c r="B94" s="50" t="s">
         <v>113</v>
@@ -4617,7 +4609,7 @@
       <c r="G94" s="45"/>
       <c r="H94" s="45"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="45"/>
       <c r="B95" s="50" t="s">
         <v>114</v>
@@ -4635,17 +4627,17 @@
       <c r="G95" s="45"/>
       <c r="H95" s="45"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F96" s="45"/>
       <c r="G96" s="45"/>
       <c r="H96" s="45"/>
     </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F97" s="45"/>
       <c r="G97" s="45"/>
       <c r="H97" s="45"/>
     </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F98" s="45"/>
       <c r="G98" s="45"/>
       <c r="H98" s="45"/>
@@ -4664,14 +4656,14 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4691,7 +4683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4714,7 +4706,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4737,7 +4729,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -4760,7 +4752,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -4783,7 +4775,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -4806,7 +4798,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -4843,15 +4835,15 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -4919,7 +4911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -4953,7 +4945,7 @@
       </c>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5009,7 +5001,7 @@
       </c>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5043,7 +5035,7 @@
       </c>
       <c r="Z5" s="8"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5077,7 +5069,7 @@
       </c>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5133,7 +5125,7 @@
       </c>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5167,7 +5159,7 @@
       </c>
       <c r="Z9" s="8"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5201,7 +5193,7 @@
       </c>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5257,7 +5249,7 @@
       </c>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5291,7 +5283,7 @@
       </c>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -5304,7 +5296,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
@@ -5337,7 +5329,7 @@
       </c>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -5392,7 +5384,7 @@
       </c>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -5425,7 +5417,7 @@
       </c>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -5438,7 +5430,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5472,7 +5464,7 @@
       </c>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5528,7 +5520,7 @@
       </c>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5562,7 +5554,7 @@
       </c>
       <c r="Z21" s="8"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5596,7 +5588,7 @@
       </c>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5652,7 +5644,7 @@
       </c>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5686,7 +5678,7 @@
       </c>
       <c r="Z25" s="8"/>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
         <v>28</v>
       </c>
@@ -5695,7 +5687,7 @@
         <v>21773583.295806497</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
         <v>29</v>
       </c>
@@ -5711,7 +5703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
       <c r="N29">
         <f>3529/'Population size'!N28*100</f>
         <v>7.0468319579830743</v>
@@ -5734,14 +5726,14 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -5809,7 +5801,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5849,7 +5841,7 @@
       </c>
       <c r="Z3" s="16"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5889,7 +5881,7 @@
       </c>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5929,7 +5921,7 @@
       </c>
       <c r="Z5" s="16"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5963,7 +5955,7 @@
       </c>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5999,7 +5991,7 @@
       </c>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6033,7 +6025,7 @@
       </c>
       <c r="Z9" s="16"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6069,7 +6061,7 @@
       </c>
       <c r="Z11" s="16"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6111,7 +6103,7 @@
       </c>
       <c r="Z12" s="16"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6147,7 +6139,7 @@
       </c>
       <c r="Z13" s="16"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
@@ -6182,7 +6174,7 @@
       </c>
       <c r="Z15" s="16"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -6223,7 +6215,7 @@
       </c>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -6258,7 +6250,7 @@
       </c>
       <c r="Z17" s="16"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6292,7 +6284,7 @@
       </c>
       <c r="Z19" s="16"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6340,7 +6332,7 @@
       </c>
       <c r="Z20" s="16"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6374,7 +6366,7 @@
       </c>
       <c r="Z21" s="16"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6408,7 +6400,7 @@
       </c>
       <c r="Z23" s="16"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6456,7 +6448,7 @@
       </c>
       <c r="Z24" s="16"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6505,14 +6497,14 @@
       <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -6580,7 +6572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6613,7 +6605,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6646,7 +6638,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6679,7 +6671,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -6711,7 +6703,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6744,7 +6736,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6777,12 +6769,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -6850,7 +6842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6883,7 +6875,7 @@
       </c>
       <c r="Y14" s="16"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6916,7 +6908,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6949,7 +6941,7 @@
       </c>
       <c r="Y16" s="16"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -6981,7 +6973,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7014,7 +7006,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7047,12 +7039,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -7120,7 +7112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7153,7 +7145,7 @@
       </c>
       <c r="Y25" s="16"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7186,7 +7178,7 @@
       </c>
       <c r="Y26" s="16"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7219,7 +7211,7 @@
       </c>
       <c r="Y27" s="16"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
@@ -7251,7 +7243,7 @@
       </c>
       <c r="Y28" s="16"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7284,7 +7276,7 @@
       </c>
       <c r="Y29" s="16"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7327,22 +7319,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -7410,7 +7402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7445,7 +7437,7 @@
       </c>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7482,7 +7474,7 @@
       </c>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7515,7 +7507,7 @@
       </c>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -7547,7 +7539,7 @@
       </c>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7580,7 +7572,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7613,12 +7605,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -7686,7 +7678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
@@ -7718,12 +7710,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" s="5">
         <v>2000</v>
       </c>
@@ -7791,7 +7783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
@@ -7853,7 +7845,7 @@
       </c>
       <c r="Y20" s="6"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="K21" s="44"/>
       <c r="L21" s="44"/>
       <c r="M21" s="44"/>
@@ -7862,7 +7854,7 @@
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
       <c r="M22" s="44"/>
@@ -7871,12 +7863,12 @@
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
     </row>
-    <row r="24" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="5">
         <v>2000</v>
       </c>
@@ -7944,7 +7936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>40</v>
       </c>
@@ -7980,15 +7972,15 @@
       </c>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
         <v>2000</v>
       </c>
@@ -8056,7 +8048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8089,7 +8081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -8122,7 +8114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -8155,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>16</v>
       </c>
@@ -8187,7 +8179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -8220,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -8253,12 +8245,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C42" s="5">
         <v>2000</v>
       </c>
@@ -8326,7 +8318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>40</v>
       </c>
@@ -8362,12 +8354,12 @@
       </c>
       <c r="Y43" s="6"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C48" s="5">
         <v>2000</v>
       </c>
@@ -8435,7 +8427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -8488,7 +8480,7 @@
       </c>
       <c r="Y49" s="24"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -8541,12 +8533,12 @@
       </c>
       <c r="Y50" s="24"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C55" s="5">
         <v>2000</v>
       </c>
@@ -8614,7 +8606,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>40</v>
       </c>
@@ -8660,14 +8652,14 @@
       <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8735,7 +8727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>40</v>
       </c>
@@ -8779,12 +8771,12 @@
       </c>
       <c r="Y3" s="24"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -8852,7 +8844,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
@@ -8886,12 +8878,12 @@
       </c>
       <c r="Y9" s="24"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -8959,7 +8951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>40</v>
       </c>
@@ -9017,7 +9009,7 @@
       </c>
       <c r="Y15" s="24"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
@@ -9031,7 +9023,7 @@
       <c r="M16" s="44"/>
       <c r="N16" s="44"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D17" s="44"/>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
@@ -9046,12 +9038,12 @@
       <c r="O17" s="44"/>
       <c r="P17" s="44"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -9119,7 +9111,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
@@ -9149,7 +9141,7 @@
       </c>
       <c r="Y21" s="33"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>49</v>
       </c>
@@ -9178,7 +9170,7 @@
       <c r="X25" s="34"/>
       <c r="Y25" s="34"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
       <c r="B26" s="34"/>
       <c r="C26" s="35">
@@ -9249,7 +9241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="35" t="s">
         <v>40</v>
@@ -9282,13 +9274,13 @@
       </c>
       <c r="Y27" s="36"/>
     </row>
-    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -9356,7 +9348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>40</v>
       </c>
@@ -9394,7 +9386,7 @@
       </c>
       <c r="Y33" s="24"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C34" s="44"/>
       <c r="D34" s="44"/>
       <c r="E34" s="44"/>
@@ -9408,7 +9400,7 @@
       <c r="M34" s="44"/>
       <c r="N34" s="44"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C35" s="44"/>
       <c r="D35" s="44"/>
       <c r="E35" s="44"/>
@@ -9423,12 +9415,12 @@
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -9496,7 +9488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -9534,15 +9526,15 @@
       </c>
       <c r="Y39" s="24"/>
     </row>
-    <row r="40" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="70" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="71">
         <v>2000</v>
       </c>
@@ -9610,7 +9602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="71" t="s">
         <v>38</v>
       </c>
@@ -9642,15 +9634,15 @@
       </c>
       <c r="Y45" s="73"/>
     </row>
-    <row r="46" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="70" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="71">
         <v>2000</v>
       </c>
@@ -9718,7 +9710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="71" t="s">
         <v>38</v>
       </c>
@@ -9750,15 +9742,15 @@
       </c>
       <c r="Y51" s="73"/>
     </row>
-    <row r="52" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="70" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="71">
         <v>2000</v>
       </c>
@@ -9826,7 +9818,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="71" t="s">
         <v>38</v>
       </c>
@@ -9858,15 +9850,15 @@
       </c>
       <c r="Y57" s="73"/>
     </row>
-    <row r="58" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="70" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="71">
         <v>2000</v>
       </c>
@@ -9934,7 +9926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="71" t="s">
         <v>38</v>
       </c>
@@ -9966,15 +9958,15 @@
       </c>
       <c r="Y63" s="73"/>
     </row>
-    <row r="64" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="70" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C68" s="71">
         <v>2000</v>
       </c>
@@ -10042,7 +10034,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="71" t="s">
         <v>38</v>
       </c>
@@ -10084,18 +10076,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="27"/>
       <c r="C2" s="5">
         <v>2000</v>
@@ -10164,7 +10156,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
@@ -10198,7 +10190,7 @@
       </c>
       <c r="Y3" s="23"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
@@ -10232,7 +10224,7 @@
       </c>
       <c r="Y4" s="23"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10265,7 +10257,7 @@
       </c>
       <c r="Y5" s="23"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -10297,7 +10289,7 @@
       </c>
       <c r="Y6" s="23"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
@@ -10331,7 +10323,7 @@
       </c>
       <c r="Y7" s="23"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
@@ -10365,15 +10357,15 @@
       </c>
       <c r="Y8" s="23"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
     </row>
-    <row r="12" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -10441,7 +10433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
@@ -10473,7 +10465,7 @@
       </c>
       <c r="Y14" s="69"/>
     </row>
-    <row r="15" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -10509,7 +10501,7 @@
       <c r="AH15" s="5"/>
       <c r="AI15" s="5"/>
     </row>
-    <row r="16" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -10545,7 +10537,7 @@
       <c r="AH16" s="5"/>
       <c r="AI16" s="5"/>
     </row>
-    <row r="17" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -10581,12 +10573,12 @@
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C19" s="5">
         <v>2000</v>
       </c>
@@ -10654,7 +10646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10675,7 +10667,7 @@
       <c r="P20" s="38"/>
       <c r="Q20" s="38"/>
       <c r="R20" s="38">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="S20" s="38"/>
       <c r="T20" s="38"/>
@@ -10687,7 +10679,7 @@
       </c>
       <c r="Y20" s="38"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10708,7 +10700,7 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="38">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="S21" s="38"/>
       <c r="T21" s="38"/>
@@ -10720,7 +10712,7 @@
       </c>
       <c r="Y21" s="38"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10741,7 +10733,7 @@
       <c r="P22" s="38"/>
       <c r="Q22" s="38"/>
       <c r="R22" s="38">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="S22" s="38"/>
       <c r="T22" s="38"/>
@@ -10753,7 +10745,7 @@
       </c>
       <c r="Y22" s="38"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>16</v>
       </c>
@@ -10773,7 +10765,7 @@
       <c r="P23" s="38"/>
       <c r="Q23" s="38"/>
       <c r="R23" s="38">
-        <v>0.55000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="S23" s="38"/>
       <c r="T23" s="38"/>
@@ -10785,7 +10777,7 @@
       </c>
       <c r="Y23" s="38"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10806,7 +10798,7 @@
       <c r="P24" s="38"/>
       <c r="Q24" s="38"/>
       <c r="R24" s="38">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="S24" s="38"/>
       <c r="T24" s="38"/>
@@ -10818,7 +10810,7 @@
       </c>
       <c r="Y24" s="38"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10839,7 +10831,7 @@
       <c r="P25" s="38"/>
       <c r="Q25" s="38"/>
       <c r="R25" s="38">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="S25" s="38"/>
       <c r="T25" s="38"/>
@@ -10851,12 +10843,12 @@
       </c>
       <c r="Y25" s="38"/>
     </row>
-    <row r="29" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -10924,7 +10916,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>38</v>
       </c>
@@ -10956,7 +10948,7 @@
       </c>
       <c r="Y31" s="6"/>
     </row>
-    <row r="32" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -10992,7 +10984,7 @@
       <c r="AH32" s="5"/>
       <c r="AI32" s="5"/>
     </row>
-    <row r="33" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -11028,7 +11020,7 @@
       <c r="AH33" s="5"/>
       <c r="AI33" s="5"/>
     </row>
-    <row r="34" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -11064,7 +11056,7 @@
       <c r="AH34" s="5"/>
       <c r="AI34" s="5"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>53</v>
       </c>
@@ -11093,7 +11085,7 @@
       <c r="X35" s="27"/>
       <c r="Y35" s="27"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
       <c r="C36" s="28">
@@ -11164,7 +11156,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
       <c r="B37" s="28" t="s">
         <v>38</v>
@@ -11257,14 +11249,14 @@
       <selection activeCell="A76" sqref="A76:XFD80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -11332,7 +11324,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11365,7 +11357,7 @@
       </c>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11398,7 +11390,7 @@
       </c>
       <c r="Y4" s="6"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11431,7 +11423,7 @@
       </c>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
@@ -11463,7 +11455,7 @@
       </c>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11496,7 +11488,7 @@
       </c>
       <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11529,12 +11521,12 @@
       </c>
       <c r="Y8" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -11602,7 +11594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11635,7 +11627,7 @@
       </c>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11668,7 +11660,7 @@
       </c>
       <c r="Y15" s="6"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11701,7 +11693,7 @@
       </c>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -11733,7 +11725,7 @@
       </c>
       <c r="Y17" s="6"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11766,7 +11758,7 @@
       </c>
       <c r="Y18" s="6"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11799,12 +11791,12 @@
       </c>
       <c r="Y19" s="6"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -11872,7 +11864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11905,7 +11897,7 @@
       </c>
       <c r="Y25" s="6"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11938,7 +11930,7 @@
       </c>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11971,7 +11963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
@@ -12003,7 +11995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12036,7 +12028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12069,12 +12061,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C35" s="5">
         <v>2000</v>
       </c>
@@ -12142,7 +12134,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12175,7 +12167,7 @@
       </c>
       <c r="Y36" s="19"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12208,7 +12200,7 @@
       </c>
       <c r="Y37" s="19"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12241,7 +12233,7 @@
       </c>
       <c r="Y38" s="19"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>16</v>
       </c>
@@ -12273,7 +12265,7 @@
       </c>
       <c r="Y39" s="19"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12306,7 +12298,7 @@
       </c>
       <c r="Y40" s="19"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12339,12 +12331,12 @@
       </c>
       <c r="Y41" s="19"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C46" s="5">
         <v>2000</v>
       </c>
@@ -12412,7 +12404,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12445,7 +12437,7 @@
       </c>
       <c r="Y47" s="19"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12482,7 +12474,7 @@
       </c>
       <c r="Y48" s="19"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12515,7 +12507,7 @@
       </c>
       <c r="Y49" s="19"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>16</v>
       </c>
@@ -12547,7 +12539,7 @@
       </c>
       <c r="Y50" s="19"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12584,7 +12576,7 @@
       </c>
       <c r="Y51" s="19"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12621,12 +12613,12 @@
       </c>
       <c r="Y52" s="19"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C57" s="5">
         <v>2000</v>
       </c>
@@ -12694,7 +12686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12729,7 +12721,7 @@
       </c>
       <c r="Y58" s="19"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12764,7 +12756,7 @@
       </c>
       <c r="Y59" s="19"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12797,7 +12789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>16</v>
       </c>
@@ -12829,7 +12821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12862,7 +12854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12895,12 +12887,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C68" s="5">
         <v>2000</v>
       </c>
@@ -12968,7 +12960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13001,7 +12993,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -13034,7 +13026,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>16</v>
       </c>
@@ -13066,7 +13058,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>

</xml_diff>

<commit_message>
changing pwids back to neither male nor female
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -4657,7 +4657,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4767,7 +4767,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
remove from demo spreadsheets
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/optima/tests/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28575" windowHeight="15975" tabRatio="805"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28580" windowHeight="15980" tabRatio="805" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,15 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -142,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="137">
   <si>
     <t>Populations</t>
   </si>
@@ -529,9 +542,6 @@
   </si>
   <si>
     <t>Average time taken to be linked to care for people with CD4&lt;200 (years)</t>
-  </si>
-  <si>
-    <t>Unit cost of treatment</t>
   </si>
   <si>
     <t>Number of VL tests recommended per person per year</t>
@@ -562,7 +572,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
@@ -572,7 +582,6 @@
     <numFmt numFmtId="169" formatCode="#,##0.000"/>
     <numFmt numFmtId="170" formatCode="#,##0.0"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1062,7 +1071,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1228,9 +1237,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1987,120 +1993,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="135.7109375" customWidth="1"/>
+    <col min="1" max="1" width="135.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="80" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="80"/>
+    </row>
+    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="80"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="77"/>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="77" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
-    </row>
-    <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
-    </row>
-    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="77"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="77" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="78"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="77"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="77" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="77"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="77" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="77"/>
+    </row>
+    <row r="13" spans="1:1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="77" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78" t="s">
+    <row r="14" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="78"/>
+    </row>
+    <row r="15" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="78" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="78"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-    </row>
-    <row r="13" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="78" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
-    </row>
-    <row r="15" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="80"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="80"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="80"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="80"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="80"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="79"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="79"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="79"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="79"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="79"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="79"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="79"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="79"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="79"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="79"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="79"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="79"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="79"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="79"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="79"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="44"/>
     </row>
   </sheetData>
@@ -2120,14 +2126,14 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2228,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2261,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2294,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -2326,7 +2332,7 @@
       </c>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2359,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2392,12 +2398,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -2465,7 +2471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2498,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2531,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2564,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
@@ -2596,7 +2602,7 @@
       </c>
       <c r="Y17" s="19"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2629,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2662,12 +2668,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -2735,7 +2741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
@@ -2781,14 +2787,14 @@
       <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2814,7 +2820,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2826,7 +2832,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2842,7 +2848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2856,7 +2862,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2870,7 +2876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -2886,7 +2892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -2898,12 +2904,12 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2929,7 +2935,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -2941,7 +2947,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -2957,7 +2963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -2971,7 +2977,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -2985,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3001,7 +3007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3013,12 +3019,12 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C24" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3044,7 +3050,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3056,7 +3062,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3070,7 +3076,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3082,7 +3088,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3094,7 +3100,7 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3106,7 +3112,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3118,12 +3124,12 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C35" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3149,7 +3155,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3161,7 +3167,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3173,7 +3179,7 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3185,7 +3191,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3199,7 +3205,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3211,7 +3217,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3223,12 +3229,12 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C46" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3254,7 +3260,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3266,7 +3272,7 @@
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3278,12 +3284,12 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C53" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3309,7 +3315,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3321,7 +3327,7 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3333,7 +3339,7 @@
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3345,7 +3351,7 @@
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3357,7 +3363,7 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3369,7 +3375,7 @@
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B59" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3381,12 +3387,12 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C64" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3412,7 +3418,7 @@
         <v>F 15+</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -3426,7 +3432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -3438,7 +3444,7 @@
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -3450,7 +3456,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" s="5" t="str">
         <f>Populations!$C$6</f>
         <v>PWID</v>
@@ -3462,7 +3468,7 @@
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B69" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -3474,7 +3480,7 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -3500,16 +3506,16 @@
       <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="44"/>
-    <col min="2" max="2" width="37.7109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="8.85546875" style="44"/>
-    <col min="10" max="10" width="18.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="44"/>
+    <col min="1" max="1" width="8.83203125" style="44"/>
+    <col min="2" max="2" width="37.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.83203125" style="44"/>
+    <col min="10" max="10" width="18.83203125" style="44" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
         <v>70</v>
       </c>
@@ -3518,7 +3524,7 @@
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="53" t="s">
@@ -3531,7 +3537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="52"/>
       <c r="B3" s="55" t="s">
         <v>71</v>
@@ -3546,7 +3552,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="52"/>
       <c r="B4" s="55" t="s">
         <v>72</v>
@@ -3561,7 +3567,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="52"/>
       <c r="B5" s="55" t="s">
         <v>73</v>
@@ -3576,7 +3582,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="52"/>
       <c r="B6" s="55" t="s">
         <v>74</v>
@@ -3591,7 +3597,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="52"/>
       <c r="B7" s="55" t="s">
         <v>75</v>
@@ -3606,7 +3612,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="52"/>
       <c r="B8" s="55" t="s">
         <v>76</v>
@@ -3621,7 +3627,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="52"/>
       <c r="B9" s="55" t="s">
         <v>77</v>
@@ -3636,33 +3642,33 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="B10" s="60"/>
       <c r="C10" s="59"/>
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="59"/>
       <c r="B11" s="60"/>
       <c r="C11" s="59"/>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="B12" s="60"/>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
@@ -3673,7 +3679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>79</v>
       </c>
@@ -3687,7 +3693,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>80</v>
       </c>
@@ -3701,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>81</v>
       </c>
@@ -3715,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>82</v>
       </c>
@@ -3729,7 +3735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>83</v>
       </c>
@@ -3743,7 +3749,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>84</v>
       </c>
@@ -3757,33 +3763,33 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="59"/>
       <c r="B21" s="60"/>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="59"/>
       <c r="B22" s="60"/>
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="59"/>
       <c r="B23" s="60"/>
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C25" s="5" t="s">
         <v>25</v>
       </c>
@@ -3794,7 +3800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>85</v>
       </c>
@@ -3808,7 +3814,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>81</v>
       </c>
@@ -3823,7 +3829,7 @@
       </c>
       <c r="G27" s="62"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>86</v>
       </c>
@@ -3837,7 +3843,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>87</v>
       </c>
@@ -3851,7 +3857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>88</v>
       </c>
@@ -3865,33 +3871,33 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="59"/>
       <c r="B31" s="60"/>
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="59"/>
       <c r="B32" s="60"/>
       <c r="C32" s="59"/>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="59"/>
       <c r="B33" s="60"/>
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C35" s="5" t="s">
         <v>25</v>
       </c>
@@ -3902,7 +3908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>89</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>90</v>
       </c>
@@ -3930,7 +3936,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>91</v>
       </c>
@@ -3944,7 +3950,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>92</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="51"/>
       <c r="B40" s="2" t="s">
         <v>118</v>
@@ -3973,10 +3979,10 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="59"/>
       <c r="B41" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C41" s="61">
         <v>2</v>
@@ -3988,28 +3994,28 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="59"/>
       <c r="B42" s="60"/>
       <c r="C42" s="59"/>
       <c r="D42" s="59"/>
       <c r="E42" s="59"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="59"/>
       <c r="B43" s="60"/>
       <c r="C43" s="59"/>
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="59"/>
       <c r="B44" s="60"/>
       <c r="C44" s="59"/>
       <c r="D44" s="59"/>
       <c r="E44" s="59"/>
     </row>
-    <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="46" t="s">
         <v>120</v>
       </c>
@@ -4018,7 +4024,7 @@
       <c r="D45" s="51"/>
       <c r="E45" s="51"/>
     </row>
-    <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="51"/>
       <c r="B46" s="51"/>
       <c r="C46" s="47" t="s">
@@ -4031,7 +4037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="51"/>
       <c r="B47" s="2" t="s">
         <v>81</v>
@@ -4046,7 +4052,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="51"/>
       <c r="B48" s="2" t="s">
         <v>89</v>
@@ -4061,7 +4067,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="51"/>
       <c r="B49" s="2" t="s">
         <v>86</v>
@@ -4076,7 +4082,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="51"/>
       <c r="B50" s="2" t="s">
         <v>90</v>
@@ -4091,7 +4097,7 @@
         <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="51"/>
       <c r="B51" s="2" t="s">
         <v>87</v>
@@ -4106,7 +4112,7 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="51"/>
       <c r="B52" s="2" t="s">
         <v>91</v>
@@ -4121,7 +4127,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="51"/>
       <c r="B53" s="2" t="s">
         <v>88</v>
@@ -4136,7 +4142,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="51"/>
       <c r="B54" s="2" t="s">
         <v>92</v>
@@ -4151,7 +4157,7 @@
         <v>0.56299999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="51"/>
       <c r="B55" s="2" t="s">
         <v>121</v>
@@ -4166,33 +4172,33 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="57"/>
       <c r="B56" s="57"/>
       <c r="C56" s="57"/>
       <c r="D56" s="57"/>
       <c r="E56" s="57"/>
     </row>
-    <row r="57" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="57"/>
       <c r="B57" s="57"/>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
       <c r="E57" s="57"/>
     </row>
-    <row r="58" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="57"/>
       <c r="B58" s="57"/>
       <c r="C58" s="57"/>
       <c r="D58" s="57"/>
       <c r="E58" s="57"/>
     </row>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" s="5" t="s">
         <v>25</v>
       </c>
@@ -4203,7 +4209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
         <v>79</v>
       </c>
@@ -4217,7 +4223,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>80</v>
       </c>
@@ -4231,7 +4237,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>94</v>
       </c>
@@ -4245,7 +4251,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>82</v>
       </c>
@@ -4259,7 +4265,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>83</v>
       </c>
@@ -4274,7 +4280,7 @@
       </c>
       <c r="F65" s="59"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>84</v>
       </c>
@@ -4289,7 +4295,7 @@
       </c>
       <c r="F66" s="59"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
         <v>116</v>
       </c>
@@ -4304,7 +4310,7 @@
       </c>
       <c r="F67" s="59"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>117</v>
       </c>
@@ -4319,7 +4325,7 @@
       </c>
       <c r="F68" s="59"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
         <v>95</v>
       </c>
@@ -4334,7 +4340,7 @@
       </c>
       <c r="F69" s="59"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="59"/>
       <c r="B70" s="60"/>
       <c r="C70" s="59"/>
@@ -4342,7 +4348,7 @@
       <c r="E70" s="59"/>
       <c r="F70" s="59"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="59"/>
       <c r="B71" s="60"/>
       <c r="C71" s="59"/>
@@ -4353,7 +4359,7 @@
       <c r="H71" s="59"/>
       <c r="I71" s="59"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="59"/>
       <c r="B72" s="60"/>
       <c r="C72" s="59"/>
@@ -4364,7 +4370,7 @@
       <c r="H72" s="59"/>
       <c r="I72" s="59"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>96</v>
       </c>
@@ -4373,7 +4379,7 @@
       <c r="H73" s="59"/>
       <c r="I73" s="59"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C74" s="5" t="s">
         <v>25</v>
       </c>
@@ -4388,7 +4394,7 @@
       <c r="H74" s="59"/>
       <c r="I74" s="59"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
         <v>97</v>
       </c>
@@ -4406,7 +4412,7 @@
       <c r="H75" s="64"/>
       <c r="I75" s="64"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
         <v>98</v>
       </c>
@@ -4424,7 +4430,7 @@
       <c r="H76" s="64"/>
       <c r="I76" s="64"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
         <v>99</v>
       </c>
@@ -4439,7 +4445,7 @@
       </c>
       <c r="F77" s="59"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
         <v>100</v>
       </c>
@@ -4457,7 +4463,7 @@
       <c r="H78" s="64"/>
       <c r="I78" s="64"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
         <v>101</v>
       </c>
@@ -4475,7 +4481,7 @@
       <c r="H79" s="64"/>
       <c r="I79" s="64"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
         <v>102</v>
       </c>
@@ -4493,7 +4499,7 @@
       <c r="H80" s="64"/>
       <c r="I80" s="64"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B81" s="2" t="s">
         <v>103</v>
       </c>
@@ -4511,7 +4517,7 @@
       <c r="H81" s="64"/>
       <c r="I81" s="64"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
         <v>104</v>
       </c>
@@ -4529,7 +4535,7 @@
       <c r="H82" s="64"/>
       <c r="I82" s="64"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B83" s="2" t="s">
         <v>105</v>
       </c>
@@ -4547,7 +4553,7 @@
       <c r="H83" s="59"/>
       <c r="I83" s="59"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="59"/>
       <c r="B84" s="60"/>
       <c r="C84" s="59"/>
@@ -4558,7 +4564,7 @@
       <c r="H84" s="59"/>
       <c r="I84" s="59"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="65"/>
       <c r="B85" s="66"/>
       <c r="C85" s="67"/>
@@ -4569,7 +4575,7 @@
       <c r="H85" s="67"/>
       <c r="I85" s="59"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="67"/>
       <c r="B86" s="66"/>
       <c r="C86" s="68"/>
@@ -4580,7 +4586,7 @@
       <c r="H86" s="67"/>
       <c r="I86" s="59"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="48" t="s">
         <v>106</v>
       </c>
@@ -4592,7 +4598,7 @@
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="45"/>
       <c r="B88" s="45"/>
       <c r="C88" s="49" t="s">
@@ -4608,7 +4614,7 @@
       <c r="G88" s="45"/>
       <c r="H88" s="45"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="45"/>
       <c r="B89" s="50" t="s">
         <v>107</v>
@@ -4626,7 +4632,7 @@
       <c r="G89" s="45"/>
       <c r="H89" s="45"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="45"/>
       <c r="B90" s="50" t="s">
         <v>108</v>
@@ -4644,7 +4650,7 @@
       <c r="G90" s="45"/>
       <c r="H90" s="45"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="45"/>
       <c r="B91" s="50" t="s">
         <v>109</v>
@@ -4662,7 +4668,7 @@
       <c r="G91" s="45"/>
       <c r="H91" s="45"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="45"/>
       <c r="B92" s="50" t="s">
         <v>110</v>
@@ -4680,7 +4686,7 @@
       <c r="G92" s="45"/>
       <c r="H92" s="45"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="45"/>
       <c r="B93" s="50" t="s">
         <v>111</v>
@@ -4698,7 +4704,7 @@
       <c r="G93" s="45"/>
       <c r="H93" s="45"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="45"/>
       <c r="B94" s="50" t="s">
         <v>112</v>
@@ -4716,7 +4722,7 @@
       <c r="G94" s="45"/>
       <c r="H94" s="45"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="45"/>
       <c r="B95" s="50" t="s">
         <v>113</v>
@@ -4734,17 +4740,17 @@
       <c r="G95" s="45"/>
       <c r="H95" s="45"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F96" s="45"/>
       <c r="G96" s="45"/>
       <c r="H96" s="45"/>
     </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F97" s="45"/>
       <c r="G97" s="45"/>
       <c r="H97" s="45"/>
     </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F98" s="45"/>
       <c r="G98" s="45"/>
       <c r="H98" s="45"/>
@@ -4763,14 +4769,14 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4790,7 +4796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4813,7 +4819,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -4836,7 +4842,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -4859,7 +4865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -4869,7 +4875,7 @@
       <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="77" t="b">
+      <c r="E6" s="76" t="b">
         <v>0</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -4882,7 +4888,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -4905,7 +4911,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -4942,15 +4948,15 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -5018,7 +5024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5052,7 +5058,7 @@
       </c>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5108,7 +5114,7 @@
       </c>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5142,7 +5148,7 @@
       </c>
       <c r="Z5" s="8"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5176,7 +5182,7 @@
       </c>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5232,7 +5238,7 @@
       </c>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -5266,7 +5272,7 @@
       </c>
       <c r="Z9" s="8"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5300,7 +5306,7 @@
       </c>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5356,7 +5362,7 @@
       </c>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -5390,7 +5396,7 @@
       </c>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -5403,7 +5409,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -5436,7 +5442,7 @@
       </c>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
@@ -5491,7 +5497,7 @@
       </c>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
@@ -5524,7 +5530,7 @@
       </c>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -5537,7 +5543,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5571,7 +5577,7 @@
       </c>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5627,7 +5633,7 @@
       </c>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -5661,7 +5667,7 @@
       </c>
       <c r="Z21" s="8"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5695,7 +5701,7 @@
       </c>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5751,7 +5757,7 @@
       </c>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -5785,7 +5791,7 @@
       </c>
       <c r="Z25" s="8"/>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
       <c r="M27" t="s">
         <v>27</v>
       </c>
@@ -5794,7 +5800,7 @@
         <v>21773583.295806497</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
       <c r="M28" t="s">
         <v>28</v>
       </c>
@@ -5810,7 +5816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
       <c r="N29">
         <f>3529/'Population size'!N28*100</f>
         <v>7.0468319579830743</v>
@@ -5833,14 +5839,14 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D2" s="5">
         <v>2000</v>
       </c>
@@ -5908,7 +5914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5948,7 +5954,7 @@
       </c>
       <c r="Z3" s="16"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -5988,7 +5994,7 @@
       </c>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6028,7 +6034,7 @@
       </c>
       <c r="Z5" s="16"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6062,7 +6068,7 @@
       </c>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6098,7 +6104,7 @@
       </c>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6132,7 +6138,7 @@
       </c>
       <c r="Z9" s="16"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6168,7 +6174,7 @@
       </c>
       <c r="Z11" s="16"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6210,7 +6216,7 @@
       </c>
       <c r="Z12" s="16"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6246,7 +6252,7 @@
       </c>
       <c r="Z13" s="16"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -6281,7 +6287,7 @@
       </c>
       <c r="Z15" s="16"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
@@ -6322,7 +6328,7 @@
       </c>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
@@ -6357,7 +6363,7 @@
       </c>
       <c r="Z17" s="16"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6391,7 +6397,7 @@
       </c>
       <c r="Z19" s="16"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6439,7 +6445,7 @@
       </c>
       <c r="Z20" s="16"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6473,7 +6479,7 @@
       </c>
       <c r="Z21" s="16"/>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6507,7 +6513,7 @@
       </c>
       <c r="Z23" s="16"/>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6555,7 +6561,7 @@
       </c>
       <c r="Z24" s="16"/>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6604,14 +6610,14 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -6679,7 +6685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6712,7 +6718,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6745,7 +6751,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6778,7 +6784,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -6810,7 +6816,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6843,7 +6849,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6876,12 +6882,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -6949,7 +6955,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6982,7 +6988,7 @@
       </c>
       <c r="Y14" s="16"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7015,7 +7021,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7048,7 +7054,7 @@
       </c>
       <c r="Y16" s="16"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
@@ -7080,7 +7086,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7113,7 +7119,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7146,12 +7152,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -7219,7 +7225,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7252,7 +7258,7 @@
       </c>
       <c r="Y25" s="16"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7285,7 +7291,7 @@
       </c>
       <c r="Y26" s="16"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7318,7 +7324,7 @@
       </c>
       <c r="Y27" s="16"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>15</v>
       </c>
@@ -7350,7 +7356,7 @@
       </c>
       <c r="Y28" s="16"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7383,7 +7389,7 @@
       </c>
       <c r="Y29" s="16"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7424,24 +7430,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y56"/>
+  <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -7509,7 +7515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -7544,7 +7550,7 @@
       </c>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -7581,7 +7587,7 @@
       </c>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -7614,7 +7620,7 @@
       </c>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -7646,7 +7652,7 @@
       </c>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -7679,7 +7685,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -7712,12 +7718,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -7785,7 +7791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -7817,12 +7823,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C19" s="5">
         <v>2000</v>
       </c>
@@ -7890,7 +7896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>39</v>
       </c>
@@ -7952,7 +7958,7 @@
       </c>
       <c r="Y20" s="6"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="K21" s="44"/>
       <c r="L21" s="44"/>
       <c r="M21" s="44"/>
@@ -7961,7 +7967,7 @@
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="K22" s="44"/>
       <c r="L22" s="44"/>
       <c r="M22" s="44"/>
@@ -7970,12 +7976,12 @@
       <c r="P22" s="44"/>
       <c r="Q22" s="44"/>
     </row>
-    <row r="24" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C25" s="5">
         <v>2000</v>
       </c>
@@ -8043,321 +8049,318 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="76"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="76"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="76">
-        <v>500</v>
-      </c>
-      <c r="O26" s="76"/>
-      <c r="P26" s="76">
-        <v>350</v>
-      </c>
-      <c r="Q26" s="76">
-        <v>300</v>
-      </c>
-      <c r="R26" s="76"/>
-      <c r="S26" s="76"/>
-      <c r="T26" s="76"/>
-      <c r="U26" s="76"/>
-      <c r="V26" s="76"/>
-      <c r="W26" s="76"/>
-      <c r="X26" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y26" s="6"/>
-    </row>
-    <row r="27" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C31" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D31" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E31" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F31" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G31" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H31" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I31" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J31" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K31" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L31" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M31" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N31" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O31" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P31" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q31" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R31" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S31" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T31" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U31" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V31" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W31" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y31" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="str">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y32" s="19">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y26" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="str">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
-      <c r="X33" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y33" s="19">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y27" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="str">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y34" s="19">
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y28" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="19"/>
-      <c r="X35" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y35" s="19">
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y29" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="str">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="19"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y36" s="19">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y30" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="str">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B31" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y31" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C36" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D36" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E36" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F36" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H36" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J36" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K36" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L36" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M36" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N36" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O36" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P36" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R36" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S36" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T36" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U36" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V36" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W36" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="6">
+        <v>500</v>
+      </c>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6">
+        <v>612</v>
+      </c>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22">
+        <v>702</v>
+      </c>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
       <c r="X37" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y37" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y37" s="6"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C42" s="5">
         <v>2000</v>
       </c>
@@ -8425,325 +8428,216 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="6">
-        <v>500</v>
-      </c>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6">
-        <v>612</v>
-      </c>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="22">
-        <v>702</v>
-      </c>
-      <c r="S43" s="22"/>
-      <c r="T43" s="22"/>
-      <c r="U43" s="22"/>
-      <c r="V43" s="22"/>
-      <c r="W43" s="22"/>
-      <c r="X43" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y43" s="6"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C48" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D48" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E48" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F48" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G48" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H48" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I48" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J48" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K48" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L48" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M48" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N48" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O48" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P48" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q48" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R48" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S48" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T48" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U48" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V48" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W48" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y48" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="str">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B43" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="C49" s="23">
+      <c r="C43" s="23">
         <v>9.0399361562071207E-2</v>
       </c>
-      <c r="D49" s="23">
+      <c r="D43" s="23">
         <v>9.0352495793761797E-2</v>
       </c>
-      <c r="E49" s="23">
+      <c r="E43" s="23">
         <v>9.03509105055256E-2</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F43" s="23">
         <v>9.0349112944317397E-2</v>
       </c>
-      <c r="G49" s="23">
+      <c r="G43" s="23">
         <v>9.0292047960886607E-2</v>
       </c>
-      <c r="H49" s="23">
+      <c r="H43" s="23">
         <v>8.3642402217548498E-2</v>
       </c>
-      <c r="I49" s="23">
+      <c r="I43" s="23">
         <v>8.3588880435537694E-2</v>
       </c>
-      <c r="J49" s="23">
+      <c r="J43" s="23">
         <v>8.3422244145891195E-2</v>
       </c>
-      <c r="K49" s="23">
+      <c r="K43" s="23">
         <v>8.3179781995007904E-2</v>
       </c>
-      <c r="L49" s="23">
+      <c r="L43" s="23">
         <v>8.2909632807747005E-2</v>
       </c>
-      <c r="M49" s="23">
+      <c r="M43" s="23">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="N49" s="23"/>
-      <c r="O49" s="23"/>
-      <c r="P49" s="23"/>
-      <c r="Q49" s="24"/>
-      <c r="R49" s="24"/>
-      <c r="S49" s="24"/>
-      <c r="T49" s="24"/>
-      <c r="U49" s="24"/>
-      <c r="V49" s="24"/>
-      <c r="W49" s="24"/>
-      <c r="X49" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y49" s="24"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B50" s="5" t="str">
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="24"/>
+      <c r="R43" s="24"/>
+      <c r="S43" s="24"/>
+      <c r="T43" s="24"/>
+      <c r="U43" s="24"/>
+      <c r="V43" s="24"/>
+      <c r="W43" s="24"/>
+      <c r="X43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y43" s="24"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B44" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
       </c>
-      <c r="C50" s="23">
+      <c r="C44" s="23">
         <v>9.0399361562071207E-2</v>
       </c>
-      <c r="D50" s="23">
+      <c r="D44" s="23">
         <v>9.0352495793761797E-2</v>
       </c>
-      <c r="E50" s="23">
+      <c r="E44" s="23">
         <v>9.03509105055256E-2</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F44" s="23">
         <v>9.0349112944317397E-2</v>
       </c>
-      <c r="G50" s="23">
+      <c r="G44" s="23">
         <v>9.0292047960886607E-2</v>
       </c>
-      <c r="H50" s="23">
+      <c r="H44" s="23">
         <v>8.3642402217548498E-2</v>
       </c>
-      <c r="I50" s="23">
+      <c r="I44" s="23">
         <v>8.3588880435537694E-2</v>
       </c>
-      <c r="J50" s="23">
+      <c r="J44" s="23">
         <v>8.3422244145891195E-2</v>
       </c>
-      <c r="K50" s="23">
+      <c r="K44" s="23">
         <v>8.3179781995007904E-2</v>
       </c>
-      <c r="L50" s="23">
+      <c r="L44" s="23">
         <v>8.2909632807747005E-2</v>
       </c>
-      <c r="M50" s="23">
+      <c r="M44" s="23">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="N50" s="23"/>
-      <c r="O50" s="23"/>
-      <c r="P50" s="23"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="24"/>
-      <c r="T50" s="24"/>
-      <c r="U50" s="24"/>
-      <c r="V50" s="24"/>
-      <c r="W50" s="24"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="24"/>
+      <c r="V44" s="24"/>
+      <c r="W44" s="24"/>
+      <c r="X44" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y44" s="24"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="C49" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D49" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E49" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F49" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G49" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H49" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I49" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J49" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K49" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L49" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M49" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N49" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O49" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P49" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q49" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R49" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S49" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T49" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U49" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V49" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W49" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y49" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B50" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="25">
+        <v>0.876</v>
+      </c>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
       <c r="X50" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y50" s="24"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C55" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D55" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E55" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F55" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G55" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H55" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I55" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J55" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K55" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L55" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M55" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N55" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O55" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P55" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q55" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R55" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S55" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T55" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U55" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V55" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W55" s="5">
-        <v>2020</v>
-      </c>
-      <c r="Y55" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="25">
-        <v>0.876</v>
-      </c>
-      <c r="N56" s="19"/>
-      <c r="O56" s="19"/>
-      <c r="P56" s="19"/>
-      <c r="Q56" s="19"/>
-      <c r="R56" s="19"/>
-      <c r="S56" s="19"/>
-      <c r="T56" s="19"/>
-      <c r="U56" s="19"/>
-      <c r="V56" s="19"/>
-      <c r="W56" s="19"/>
-      <c r="X56" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y56" s="19"/>
+      <c r="Y50" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -8759,14 +8653,14 @@
       <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -8834,7 +8728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
@@ -8878,12 +8772,12 @@
       </c>
       <c r="Y3" s="24"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C8" s="5">
         <v>2000</v>
       </c>
@@ -8951,7 +8845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>39</v>
       </c>
@@ -8985,12 +8879,12 @@
       </c>
       <c r="Y9" s="24"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C14" s="5">
         <v>2000</v>
       </c>
@@ -9058,7 +8952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>39</v>
       </c>
@@ -9116,7 +9010,7 @@
       </c>
       <c r="Y15" s="24"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
@@ -9130,7 +9024,7 @@
       <c r="M16" s="44"/>
       <c r="N16" s="44"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D17" s="44"/>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
@@ -9145,12 +9039,12 @@
       <c r="O17" s="44"/>
       <c r="P17" s="44"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C20" s="5">
         <v>2000</v>
       </c>
@@ -9218,7 +9112,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
@@ -9248,7 +9142,7 @@
       </c>
       <c r="Y21" s="33"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>48</v>
       </c>
@@ -9277,7 +9171,7 @@
       <c r="X25" s="34"/>
       <c r="Y25" s="34"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="34"/>
       <c r="B26" s="34"/>
       <c r="C26" s="35">
@@ -9348,7 +9242,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="35" t="s">
         <v>39</v>
@@ -9381,13 +9275,13 @@
       </c>
       <c r="Y27" s="36"/>
     </row>
-    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C32" s="5">
         <v>2000</v>
       </c>
@@ -9455,7 +9349,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>39</v>
       </c>
@@ -9493,7 +9387,7 @@
       </c>
       <c r="Y33" s="24"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C34" s="44"/>
       <c r="D34" s="44"/>
       <c r="E34" s="44"/>
@@ -9507,7 +9401,7 @@
       <c r="M34" s="44"/>
       <c r="N34" s="44"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C35" s="44"/>
       <c r="D35" s="44"/>
       <c r="E35" s="44"/>
@@ -9522,12 +9416,12 @@
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C38" s="5">
         <v>2000</v>
       </c>
@@ -9595,7 +9489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>39</v>
       </c>
@@ -9633,15 +9527,15 @@
       </c>
       <c r="Y39" s="24"/>
     </row>
-    <row r="40" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="70" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C44" s="71">
         <v>2000</v>
       </c>
@@ -9709,7 +9603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="71" t="s">
         <v>37</v>
       </c>
@@ -9741,15 +9635,15 @@
       </c>
       <c r="Y45" s="73"/>
     </row>
-    <row r="46" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="70" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C50" s="71">
         <v>2000</v>
       </c>
@@ -9817,7 +9711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="71" t="s">
         <v>37</v>
       </c>
@@ -9849,15 +9743,15 @@
       </c>
       <c r="Y51" s="73"/>
     </row>
-    <row r="52" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="70" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C56" s="71">
         <v>2000</v>
       </c>
@@ -9925,7 +9819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="71" t="s">
         <v>37</v>
       </c>
@@ -9957,15 +9851,15 @@
       </c>
       <c r="Y57" s="73"/>
     </row>
-    <row r="58" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="70" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C62" s="71">
         <v>2000</v>
       </c>
@@ -10033,7 +9927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="71" t="s">
         <v>37</v>
       </c>
@@ -10065,15 +9959,15 @@
       </c>
       <c r="Y63" s="73"/>
     </row>
-    <row r="64" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="70" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C68" s="71">
         <v>2000</v>
       </c>
@@ -10141,7 +10035,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="71" t="s">
         <v>37</v>
       </c>
@@ -10187,14 +10081,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="27"/>
       <c r="C2" s="5">
         <v>2000</v>
@@ -10263,7 +10157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
@@ -10297,7 +10191,7 @@
       </c>
       <c r="Y3" s="23"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
@@ -10331,7 +10225,7 @@
       </c>
       <c r="Y4" s="23"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10364,7 +10258,7 @@
       </c>
       <c r="Y5" s="23"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -10396,7 +10290,7 @@
       </c>
       <c r="Y6" s="23"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
@@ -10430,7 +10324,7 @@
       </c>
       <c r="Y7" s="23"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
@@ -10464,15 +10358,15 @@
       </c>
       <c r="Y8" s="23"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
     </row>
-    <row r="12" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="75" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -10540,7 +10434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -10572,7 +10466,7 @@
       </c>
       <c r="Y14" s="69"/>
     </row>
-    <row r="15" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -10608,7 +10502,7 @@
       <c r="AH15" s="5"/>
       <c r="AI15" s="5"/>
     </row>
-    <row r="16" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -10644,7 +10538,7 @@
       <c r="AH16" s="5"/>
       <c r="AI16" s="5"/>
     </row>
-    <row r="17" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -10680,12 +10574,12 @@
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C19" s="5">
         <v>2000</v>
       </c>
@@ -10753,7 +10647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -10786,7 +10680,7 @@
       </c>
       <c r="Y20" s="38"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -10819,7 +10713,7 @@
       </c>
       <c r="Y21" s="38"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -10852,7 +10746,7 @@
       </c>
       <c r="Y22" s="38"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
@@ -10884,7 +10778,7 @@
       </c>
       <c r="Y23" s="38"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -10917,7 +10811,7 @@
       </c>
       <c r="Y24" s="38"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -10950,12 +10844,12 @@
       </c>
       <c r="Y25" s="38"/>
     </row>
-    <row r="29" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C30" s="5">
         <v>2000</v>
       </c>
@@ -11023,7 +10917,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>37</v>
       </c>
@@ -11055,7 +10949,7 @@
       </c>
       <c r="Y31" s="6"/>
     </row>
-    <row r="32" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -11091,7 +10985,7 @@
       <c r="AH32" s="5"/>
       <c r="AI32" s="5"/>
     </row>
-    <row r="33" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -11127,7 +11021,7 @@
       <c r="AH33" s="5"/>
       <c r="AI33" s="5"/>
     </row>
-    <row r="34" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -11163,7 +11057,7 @@
       <c r="AH34" s="5"/>
       <c r="AI34" s="5"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
         <v>52</v>
       </c>
@@ -11192,7 +11086,7 @@
       <c r="X35" s="27"/>
       <c r="Y35" s="27"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
       <c r="C36" s="28">
@@ -11263,7 +11157,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" s="27"/>
       <c r="B37" s="28" t="s">
         <v>37</v>
@@ -11356,14 +11250,14 @@
       <selection activeCell="A76" sqref="A76:XFD80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -11431,7 +11325,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11464,7 +11358,7 @@
       </c>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11497,7 +11391,7 @@
       </c>
       <c r="Y4" s="6"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11530,7 +11424,7 @@
       </c>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -11562,7 +11456,7 @@
       </c>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11595,7 +11489,7 @@
       </c>
       <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11628,12 +11522,12 @@
       </c>
       <c r="Y8" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -11701,7 +11595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -11734,7 +11628,7 @@
       </c>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -11767,7 +11661,7 @@
       </c>
       <c r="Y15" s="6"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -11800,7 +11694,7 @@
       </c>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
@@ -11832,7 +11726,7 @@
       </c>
       <c r="Y17" s="6"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -11865,7 +11759,7 @@
       </c>
       <c r="Y18" s="6"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -11898,12 +11792,12 @@
       </c>
       <c r="Y19" s="6"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -11971,7 +11865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12004,7 +11898,7 @@
       </c>
       <c r="Y25" s="6"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12037,7 +11931,7 @@
       </c>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12070,7 +11964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>15</v>
       </c>
@@ -12102,7 +11996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12135,7 +12029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12168,12 +12062,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C35" s="5">
         <v>2000</v>
       </c>
@@ -12241,7 +12135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12274,7 +12168,7 @@
       </c>
       <c r="Y36" s="19"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12307,7 +12201,7 @@
       </c>
       <c r="Y37" s="19"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12340,7 +12234,7 @@
       </c>
       <c r="Y38" s="19"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
@@ -12372,7 +12266,7 @@
       </c>
       <c r="Y39" s="19"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12405,7 +12299,7 @@
       </c>
       <c r="Y40" s="19"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12438,12 +12332,12 @@
       </c>
       <c r="Y41" s="19"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C46" s="5">
         <v>2000</v>
       </c>
@@ -12511,7 +12405,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12544,7 +12438,7 @@
       </c>
       <c r="Y47" s="19"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B48" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12581,7 +12475,7 @@
       </c>
       <c r="Y48" s="19"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12614,7 +12508,7 @@
       </c>
       <c r="Y49" s="19"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B50" s="5" t="s">
         <v>15</v>
       </c>
@@ -12646,7 +12540,7 @@
       </c>
       <c r="Y50" s="19"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B51" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12683,7 +12577,7 @@
       </c>
       <c r="Y51" s="19"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B52" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12720,12 +12614,12 @@
       </c>
       <c r="Y52" s="19"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C57" s="5">
         <v>2000</v>
       </c>
@@ -12793,7 +12687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -12828,7 +12722,7 @@
       </c>
       <c r="Y58" s="19"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B59" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -12863,7 +12757,7 @@
       </c>
       <c r="Y59" s="19"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -12896,7 +12790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B61" s="5" t="s">
         <v>15</v>
       </c>
@@ -12928,7 +12822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B62" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -12961,7 +12855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B63" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -12994,12 +12888,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C68" s="5">
         <v>2000</v>
       </c>
@@ -13067,7 +12961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B69" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -13100,7 +12994,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B70" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -13133,7 +13027,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B71" s="5" t="s">
         <v>15</v>
       </c>
@@ -13165,7 +13059,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B72" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>

</xml_diff>

<commit_message>
going to try without or
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -560,7 +560,7 @@
     <t>Proportion of those with VL failure who are provided with effective adherence support or a successful new regimen (%/year)</t>
   </si>
   <si>
-    <t>Spreadsheet created with Optima version 2.8.1</t>
+    <t>Spreadsheet created with Optima version 2.9.0</t>
   </si>
 </sst>
 </file>
@@ -2045,7 +2045,7 @@
   <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update default suppressive ART efficacy
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rowan.martin-hughes\Documents\GitHub\optima\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070200CB-6C22-4226-B3A9-69EB93746E17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2568C48D-952E-4773-8052-B9DB10BA0674}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5055" windowWidth="29040" windowHeight="15990" tabRatio="805" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1323,11 +1323,11 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="238">
@@ -2093,8 +2093,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,15 +2103,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
+      <c r="A2" s="84"/>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83"/>
+      <c r="A3" s="84"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="77"/>
@@ -2133,7 +2133,7 @@
       <c r="A8" s="77"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="83" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3605,8 +3605,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4646,13 +4646,13 @@
         <v>102</v>
       </c>
       <c r="C83" s="63">
+        <v>1</v>
+      </c>
+      <c r="D83" s="63">
         <v>0.92</v>
       </c>
-      <c r="D83" s="63">
-        <v>0.8</v>
-      </c>
       <c r="E83" s="63">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F83" s="59"/>
       <c r="G83" s="59"/>

</xml_diff>

<commit_message>
Update version in databook details also
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2888DBD-73B4-4748-865F-6CC488176A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EA7740-1FC9-4F87-A885-78031AB05A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="805" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
     <t>ARV-based post-exposure prophylaxis</t>
   </si>
   <si>
-    <t>Spreadsheet created with Optima version 2.10.0</t>
+    <t>Spreadsheet created with Optima version 2.10.1</t>
   </si>
 </sst>
 </file>
@@ -1323,13 +1323,13 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="170" fontId="10" fillId="5" borderId="1" xfId="124" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="5" borderId="1" xfId="124" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="238">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2094,8 +2094,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,7 +2134,7 @@
       <c r="A8" s="77"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="85" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3606,8 +3606,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="K81" sqref="K81"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="I98" sqref="I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4726,13 +4726,13 @@
       <c r="B89" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="C89" s="85">
+      <c r="C89" s="83">
         <v>0.18099999999999999</v>
       </c>
-      <c r="D89" s="85">
+      <c r="D89" s="83">
         <v>0.121</v>
       </c>
-      <c r="E89" s="85">
+      <c r="E89" s="83">
         <v>0.249</v>
       </c>
       <c r="F89" s="45"/>
@@ -4744,13 +4744,13 @@
       <c r="B90" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="C90" s="85">
+      <c r="C90" s="83">
         <v>0.01</v>
       </c>
-      <c r="D90" s="85">
+      <c r="D90" s="83">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E90" s="85">
+      <c r="E90" s="83">
         <v>1.4E-2</v>
       </c>
       <c r="F90" s="45"/>
@@ -4762,13 +4762,13 @@
       <c r="B91" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C91" s="85">
+      <c r="C91" s="83">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D91" s="85">
+      <c r="D91" s="83">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E91" s="85">
+      <c r="E91" s="83">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F91" s="45"/>
@@ -4780,13 +4780,13 @@
       <c r="B92" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="C92" s="85">
+      <c r="C92" s="83">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="D92" s="85">
+      <c r="D92" s="83">
         <v>5.5E-2</v>
       </c>
-      <c r="E92" s="85">
+      <c r="E92" s="83">
         <v>0.107</v>
       </c>
       <c r="F92" s="45"/>
@@ -4798,13 +4798,13 @@
       <c r="B93" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="C93" s="85">
+      <c r="C93" s="83">
         <v>0.28899999999999998</v>
       </c>
-      <c r="D93" s="85">
+      <c r="D93" s="83">
         <v>0.128</v>
       </c>
-      <c r="E93" s="85">
+      <c r="E93" s="83">
         <v>0.499</v>
       </c>
       <c r="F93" s="45"/>
@@ -4816,13 +4816,13 @@
       <c r="B94" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="C94" s="85">
+      <c r="C94" s="83">
         <v>0.58199999999999996</v>
       </c>
-      <c r="D94" s="85">
+      <c r="D94" s="83">
         <v>0.40600000000000003</v>
       </c>
-      <c r="E94" s="85">
+      <c r="E94" s="83">
         <v>0.74299999999999999</v>
       </c>
       <c r="F94" s="45"/>
@@ -4834,13 +4834,13 @@
       <c r="B95" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="C95" s="85">
+      <c r="C95" s="83">
         <v>7.8E-2</v>
       </c>
-      <c r="D95" s="85">
+      <c r="D95" s="83">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="E95" s="85">
+      <c r="E95" s="83">
         <v>0.111</v>
       </c>
       <c r="F95" s="45"/>

</xml_diff>

<commit_message>
Update demo databooks to 2_11_0
</commit_message>
<xml_diff>
--- a/tests/concentrated.xlsx
+++ b/tests/concentrated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\optima\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rowan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EA7740-1FC9-4F87-A885-78031AB05A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22697A3D-4243-4ECE-AA6A-5EAF2F12129A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="805" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Partnerships &amp; transitions" sheetId="11" r:id="rId11"/>
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,6 +35,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -162,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="142">
   <si>
     <t>Populations</t>
   </si>
@@ -333,9 +334,6 @@
   </si>
   <si>
     <t>Percentage of people who used a condom at last act with commercial partners</t>
-  </si>
-  <si>
-    <t>Percentage of males who have been circumcised</t>
   </si>
   <si>
     <t>Average number of injections per person per year</t>
@@ -518,28 +516,10 @@
     <t>CD4 change due to non-suppressive ART (%/year)</t>
   </si>
   <si>
-    <t>PLHIV aware of their status (%)</t>
-  </si>
-  <si>
-    <t>Diagnosed PLHIV in care (%)</t>
-  </si>
-  <si>
-    <t>PLHIV in care on treatment (%)</t>
-  </si>
-  <si>
-    <t>Pregnant women on PMTCT (%)</t>
-  </si>
-  <si>
-    <t>People on ART with viral suppression (%)</t>
-  </si>
-  <si>
     <t>Percentage of people with CD4&lt;200 lost to follow-up (%/year)</t>
   </si>
   <si>
     <t>Average time taken to be linked to care for people with CD4&lt;200 (years)</t>
-  </si>
-  <si>
-    <t>Number of VL tests recommended per person per year</t>
   </si>
   <si>
     <t>O P T I M A   H I V</t>
@@ -569,13 +549,37 @@
     <t>Proportion of those with VL failure who are provided with effective adherence support or a successful new regimen (%/year)</t>
   </si>
   <si>
+    <t>Spreadsheet created with Optima version 2.11.0</t>
+  </si>
+  <si>
+    <t>Percentage of people who age into the next age category per year</t>
+  </si>
+  <si>
     <t>Proportion of exposure events covered by ARV-based pre-exposure prophylaxis</t>
   </si>
   <si>
     <t>Proportion of exposure events covered by ARV-based post-exposure prophylaxis</t>
   </si>
   <si>
-    <t>Average time taken to be returned to care after loss to follow-up (years)</t>
+    <t>Percentage of people lost to follow-up who are returned to care per year (%/year)</t>
+  </si>
+  <si>
+    <t>Percent of people living with HIV who know their status</t>
+  </si>
+  <si>
+    <t>Percent of people who know their status who are retained in care</t>
+  </si>
+  <si>
+    <t>Percent of people who know their status who are on ART</t>
+  </si>
+  <si>
+    <t>Coverage of pregnant women who receive ARV for PMTCT</t>
+  </si>
+  <si>
+    <t>Percent of people on ART who achieve viral suppression</t>
+  </si>
+  <si>
+    <t>Percentage of males who have been traditionally circumcised</t>
   </si>
   <si>
     <t>Number of voluntary medical male circumcisions</t>
@@ -585,9 +589,6 @@
   </si>
   <si>
     <t>ARV-based post-exposure prophylaxis</t>
-  </si>
-  <si>
-    <t>Spreadsheet created with Optima version 2.10.1</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1138,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1323,12 +1324,11 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="10" fillId="5" borderId="1" xfId="124" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="237" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="238">
@@ -2091,11 +2091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2104,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2119,7 +2118,7 @@
     </row>
     <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -2127,15 +2126,15 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="77"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="85" t="s">
-        <v>141</v>
+      <c r="A9" s="83" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -2143,7 +2142,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -2151,7 +2150,7 @@
     </row>
     <row r="13" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2159,7 +2158,7 @@
     </row>
     <row r="15" spans="1:1" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="78" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2221,7 +2220,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2232,7 +2230,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -2502,7 +2500,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -2772,7 +2770,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -2883,7 +2881,6 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2894,7 +2891,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3009,7 +3006,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3124,7 +3121,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3229,7 +3226,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3334,7 +3331,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3389,7 +3386,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3492,7 +3489,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3603,11 +3600,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3621,7 +3617,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -3644,7 +3640,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="58">
         <v>4.0000000000000002E-4</v>
@@ -3659,7 +3655,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
       <c r="B4" s="55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="58">
         <v>8.0000000000000004E-4</v>
@@ -3674,7 +3670,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
       <c r="B5" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="58">
         <v>1.1000000000000001E-3</v>
@@ -3689,7 +3685,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="58">
         <v>1.38E-2</v>
@@ -3704,7 +3700,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="58">
         <v>8.0000000000000002E-3</v>
@@ -3719,7 +3715,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="58">
         <v>0.36699999999999999</v>
@@ -3734,7 +3730,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="B9" s="55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="58">
         <v>0.20499999999999999</v>
@@ -3769,7 +3765,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3785,7 +3781,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="61">
         <v>5.6</v>
@@ -3799,7 +3795,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="61">
         <v>1</v>
@@ -3813,7 +3809,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" s="61">
         <v>1</v>
@@ -3827,7 +3823,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="61">
         <v>1</v>
@@ -3841,7 +3837,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" s="61">
         <v>3.49</v>
@@ -3855,7 +3851,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="61">
         <v>7.17</v>
@@ -3890,7 +3886,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3906,7 +3902,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="61">
         <v>0.24</v>
@@ -3920,7 +3916,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="61">
         <v>0.95</v>
@@ -3935,7 +3931,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="61">
         <v>3</v>
@@ -3949,7 +3945,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="61">
         <v>3.74</v>
@@ -3963,7 +3959,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="61">
         <v>1.5</v>
@@ -3998,7 +3994,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4014,7 +4010,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C36" s="61">
         <v>2.2000000000000002</v>
@@ -4028,7 +4024,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" s="61">
         <v>1.42</v>
@@ -4042,7 +4038,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="61">
         <v>2.14</v>
@@ -4056,7 +4052,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C39" s="61">
         <v>0.66</v>
@@ -4071,7 +4067,7 @@
     <row r="40" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
       <c r="B40" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C40" s="61">
         <v>0.2</v>
@@ -4085,18 +4081,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
-      <c r="B41" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="61">
-        <v>1</v>
-      </c>
-      <c r="D41" s="61">
-        <v>0.5</v>
-      </c>
-      <c r="E41" s="61">
-        <v>1.5</v>
-      </c>
+      <c r="B41" s="60"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="59"/>
@@ -4112,154 +4100,154 @@
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
+    <row r="44" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
     </row>
     <row r="45" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="46" t="s">
-        <v>117</v>
-      </c>
+      <c r="A45" s="51"/>
       <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
+      <c r="C45" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="47" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="46" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" s="47" t="s">
-        <v>23</v>
+      <c r="B46" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="58">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D46" s="58">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E46" s="58">
+        <v>0.27500000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
       <c r="B47" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C47" s="58">
-        <v>2.5999999999999999E-2</v>
+        <v>0.15</v>
       </c>
       <c r="D47" s="58">
-        <v>5.0000000000000001E-3</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E47" s="58">
-        <v>0.27500000000000002</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
       <c r="B48" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C48" s="58">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D48" s="58">
-        <v>3.7999999999999999E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E48" s="58">
-        <v>0.88500000000000001</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
       <c r="B49" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C49" s="58">
-        <v>0.1</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D49" s="58">
-        <v>2.1999999999999999E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E49" s="58">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
       <c r="B50" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C50" s="58">
-        <v>5.2999999999999999E-2</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="D50" s="58">
-        <v>8.0000000000000002E-3</v>
+        <v>0.05</v>
       </c>
       <c r="E50" s="58">
-        <v>0.82699999999999996</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
       <c r="B51" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C51" s="58">
-        <v>0.16200000000000001</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="D51" s="58">
-        <v>0.05</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="E51" s="58">
-        <v>0.86899999999999999</v>
+        <v>0.68600000000000005</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
       <c r="B52" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C52" s="58">
-        <v>0.11700000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="D52" s="58">
-        <v>3.2000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="E52" s="58">
-        <v>0.68600000000000005</v>
+        <v>0.72299999999999998</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
       <c r="B53" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C53" s="58">
-        <v>0.09</v>
+        <v>0.111</v>
       </c>
       <c r="D53" s="58">
-        <v>1.9E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="E53" s="58">
-        <v>0.72299999999999998</v>
+        <v>0.56299999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="51"/>
-      <c r="B54" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="58">
-        <v>0.111</v>
-      </c>
-      <c r="D54" s="58">
-        <v>4.7E-2</v>
-      </c>
-      <c r="E54" s="58">
-        <v>0.56299999999999994</v>
-      </c>
+      <c r="A54" s="57"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
     </row>
     <row r="55" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="57"/>
@@ -4275,27 +4263,34 @@
       <c r="D56" s="57"/>
       <c r="E56" s="57"/>
     </row>
-    <row r="57" spans="1:6" s="56" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="57"/>
+    <row r="57" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>91</v>
+      <c r="C58" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>23</v>
+      <c r="B59" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="58">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D59" s="58">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E59" s="58">
+        <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4314,73 +4309,74 @@
     </row>
     <row r="61" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C61" s="58">
-        <v>3.5999999999999999E-3</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="D61" s="58">
-        <v>2.8999999999999998E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="E61" s="58">
-        <v>4.4000000000000003E-3</v>
+        <v>7.1000000000000004E-3</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C62" s="58">
-        <v>5.7999999999999996E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="D62" s="58">
-        <v>4.7999999999999996E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E62" s="58">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.01E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C63" s="58">
-        <v>8.8000000000000005E-3</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D63" s="58">
-        <v>7.4999999999999997E-3</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="E63" s="58">
-        <v>1.01E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F63" s="59"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C64" s="58">
-        <v>5.8999999999999997E-2</v>
+        <v>0.32300000000000001</v>
       </c>
       <c r="D64" s="58">
-        <v>5.3999999999999999E-2</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="E64" s="58">
-        <v>7.9000000000000001E-2</v>
+        <v>0.432</v>
       </c>
       <c r="F64" s="59"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="C65" s="58">
-        <v>0.32300000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="D65" s="58">
-        <v>0.29599999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="E65" s="58">
-        <v>0.432</v>
+        <v>0.3</v>
       </c>
       <c r="F65" s="59"/>
     </row>
@@ -4389,44 +4385,37 @@
         <v>113</v>
       </c>
       <c r="C66" s="58">
-        <v>0.23</v>
+        <v>0.48780000000000001</v>
       </c>
       <c r="D66" s="58">
-        <v>0.15</v>
+        <v>0.28349999999999997</v>
       </c>
       <c r="E66" s="58">
-        <v>0.3</v>
+        <v>0.8417</v>
       </c>
       <c r="F66" s="59"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C67" s="58">
-        <v>0.48780000000000001</v>
+        <v>2.17</v>
       </c>
       <c r="D67" s="58">
-        <v>0.28349999999999997</v>
+        <v>1.27</v>
       </c>
       <c r="E67" s="58">
-        <v>0.8417</v>
+        <v>3.71</v>
       </c>
       <c r="F67" s="59"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68" s="58">
-        <v>2.17</v>
-      </c>
-      <c r="D68" s="58">
-        <v>1.27</v>
-      </c>
-      <c r="E68" s="58">
-        <v>3.71</v>
-      </c>
+      <c r="A68" s="59"/>
+      <c r="B68" s="60"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="59"/>
       <c r="F68" s="59"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -4436,6 +4425,9 @@
       <c r="D69" s="59"/>
       <c r="E69" s="59"/>
       <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="59"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="59"/>
@@ -4449,19 +4441,23 @@
       <c r="I70" s="59"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="59"/>
-      <c r="B71" s="60"/>
-      <c r="C71" s="59"/>
-      <c r="D71" s="59"/>
-      <c r="E71" s="59"/>
+      <c r="A71" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="F71" s="59"/>
       <c r="G71" s="59"/>
       <c r="H71" s="59"/>
       <c r="I71" s="59"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>94</v>
+      <c r="C72" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="F72" s="59"/>
       <c r="G72" s="59"/>
@@ -4469,32 +4465,35 @@
       <c r="I72" s="59"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C73" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>23</v>
+      <c r="B73" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="63">
+        <v>0.95</v>
+      </c>
+      <c r="D73" s="63">
+        <v>0.8</v>
+      </c>
+      <c r="E73" s="63">
+        <v>0.98</v>
       </c>
       <c r="F73" s="59"/>
-      <c r="G73" s="59"/>
-      <c r="H73" s="59"/>
-      <c r="I73" s="59"/>
+      <c r="G73" s="64"/>
+      <c r="H73" s="64"/>
+      <c r="I73" s="64"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C74" s="63">
-        <v>0.95</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D74" s="63">
-        <v>0.8</v>
+        <v>0.47</v>
       </c>
       <c r="E74" s="63">
-        <v>0.98</v>
+        <v>0.67</v>
       </c>
       <c r="F74" s="59"/>
       <c r="G74" s="64"/>
@@ -4506,46 +4505,46 @@
         <v>96</v>
       </c>
       <c r="C75" s="63">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="D75" s="63">
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="E75" s="63">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="F75" s="59"/>
-      <c r="G75" s="64"/>
-      <c r="H75" s="64"/>
-      <c r="I75" s="64"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C76" s="63">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="D76" s="63">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E76" s="63">
-        <v>0.68</v>
+        <v>5.19</v>
       </c>
       <c r="F76" s="59"/>
+      <c r="G76" s="64"/>
+      <c r="H76" s="64"/>
+      <c r="I76" s="64"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C77" s="63">
-        <v>2.65</v>
+        <v>0.54</v>
       </c>
       <c r="D77" s="63">
-        <v>1.35</v>
+        <v>0.33</v>
       </c>
       <c r="E77" s="63">
-        <v>5.19</v>
+        <v>0.68</v>
       </c>
       <c r="F77" s="59"/>
       <c r="G77" s="64"/>
@@ -4557,13 +4556,13 @@
         <v>99</v>
       </c>
       <c r="C78" s="63">
-        <v>0.54</v>
+        <v>0.9</v>
       </c>
       <c r="D78" s="63">
-        <v>0.33</v>
+        <v>0.82</v>
       </c>
       <c r="E78" s="63">
-        <v>0.68</v>
+        <v>0.93</v>
       </c>
       <c r="F78" s="59"/>
       <c r="G78" s="64"/>
@@ -4572,16 +4571,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="C79" s="63">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="D79" s="63">
-        <v>0.82</v>
+        <v>0.92</v>
       </c>
       <c r="E79" s="63">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="F79" s="59"/>
       <c r="G79" s="64"/>
@@ -4590,16 +4589,16 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C80" s="63">
-        <v>0.95</v>
+        <v>0.73</v>
       </c>
       <c r="D80" s="63">
-        <v>0.92</v>
+        <v>0.65</v>
       </c>
       <c r="E80" s="63">
-        <v>0.97</v>
+        <v>0.8</v>
       </c>
       <c r="F80" s="59"/>
       <c r="G80" s="64"/>
@@ -4608,13 +4607,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="C81" s="63">
-        <v>0.73</v>
+        <v>0.5</v>
       </c>
       <c r="D81" s="63">
-        <v>0.65</v>
+        <v>0.3</v>
       </c>
       <c r="E81" s="63">
         <v>0.8</v>
@@ -4629,93 +4628,93 @@
         <v>101</v>
       </c>
       <c r="C82" s="63">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D82" s="63">
-        <v>0.3</v>
+        <v>0.92</v>
       </c>
       <c r="E82" s="63">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F82" s="59"/>
-      <c r="G82" s="64"/>
-      <c r="H82" s="64"/>
-      <c r="I82" s="64"/>
+      <c r="G82" s="59"/>
+      <c r="H82" s="59"/>
+      <c r="I82" s="59"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C83" s="63">
-        <v>1</v>
-      </c>
-      <c r="D83" s="63">
-        <v>0.92</v>
-      </c>
-      <c r="E83" s="63">
-        <v>1</v>
-      </c>
+      <c r="A83" s="59"/>
+      <c r="B83" s="60"/>
+      <c r="C83" s="59"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="59"/>
       <c r="F83" s="59"/>
       <c r="G83" s="59"/>
       <c r="H83" s="59"/>
       <c r="I83" s="59"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="59"/>
-      <c r="B84" s="60"/>
-      <c r="C84" s="59"/>
-      <c r="D84" s="59"/>
-      <c r="E84" s="59"/>
-      <c r="F84" s="59"/>
-      <c r="G84" s="59"/>
-      <c r="H84" s="59"/>
+      <c r="A84" s="65"/>
+      <c r="B84" s="66"/>
+      <c r="C84" s="67"/>
+      <c r="D84" s="67"/>
+      <c r="E84" s="67"/>
+      <c r="F84" s="67"/>
+      <c r="G84" s="67"/>
+      <c r="H84" s="67"/>
       <c r="I84" s="59"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="65"/>
+      <c r="A85" s="67"/>
       <c r="B85" s="66"/>
-      <c r="C85" s="67"/>
-      <c r="D85" s="67"/>
-      <c r="E85" s="67"/>
+      <c r="C85" s="68"/>
+      <c r="D85" s="68"/>
+      <c r="E85" s="68"/>
       <c r="F85" s="67"/>
       <c r="G85" s="67"/>
       <c r="H85" s="67"/>
       <c r="I85" s="59"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="67"/>
-      <c r="B86" s="66"/>
-      <c r="C86" s="68"/>
-      <c r="D86" s="68"/>
-      <c r="E86" s="68"/>
-      <c r="F86" s="67"/>
-      <c r="G86" s="67"/>
-      <c r="H86" s="67"/>
-      <c r="I86" s="59"/>
+      <c r="A86" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="45"/>
+      <c r="C86" s="45"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="45"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="45"/>
+      <c r="H86" s="45"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="48" t="s">
-        <v>103</v>
-      </c>
+      <c r="A87" s="45"/>
       <c r="B87" s="45"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="45"/>
+      <c r="C87" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D87" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E87" s="49" t="s">
+        <v>23</v>
+      </c>
       <c r="F87" s="45"/>
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="45"/>
-      <c r="B88" s="45"/>
-      <c r="C88" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="D88" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E88" s="49" t="s">
-        <v>23</v>
+      <c r="B88" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C88" s="61">
+        <v>7.8E-2</v>
+      </c>
+      <c r="D88" s="61">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E88" s="61">
+        <v>0.111</v>
       </c>
       <c r="F88" s="45"/>
       <c r="G88" s="45"/>
@@ -4726,14 +4725,14 @@
       <c r="B89" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="C89" s="83">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="D89" s="83">
-        <v>0.121</v>
-      </c>
-      <c r="E89" s="83">
-        <v>0.249</v>
+      <c r="C89" s="61">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D89" s="61">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E89" s="61">
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F89" s="45"/>
       <c r="G89" s="45"/>
@@ -4744,14 +4743,14 @@
       <c r="B90" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="C90" s="83">
-        <v>0.01</v>
-      </c>
-      <c r="D90" s="83">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E90" s="83">
-        <v>1.4E-2</v>
+      <c r="C90" s="61">
+        <v>0.02</v>
+      </c>
+      <c r="D90" s="61">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E90" s="61">
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F90" s="45"/>
       <c r="G90" s="45"/>
@@ -4762,14 +4761,14 @@
       <c r="B91" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C91" s="83">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D91" s="83">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="E91" s="83">
-        <v>3.5000000000000003E-2</v>
+      <c r="C91" s="61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D91" s="61">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E91" s="61">
+        <v>9.4E-2</v>
       </c>
       <c r="F91" s="45"/>
       <c r="G91" s="45"/>
@@ -4780,14 +4779,14 @@
       <c r="B92" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="C92" s="83">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="D92" s="83">
-        <v>5.5E-2</v>
-      </c>
-      <c r="E92" s="83">
-        <v>0.107</v>
+      <c r="C92" s="61">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D92" s="61">
+        <v>0.114</v>
+      </c>
+      <c r="E92" s="61">
+        <v>0.47399999999999998</v>
       </c>
       <c r="F92" s="45"/>
       <c r="G92" s="45"/>
@@ -4798,14 +4797,14 @@
       <c r="B93" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="C93" s="83">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="D93" s="83">
-        <v>0.128</v>
-      </c>
-      <c r="E93" s="83">
-        <v>0.499</v>
+      <c r="C93" s="61">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D93" s="61">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E93" s="61">
+        <v>0.71499999999999997</v>
       </c>
       <c r="F93" s="45"/>
       <c r="G93" s="45"/>
@@ -4816,33 +4815,20 @@
       <c r="B94" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="C94" s="83">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="D94" s="83">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="E94" s="83">
-        <v>0.74299999999999999</v>
+      <c r="C94" s="61">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D94" s="61">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="E94" s="61">
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="F94" s="45"/>
       <c r="G94" s="45"/>
       <c r="H94" s="45"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="45"/>
-      <c r="B95" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C95" s="83">
-        <v>7.8E-2</v>
-      </c>
-      <c r="D95" s="83">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E95" s="83">
-        <v>0.111</v>
-      </c>
       <c r="F95" s="45"/>
       <c r="G95" s="45"/>
       <c r="H95" s="45"/>
@@ -4856,11 +4842,6 @@
       <c r="F97" s="45"/>
       <c r="G97" s="45"/>
       <c r="H97" s="45"/>
-    </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F98" s="45"/>
-      <c r="G98" s="45"/>
-      <c r="H98" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4870,7 +4851,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5048,7 +5028,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5940,7 +5919,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6712,21 +6690,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:Y30"/>
+  <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD22"/>
+      <selection sqref="A1:AZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5">
         <v>2000</v>
       </c>
@@ -6794,7 +6771,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
@@ -6824,10 +6801,10 @@
         <v>24</v>
       </c>
       <c r="Y3" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
@@ -6857,10 +6834,10 @@
         <v>24</v>
       </c>
       <c r="Y4" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
@@ -6890,10 +6867,10 @@
         <v>24</v>
       </c>
       <c r="Y5" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
@@ -6922,10 +6899,10 @@
         <v>24</v>
       </c>
       <c r="Y6" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
@@ -6955,10 +6932,10 @@
         <v>24</v>
       </c>
       <c r="Y7" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
@@ -6988,17 +6965,18 @@
         <v>24</v>
       </c>
       <c r="Y8" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>2000</v>
       </c>
@@ -7066,207 +7044,211 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>7</v>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="str">
+        <f>Populations!$C$3</f>
+        <v>FSW</v>
       </c>
       <c r="C14" s="16"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="80">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="N14" s="80"/>
-      <c r="O14" s="80"/>
-      <c r="P14" s="80"/>
-      <c r="Q14" s="80"/>
-      <c r="R14" s="80"/>
-      <c r="S14" s="80"/>
-      <c r="T14" s="80"/>
-      <c r="U14" s="80"/>
-      <c r="V14" s="80"/>
-      <c r="W14" s="80"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
       <c r="X14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y14" s="16"/>
-    </row>
-    <row r="15" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="82"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="82"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="82"/>
-      <c r="T15" s="82"/>
-      <c r="U15" s="82"/>
-      <c r="V15" s="82"/>
-      <c r="W15" s="82"/>
+      <c r="Y14" s="16">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="str">
+        <f>Populations!$C$4</f>
+        <v>Clients</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
       <c r="X15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y15" s="81">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="N16" s="82"/>
-      <c r="O16" s="82"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="82"/>
-      <c r="R16" s="82"/>
-      <c r="S16" s="82"/>
-      <c r="T16" s="82"/>
-      <c r="U16" s="82"/>
-      <c r="V16" s="82"/>
-      <c r="W16" s="82"/>
+      <c r="Y15" s="16">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
       <c r="X16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y16" s="81"/>
-    </row>
-    <row r="17" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y16" s="16">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="82"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="82"/>
-      <c r="R17" s="82"/>
-      <c r="S17" s="82"/>
-      <c r="T17" s="82"/>
-      <c r="U17" s="82"/>
-      <c r="V17" s="82"/>
-      <c r="W17" s="82"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
       <c r="X17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y17" s="81">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="82"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="82"/>
-      <c r="T18" s="82"/>
-      <c r="U18" s="82"/>
-      <c r="V18" s="82"/>
-      <c r="W18" s="82"/>
+      <c r="Y17" s="16">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="str">
+        <f>Populations!$C$7</f>
+        <v>M 15+</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
       <c r="X18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y18" s="81">
+      <c r="Y18" s="16">
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="82"/>
-      <c r="S19" s="82"/>
-      <c r="T19" s="82"/>
-      <c r="U19" s="82"/>
-      <c r="V19" s="82"/>
-      <c r="W19" s="82"/>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="str">
+        <f>Populations!$C$8</f>
+        <v>F 15+</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
       <c r="X19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y19" s="81">
+      <c r="Y19" s="16">
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="5">
         <v>2000</v>
       </c>
@@ -7334,202 +7316,470 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="str">
+    <row r="25" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="80">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N25" s="80"/>
+      <c r="O25" s="80"/>
+      <c r="P25" s="80"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="80"/>
+      <c r="S25" s="80"/>
+      <c r="T25" s="80"/>
+      <c r="U25" s="80"/>
+      <c r="V25" s="80"/>
+      <c r="W25" s="80"/>
+      <c r="X25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y25" s="16"/>
+    </row>
+    <row r="26" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="81"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
+      <c r="N26" s="82"/>
+      <c r="O26" s="82"/>
+      <c r="P26" s="82"/>
+      <c r="Q26" s="82"/>
+      <c r="R26" s="82"/>
+      <c r="S26" s="82"/>
+      <c r="T26" s="82"/>
+      <c r="U26" s="82"/>
+      <c r="V26" s="82"/>
+      <c r="W26" s="82"/>
+      <c r="X26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y26" s="81">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="81"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N27" s="82"/>
+      <c r="O27" s="82"/>
+      <c r="P27" s="82"/>
+      <c r="Q27" s="82"/>
+      <c r="R27" s="82"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="82"/>
+      <c r="U27" s="82"/>
+      <c r="V27" s="82"/>
+      <c r="W27" s="82"/>
+      <c r="X27" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y27" s="81"/>
+    </row>
+    <row r="28" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="81"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="82"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="82"/>
+      <c r="S28" s="82"/>
+      <c r="T28" s="82"/>
+      <c r="U28" s="82"/>
+      <c r="V28" s="82"/>
+      <c r="W28" s="82"/>
+      <c r="X28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y28" s="81">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="81"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="82"/>
+      <c r="N29" s="82"/>
+      <c r="O29" s="82"/>
+      <c r="P29" s="82"/>
+      <c r="Q29" s="82"/>
+      <c r="R29" s="82"/>
+      <c r="S29" s="82"/>
+      <c r="T29" s="82"/>
+      <c r="U29" s="82"/>
+      <c r="V29" s="82"/>
+      <c r="W29" s="82"/>
+      <c r="X29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y29" s="81">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="82"/>
+      <c r="N30" s="82"/>
+      <c r="O30" s="82"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="82"/>
+      <c r="R30" s="82"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="82"/>
+      <c r="V30" s="82"/>
+      <c r="W30" s="82"/>
+      <c r="X30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y30" s="81">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="C35" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D35" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F35" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G35" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H35" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I35" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J35" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K35" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L35" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M35" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N35" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O35" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P35" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R35" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S35" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T35" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U35" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V35" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W35" s="5">
+        <v>2020</v>
+      </c>
+      <c r="Y35" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="str">
         <f>Populations!$C$3</f>
         <v>FSW</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16">
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y25" s="16"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="str">
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y36" s="16"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="str">
         <f>Populations!$C$4</f>
         <v>Clients</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16">
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y26" s="16"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="str">
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y37" s="16"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="str">
         <f>Populations!$C$5</f>
         <v>MSM</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16">
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y27" s="16"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y38" s="16"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16">
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y28" s="16"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="str">
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y39" s="16"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="str">
         <f>Populations!$C$7</f>
         <v>M 15+</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y29" s="16"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="str">
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y40" s="16"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="str">
         <f>Populations!$C$8</f>
         <v>F 15+</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16">
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y30" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y41" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7539,11 +7789,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:AZ42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8088,7 +8337,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -8358,7 +8607,7 @@
     </row>
     <row r="35" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -9030,7 +9279,6 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Y93"/>
   <sheetViews>
     <sheetView topLeftCell="A62" workbookViewId="0">
@@ -10460,7 +10708,7 @@
     <row r="56" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="70" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -10632,7 +10880,7 @@
     <row r="64" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="70" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -10804,7 +11052,7 @@
     <row r="72" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="70" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -10976,7 +11224,7 @@
     <row r="80" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="81" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="70" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -11144,7 +11392,7 @@
     <row r="88" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="89" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="70" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -11319,18 +11567,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:AZ45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -11424,7 +11671,7 @@
       <c r="P3" s="23"/>
       <c r="Q3" s="23"/>
       <c r="R3" s="69">
-        <v>1</v>
+        <v>0.9063462346100909</v>
       </c>
       <c r="S3" s="23"/>
       <c r="T3" s="23"/>
@@ -11458,7 +11705,7 @@
       <c r="P4" s="23"/>
       <c r="Q4" s="23"/>
       <c r="R4" s="69">
-        <v>1</v>
+        <v>0.9063462346100909</v>
       </c>
       <c r="S4" s="23"/>
       <c r="T4" s="23"/>
@@ -11491,7 +11738,7 @@
       <c r="P5" s="23"/>
       <c r="Q5" s="23"/>
       <c r="R5" s="69">
-        <v>1</v>
+        <v>0.9063462346100909</v>
       </c>
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
@@ -11523,7 +11770,7 @@
       <c r="P6" s="23"/>
       <c r="Q6" s="23"/>
       <c r="R6" s="69">
-        <v>1</v>
+        <v>0.9063462346100909</v>
       </c>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
@@ -11557,7 +11804,7 @@
       <c r="P7" s="23"/>
       <c r="Q7" s="23"/>
       <c r="R7" s="69">
-        <v>1</v>
+        <v>0.9063462346100909</v>
       </c>
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
@@ -11591,7 +11838,7 @@
       <c r="P8" s="23"/>
       <c r="Q8" s="23"/>
       <c r="R8" s="69">
-        <v>1</v>
+        <v>0.9063462346100909</v>
       </c>
       <c r="S8" s="23"/>
       <c r="T8" s="23"/>
@@ -11608,7 +11855,7 @@
     </row>
     <row r="12" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -12091,7 +12338,7 @@
     </row>
     <row r="29" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -12304,7 +12551,7 @@
     </row>
     <row r="35" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -12763,7 +13010,7 @@
     </row>
     <row r="52" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B52" s="34"/>
       <c r="C52" s="34"/>
@@ -12901,7 +13148,7 @@
     <row r="57" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:25" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B58" s="34"/>
       <c r="C58" s="34"/>
@@ -13043,11 +13290,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:AZ81"/>
+  <dimension ref="A1:AZ83"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="Y81" sqref="Y81"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77:AZ83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14690,7 +14936,7 @@
     </row>
     <row r="67" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:52" x14ac:dyDescent="0.25">
@@ -14892,132 +15138,34 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B76" s="44"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="44"/>
-      <c r="G76" s="44"/>
-      <c r="H76" s="44"/>
-      <c r="I76" s="44"/>
-      <c r="J76" s="44"/>
-      <c r="K76" s="44"/>
-      <c r="L76" s="44"/>
-      <c r="M76" s="44"/>
-      <c r="N76" s="44"/>
-      <c r="O76" s="44"/>
-      <c r="P76" s="44"/>
-      <c r="Q76" s="44"/>
-      <c r="R76" s="44"/>
-      <c r="S76" s="44"/>
-      <c r="T76" s="44"/>
-      <c r="U76" s="44"/>
-      <c r="V76" s="44"/>
-      <c r="W76" s="44"/>
-      <c r="X76" s="44"/>
-      <c r="Y76" s="44"/>
-      <c r="Z76" s="44"/>
-      <c r="AA76" s="44"/>
-      <c r="AB76" s="44"/>
-      <c r="AC76" s="44"/>
-      <c r="AD76" s="44"/>
-      <c r="AE76" s="44"/>
-      <c r="AF76" s="44"/>
-      <c r="AG76" s="44"/>
-      <c r="AH76" s="44"/>
-      <c r="AI76" s="44"/>
-      <c r="AJ76" s="44"/>
-      <c r="AK76" s="44"/>
-      <c r="AL76" s="44"/>
-      <c r="AM76" s="44"/>
-      <c r="AN76" s="44"/>
-      <c r="AO76" s="44"/>
-      <c r="AP76" s="44"/>
-      <c r="AQ76" s="44"/>
-      <c r="AR76" s="44"/>
-      <c r="AS76" s="44"/>
-      <c r="AT76" s="44"/>
-      <c r="AU76" s="44"/>
-      <c r="AV76" s="44"/>
-      <c r="AW76" s="44"/>
-      <c r="AX76" s="44"/>
-      <c r="AY76" s="44"/>
-      <c r="AZ76" s="44"/>
-    </row>
     <row r="77" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
+      <c r="A77" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="B77" s="44"/>
-      <c r="C77" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D77" s="5">
-        <v>2001</v>
-      </c>
-      <c r="E77" s="5">
-        <v>2002</v>
-      </c>
-      <c r="F77" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G77" s="5">
-        <v>2004</v>
-      </c>
-      <c r="H77" s="5">
-        <v>2005</v>
-      </c>
-      <c r="I77" s="5">
-        <v>2006</v>
-      </c>
-      <c r="J77" s="5">
-        <v>2007</v>
-      </c>
-      <c r="K77" s="5">
-        <v>2008</v>
-      </c>
-      <c r="L77" s="5">
-        <v>2009</v>
-      </c>
-      <c r="M77" s="5">
-        <v>2010</v>
-      </c>
-      <c r="N77" s="5">
-        <v>2011</v>
-      </c>
-      <c r="O77" s="5">
-        <v>2012</v>
-      </c>
-      <c r="P77" s="5">
-        <v>2013</v>
-      </c>
-      <c r="Q77" s="5">
-        <v>2014</v>
-      </c>
-      <c r="R77" s="5">
-        <v>2015</v>
-      </c>
-      <c r="S77" s="5">
-        <v>2016</v>
-      </c>
-      <c r="T77" s="5">
-        <v>2017</v>
-      </c>
-      <c r="U77" s="5">
-        <v>2018</v>
-      </c>
-      <c r="V77" s="5">
-        <v>2019</v>
-      </c>
-      <c r="W77" s="5">
-        <v>2020</v>
-      </c>
+      <c r="C77" s="44"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="44"/>
+      <c r="I77" s="44"/>
+      <c r="J77" s="44"/>
+      <c r="K77" s="44"/>
+      <c r="L77" s="44"/>
+      <c r="M77" s="44"/>
+      <c r="N77" s="44"/>
+      <c r="O77" s="44"/>
+      <c r="P77" s="44"/>
+      <c r="Q77" s="44"/>
+      <c r="R77" s="44"/>
+      <c r="S77" s="44"/>
+      <c r="T77" s="44"/>
+      <c r="U77" s="44"/>
+      <c r="V77" s="44"/>
+      <c r="W77" s="44"/>
       <c r="X77" s="44"/>
-      <c r="Y77" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="Y77" s="44"/>
       <c r="Z77" s="44"/>
       <c r="AA77" s="44"/>
       <c r="AB77" s="44"/>
@@ -15048,36 +15196,73 @@
     </row>
     <row r="78" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A78" s="44"/>
-      <c r="B78" s="5" t="str">
-        <f>Populations!$C$4</f>
-        <v>Clients</v>
-      </c>
-      <c r="C78" s="19"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="19"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="19"/>
-      <c r="J78" s="19"/>
-      <c r="K78" s="19"/>
-      <c r="L78" s="19"/>
-      <c r="M78" s="19"/>
-      <c r="N78" s="19"/>
-      <c r="O78" s="19"/>
-      <c r="P78" s="19"/>
-      <c r="Q78" s="19"/>
-      <c r="R78" s="19"/>
-      <c r="S78" s="19"/>
-      <c r="T78" s="19"/>
-      <c r="U78" s="19"/>
-      <c r="V78" s="19"/>
-      <c r="W78" s="19"/>
-      <c r="X78" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y78" s="20">
-        <v>0</v>
+      <c r="B78" s="44"/>
+      <c r="C78" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D78" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E78" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F78" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G78" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H78" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I78" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J78" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K78" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L78" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M78" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N78" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O78" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P78" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q78" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R78" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S78" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T78" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U78" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V78" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W78" s="5">
+        <v>2020</v>
+      </c>
+      <c r="X78" s="44"/>
+      <c r="Y78" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="Z78" s="44"/>
       <c r="AA78" s="44"/>
@@ -15110,8 +15295,8 @@
     <row r="79" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A79" s="44"/>
       <c r="B79" s="5" t="str">
-        <f>Populations!$C$5</f>
-        <v>MSM</v>
+        <f>Populations!$C$4</f>
+        <v>Clients</v>
       </c>
       <c r="C79" s="19"/>
       <c r="D79" s="19"/>
@@ -15137,8 +15322,8 @@
       <c r="X79" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y79" s="20">
-        <v>0</v>
+      <c r="Y79" s="19">
+        <v>0.06</v>
       </c>
       <c r="Z79" s="44"/>
       <c r="AA79" s="44"/>
@@ -15170,8 +15355,9 @@
     </row>
     <row r="80" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A80" s="44"/>
-      <c r="B80" s="5" t="s">
-        <v>15</v>
+      <c r="B80" s="5" t="str">
+        <f>Populations!$C$5</f>
+        <v>MSM</v>
       </c>
       <c r="C80" s="19"/>
       <c r="D80" s="19"/>
@@ -15197,8 +15383,8 @@
       <c r="X80" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y80" s="20">
-        <v>0</v>
+      <c r="Y80" s="19">
+        <v>0.06</v>
       </c>
       <c r="Z80" s="44"/>
       <c r="AA80" s="44"/>
@@ -15230,9 +15416,8 @@
     </row>
     <row r="81" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A81" s="44"/>
-      <c r="B81" s="5" t="str">
-        <f>Populations!$C$7</f>
-        <v>M 15+</v>
+      <c r="B81" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C81" s="19"/>
       <c r="D81" s="19"/>
@@ -15258,8 +15443,8 @@
       <c r="X81" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Y81" s="20">
-        <v>0</v>
+      <c r="Y81" s="19">
+        <v>0.06</v>
       </c>
       <c r="Z81" s="44"/>
       <c r="AA81" s="44"/>
@@ -15289,6 +15474,121 @@
       <c r="AY81" s="44"/>
       <c r="AZ81" s="44"/>
     </row>
+    <row r="82" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A82" s="44"/>
+      <c r="B82" s="5" t="str">
+        <f>Populations!$C$7</f>
+        <v>M 15+</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="19"/>
+      <c r="J82" s="19"/>
+      <c r="K82" s="19"/>
+      <c r="L82" s="19"/>
+      <c r="M82" s="19"/>
+      <c r="N82" s="19"/>
+      <c r="O82" s="19"/>
+      <c r="P82" s="19"/>
+      <c r="Q82" s="19"/>
+      <c r="R82" s="19"/>
+      <c r="S82" s="19"/>
+      <c r="T82" s="19"/>
+      <c r="U82" s="19"/>
+      <c r="V82" s="19"/>
+      <c r="W82" s="19"/>
+      <c r="X82" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y82" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="Z82" s="44"/>
+      <c r="AA82" s="44"/>
+      <c r="AB82" s="44"/>
+      <c r="AC82" s="44"/>
+      <c r="AD82" s="44"/>
+      <c r="AE82" s="44"/>
+      <c r="AF82" s="44"/>
+      <c r="AG82" s="44"/>
+      <c r="AH82" s="44"/>
+      <c r="AI82" s="44"/>
+      <c r="AJ82" s="44"/>
+      <c r="AK82" s="44"/>
+      <c r="AL82" s="44"/>
+      <c r="AM82" s="44"/>
+      <c r="AN82" s="44"/>
+      <c r="AO82" s="44"/>
+      <c r="AP82" s="44"/>
+      <c r="AQ82" s="44"/>
+      <c r="AR82" s="44"/>
+      <c r="AS82" s="44"/>
+      <c r="AT82" s="44"/>
+      <c r="AU82" s="44"/>
+      <c r="AV82" s="44"/>
+      <c r="AW82" s="44"/>
+      <c r="AX82" s="44"/>
+      <c r="AY82" s="44"/>
+      <c r="AZ82" s="44"/>
+    </row>
+    <row r="83" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="44"/>
+      <c r="L83" s="44"/>
+      <c r="M83" s="44"/>
+      <c r="N83" s="44"/>
+      <c r="O83" s="44"/>
+      <c r="P83" s="44"/>
+      <c r="Q83" s="44"/>
+      <c r="R83" s="44"/>
+      <c r="S83" s="44"/>
+      <c r="T83" s="44"/>
+      <c r="U83" s="44"/>
+      <c r="V83" s="44"/>
+      <c r="W83" s="44"/>
+      <c r="X83" s="44"/>
+      <c r="Y83" s="44"/>
+      <c r="Z83" s="44"/>
+      <c r="AA83" s="44"/>
+      <c r="AB83" s="44"/>
+      <c r="AC83" s="44"/>
+      <c r="AD83" s="44"/>
+      <c r="AE83" s="44"/>
+      <c r="AF83" s="44"/>
+      <c r="AG83" s="44"/>
+      <c r="AH83" s="44"/>
+      <c r="AI83" s="44"/>
+      <c r="AJ83" s="44"/>
+      <c r="AK83" s="44"/>
+      <c r="AL83" s="44"/>
+      <c r="AM83" s="44"/>
+      <c r="AN83" s="44"/>
+      <c r="AO83" s="44"/>
+      <c r="AP83" s="44"/>
+      <c r="AQ83" s="44"/>
+      <c r="AR83" s="44"/>
+      <c r="AS83" s="44"/>
+      <c r="AT83" s="44"/>
+      <c r="AU83" s="44"/>
+      <c r="AV83" s="44"/>
+      <c r="AW83" s="44"/>
+      <c r="AX83" s="44"/>
+      <c r="AY83" s="44"/>
+      <c r="AZ83" s="44"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>